<commit_message>
- Updated milestone tracking, now in both Open Office and Excel formats.
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="129">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -221,7 +221,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">01/31/2021
 </t>
@@ -232,7 +231,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(run on 02/04/2021)</t>
     </r>
@@ -245,7 +243,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">02/07/2021
 </t>
@@ -256,7 +253,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(run on 02/08/2021)</t>
     </r>
@@ -269,7 +265,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">02/21/2021
 </t>
@@ -280,7 +275,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(run on 02/22/2021)</t>
     </r>
@@ -293,7 +287,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">03/07/2021
 </t>
@@ -304,7 +297,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(some results on 03/08/2021)</t>
     </r>
@@ -317,7 +309,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">03/14/2021
 </t>
@@ -328,7 +319,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(run on 03/17/2021)</t>
     </r>
@@ -341,7 +331,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">04/11/2021
 </t>
@@ -352,7 +341,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">also 4/12/21)</t>
     </r>
@@ -365,7 +353,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">04/18/2021
 </t>
@@ -376,7 +363,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(run on  4/19/21)</t>
     </r>
@@ -389,7 +375,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">05/16/2021
 </t>
@@ -400,7 +385,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(run on  5/19/21)</t>
     </r>
@@ -413,7 +397,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">05/30/2021
 </t>
@@ -424,7 +407,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(run  on 5/31 
 and 6/1/21)</t>
@@ -464,9 +446,6 @@
   </si>
   <si>
     <t xml:space="preserve">GtkBuilder Added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Parallel</t>
   </si>
   <si>
     <t xml:space="preserve">CardDeck</t>
@@ -625,7 +604,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -647,7 +625,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -655,14 +632,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -670,7 +645,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -678,28 +652,24 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -707,7 +677,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -715,21 +684,18 @@
       <color rgb="FF0000EE"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -737,7 +703,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -746,7 +711,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -754,7 +718,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -762,28 +725,24 @@
       <color rgb="FF444D56"/>
       <name val="Consolas"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -791,7 +750,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -799,14 +757,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1292,15 +1248,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9720</xdr:colOff>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>689400</xdr:colOff>
+      <xdr:colOff>690480</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1313,7 +1269,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2220480" y="11669760"/>
+          <a:off x="2221560" y="11670840"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1329,13 +1285,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9720</xdr:colOff>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>654840</xdr:colOff>
+      <xdr:colOff>655920</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
@@ -1350,7 +1306,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2220480" y="14280120"/>
+          <a:off x="2221560" y="14280120"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1366,13 +1322,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9720</xdr:colOff>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>23400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>497520</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>110</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:to>
@@ -1387,7 +1343,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2220480" y="16575840"/>
+          <a:off x="2221560" y="16575840"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1403,13 +1359,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9360</xdr:colOff>
+      <xdr:colOff>10440</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>23400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>450720</xdr:colOff>
+      <xdr:colOff>451800</xdr:colOff>
       <xdr:row>126</xdr:row>
       <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
@@ -1424,7 +1380,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2220120" y="19730520"/>
+          <a:off x="2221200" y="19730520"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1440,15 +1396,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>38880</xdr:colOff>
+      <xdr:colOff>39960</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>475560</xdr:colOff>
+      <xdr:colOff>476640</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1461,7 +1417,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2249640" y="22513320"/>
+          <a:off x="2250720" y="22514400"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1477,13 +1433,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:colOff>7920</xdr:colOff>
       <xdr:row>143</xdr:row>
       <xdr:rowOff>23400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>882720</xdr:colOff>
+      <xdr:colOff>883800</xdr:colOff>
       <xdr:row>155</xdr:row>
       <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
@@ -1498,7 +1454,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2217600" y="24988320"/>
+          <a:off x="2218680" y="24988320"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1553,13 +1509,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>360360</xdr:colOff>
       <xdr:row>158</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>910440</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1572,7 +1528,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3210120" y="27601920"/>
+          <a:off x="3210120" y="27603000"/>
           <a:ext cx="8718120" cy="1964880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1590,13 +1546,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>209880</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:rowOff>165600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>619920</xdr:colOff>
       <xdr:row>200</xdr:row>
-      <xdr:rowOff>77400</xdr:rowOff>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1609,7 +1565,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3059640" y="32840640"/>
+          <a:off x="3059640" y="32841720"/>
           <a:ext cx="9787680" cy="2191320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1627,13 +1583,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>306720</xdr:colOff>
       <xdr:row>201</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>410040</xdr:colOff>
       <xdr:row>213</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:rowOff>117000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1646,7 +1602,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3156480" y="35239320"/>
+          <a:off x="3156480" y="35240400"/>
           <a:ext cx="9480960" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2658,6 +2614,43 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>8280</xdr:colOff>
+      <xdr:row>585</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1190160</xdr:colOff>
+      <xdr:row>598</xdr:row>
+      <xdr:rowOff>146520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Image 36" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId39"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2219040" y="102438720"/>
+          <a:ext cx="9988920" cy="2415960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2666,10 +2659,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W570"/>
+  <dimension ref="A1:W587"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A568" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2733,11 +2726,11 @@
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>755.97</v>
+        <v>721.07</v>
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>194.38746</v>
+        <v>202.62068</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2749,11 +2742,11 @@
       </c>
       <c r="O6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>214.34</v>
+        <v>206.34</v>
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>82.78609</v>
+        <v>84.56981</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2765,11 +2758,11 @@
       </c>
       <c r="O7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>312.87</v>
+        <v>283.06</v>
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>83.1724</v>
+        <v>82.23518</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,11 +2779,11 @@
       </c>
       <c r="O8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1604.37</v>
+        <v>1564.59</v>
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>368.39365</v>
+        <v>367.02511</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2803,11 +2796,11 @@
       <c r="N9" s="3"/>
       <c r="O9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>153.88</v>
+        <v>154.26</v>
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>47.34358</v>
+        <v>46.60427</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2833,11 +2826,11 @@
       <c r="N11" s="3"/>
       <c r="O11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>129.97843</v>
+        <v>134.45877</v>
       </c>
       <c r="P11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>129.97843</v>
+        <v>134.45877</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2850,11 +2843,11 @@
       <c r="N12" s="3"/>
       <c r="O12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>109.22</v>
+        <v>109.11</v>
       </c>
       <c r="P12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>41.9856</v>
+        <v>44.2461</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2867,11 +2860,11 @@
       <c r="N13" s="3"/>
       <c r="O13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>564.64</v>
+        <v>588.87</v>
       </c>
       <c r="P13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>145.00068</v>
+        <v>156.91935</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2888,11 +2881,11 @@
       </c>
       <c r="O14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>330.4</v>
+        <v>336.18</v>
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>111.97882</v>
+        <v>122.50085</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,11 +2898,11 @@
       </c>
       <c r="O15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>418.45</v>
+        <v>414.92</v>
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>130.95272</v>
+        <v>133.83578</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,11 +2919,11 @@
       </c>
       <c r="O16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>3099.3</v>
+        <v>2672.48</v>
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>635.1125</v>
+        <v>647.08731</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2942,11 +2935,11 @@
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>282.23</v>
+        <v>233.89</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
-        <v>54.4993</v>
+        <v>56.3747</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2958,11 +2951,11 @@
       </c>
       <c r="O18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>700.31</v>
+        <v>679.99</v>
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>184.17036</v>
+        <v>187.68721</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2978,11 +2971,11 @@
       </c>
       <c r="O19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>864.4</v>
+        <v>867.6</v>
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>216.28429</v>
+        <v>222.75538</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2994,11 +2987,11 @@
       </c>
       <c r="O20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>142.58</v>
+        <v>138.85</v>
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>54.75699</v>
+        <v>55.86961</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3010,11 +3003,11 @@
       </c>
       <c r="O21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>476.07</v>
+        <v>461.76</v>
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>148.27171</v>
+        <v>148.24599</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3026,11 +3019,11 @@
       </c>
       <c r="O22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>440.5</v>
+        <v>409.87</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>127.34753</v>
+        <v>132.70001</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3042,11 +3035,11 @@
       </c>
       <c r="O23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>274.58</v>
+        <v>257.73</v>
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>94.24321</v>
+        <v>95.84901</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,11 +3051,11 @@
       </c>
       <c r="O24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>296.43</v>
+        <v>282.56</v>
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>86.45133</v>
+        <v>87.66823</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3075,11 +3068,11 @@
       <c r="N25" s="1"/>
       <c r="O25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>364.39</v>
+        <v>335.87</v>
       </c>
       <c r="P25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>92.84857</v>
+        <v>95.01073</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3091,11 +3084,11 @@
       </c>
       <c r="O26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>909.25</v>
+        <v>802.45</v>
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>236.01994</v>
+        <v>240.82268</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,11 +3100,11 @@
       </c>
       <c r="O27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>204.56</v>
+        <v>181.05</v>
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>50.98505</v>
+        <v>52.09334</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,11 +3116,11 @@
       </c>
       <c r="O28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>466.16</v>
+        <v>424.32</v>
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>120.99359</v>
+        <v>123.55108</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3143,11 +3136,11 @@
       </c>
       <c r="O29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1817.3</v>
+        <v>1731.28</v>
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>440.70349</v>
+        <v>455.05082</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3159,11 +3152,11 @@
       </c>
       <c r="O30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>44.19</v>
+        <v>46.35</v>
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>21.10584</v>
+        <v>22.31878</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3175,11 +3168,11 @@
       </c>
       <c r="O31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>31.9</v>
+        <v>31.52</v>
       </c>
       <c r="P31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>24.54437</v>
+        <v>26.58519</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3191,11 +3184,11 @@
       </c>
       <c r="O32" s="8" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>164.79</v>
+        <v>159.68</v>
       </c>
       <c r="P32" s="8" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>56.19962</v>
+        <v>60.24165</v>
       </c>
       <c r="Q32" s="8"/>
     </row>
@@ -3204,7 +3197,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="4" t="n">
-        <v>8198</v>
+        <v>9529</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
@@ -3324,7 +3317,7 @@
       </c>
       <c r="C47" s="4" t="n">
         <f aca="false">SUM(C4:C45)</f>
-        <v>570557</v>
+        <v>571888</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!A:A)), Miletone_Tracking!A:A)</f>
@@ -3335,11 +3328,11 @@
       </c>
       <c r="O47" s="0" t="n">
         <f aca="false">INDEX(Regular_Timings!34:34,COUNT(Regular_Timings!34:34,1,1))</f>
-        <v>16684.01</v>
+        <v>15688.1</v>
       </c>
       <c r="P47" s="0" t="n">
         <f aca="false">INDEX(Parallel_Timings!34:34,COUNT(Parallel_Timings!34:34,1,1))</f>
-        <v>4087.71284</v>
+        <v>4223.42963</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,7 +3347,7 @@
       </c>
       <c r="P48" s="16" t="n">
         <f aca="false">O47/P47</f>
-        <v>4.08150245700723</v>
+        <v>3.71454040303259</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,6 +3573,11 @@
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S570" s="17" t="n">
         <v>44325</v>
+      </c>
+    </row>
+    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S587" s="17" t="n">
+        <v>44367</v>
       </c>
     </row>
   </sheetData>
@@ -3601,12 +3599,12 @@
   </sheetPr>
   <dimension ref="A2:BK108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="AG5" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AG1" activeCellId="0" sqref="AG1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="P49" activeCellId="0" sqref="P49"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+      <selection pane="bottomRight" activeCell="G49" activeCellId="0" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3729,6 +3727,9 @@
       </c>
       <c r="AI4" s="22" t="n">
         <v>44360</v>
+      </c>
+      <c r="AJ4" s="22" t="n">
+        <v>44367</v>
       </c>
     </row>
     <row r="5" s="18" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3782,6 +3783,9 @@
       <c r="AI5" s="0" t="n">
         <v>1178.67</v>
       </c>
+      <c r="AJ5" s="0" t="n">
+        <v>1132.27</v>
+      </c>
     </row>
     <row r="6" s="10" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="27" t="s">
@@ -3885,6 +3889,9 @@
       <c r="AI6" s="0" t="n">
         <v>755.97</v>
       </c>
+      <c r="AJ6" s="0" t="n">
+        <v>721.07</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
@@ -3989,6 +3996,9 @@
       <c r="AI7" s="0" t="n">
         <v>214.34</v>
       </c>
+      <c r="AJ7" s="0" t="n">
+        <v>206.34</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
@@ -4081,6 +4091,9 @@
       <c r="AI8" s="0" t="n">
         <v>312.87</v>
       </c>
+      <c r="AJ8" s="0" t="n">
+        <v>283.06</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
@@ -4185,6 +4198,9 @@
       <c r="AI9" s="0" t="n">
         <v>1604.37</v>
       </c>
+      <c r="AJ9" s="0" t="n">
+        <v>1564.59</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
@@ -4289,6 +4305,9 @@
       <c r="AI10" s="0" t="n">
         <v>153.88</v>
       </c>
+      <c r="AJ10" s="0" t="n">
+        <v>154.26</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
@@ -4393,6 +4412,9 @@
       <c r="AI11" s="0" t="n">
         <v>462.26</v>
       </c>
+      <c r="AJ11" s="0" t="n">
+        <v>460.18</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
@@ -4470,6 +4492,9 @@
       <c r="AI12" s="0" t="n">
         <v>109.22</v>
       </c>
+      <c r="AJ12" s="0" t="n">
+        <v>109.11</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
@@ -4535,6 +4560,9 @@
       <c r="AI13" s="0" t="n">
         <v>564.64</v>
       </c>
+      <c r="AJ13" s="0" t="n">
+        <v>588.87</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
@@ -4639,6 +4667,9 @@
       <c r="AI14" s="0" t="n">
         <v>330.4</v>
       </c>
+      <c r="AJ14" s="0" t="n">
+        <v>336.18</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
@@ -4743,6 +4774,9 @@
       <c r="AI15" s="0" t="n">
         <v>418.45</v>
       </c>
+      <c r="AJ15" s="0" t="n">
+        <v>414.92</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="27" t="s">
@@ -4847,6 +4881,9 @@
       <c r="AI16" s="0" t="n">
         <v>3099.3</v>
       </c>
+      <c r="AJ16" s="0" t="n">
+        <v>2672.48</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="s">
@@ -4870,6 +4907,9 @@
       <c r="AI17" s="0" t="n">
         <v>282.23</v>
       </c>
+      <c r="AJ17" s="0" t="n">
+        <v>233.89</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="27" t="s">
@@ -4974,6 +5014,9 @@
       <c r="AI18" s="0" t="n">
         <v>700.31</v>
       </c>
+      <c r="AJ18" s="0" t="n">
+        <v>679.99</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="27" t="s">
@@ -5078,6 +5121,9 @@
       <c r="AI19" s="0" t="n">
         <v>864.4</v>
       </c>
+      <c r="AJ19" s="0" t="n">
+        <v>867.6</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="27" t="s">
@@ -5182,6 +5228,9 @@
       <c r="AI20" s="0" t="n">
         <v>142.58</v>
       </c>
+      <c r="AJ20" s="0" t="n">
+        <v>138.85</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="27" t="s">
@@ -5286,6 +5335,9 @@
       <c r="AI21" s="0" t="n">
         <v>476.07</v>
       </c>
+      <c r="AJ21" s="0" t="n">
+        <v>461.76</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="27" t="s">
@@ -5390,6 +5442,9 @@
       <c r="AI22" s="0" t="n">
         <v>440.5</v>
       </c>
+      <c r="AJ22" s="0" t="n">
+        <v>409.87</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="27" t="s">
@@ -5494,6 +5549,9 @@
       <c r="AI23" s="0" t="n">
         <v>274.58</v>
       </c>
+      <c r="AJ23" s="0" t="n">
+        <v>257.73</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="s">
@@ -5598,6 +5656,9 @@
       <c r="AI24" s="0" t="n">
         <v>296.43</v>
       </c>
+      <c r="AJ24" s="0" t="n">
+        <v>282.56</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="s">
@@ -5702,6 +5763,9 @@
       <c r="AI25" s="0" t="n">
         <v>364.39</v>
       </c>
+      <c r="AJ25" s="0" t="n">
+        <v>335.87</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="s">
@@ -5806,6 +5870,9 @@
       <c r="AI26" s="0" t="n">
         <v>909.25</v>
       </c>
+      <c r="AJ26" s="0" t="n">
+        <v>802.45</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27" t="s">
@@ -5910,6 +5977,9 @@
       <c r="AI27" s="0" t="n">
         <v>204.56</v>
       </c>
+      <c r="AJ27" s="0" t="n">
+        <v>181.05</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="27" t="s">
@@ -5960,6 +6030,9 @@
       <c r="AI28" s="0" t="n">
         <v>466.16</v>
       </c>
+      <c r="AJ28" s="0" t="n">
+        <v>424.32</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="27" t="s">
@@ -6064,6 +6137,9 @@
       <c r="AI29" s="0" t="n">
         <v>1817.3</v>
       </c>
+      <c r="AJ29" s="0" t="n">
+        <v>1731.28</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="27" t="s">
@@ -6168,6 +6244,9 @@
       <c r="AI30" s="0" t="n">
         <v>44.19</v>
       </c>
+      <c r="AJ30" s="0" t="n">
+        <v>46.35</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="29" t="s">
@@ -6272,6 +6351,9 @@
       <c r="AI31" s="0" t="n">
         <v>31.9</v>
       </c>
+      <c r="AJ31" s="0" t="n">
+        <v>31.52</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
@@ -6376,6 +6458,9 @@
       <c r="AI32" s="0" t="n">
         <v>164.79</v>
       </c>
+      <c r="AJ32" s="0" t="n">
+        <v>159.68</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -6513,8 +6598,12 @@
         <f aca="false">SUM(AI$5:AI$32)</f>
         <v>16684.01</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AJ34" s="0" t="n">
+        <f aca="false">SUM(AJ$5:AJ$32)</f>
+        <v>15688.1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
         <v>74</v>
       </c>
@@ -6646,6 +6735,10 @@
       <c r="AI35" s="31" t="n">
         <f aca="false">AI34/AH34</f>
         <v>1.04927844854803</v>
+      </c>
+      <c r="AJ35" s="31" t="n">
+        <f aca="false">AJ34/AI34</f>
+        <v>0.940307515998851</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6679,320 +6772,144 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O48" s="0" t="s">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E49" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E50" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E51" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E52" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E55" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E56" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E63" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E64" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E66" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E69" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E71" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E72" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E74" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="P48" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N49" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="O49" s="0" t="n">
-        <v>1178.67</v>
-      </c>
-      <c r="P49" s="0" t="n">
-        <v>242.91251</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N50" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="O50" s="0" t="n">
-        <v>755.97</v>
-      </c>
-      <c r="P50" s="0" t="n">
-        <v>194.38746</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N51" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="O51" s="0" t="n">
-        <v>214.34</v>
-      </c>
-      <c r="P51" s="0" t="n">
-        <v>82.78609</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N52" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="O52" s="0" t="n">
-        <v>312.87</v>
-      </c>
-      <c r="P52" s="0" t="n">
-        <v>83.1724</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N53" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="O53" s="0" t="n">
-        <v>1604.37</v>
-      </c>
-      <c r="P53" s="0" t="n">
-        <v>368.39365</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N54" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="O54" s="0" t="n">
-        <v>153.88</v>
-      </c>
-      <c r="P54" s="0" t="n">
-        <v>47.34358</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N55" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="O55" s="0" t="n">
-        <v>462.26</v>
-      </c>
-      <c r="P55" s="0" t="n">
-        <v>129.97843</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N56" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="O56" s="0" t="n">
-        <v>109.22</v>
-      </c>
-      <c r="P56" s="0" t="n">
-        <v>41.9856</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N57" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="O57" s="0" t="n">
-        <v>564.64</v>
-      </c>
-      <c r="P57" s="0" t="n">
-        <v>145.00068</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N58" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="O58" s="0" t="n">
-        <v>330.4</v>
-      </c>
-      <c r="P58" s="0" t="n">
-        <v>111.97882</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N59" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="O59" s="0" t="n">
-        <v>418.45</v>
-      </c>
-      <c r="P59" s="0" t="n">
-        <v>130.95272</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N60" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="O60" s="0" t="n">
-        <v>3099.3</v>
-      </c>
-      <c r="P60" s="0" t="n">
-        <v>635.1125</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N61" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="O61" s="0" t="n">
-        <v>282.23</v>
-      </c>
-      <c r="P61" s="0" t="n">
-        <v>54.4993</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N62" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="O62" s="0" t="n">
-        <v>700.31</v>
-      </c>
-      <c r="P62" s="0" t="n">
-        <v>184.17036</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N63" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="O63" s="0" t="n">
-        <v>864.4</v>
-      </c>
-      <c r="P63" s="0" t="n">
-        <v>216.28429</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N64" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="O64" s="0" t="n">
-        <v>142.58</v>
-      </c>
-      <c r="P64" s="0" t="n">
-        <v>54.75699</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N65" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O65" s="0" t="n">
-        <v>476.07</v>
-      </c>
-      <c r="P65" s="0" t="n">
-        <v>148.27171</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N66" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="O66" s="0" t="n">
-        <v>440.5</v>
-      </c>
-      <c r="P66" s="0" t="n">
-        <v>127.34753</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N67" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="O67" s="0" t="n">
-        <v>274.58</v>
-      </c>
-      <c r="P67" s="0" t="n">
-        <v>94.24321</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N68" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="O68" s="0" t="n">
-        <v>296.43</v>
-      </c>
-      <c r="P68" s="0" t="n">
-        <v>86.45133</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N69" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="O69" s="0" t="n">
-        <v>364.39</v>
-      </c>
-      <c r="P69" s="0" t="n">
-        <v>92.84857</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N70" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O70" s="0" t="n">
-        <v>909.25</v>
-      </c>
-      <c r="P70" s="0" t="n">
-        <v>236.01994</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N71" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O71" s="0" t="n">
-        <v>204.56</v>
-      </c>
-      <c r="P71" s="0" t="n">
-        <v>50.98505</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N72" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="O72" s="0" t="n">
-        <v>466.16</v>
-      </c>
-      <c r="P72" s="0" t="n">
-        <v>120.99359</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N73" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="O73" s="0" t="n">
-        <v>1817.3</v>
-      </c>
-      <c r="P73" s="0" t="n">
-        <v>440.70349</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N74" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="O74" s="0" t="n">
-        <v>44.19</v>
-      </c>
-      <c r="P74" s="0" t="n">
-        <v>21.10584</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N75" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="O75" s="0" t="n">
-        <v>31.9</v>
-      </c>
-      <c r="P75" s="0" t="n">
-        <v>24.54437</v>
-      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N76" s="0" t="s">
+      <c r="E76" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="O76" s="0" t="n">
-        <v>164.79</v>
-      </c>
-      <c r="P76" s="0" t="n">
-        <v>56.19962</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7274,7 +7191,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI107" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BJ107" s="0" t="n">
         <v>27.54</v>
@@ -7310,14 +7227,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AI37"/>
+  <dimension ref="A2:AJ37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AD23" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AD1" activeCellId="0" sqref="AD1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="AK31" activeCellId="0" sqref="AK31"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7339,7 +7256,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" s="37" customFormat="true" ht="43.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="37" customFormat="true" ht="43.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
       <c r="C4" s="35" t="n">
@@ -7437,6 +7354,9 @@
       </c>
       <c r="AI4" s="22" t="n">
         <v>44360</v>
+      </c>
+      <c r="AJ4" s="22" t="n">
+        <v>44367</v>
       </c>
     </row>
     <row r="5" s="37" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7488,6 +7408,9 @@
       <c r="AI5" s="0" t="n">
         <v>242.91251</v>
       </c>
+      <c r="AJ5" s="0" t="n">
+        <v>257.4753</v>
+      </c>
     </row>
     <row r="6" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -7590,6 +7513,9 @@
       <c r="AI6" s="0" t="n">
         <v>194.38746</v>
       </c>
+      <c r="AJ6" s="0" t="n">
+        <v>202.62068</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="29" t="s">
@@ -7691,6 +7617,9 @@
       <c r="AI7" s="0" t="n">
         <v>82.78609</v>
       </c>
+      <c r="AJ7" s="0" t="n">
+        <v>84.56981</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="29" t="s">
@@ -7780,6 +7709,9 @@
       <c r="AI8" s="0" t="n">
         <v>83.1724</v>
       </c>
+      <c r="AJ8" s="0" t="n">
+        <v>82.23518</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="27" t="s">
@@ -7881,6 +7813,9 @@
       <c r="AI9" s="0" t="n">
         <v>368.39365</v>
       </c>
+      <c r="AJ9" s="0" t="n">
+        <v>367.02511</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="29" t="s">
@@ -7982,6 +7917,9 @@
       <c r="AI10" s="0" t="n">
         <v>47.34358</v>
       </c>
+      <c r="AJ10" s="0" t="n">
+        <v>46.60427</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="29" t="s">
@@ -8083,6 +8021,9 @@
       <c r="AI11" s="0" t="n">
         <v>129.97843</v>
       </c>
+      <c r="AJ11" s="0" t="n">
+        <v>134.45877</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="29" t="s">
@@ -8157,6 +8098,9 @@
       <c r="AI12" s="0" t="n">
         <v>41.9856</v>
       </c>
+      <c r="AJ12" s="0" t="n">
+        <v>44.2461</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="29" t="s">
@@ -8219,6 +8163,9 @@
       <c r="AI13" s="0" t="n">
         <v>145.00068</v>
       </c>
+      <c r="AJ13" s="0" t="n">
+        <v>156.91935</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="27" t="s">
@@ -8320,6 +8267,9 @@
       <c r="AI14" s="0" t="n">
         <v>111.97882</v>
       </c>
+      <c r="AJ14" s="0" t="n">
+        <v>122.50085</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="27" t="s">
@@ -8421,6 +8371,9 @@
       <c r="AI15" s="0" t="n">
         <v>130.95272</v>
       </c>
+      <c r="AJ15" s="0" t="n">
+        <v>133.83578</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="27" t="s">
@@ -8521,6 +8474,9 @@
       </c>
       <c r="AI16" s="0" t="n">
         <v>635.1125</v>
+      </c>
+      <c r="AJ16" s="0" t="n">
+        <v>647.08731</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8540,6 +8496,9 @@
       <c r="AI17" s="0" t="n">
         <v>54.4993</v>
       </c>
+      <c r="AJ17" s="0" t="n">
+        <v>56.3747</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="27" t="s">
@@ -8641,6 +8600,9 @@
       <c r="AI18" s="0" t="n">
         <v>184.17036</v>
       </c>
+      <c r="AJ18" s="0" t="n">
+        <v>187.68721</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="27" t="s">
@@ -8742,6 +8704,9 @@
       <c r="AI19" s="0" t="n">
         <v>216.28429</v>
       </c>
+      <c r="AJ19" s="0" t="n">
+        <v>222.75538</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="27" t="s">
@@ -8843,6 +8808,9 @@
       <c r="AI20" s="0" t="n">
         <v>54.75699</v>
       </c>
+      <c r="AJ20" s="0" t="n">
+        <v>55.86961</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="27" t="s">
@@ -8944,6 +8912,9 @@
       <c r="AI21" s="0" t="n">
         <v>148.27171</v>
       </c>
+      <c r="AJ21" s="0" t="n">
+        <v>148.24599</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="27" t="s">
@@ -9045,6 +9016,9 @@
       <c r="AI22" s="0" t="n">
         <v>127.34753</v>
       </c>
+      <c r="AJ22" s="0" t="n">
+        <v>132.70001</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="27" t="s">
@@ -9146,6 +9120,9 @@
       <c r="AI23" s="0" t="n">
         <v>94.24321</v>
       </c>
+      <c r="AJ23" s="0" t="n">
+        <v>95.84901</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="27" t="s">
@@ -9247,6 +9224,9 @@
       <c r="AI24" s="0" t="n">
         <v>86.45133</v>
       </c>
+      <c r="AJ24" s="0" t="n">
+        <v>87.66823</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="27" t="s">
@@ -9348,6 +9328,9 @@
       <c r="AI25" s="0" t="n">
         <v>92.84857</v>
       </c>
+      <c r="AJ25" s="0" t="n">
+        <v>95.01073</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
@@ -9449,6 +9432,9 @@
       <c r="AI26" s="0" t="n">
         <v>236.01994</v>
       </c>
+      <c r="AJ26" s="0" t="n">
+        <v>240.82268</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="27" t="s">
@@ -9550,6 +9536,9 @@
       <c r="AI27" s="0" t="n">
         <v>50.98505</v>
       </c>
+      <c r="AJ27" s="0" t="n">
+        <v>52.09334</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="27" t="s">
@@ -9597,6 +9586,9 @@
       <c r="AI28" s="0" t="n">
         <v>120.99359</v>
       </c>
+      <c r="AJ28" s="0" t="n">
+        <v>123.55108</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="27" t="s">
@@ -9698,6 +9690,9 @@
       <c r="AI29" s="0" t="n">
         <v>440.70349</v>
       </c>
+      <c r="AJ29" s="0" t="n">
+        <v>455.05082</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="27" t="s">
@@ -9799,6 +9794,9 @@
       <c r="AI30" s="0" t="n">
         <v>21.10584</v>
       </c>
+      <c r="AJ30" s="0" t="n">
+        <v>22.31878</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="29" t="s">
@@ -9900,6 +9898,9 @@
       <c r="AI31" s="0" t="n">
         <v>24.54437</v>
       </c>
+      <c r="AJ31" s="0" t="n">
+        <v>26.58519</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="29" t="s">
@@ -10001,6 +10002,9 @@
       <c r="AI32" s="0" t="n">
         <v>56.19962</v>
       </c>
+      <c r="AJ32" s="0" t="n">
+        <v>60.24165</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
@@ -10134,10 +10138,14 @@
         <f aca="false">SUM(AI$5:AI$32)</f>
         <v>4223.42963</v>
       </c>
+      <c r="AJ34" s="0" t="n">
+        <f aca="false">SUM(AJ$5:AJ$32)</f>
+        <v>4342.40292</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" s="42" t="n">
         <f aca="false">1/(C34/Regular_Timings!C34)</f>
@@ -10266,6 +10274,10 @@
       <c r="AI35" s="42" t="n">
         <f aca="false">Regular_Timings!AI34/AI34</f>
         <v>3.95034639182564</v>
+      </c>
+      <c r="AJ35" s="42" t="n">
+        <f aca="false">Regular_Timings!AJ34/AJ34</f>
+        <v>3.61276930976272</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10275,7 +10287,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AC37" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -10296,7 +10308,7 @@
   </sheetPr>
   <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -10312,7 +10324,7 @@
         <v>50</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>38</v>
@@ -10338,182 +10350,182 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="I3" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="Q3" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="T3" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="X3" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="AB3" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AF3" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="AF3" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="T4" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="44" t="s">
         <v>107</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Updated milestone tracking
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -1248,15 +1248,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>10800</xdr:colOff>
+      <xdr:colOff>11520</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:rowOff>26640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>690480</xdr:colOff>
+      <xdr:colOff>691200</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>39960</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1269,7 +1269,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2221560" y="11670840"/>
+          <a:off x="2222280" y="11671560"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1285,13 +1285,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>10800</xdr:colOff>
+      <xdr:colOff>11520</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>6120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>655920</xdr:colOff>
+      <xdr:colOff>656640</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
@@ -1306,7 +1306,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2221560" y="14280120"/>
+          <a:off x="2222280" y="14280120"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1322,13 +1322,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>10800</xdr:colOff>
+      <xdr:colOff>11520</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>23400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>498600</xdr:colOff>
+      <xdr:colOff>499320</xdr:colOff>
       <xdr:row>110</xdr:row>
       <xdr:rowOff>7560</xdr:rowOff>
     </xdr:to>
@@ -1343,7 +1343,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2221560" y="16575840"/>
+          <a:off x="2222280" y="16575840"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1359,13 +1359,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
+      <xdr:colOff>11160</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>23400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>451800</xdr:colOff>
+      <xdr:colOff>452520</xdr:colOff>
       <xdr:row>126</xdr:row>
       <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
@@ -1380,7 +1380,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2221200" y="19730520"/>
+          <a:off x="2221920" y="19730520"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1396,15 +1396,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>39960</xdr:colOff>
+      <xdr:colOff>40680</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>476640</xdr:colOff>
+      <xdr:colOff>477360</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1417,7 +1417,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2250720" y="22514400"/>
+          <a:off x="2251440" y="22515120"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1433,13 +1433,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>143</xdr:row>
       <xdr:rowOff>23400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>883800</xdr:colOff>
+      <xdr:colOff>884520</xdr:colOff>
       <xdr:row>155</xdr:row>
       <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
@@ -1454,7 +1454,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2218680" y="24988320"/>
+          <a:off x="2219400" y="24988320"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1509,13 +1509,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>360360</xdr:colOff>
       <xdr:row>158</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>910440</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1528,7 +1528,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3210120" y="27603000"/>
+          <a:off x="3210120" y="27603720"/>
           <a:ext cx="8718120" cy="1964880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1546,13 +1546,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>209880</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>619920</xdr:colOff>
       <xdr:row>200</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1565,7 +1565,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3059640" y="32841720"/>
+          <a:off x="3059640" y="32842440"/>
           <a:ext cx="9787680" cy="2191320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1583,13 +1583,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>306720</xdr:colOff>
       <xdr:row>201</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>410040</xdr:colOff>
       <xdr:row>213</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1602,7 +1602,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3156480" y="35240400"/>
+          <a:off x="3156480" y="35241120"/>
           <a:ext cx="9480960" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2651,6 +2651,43 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>601</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>41760</xdr:colOff>
+      <xdr:row>615</xdr:row>
+      <xdr:rowOff>160920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Image 37" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId40"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2210760" y="105233760"/>
+          <a:ext cx="10058400" cy="2614680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2659,10 +2696,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W587"/>
+  <dimension ref="A1:W603"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A586" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S615" activeCellId="0" sqref="S615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3197,7 +3234,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="4" t="n">
-        <v>9529</v>
+        <v>10892</v>
       </c>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
@@ -3317,7 +3354,7 @@
       </c>
       <c r="C47" s="4" t="n">
         <f aca="false">SUM(C4:C45)</f>
-        <v>571888</v>
+        <v>573251</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!A:A)), Miletone_Tracking!A:A)</f>
@@ -3578,6 +3615,11 @@
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S587" s="17" t="n">
         <v>44367</v>
+      </c>
+    </row>
+    <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S603" s="17" t="n">
+        <v>44370</v>
       </c>
     </row>
   </sheetData>
@@ -6603,7 +6645,7 @@
         <v>15688.1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="23.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
         <v>74</v>
       </c>
@@ -7229,12 +7271,12 @@
   </sheetPr>
   <dimension ref="A2:AJ37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E30" activeCellId="0" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="AF4" activeCellId="0" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7256,7 +7298,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" s="37" customFormat="true" ht="43.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="37" customFormat="true" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
       <c r="C4" s="35" t="n">

</xml_diff>

<commit_message>
- Updated milestone tracking. Notes 580,000 LOC
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="132">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -58,76 +58,76 @@
     <t xml:space="preserve">JSON-GLib</t>
   </si>
   <si>
+    <t xml:space="preserve">SOUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSSDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUPnP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pango</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GtkPlus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GtkBuilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SourceViewGTK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebkitGTK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMTK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GooCanvas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WNCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GtkClutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Champlain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GStreamer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSVG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CardDecks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICal-GLib</t>
+  </si>
+  <si>
     <t xml:space="preserve">EDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOUP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSSDP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUPnP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pango</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GtkPlus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GtkBuilder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SourceViewGTK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WebkitGTK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMTK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEPL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GooCanvas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slope</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WNCK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COGL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clutter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GtkClutter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Champlain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GStreamer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSVG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CardDecks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICal-GLib</t>
   </si>
   <si>
     <t xml:space="preserve">Sheet</t>
@@ -413,6 +413,28 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">07/04/2021
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">(run  on 7/6/21)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">ICal</t>
   </si>
   <si>
@@ -448,6 +470,9 @@
     <t xml:space="preserve">GtkBuilder Added</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-Parallel</t>
+  </si>
+  <si>
     <t xml:space="preserve">CardDeck</t>
   </si>
   <si>
@@ -584,6 +609,9 @@
   </si>
   <si>
     <t xml:space="preserve">Crossed 570,000 on 06/13/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crossed 580,000 on 07/08/21</t>
   </si>
 </sst>
 </file>
@@ -936,7 +964,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -959,6 +987,10 @@
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1049,10 +1081,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1075,6 +1103,10 @@
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1213,13 +1245,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>738360</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>186480</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1232,7 +1264,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="738360" y="9214920"/>
+          <a:off x="738360" y="9216000"/>
           <a:ext cx="9703800" cy="2053800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1248,15 +1280,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>11520</xdr:colOff>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>26640</xdr:rowOff>
+      <xdr:rowOff>28440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>691200</xdr:colOff>
+      <xdr:colOff>694080</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1269,7 +1301,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2222280" y="11671560"/>
+          <a:off x="2225160" y="11673360"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1285,15 +1317,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>11520</xdr:colOff>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
+      <xdr:colOff>659520</xdr:colOff>
       <xdr:row>93</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1306,7 +1338,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2222280" y="14280120"/>
+          <a:off x="2225160" y="14281200"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1322,15 +1354,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>11520</xdr:colOff>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>499320</xdr:colOff>
+      <xdr:colOff>502200</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1343,7 +1375,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2222280" y="16575840"/>
+          <a:off x="2225160" y="16576920"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1359,15 +1391,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>11160</xdr:colOff>
+      <xdr:colOff>14040</xdr:colOff>
       <xdr:row>113</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>452520</xdr:colOff>
+      <xdr:colOff>455400</xdr:colOff>
       <xdr:row>126</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1380,7 +1412,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2221920" y="19730520"/>
+          <a:off x="2224800" y="19731600"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1396,15 +1428,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>40680</xdr:colOff>
+      <xdr:colOff>43560</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>477360</xdr:colOff>
+      <xdr:colOff>480240</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1417,7 +1449,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2251440" y="22515120"/>
+          <a:off x="2254320" y="22516920"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1433,15 +1465,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>11520</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>884520</xdr:colOff>
+      <xdr:colOff>887400</xdr:colOff>
       <xdr:row>155</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1454,7 +1486,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2219400" y="24988320"/>
+          <a:off x="2222280" y="24989400"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1472,13 +1504,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
       <xdr:row>173</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>595800</xdr:colOff>
       <xdr:row>185</xdr:row>
-      <xdr:rowOff>64800</xdr:rowOff>
+      <xdr:rowOff>65880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1491,7 +1523,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3115080" y="30252240"/>
+          <a:off x="3115080" y="30253320"/>
           <a:ext cx="9708120" cy="2138400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1509,13 +1541,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>360360</xdr:colOff>
       <xdr:row>158</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>910440</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>48960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1528,7 +1560,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3210120" y="27603720"/>
+          <a:off x="3210120" y="27605520"/>
           <a:ext cx="8718120" cy="1964880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1546,13 +1578,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>209880</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:rowOff>168120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>619920</xdr:colOff>
       <xdr:row>200</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1565,7 +1597,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3059640" y="32842440"/>
+          <a:off x="3059640" y="32844240"/>
           <a:ext cx="9787680" cy="2191320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1583,13 +1615,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>306720</xdr:colOff>
       <xdr:row>201</xdr:row>
-      <xdr:rowOff>111240</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>410040</xdr:colOff>
       <xdr:row>213</xdr:row>
-      <xdr:rowOff>117720</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1602,7 +1634,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3156480" y="35241120"/>
+          <a:off x="3156480" y="35242920"/>
           <a:ext cx="9480960" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1620,13 +1652,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>275040</xdr:colOff>
       <xdr:row>214</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>58680</xdr:colOff>
       <xdr:row>225</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1639,7 +1671,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3124800" y="37437840"/>
+          <a:off x="3124800" y="37438920"/>
           <a:ext cx="9161280" cy="2044800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2698,8 +2730,8 @@
   </sheetPr>
   <dimension ref="A1:W603"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A586" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S615" activeCellId="0" sqref="S615"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2726,7 +2758,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="n">
-        <v>44357</v>
+        <v>44385</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>2</v>
@@ -2758,16 +2790,16 @@
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="n">
-        <v>35099</v>
+      <c r="C5" s="6" t="n">
+        <v>35374</v>
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>721.07</v>
+        <v>721.09</v>
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>202.62068</v>
+        <v>201.08922</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2775,15 +2807,15 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>4647</v>
+        <v>4649</v>
       </c>
       <c r="O6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>206.34</v>
+        <v>207.11</v>
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>84.56981</v>
+        <v>85.80095</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2791,15 +2823,15 @@
         <v>8</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>6329</v>
+        <v>6344</v>
       </c>
       <c r="O7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>283.06</v>
+        <v>283.49</v>
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>82.23518</v>
+        <v>89.23264</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2816,11 +2848,11 @@
       </c>
       <c r="O8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1564.59</v>
+        <v>1549.65</v>
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>367.02511</v>
+        <v>394.37914</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2833,11 +2865,11 @@
       <c r="N9" s="3"/>
       <c r="O9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>154.26</v>
+        <v>153.26</v>
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>46.60427</v>
+        <v>49.68901</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2845,63 +2877,71 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>39081</v>
-      </c>
-      <c r="E10" s="0" t="str">
-        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!AF:AF)), Miletone_Tracking!AF:AF)</f>
-        <v>Crossed 20,000 lines on 04/21/21</v>
+        <v>13418</v>
       </c>
       <c r="N10" s="3"/>
+      <c r="O10" s="0" t="n">
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
+        <v>149.73393</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
+        <v>149.73393</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>13418</v>
+        <v>1821</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>134.45877</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
+        <v>108.67</v>
       </c>
       <c r="P11" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>134.45877</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
+        <v>46.49996</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="4" t="n">
-        <v>1821</v>
+      <c r="C12" s="6" t="n">
+        <v>12474</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>109.11</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
+        <v>585.16</v>
       </c>
       <c r="P12" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>44.2461</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
+        <v>165.68603</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>12524</v>
-      </c>
-      <c r="N13" s="3"/>
+        <v>8998</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!M:M)), Miletone_Tracking!M:M)</f>
+        <v>Crossed 10,000 on 12/02/2019</v>
+      </c>
       <c r="O13" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>588.87</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
+        <v>334.56</v>
       </c>
       <c r="P13" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>156.91935</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
+        <v>126.72426</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2910,36 +2950,35 @@
         <v>15</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>8998</v>
-      </c>
-      <c r="E14" s="0" t="str">
-        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!M:M)), Miletone_Tracking!M:M)</f>
-        <v>Crossed 10,000 on 12/02/2019</v>
+        <v>15698</v>
       </c>
       <c r="O14" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>336.18</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
+        <v>410.34</v>
       </c>
       <c r="P14" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>122.50085</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
+        <v>146.36531</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="4" t="n">
-        <v>15698</v>
+      <c r="C15" s="6" t="n">
+        <v>89388</v>
+      </c>
+      <c r="E15" s="0" t="str">
+        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!E:E)), Miletone_Tracking!E:E)</f>
+        <v>Split to 85,550 on 01/04/20</v>
       </c>
       <c r="O15" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>414.92</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
+        <v>2668.12</v>
       </c>
       <c r="P15" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>133.83578</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
+        <v>706.35853</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,20 +2986,15 @@
         <v>17</v>
       </c>
       <c r="C16" s="4" t="n">
-        <f aca="false">89390-616</f>
-        <v>88774</v>
-      </c>
-      <c r="E16" s="0" t="str">
-        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!E:E)), Miletone_Tracking!E:E)</f>
-        <v>Split to 85,550 on 01/04/20</v>
+        <v>2490</v>
       </c>
       <c r="O16" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>2672.48</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
+        <v>229.12</v>
       </c>
       <c r="P16" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>647.08731</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
+        <v>15.64652</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2968,15 +3002,15 @@
         <v>18</v>
       </c>
       <c r="C17" s="4" t="n">
-        <v>1893</v>
+        <v>11666</v>
       </c>
       <c r="O17" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>233.89</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
+        <v>666.57</v>
       </c>
       <c r="P17" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
-        <v>56.3747</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
+        <v>201.24464</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2984,15 +3018,19 @@
         <v>19</v>
       </c>
       <c r="C18" s="4" t="n">
-        <v>11668</v>
+        <v>15279</v>
+      </c>
+      <c r="E18" s="0" t="str">
+        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!Q:Q)), Miletone_Tracking!Q:Q)</f>
+        <v>Crossed 15,000 on 01/24/20</v>
       </c>
       <c r="O18" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>679.99</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
+        <v>815.33</v>
       </c>
       <c r="P18" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>187.68721</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
+        <v>233.38656</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3000,19 +3038,15 @@
         <v>20</v>
       </c>
       <c r="C19" s="4" t="n">
-        <v>15278</v>
-      </c>
-      <c r="E19" s="0" t="str">
-        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!Q:Q)), Miletone_Tracking!Q:Q)</f>
-        <v>Crossed 15,000 on 01/24/20</v>
+        <v>2242</v>
       </c>
       <c r="O19" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>867.6</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
+        <v>135.95</v>
       </c>
       <c r="P19" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>222.75538</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
+        <v>57.87874</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,31 +3054,31 @@
         <v>21</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>2242</v>
+        <v>4002</v>
       </c>
       <c r="O20" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>138.85</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
+        <v>456.1</v>
       </c>
       <c r="P20" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>55.86961</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
+        <v>158.57442</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="4" t="n">
-        <v>4002</v>
+      <c r="C21" s="6" t="n">
+        <v>11420</v>
       </c>
       <c r="O21" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>461.76</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
+        <v>412.46</v>
       </c>
       <c r="P21" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>148.24599</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
+        <v>137.82394</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3052,15 +3086,15 @@
         <v>23</v>
       </c>
       <c r="C22" s="4" t="n">
-        <v>11418</v>
+        <v>2936</v>
       </c>
       <c r="O22" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>409.87</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
+        <v>258.54</v>
       </c>
       <c r="P22" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>132.70001</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
+        <v>100.28026</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,15 +3102,15 @@
         <v>24</v>
       </c>
       <c r="C23" s="4" t="n">
-        <v>2934</v>
+        <v>4261</v>
       </c>
       <c r="O23" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>257.73</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
+        <v>279.62</v>
       </c>
       <c r="P23" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>95.84901</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
+        <v>93.20633</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3084,80 +3118,84 @@
         <v>25</v>
       </c>
       <c r="C24" s="4" t="n">
-        <v>4259</v>
-      </c>
+        <v>11312</v>
+      </c>
+      <c r="N24" s="1"/>
       <c r="O24" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>282.56</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
+        <v>333.04</v>
       </c>
       <c r="P24" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>87.66823</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
+        <v>102.98585</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="4" t="n">
-        <v>11310</v>
-      </c>
-      <c r="N25" s="1"/>
+        <v>28579</v>
+      </c>
       <c r="O25" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>335.87</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
+        <v>805.76</v>
       </c>
       <c r="P25" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>95.01073</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
+        <v>259.49712</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="4" t="n">
-        <v>28564</v>
+        <v>1404</v>
       </c>
       <c r="O26" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>802.45</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
+        <v>179.86</v>
       </c>
       <c r="P26" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>240.82268</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
+        <v>53.681</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="4" t="n">
-        <v>1404</v>
+        <v>9645</v>
       </c>
       <c r="O27" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>181.05</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
+        <v>421.24</v>
       </c>
       <c r="P27" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>52.09334</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
+        <v>131.4421</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="4" t="n">
-        <v>9643</v>
+        <v>66230</v>
+      </c>
+      <c r="E28" s="0" t="str">
+        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!T:T)), Miletone_Tracking!T:T)</f>
+        <v>Crossed 50,000 lines on 05/08/20</v>
       </c>
       <c r="O28" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>424.32</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
+        <v>1704.92</v>
       </c>
       <c r="P28" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>123.55108</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
+        <v>473.3997</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,87 +3203,80 @@
         <v>30</v>
       </c>
       <c r="C29" s="4" t="n">
-        <v>66206</v>
-      </c>
-      <c r="E29" s="0" t="str">
-        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!T:T)), Miletone_Tracking!T:T)</f>
-        <v>Crossed 50,000 lines on 05/08/20</v>
+        <v>1044</v>
       </c>
       <c r="O29" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1731.28</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
+        <v>44.53</v>
       </c>
       <c r="P29" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>455.05082</v>
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
+        <v>23.57155</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="4" t="n">
-        <v>1044</v>
+        <v>207</v>
       </c>
       <c r="O30" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>46.35</v>
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
+        <v>31.58</v>
       </c>
       <c r="P30" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>22.31878</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
+        <v>25.34196</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="4" t="n">
-        <v>207</v>
-      </c>
-      <c r="O31" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>31.52</v>
-      </c>
-      <c r="P31" s="0" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>26.58519</v>
-      </c>
+        <v>3625</v>
+      </c>
+      <c r="O31" s="9" t="n">
+        <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
+        <v>163.64</v>
+      </c>
+      <c r="P31" s="9" t="n">
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
+        <v>62.46432</v>
+      </c>
+      <c r="Q31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="4" t="n">
-        <v>3610</v>
-      </c>
-      <c r="O32" s="8" t="n">
-        <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>159.68</v>
-      </c>
-      <c r="P32" s="8" t="n">
-        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>60.24165</v>
-      </c>
-      <c r="Q32" s="8"/>
+        <v>17108</v>
+      </c>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="4" t="n">
-        <v>10892</v>
-      </c>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-    </row>
-    <row r="34" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="10" t="s">
+        <v>39105</v>
+      </c>
+      <c r="E33" s="0" t="str">
+        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!AF:AF)), Miletone_Tracking!AF:AF)</f>
+        <v>Crossed 20,000 lines on 04/21/21</v>
+      </c>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="11" t="n">
-        <v>5143</v>
+      <c r="C34" s="12" t="n">
+        <v>5260</v>
       </c>
       <c r="O34" s="0"/>
       <c r="P34" s="0"/>
@@ -3258,7 +3289,7 @@
         <v>36</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>566</v>
+        <v>878</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,7 +3297,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="4" t="n">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,10 +3307,6 @@
       <c r="C38" s="4" t="n">
         <v>22184</v>
       </c>
-      <c r="E38" s="0" t="str">
-        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!I:I)), Miletone_Tracking!I:I)</f>
-        <v>Crossed 20,000 on 12/19/19</v>
-      </c>
     </row>
     <row r="39" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
@@ -3294,7 +3321,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="4" t="n">
-        <v>20958</v>
+        <v>21021</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3311,12 +3338,12 @@
         <f aca="false">4650-865</f>
         <v>3785</v>
       </c>
-      <c r="I42" s="12" t="s">
+      <c r="I42" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B43" s="0" t="s">
@@ -3326,7 +3353,7 @@
         <f aca="false">10319-580</f>
         <v>9739</v>
       </c>
-      <c r="I43" s="14" t="s">
+      <c r="I43" s="15" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3337,7 +3364,7 @@
       <c r="C44" s="0" t="n">
         <v>23768</v>
       </c>
-      <c r="E44" s="15"/>
+      <c r="E44" s="16"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
@@ -3346,7 +3373,7 @@
       <c r="C45" s="0" t="n">
         <v>3357</v>
       </c>
-      <c r="E45" s="15"/>
+      <c r="E45" s="16"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="4" t="s">
@@ -3354,22 +3381,22 @@
       </c>
       <c r="C47" s="4" t="n">
         <f aca="false">SUM(C4:C45)</f>
-        <v>573251</v>
+        <v>581502</v>
       </c>
       <c r="E47" s="0" t="str">
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!A:A)), Miletone_Tracking!A:A)</f>
-        <v>Crossed 570,000 on 06/13/21</v>
+        <v>Crossed 580,000 on 07/08/21</v>
       </c>
       <c r="N47" s="0" t="s">
         <v>50</v>
       </c>
       <c r="O47" s="0" t="n">
-        <f aca="false">INDEX(Regular_Timings!34:34,COUNT(Regular_Timings!34:34,1,1))</f>
-        <v>15688.1</v>
+        <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
+        <v>15540.43</v>
       </c>
       <c r="P47" s="0" t="n">
-        <f aca="false">INDEX(Parallel_Timings!34:34,COUNT(Parallel_Timings!34:34,1,1))</f>
-        <v>4223.42963</v>
+        <f aca="false">INDEX(Parallel_Timings!35:35,COUNT(Parallel_Timings!35:35,1,1))</f>
+        <v>4313.62711</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3382,9 +3409,9 @@
       <c r="N48" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="P48" s="16" t="n">
+      <c r="P48" s="17" t="n">
         <f aca="false">O47/P47</f>
-        <v>3.71454040303259</v>
+        <v>3.60263639014453</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3423,7 +3450,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S145" s="17" t="n">
+      <c r="S145" s="18" t="n">
         <v>43729</v>
       </c>
     </row>
@@ -3433,7 +3460,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S161" s="17" t="n">
+      <c r="S161" s="18" t="n">
         <v>43780</v>
       </c>
     </row>
@@ -3443,152 +3470,152 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S174" s="17" t="n">
+      <c r="S174" s="18" t="n">
         <v>43765</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S189" s="17" t="n">
+      <c r="S189" s="18" t="n">
         <v>43799</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S203" s="17" t="n">
+      <c r="S203" s="18" t="n">
         <v>43814</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S215" s="17" t="n">
+      <c r="S215" s="18" t="n">
         <v>43827</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S230" s="17" t="n">
+      <c r="S230" s="18" t="n">
         <v>43930</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S244" s="17" t="n">
+      <c r="S244" s="18" t="n">
         <v>43939</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S257" s="17" t="n">
+      <c r="S257" s="18" t="n">
         <v>43955</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S265" s="17"/>
+      <c r="S265" s="18"/>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S266" s="17"/>
+      <c r="S266" s="18"/>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S267" s="17"/>
+      <c r="S267" s="18"/>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S268" s="17"/>
+      <c r="S268" s="18"/>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S269" s="17"/>
+      <c r="S269" s="18"/>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S270" s="17" t="n">
+      <c r="S270" s="18" t="n">
         <v>43968</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S284" s="17" t="n">
+      <c r="S284" s="18" t="n">
         <v>44025</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S297" s="17" t="n">
+      <c r="S297" s="18" t="n">
         <v>44031</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S309" s="17" t="n">
+      <c r="S309" s="18" t="n">
         <v>44050</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S323" s="17" t="n">
+      <c r="S323" s="18" t="n">
         <v>44053</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S336" s="17" t="n">
+      <c r="S336" s="18" t="n">
         <v>44072</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S349" s="17" t="n">
+      <c r="S349" s="18" t="n">
         <v>44094</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S364" s="17" t="n">
+      <c r="S364" s="18" t="n">
         <v>44101</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S378" s="17" t="n">
+      <c r="S378" s="18" t="n">
         <v>44125</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S392" s="17" t="n">
+      <c r="S392" s="18" t="n">
         <v>44130</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S405" s="17" t="n">
+      <c r="S405" s="18" t="n">
         <v>44136</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S419" s="17" t="n">
+      <c r="S419" s="18" t="n">
         <v>44157</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S432" s="17" t="n">
+      <c r="S432" s="18" t="n">
         <v>44164</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S444" s="17" t="n">
+      <c r="S444" s="18" t="n">
         <v>44171</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S459" s="17" t="n">
+      <c r="S459" s="18" t="n">
         <v>44199</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S471" s="17" t="n">
+      <c r="S471" s="18" t="n">
         <v>44218</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S484" s="17" t="n">
+      <c r="S484" s="18" t="n">
         <v>44220</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S498" s="17" t="n">
+      <c r="S498" s="18" t="n">
         <v>44241</v>
       </c>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S511" s="17" t="n">
+      <c r="S511" s="18" t="n">
         <v>44241</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S527" s="17" t="n">
+      <c r="S527" s="18" t="n">
         <v>44284</v>
       </c>
     </row>
@@ -3598,27 +3625,27 @@
       </c>
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S541" s="17" t="n">
+      <c r="S541" s="18" t="n">
         <v>44290</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S556" s="17" t="n">
+      <c r="S556" s="18" t="n">
         <v>44318</v>
       </c>
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S570" s="17" t="n">
+      <c r="S570" s="18" t="n">
         <v>44325</v>
       </c>
     </row>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S587" s="17" t="n">
+      <c r="S587" s="18" t="n">
         <v>44367</v>
       </c>
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S603" s="17" t="n">
+      <c r="S603" s="18" t="n">
         <v>44370</v>
       </c>
     </row>
@@ -3639,14 +3666,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:BK108"/>
+  <dimension ref="A2:BK109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
-      <selection pane="bottomRight" activeCell="G49" activeCellId="0" sqref="G49"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AL4" activeCellId="0" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3670,140 +3697,146 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" s="18" customFormat="true" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="19" t="n">
+    <row r="4" s="19" customFormat="true" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C4" s="20" t="n">
         <v>44136</v>
       </c>
-      <c r="D4" s="20" t="n">
+      <c r="D4" s="21" t="n">
         <v>44143</v>
       </c>
-      <c r="E4" s="21" t="n">
+      <c r="E4" s="22" t="n">
         <v>44151</v>
       </c>
-      <c r="F4" s="21" t="n">
+      <c r="F4" s="22" t="n">
         <v>44157</v>
       </c>
-      <c r="G4" s="19" t="n">
+      <c r="G4" s="20" t="n">
         <v>44164</v>
       </c>
-      <c r="H4" s="22" t="n">
+      <c r="H4" s="23" t="n">
         <v>44171</v>
       </c>
-      <c r="I4" s="22" t="n">
+      <c r="I4" s="23" t="n">
         <v>44178</v>
       </c>
-      <c r="J4" s="21" t="n">
+      <c r="J4" s="22" t="n">
         <v>44185</v>
       </c>
-      <c r="K4" s="21" t="n">
+      <c r="K4" s="22" t="n">
         <v>44192</v>
       </c>
-      <c r="L4" s="21" t="n">
+      <c r="L4" s="22" t="n">
         <v>43833</v>
       </c>
-      <c r="M4" s="21" t="n">
+      <c r="M4" s="22" t="n">
         <v>44206</v>
       </c>
-      <c r="N4" s="21" t="n">
+      <c r="N4" s="22" t="n">
         <v>44213</v>
       </c>
-      <c r="O4" s="21" t="n">
+      <c r="O4" s="22" t="n">
         <v>44220</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="R4" s="21" t="n">
+      <c r="R4" s="22" t="n">
         <v>44241</v>
       </c>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="21" t="n">
+      <c r="T4" s="22" t="n">
         <v>44255</v>
       </c>
-      <c r="U4" s="23" t="s">
+      <c r="U4" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="V4" s="23" t="s">
+      <c r="V4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="24" t="n">
+      <c r="W4" s="25" t="n">
         <v>44276</v>
       </c>
-      <c r="X4" s="24" t="n">
+      <c r="X4" s="25" t="n">
         <v>44283</v>
       </c>
-      <c r="Y4" s="24" t="n">
+      <c r="Y4" s="25" t="n">
         <v>44290</v>
       </c>
-      <c r="Z4" s="23" t="s">
+      <c r="Z4" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="AA4" s="23" t="s">
+      <c r="AA4" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="21" t="n">
+      <c r="AB4" s="22" t="n">
         <v>44311</v>
       </c>
-      <c r="AC4" s="22" t="n">
+      <c r="AC4" s="23" t="n">
         <v>44318</v>
       </c>
-      <c r="AD4" s="22" t="n">
+      <c r="AD4" s="23" t="n">
         <v>44325</v>
       </c>
-      <c r="AE4" s="25" t="s">
+      <c r="AE4" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="AF4" s="22" t="n">
+      <c r="AF4" s="23" t="n">
         <v>44339</v>
       </c>
-      <c r="AG4" s="25" t="s">
+      <c r="AG4" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="AH4" s="22" t="n">
+      <c r="AH4" s="23" t="n">
         <v>44353</v>
       </c>
-      <c r="AI4" s="22" t="n">
+      <c r="AI4" s="23" t="n">
         <v>44360</v>
       </c>
-      <c r="AJ4" s="22" t="n">
+      <c r="AJ4" s="23" t="n">
         <v>44367</v>
       </c>
-    </row>
-    <row r="5" s="18" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
+      <c r="AK4" s="23" t="n">
+        <v>44374</v>
+      </c>
+      <c r="AL4" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
+    </row>
+    <row r="5" s="19" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="22"/>
       <c r="AC5" s="0" t="n">
         <v>636.13</v>
       </c>
@@ -3828,16 +3861,22 @@
       <c r="AJ5" s="0" t="n">
         <v>1132.27</v>
       </c>
-    </row>
-    <row r="6" s="10" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="AK5" s="0" t="n">
+        <v>1065.15</v>
+      </c>
+      <c r="AL5" s="0" t="n">
+        <v>1121.77</v>
+      </c>
+    </row>
+    <row r="6" s="11" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0" t="n">
         <v>509.17</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="11" t="n">
         <v>561.22</v>
       </c>
       <c r="E6" s="0"/>
@@ -3889,7 +3928,7 @@
       <c r="U6" s="0" t="n">
         <v>682.7</v>
       </c>
-      <c r="V6" s="28" t="n">
+      <c r="V6" s="6" t="n">
         <v>730.42</v>
       </c>
       <c r="W6" s="0" t="n">
@@ -3933,6 +3972,12 @@
       </c>
       <c r="AJ6" s="0" t="n">
         <v>721.07</v>
+      </c>
+      <c r="AK6" s="0" t="n">
+        <v>700.97</v>
+      </c>
+      <c r="AL6" s="0" t="n">
+        <v>721.09</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4041,6 +4086,12 @@
       <c r="AJ7" s="0" t="n">
         <v>206.34</v>
       </c>
+      <c r="AK7" s="0" t="n">
+        <v>206.72</v>
+      </c>
+      <c r="AL7" s="0" t="n">
+        <v>207.11</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
@@ -4136,9 +4187,15 @@
       <c r="AJ8" s="0" t="n">
         <v>283.06</v>
       </c>
+      <c r="AK8" s="0" t="n">
+        <v>293.24</v>
+      </c>
+      <c r="AL8" s="0" t="n">
+        <v>283.49</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -4242,6 +4299,12 @@
       </c>
       <c r="AJ9" s="0" t="n">
         <v>1564.59</v>
+      </c>
+      <c r="AK9" s="0" t="n">
+        <v>1542.62</v>
+      </c>
+      <c r="AL9" s="0" t="n">
+        <v>1549.65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4350,10 +4413,16 @@
       <c r="AJ10" s="0" t="n">
         <v>154.26</v>
       </c>
+      <c r="AK10" s="0" t="n">
+        <v>148.7</v>
+      </c>
+      <c r="AL10" s="0" t="n">
+        <v>153.26</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>329.82</v>
@@ -4457,10 +4526,16 @@
       <c r="AJ11" s="0" t="n">
         <v>460.18</v>
       </c>
+      <c r="AK11" s="0" t="n">
+        <v>443.06</v>
+      </c>
+      <c r="AL11" s="0" t="n">
+        <v>458.95</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>87.98</v>
@@ -4537,10 +4612,16 @@
       <c r="AJ12" s="0" t="n">
         <v>109.11</v>
       </c>
+      <c r="AK12" s="0" t="n">
+        <v>104.71</v>
+      </c>
+      <c r="AL12" s="0" t="n">
+        <v>108.67</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>511.4</v>
@@ -4605,10 +4686,16 @@
       <c r="AJ13" s="0" t="n">
         <v>588.87</v>
       </c>
+      <c r="AK13" s="0" t="n">
+        <v>566.37</v>
+      </c>
+      <c r="AL13" s="0" t="n">
+        <v>585.16</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
-        <v>15</v>
+      <c r="A14" s="28" t="s">
+        <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>248.23</v>
@@ -4712,10 +4799,16 @@
       <c r="AJ14" s="0" t="n">
         <v>336.18</v>
       </c>
+      <c r="AK14" s="0" t="n">
+        <v>322.41</v>
+      </c>
+      <c r="AL14" s="0" t="n">
+        <v>334.56</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="s">
-        <v>16</v>
+      <c r="A15" s="28" t="s">
+        <v>15</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>309.51</v>
@@ -4819,10 +4912,16 @@
       <c r="AJ15" s="0" t="n">
         <v>414.92</v>
       </c>
+      <c r="AK15" s="0" t="n">
+        <v>397.11</v>
+      </c>
+      <c r="AL15" s="0" t="n">
+        <v>410.34</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27" t="s">
-        <v>17</v>
+      <c r="A16" s="28" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2194.98</v>
@@ -4926,10 +5025,16 @@
       <c r="AJ16" s="0" t="n">
         <v>2672.48</v>
       </c>
+      <c r="AK16" s="0" t="n">
+        <v>2554.98</v>
+      </c>
+      <c r="AL16" s="0" t="n">
+        <v>2668.12</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="s">
-        <v>18</v>
+      <c r="A17" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="AD17" s="0" t="n">
         <v>218.85</v>
@@ -4952,10 +5057,16 @@
       <c r="AJ17" s="0" t="n">
         <v>233.89</v>
       </c>
+      <c r="AK17" s="0" t="n">
+        <v>221.49</v>
+      </c>
+      <c r="AL17" s="0" t="n">
+        <v>229.12</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27" t="s">
-        <v>19</v>
+      <c r="A18" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>508.87</v>
@@ -5059,10 +5170,16 @@
       <c r="AJ18" s="0" t="n">
         <v>679.99</v>
       </c>
+      <c r="AK18" s="0" t="n">
+        <v>636.59</v>
+      </c>
+      <c r="AL18" s="0" t="n">
+        <v>666.57</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27" t="s">
-        <v>20</v>
+      <c r="A19" s="28" t="s">
+        <v>19</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>621.42</v>
@@ -5166,10 +5283,16 @@
       <c r="AJ19" s="0" t="n">
         <v>867.6</v>
       </c>
+      <c r="AK19" s="0" t="n">
+        <v>777.85</v>
+      </c>
+      <c r="AL19" s="0" t="n">
+        <v>815.33</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27" t="s">
-        <v>21</v>
+      <c r="A20" s="28" t="s">
+        <v>20</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>96.76</v>
@@ -5273,10 +5396,16 @@
       <c r="AJ20" s="0" t="n">
         <v>138.85</v>
       </c>
+      <c r="AK20" s="0" t="n">
+        <v>127.5</v>
+      </c>
+      <c r="AL20" s="0" t="n">
+        <v>135.95</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="27" t="s">
-        <v>22</v>
+      <c r="A21" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>369.58</v>
@@ -5380,10 +5509,16 @@
       <c r="AJ21" s="0" t="n">
         <v>461.76</v>
       </c>
+      <c r="AK21" s="0" t="n">
+        <v>433.56</v>
+      </c>
+      <c r="AL21" s="0" t="n">
+        <v>456.1</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="s">
-        <v>23</v>
+      <c r="A22" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>301.53</v>
@@ -5460,7 +5595,7 @@
       <c r="AA22" s="0" t="n">
         <v>407.53</v>
       </c>
-      <c r="AB22" s="10" t="n">
+      <c r="AB22" s="11" t="n">
         <v>375.94</v>
       </c>
       <c r="AC22" s="0" t="n">
@@ -5487,10 +5622,16 @@
       <c r="AJ22" s="0" t="n">
         <v>409.87</v>
       </c>
+      <c r="AK22" s="0" t="n">
+        <v>393.03</v>
+      </c>
+      <c r="AL22" s="0" t="n">
+        <v>412.46</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27" t="s">
-        <v>24</v>
+      <c r="A23" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>190.42</v>
@@ -5594,10 +5735,16 @@
       <c r="AJ23" s="0" t="n">
         <v>257.73</v>
       </c>
+      <c r="AK23" s="0" t="n">
+        <v>246.15</v>
+      </c>
+      <c r="AL23" s="0" t="n">
+        <v>258.54</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27" t="s">
-        <v>25</v>
+      <c r="A24" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>209.15</v>
@@ -5701,10 +5848,16 @@
       <c r="AJ24" s="0" t="n">
         <v>282.56</v>
       </c>
+      <c r="AK24" s="0" t="n">
+        <v>266.93</v>
+      </c>
+      <c r="AL24" s="0" t="n">
+        <v>279.62</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="27" t="s">
-        <v>26</v>
+      <c r="A25" s="28" t="s">
+        <v>25</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>242.4</v>
@@ -5808,10 +5961,16 @@
       <c r="AJ25" s="0" t="n">
         <v>335.87</v>
       </c>
+      <c r="AK25" s="0" t="n">
+        <v>316.55</v>
+      </c>
+      <c r="AL25" s="0" t="n">
+        <v>333.04</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>597.06</v>
@@ -5915,10 +6074,16 @@
       <c r="AJ26" s="0" t="n">
         <v>802.45</v>
       </c>
+      <c r="AK26" s="0" t="n">
+        <v>770.94</v>
+      </c>
+      <c r="AL26" s="0" t="n">
+        <v>805.76</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="27" t="s">
-        <v>28</v>
+      <c r="A27" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>124.46</v>
@@ -6004,7 +6169,7 @@
       <c r="AD27" s="0" t="n">
         <v>167.39</v>
       </c>
-      <c r="AE27" s="28" t="n">
+      <c r="AE27" s="6" t="n">
         <v>168.41</v>
       </c>
       <c r="AF27" s="0" t="n">
@@ -6022,10 +6187,16 @@
       <c r="AJ27" s="0" t="n">
         <v>181.05</v>
       </c>
+      <c r="AK27" s="0" t="n">
+        <v>171.16</v>
+      </c>
+      <c r="AL27" s="0" t="n">
+        <v>179.86</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="27" t="s">
-        <v>29</v>
+      <c r="A28" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="U28" s="0" t="n">
         <v>430.65</v>
@@ -6075,10 +6246,16 @@
       <c r="AJ28" s="0" t="n">
         <v>424.32</v>
       </c>
+      <c r="AK28" s="0" t="n">
+        <v>402.58</v>
+      </c>
+      <c r="AL28" s="0" t="n">
+        <v>421.24</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="27" t="s">
-        <v>30</v>
+      <c r="A29" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>1348.93</v>
@@ -6182,10 +6359,16 @@
       <c r="AJ29" s="0" t="n">
         <v>1731.28</v>
       </c>
+      <c r="AK29" s="0" t="n">
+        <v>1636.37</v>
+      </c>
+      <c r="AL29" s="0" t="n">
+        <v>1704.92</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="27" t="s">
-        <v>31</v>
+      <c r="A30" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>30.85</v>
@@ -6289,10 +6472,16 @@
       <c r="AJ30" s="0" t="n">
         <v>46.35</v>
       </c>
+      <c r="AK30" s="0" t="n">
+        <v>42.28</v>
+      </c>
+      <c r="AL30" s="0" t="n">
+        <v>44.53</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>22.21</v>
@@ -6396,10 +6585,16 @@
       <c r="AJ31" s="0" t="n">
         <v>31.52</v>
       </c>
+      <c r="AK31" s="0" t="n">
+        <v>30.52</v>
+      </c>
+      <c r="AL31" s="0" t="n">
+        <v>31.58</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>117.34</v>
@@ -6503,753 +6698,789 @@
       <c r="AJ32" s="0" t="n">
         <v>159.68</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="0" t="n">
+      <c r="AK32" s="0" t="n">
+        <v>156.35</v>
+      </c>
+      <c r="AL32" s="0" t="n">
+        <v>163.64</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
         <v>9790.18</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D35" s="0" t="n">
         <f aca="false">SUM(D$6:D$32)</f>
         <v>10337.28</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E35" s="0" t="n">
         <f aca="false">SUM(E$6:E$32)</f>
         <v>9477.73</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F35" s="0" t="n">
         <f aca="false">SUM(F$6:F$32)</f>
         <v>10458.76</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G35" s="0" t="n">
         <f aca="false">SUM(G$6:G$32)</f>
         <v>10875.79</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H35" s="0" t="n">
         <f aca="false">SUM(H$6:H$32)</f>
         <v>11600.74</v>
       </c>
-      <c r="I34" s="0" t="n">
+      <c r="I35" s="0" t="n">
         <f aca="false">SUM(I$6:I$32)</f>
         <v>11859.09</v>
       </c>
-      <c r="J34" s="0" t="n">
+      <c r="J35" s="0" t="n">
         <f aca="false">SUM(J$6:J$32)</f>
         <v>11489.62</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="K35" s="0" t="n">
         <f aca="false">SUM(K$6:K$32)</f>
         <v>11576.56</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="L35" s="0" t="n">
         <f aca="false">SUM(L$6:L$32)</f>
         <v>11966.15</v>
       </c>
-      <c r="M34" s="0" t="n">
+      <c r="M35" s="0" t="n">
         <f aca="false">SUM(M$6:M$32)</f>
         <v>11641.86</v>
       </c>
-      <c r="N34" s="0" t="n">
+      <c r="N35" s="0" t="n">
         <f aca="false">SUM(N$6:N$32)</f>
         <v>12450.34</v>
       </c>
-      <c r="O34" s="0" t="n">
+      <c r="O35" s="0" t="n">
         <f aca="false">SUM(O$6:O$32)</f>
         <v>12937.65</v>
       </c>
-      <c r="P34" s="0" t="n">
+      <c r="P35" s="0" t="n">
         <f aca="false">SUM(P$6:P$32)</f>
         <v>13285.67</v>
       </c>
-      <c r="Q34" s="0" t="n">
+      <c r="Q35" s="0" t="n">
         <f aca="false">SUM(Q$6:Q$32)</f>
         <v>13349.21</v>
       </c>
-      <c r="R34" s="0" t="n">
+      <c r="R35" s="0" t="n">
         <f aca="false">SUM(R$6:R$32)</f>
         <v>13674.81</v>
       </c>
-      <c r="S34" s="0" t="n">
+      <c r="S35" s="0" t="n">
         <f aca="false">SUM(S$6:S$32)</f>
         <v>13603.51</v>
       </c>
-      <c r="T34" s="0" t="n">
+      <c r="T35" s="0" t="n">
         <f aca="false">SUM(T$6:T$32)</f>
         <v>13543.13</v>
       </c>
-      <c r="U34" s="0" t="n">
+      <c r="U35" s="0" t="n">
         <f aca="false">SUM(U$6:U$32)</f>
         <v>14943.86</v>
       </c>
-      <c r="V34" s="0" t="n">
+      <c r="V35" s="0" t="n">
         <f aca="false">SUM(V$6:V$32)</f>
         <v>14183.58</v>
       </c>
-      <c r="W34" s="0" t="n">
+      <c r="W35" s="0" t="n">
         <f aca="false">SUM(W$6:W$32)</f>
         <v>14048.98</v>
       </c>
-      <c r="X34" s="0" t="n">
+      <c r="X35" s="0" t="n">
         <f aca="false">SUM(X$6:X$32)</f>
         <v>13534.81</v>
       </c>
-      <c r="Y34" s="0" t="n">
+      <c r="Y35" s="0" t="n">
         <f aca="false">SUM(Y$6:Y$32)</f>
         <v>14136.64</v>
       </c>
-      <c r="Z34" s="0" t="n">
+      <c r="Z35" s="0" t="n">
         <f aca="false">SUM(Z$6:Z$32)</f>
         <v>12760.59</v>
       </c>
-      <c r="AA34" s="0" t="n">
+      <c r="AA35" s="0" t="n">
         <f aca="false">SUM(AA$6:AA$32)</f>
         <v>14579.26</v>
       </c>
-      <c r="AB34" s="0" t="n">
+      <c r="AB35" s="0" t="n">
         <f aca="false">SUM(AB$6:AB$32)</f>
         <v>13658.59</v>
       </c>
-      <c r="AC34" s="0" t="n">
+      <c r="AC35" s="0" t="n">
         <f aca="false">SUM(AC$5:AC$32)</f>
         <v>14093.95</v>
       </c>
-      <c r="AD34" s="0" t="n">
+      <c r="AD35" s="0" t="n">
         <f aca="false">SUM(AD$5:AD$32)</f>
         <v>15691.06</v>
       </c>
-      <c r="AE34" s="0" t="n">
+      <c r="AE35" s="0" t="n">
         <f aca="false">SUM(AE$5:AE$32)</f>
         <v>15719.61</v>
       </c>
-      <c r="AF34" s="0" t="n">
+      <c r="AF35" s="0" t="n">
         <f aca="false">SUM(AF$5:AF$32)</f>
         <v>16257.9</v>
       </c>
-      <c r="AG34" s="0" t="n">
+      <c r="AG35" s="0" t="n">
         <f aca="false">SUM(AG$5:AG$32)</f>
         <v>16386.75</v>
       </c>
-      <c r="AH34" s="0" t="n">
+      <c r="AH35" s="0" t="n">
         <f aca="false">SUM(AH$5:AH$32)</f>
         <v>15900.46</v>
       </c>
-      <c r="AI34" s="0" t="n">
+      <c r="AI35" s="0" t="n">
         <f aca="false">SUM(AI$5:AI$32)</f>
         <v>16684.01</v>
       </c>
-      <c r="AJ34" s="0" t="n">
+      <c r="AJ35" s="0" t="n">
         <f aca="false">SUM(AJ$5:AJ$32)</f>
         <v>15688.1</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31" t="n">
-        <f aca="false">D34/C34</f>
+      <c r="AK35" s="0" t="n">
+        <f aca="false">SUM(AK$5:AK$32)</f>
+        <v>14975.89</v>
+      </c>
+      <c r="AL35" s="0" t="n">
+        <f aca="false">SUM(AL$5:AL$32)</f>
+        <v>15540.43</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31" t="n">
+        <f aca="false">D35/C35</f>
         <v>1.0558825271854</v>
       </c>
-      <c r="E35" s="31" t="n">
-        <f aca="false">E34/D34</f>
+      <c r="E36" s="31" t="n">
+        <f aca="false">E35/D35</f>
         <v>0.916849500061912</v>
       </c>
-      <c r="F35" s="31" t="n">
-        <f aca="false">F34/E34</f>
+      <c r="F36" s="31" t="n">
+        <f aca="false">F35/E35</f>
         <v>1.10350896258914</v>
       </c>
-      <c r="G35" s="31" t="n">
-        <f aca="false">G34/F34</f>
+      <c r="G36" s="31" t="n">
+        <f aca="false">G35/F35</f>
         <v>1.03987375176407</v>
       </c>
-      <c r="H35" s="31" t="n">
-        <f aca="false">H34/G34</f>
+      <c r="H36" s="31" t="n">
+        <f aca="false">H35/G35</f>
         <v>1.06665722673939</v>
       </c>
-      <c r="I35" s="31" t="n">
-        <f aca="false">I34/H34</f>
+      <c r="I36" s="31" t="n">
+        <f aca="false">I35/H35</f>
         <v>1.02227013104336</v>
       </c>
-      <c r="J35" s="31" t="n">
-        <f aca="false">J34/I34</f>
+      <c r="J36" s="31" t="n">
+        <f aca="false">J35/I35</f>
         <v>0.968844995695285</v>
       </c>
-      <c r="K35" s="31" t="n">
-        <f aca="false">K34/J34</f>
+      <c r="K36" s="31" t="n">
+        <f aca="false">K35/J35</f>
         <v>1.00756682988645</v>
       </c>
-      <c r="L35" s="31" t="n">
-        <f aca="false">L34/K34</f>
+      <c r="L36" s="31" t="n">
+        <f aca="false">L35/K35</f>
         <v>1.03365334779935</v>
       </c>
-      <c r="M35" s="31" t="n">
-        <f aca="false">M34/L34</f>
+      <c r="M36" s="31" t="n">
+        <f aca="false">M35/L35</f>
         <v>0.972899387020888</v>
       </c>
-      <c r="N35" s="31" t="n">
-        <f aca="false">N34/M34</f>
+      <c r="N36" s="31" t="n">
+        <f aca="false">N35/M35</f>
         <v>1.06944594764067</v>
       </c>
-      <c r="O35" s="31" t="n">
-        <f aca="false">O34/N34</f>
+      <c r="O36" s="31" t="n">
+        <f aca="false">O35/N35</f>
         <v>1.03914029657021</v>
       </c>
-      <c r="P35" s="31" t="n">
-        <f aca="false">P34/O34</f>
+      <c r="P36" s="31" t="n">
+        <f aca="false">P35/O35</f>
         <v>1.0268997847368</v>
       </c>
-      <c r="Q35" s="31" t="n">
-        <f aca="false">Q34/P34</f>
+      <c r="Q36" s="31" t="n">
+        <f aca="false">Q35/P35</f>
         <v>1.00478259658715</v>
       </c>
-      <c r="R35" s="31" t="n">
-        <f aca="false">R34/Q34</f>
+      <c r="R36" s="31" t="n">
+        <f aca="false">R35/Q35</f>
         <v>1.02439095646859</v>
       </c>
-      <c r="S35" s="31" t="n">
-        <f aca="false">S34/R34</f>
+      <c r="S36" s="31" t="n">
+        <f aca="false">S35/R35</f>
         <v>0.994786033590229</v>
       </c>
-      <c r="T35" s="31" t="n">
-        <f aca="false">T34/S34</f>
+      <c r="T36" s="31" t="n">
+        <f aca="false">T35/S35</f>
         <v>0.995561439657853</v>
       </c>
-      <c r="U35" s="31" t="n">
-        <f aca="false">U34/T34</f>
+      <c r="U36" s="31" t="n">
+        <f aca="false">U35/T35</f>
         <v>1.10342734655874</v>
       </c>
-      <c r="V35" s="31" t="n">
-        <f aca="false">V34/U34</f>
+      <c r="V36" s="31" t="n">
+        <f aca="false">V35/U35</f>
         <v>0.949124255714387</v>
       </c>
-      <c r="W35" s="31" t="n">
-        <f aca="false">W34/V34</f>
+      <c r="W36" s="31" t="n">
+        <f aca="false">W35/V35</f>
         <v>0.990510153289931</v>
       </c>
-      <c r="X35" s="31" t="n">
-        <f aca="false">X34/W34</f>
+      <c r="X36" s="31" t="n">
+        <f aca="false">X35/W35</f>
         <v>0.963401613497919</v>
       </c>
-      <c r="Y35" s="31" t="n">
-        <f aca="false">Y34/X34</f>
+      <c r="Y36" s="31" t="n">
+        <f aca="false">Y35/X35</f>
         <v>1.04446534528375</v>
       </c>
-      <c r="Z35" s="31" t="n">
-        <f aca="false">Z34/Y34</f>
+      <c r="Z36" s="31" t="n">
+        <f aca="false">Z35/Y35</f>
         <v>0.902660745410508</v>
       </c>
-      <c r="AA35" s="31" t="n">
-        <f aca="false">AA34/Z34</f>
+      <c r="AA36" s="31" t="n">
+        <f aca="false">AA35/Z35</f>
         <v>1.14252240687931</v>
       </c>
-      <c r="AB35" s="31" t="n">
-        <f aca="false">AB34/AA34</f>
+      <c r="AB36" s="31" t="n">
+        <f aca="false">AB35/AA35</f>
         <v>0.936850704356737</v>
       </c>
-      <c r="AC35" s="31" t="n">
-        <f aca="false">AC34/AB34</f>
+      <c r="AC36" s="31" t="n">
+        <f aca="false">AC35/AB35</f>
         <v>1.03187444677672</v>
       </c>
-      <c r="AD35" s="31" t="n">
-        <f aca="false">AD34/AC34</f>
+      <c r="AD36" s="31" t="n">
+        <f aca="false">AD35/AC35</f>
         <v>1.11331883538682</v>
       </c>
-      <c r="AE35" s="31" t="n">
-        <f aca="false">AE34/AD34</f>
+      <c r="AE36" s="31" t="n">
+        <f aca="false">AE35/AD35</f>
         <v>1.00181950741378</v>
       </c>
-      <c r="AF35" s="31" t="n">
-        <f aca="false">AF34/AE34</f>
+      <c r="AF36" s="31" t="n">
+        <f aca="false">AF35/AE35</f>
         <v>1.03424321595765</v>
       </c>
-      <c r="AG35" s="31" t="n">
-        <f aca="false">AG34/AF34</f>
+      <c r="AG36" s="31" t="n">
+        <f aca="false">AG35/AF35</f>
         <v>1.00792537781632</v>
       </c>
-      <c r="AH35" s="31" t="n">
-        <f aca="false">AH34/AG34</f>
+      <c r="AH36" s="31" t="n">
+        <f aca="false">AH35/AG35</f>
         <v>0.970324194852549</v>
       </c>
-      <c r="AI35" s="31" t="n">
-        <f aca="false">AI34/AH34</f>
+      <c r="AI36" s="31" t="n">
+        <f aca="false">AI35/AH35</f>
         <v>1.04927844854803</v>
       </c>
-      <c r="AJ35" s="31" t="n">
-        <f aca="false">AJ34/AI34</f>
+      <c r="AJ36" s="31" t="n">
+        <f aca="false">AJ35/AI35</f>
         <v>0.940307515998851</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="32" t="s">
+      <c r="AK36" s="31" t="n">
+        <f aca="false">AK35/AJ35</f>
+        <v>0.954601895704387</v>
+      </c>
+      <c r="AL36" s="31" t="n">
+        <f aca="false">AL35/AK35</f>
+        <v>1.03769659098725</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="L37" s="33" t="s">
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="O37" s="34" t="s">
+      <c r="L38" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="P37" s="33" t="s">
+      <c r="O38" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="U37" s="33" t="s">
+      <c r="P38" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="AC37" s="33" t="s">
+      <c r="U38" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="AD37" s="33" t="s">
+      <c r="AC38" s="33" t="s">
         <v>82</v>
       </c>
+      <c r="AD38" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL38" s="35"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB45" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC45" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA46" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA47" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA48" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E49" s="0" t="s">
-        <v>72</v>
+      <c r="AA49" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E50" s="0" t="s">
-        <v>6</v>
+      <c r="AA50" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E51" s="0" t="s">
-        <v>7</v>
+      <c r="AA51" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E52" s="0" t="s">
-        <v>8</v>
+      <c r="AA52" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E53" s="0" t="s">
-        <v>9</v>
+      <c r="AA53" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E54" s="0" t="s">
-        <v>10</v>
+      <c r="AA54" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E55" s="0" t="s">
-        <v>12</v>
+      <c r="AA55" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E56" s="0" t="s">
-        <v>13</v>
+      <c r="AA56" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E57" s="0" t="s">
-        <v>14</v>
+      <c r="AA57" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E58" s="0" t="s">
-        <v>15</v>
+      <c r="AA58" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E59" s="0" t="s">
-        <v>16</v>
+      <c r="AA59" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E60" s="0" t="s">
-        <v>17</v>
+      <c r="AA60" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E61" s="0" t="s">
-        <v>18</v>
+      <c r="AA61" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E62" s="0" t="s">
-        <v>19</v>
+      <c r="AA62" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E63" s="0" t="s">
-        <v>20</v>
+      <c r="AA63" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E64" s="0" t="s">
-        <v>21</v>
+      <c r="AA64" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E65" s="0" t="s">
-        <v>22</v>
+      <c r="AA65" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E66" s="0" t="s">
-        <v>23</v>
+      <c r="AA66" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E67" s="0" t="s">
-        <v>24</v>
+      <c r="AA67" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E68" s="0" t="s">
-        <v>25</v>
+      <c r="AA68" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E69" s="0" t="s">
-        <v>26</v>
+      <c r="AA69" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E70" s="0" t="s">
-        <v>27</v>
+      <c r="AA70" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E71" s="0" t="s">
-        <v>28</v>
+      <c r="AA71" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E72" s="0" t="s">
-        <v>29</v>
+      <c r="AA72" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E73" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E74" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E75" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E76" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="BI81" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="BJ81" s="0" t="n">
-        <v>636.13</v>
+      <c r="AA73" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI82" s="0" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="BJ82" s="0" t="n">
-        <v>683.07</v>
-      </c>
-      <c r="BK82" s="0" t="n">
-        <v>184.02927</v>
+        <v>636.13</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI83" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ83" s="0" t="n">
-        <v>189.3</v>
+        <v>683.07</v>
       </c>
       <c r="BK83" s="0" t="n">
-        <v>72.85334</v>
+        <v>184.02927</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI84" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BJ84" s="0" t="n">
-        <v>257.48</v>
+        <v>189.3</v>
       </c>
       <c r="BK84" s="0" t="n">
-        <v>76.28002</v>
+        <v>72.85334</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI85" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="BJ85" s="0" t="n">
-        <v>1440.74</v>
+        <v>257.48</v>
       </c>
       <c r="BK85" s="0" t="n">
-        <v>349.71263</v>
+        <v>76.28002</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI86" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="BJ86" s="0" t="n">
-        <v>141.39</v>
+        <v>1440.74</v>
       </c>
       <c r="BK86" s="0" t="n">
-        <v>38.67067</v>
+        <v>349.71263</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI87" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="BJ87" s="0" t="n">
-        <v>420.46</v>
+        <v>141.39</v>
       </c>
       <c r="BK87" s="0" t="n">
-        <v>82.07111</v>
+        <v>38.67067</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI88" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="BJ88" s="0" t="n">
-        <v>96.99</v>
+        <v>420.46</v>
       </c>
       <c r="BK88" s="0" t="n">
-        <v>40.81308</v>
+        <v>82.07111</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI89" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="BJ89" s="0" t="n">
-        <v>547.6</v>
+        <v>96.99</v>
       </c>
       <c r="BK89" s="0" t="n">
-        <v>154.66179</v>
+        <v>40.81308</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI90" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BJ90" s="0" t="n">
-        <v>314.62</v>
+        <v>547.6</v>
       </c>
       <c r="BK90" s="0" t="n">
-        <v>108.24716</v>
+        <v>154.66179</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI91" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="BJ91" s="0" t="n">
-        <v>400.01</v>
+        <v>314.62</v>
       </c>
       <c r="BK91" s="0" t="n">
-        <v>125.53587</v>
+        <v>108.24716</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI92" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="BJ92" s="0" t="n">
-        <v>2630.57</v>
+        <v>400.01</v>
       </c>
       <c r="BK92" s="0" t="n">
-        <v>618.08973</v>
+        <v>125.53587</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI93" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="BJ93" s="0" t="n">
+        <v>2630.57</v>
+      </c>
+      <c r="BK93" s="0" t="n">
+        <v>618.08973</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI94" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="BJ94" s="0" t="n">
-        <v>627.3</v>
-      </c>
-      <c r="BK94" s="0" t="n">
-        <v>170.75118</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI95" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BJ95" s="0" t="n">
-        <v>793.5</v>
+        <v>627.3</v>
       </c>
       <c r="BK95" s="0" t="n">
-        <v>207.23633</v>
+        <v>170.75118</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI96" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="BJ96" s="0" t="n">
-        <v>128.01</v>
+        <v>793.5</v>
       </c>
       <c r="BK96" s="0" t="n">
-        <v>53.48696</v>
+        <v>207.23633</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI97" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="BJ97" s="0" t="n">
-        <v>433.45</v>
+        <v>128.01</v>
       </c>
       <c r="BK97" s="0" t="n">
-        <v>136.36899</v>
+        <v>53.48696</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI98" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="BJ98" s="0" t="n">
-        <v>384.37</v>
+        <v>433.45</v>
       </c>
       <c r="BK98" s="0" t="n">
-        <v>116.54091</v>
+        <v>136.36899</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI99" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="BJ99" s="0" t="n">
-        <v>241.07</v>
+        <v>384.37</v>
       </c>
       <c r="BK99" s="0" t="n">
-        <v>85.85521</v>
+        <v>116.54091</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI100" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="BJ100" s="0" t="n">
-        <v>261.63</v>
+        <v>241.07</v>
       </c>
       <c r="BK100" s="0" t="n">
-        <v>81.64308</v>
+        <v>85.85521</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI101" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="BJ101" s="0" t="n">
-        <v>309.31</v>
+        <v>261.63</v>
       </c>
       <c r="BK101" s="0" t="n">
-        <v>83.81372</v>
+        <v>81.64308</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI102" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="BJ102" s="0" t="n">
-        <v>777.04</v>
+        <v>309.31</v>
       </c>
       <c r="BK102" s="0" t="n">
-        <v>222.50691</v>
+        <v>83.81372</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI103" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="BJ103" s="0" t="n">
-        <v>159.26</v>
+        <v>777.04</v>
       </c>
       <c r="BK103" s="0" t="n">
-        <v>44.91844</v>
+        <v>222.50691</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI104" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="BJ104" s="0" t="n">
-        <v>385.36</v>
+        <v>159.26</v>
       </c>
       <c r="BK104" s="0" t="n">
-        <v>109.12426</v>
+        <v>44.91844</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI105" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="BJ105" s="0" t="n">
-        <v>1620.35</v>
+        <v>385.36</v>
       </c>
       <c r="BK105" s="0" t="n">
-        <v>418.55554</v>
+        <v>109.12426</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI106" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="BJ106" s="0" t="n">
-        <v>38.92</v>
+        <v>1620.35</v>
       </c>
       <c r="BK106" s="0" t="n">
-        <v>19.64096</v>
+        <v>418.55554</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI107" s="0" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="BJ107" s="0" t="n">
-        <v>27.54</v>
+        <v>38.92</v>
       </c>
       <c r="BK107" s="0" t="n">
-        <v>21.33641</v>
+        <v>19.64096</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI108" s="0" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="BJ108" s="0" t="n">
+        <v>27.54</v>
+      </c>
+      <c r="BK108" s="0" t="n">
+        <v>21.33641</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BI109" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="BJ109" s="0" t="n">
         <v>148.48</v>
       </c>
-      <c r="BK108" s="0" t="n">
+      <c r="BK109" s="0" t="n">
         <v>54.7953</v>
       </c>
     </row>
@@ -7269,14 +7500,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AJ37"/>
+  <dimension ref="A2:AL38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AF4" activeCellId="0" sqref="AF4"/>
+      <selection pane="bottomRight" activeCell="AK36" activeCellId="0" sqref="AK36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7298,141 +7529,147 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" s="37" customFormat="true" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="38" customFormat="true" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
-      <c r="C4" s="35" t="n">
+      <c r="C4" s="36" t="n">
         <v>44136</v>
       </c>
-      <c r="D4" s="36" t="n">
+      <c r="D4" s="37" t="n">
         <v>44144</v>
       </c>
-      <c r="E4" s="35" t="n">
+      <c r="E4" s="36" t="n">
         <v>44151</v>
       </c>
-      <c r="F4" s="35" t="n">
+      <c r="F4" s="36" t="n">
         <v>44157</v>
       </c>
-      <c r="G4" s="35" t="n">
+      <c r="G4" s="36" t="n">
         <v>44164</v>
       </c>
-      <c r="H4" s="35" t="n">
+      <c r="H4" s="36" t="n">
         <v>44171</v>
       </c>
-      <c r="I4" s="35" t="n">
+      <c r="I4" s="36" t="n">
         <v>44178</v>
       </c>
-      <c r="J4" s="35" t="n">
+      <c r="J4" s="36" t="n">
         <v>44185</v>
       </c>
-      <c r="K4" s="35" t="n">
+      <c r="K4" s="36" t="n">
         <v>44192</v>
       </c>
-      <c r="L4" s="35" t="n">
+      <c r="L4" s="36" t="n">
         <v>43833</v>
       </c>
-      <c r="M4" s="35" t="n">
+      <c r="M4" s="36" t="n">
         <v>44206</v>
       </c>
-      <c r="N4" s="35" t="n">
+      <c r="N4" s="36" t="n">
         <v>44213</v>
       </c>
-      <c r="O4" s="35" t="n">
+      <c r="O4" s="36" t="n">
         <v>44220</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="R4" s="24" t="n">
+      <c r="R4" s="25" t="n">
         <v>44241</v>
       </c>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="T4" s="24" t="n">
+      <c r="T4" s="25" t="n">
         <v>44255</v>
       </c>
-      <c r="U4" s="23" t="s">
+      <c r="U4" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="V4" s="23" t="s">
+      <c r="V4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="24" t="n">
+      <c r="W4" s="25" t="n">
         <v>44276</v>
       </c>
-      <c r="X4" s="24" t="n">
+      <c r="X4" s="25" t="n">
         <v>44276</v>
       </c>
-      <c r="Y4" s="24" t="n">
+      <c r="Y4" s="25" t="n">
         <v>44290</v>
       </c>
-      <c r="Z4" s="23" t="s">
+      <c r="Z4" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="AA4" s="23" t="s">
+      <c r="AA4" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="21" t="n">
+      <c r="AB4" s="22" t="n">
         <v>44311</v>
       </c>
-      <c r="AC4" s="21" t="n">
+      <c r="AC4" s="22" t="n">
         <v>44318</v>
       </c>
-      <c r="AD4" s="35" t="n">
+      <c r="AD4" s="36" t="n">
         <v>44325</v>
       </c>
-      <c r="AE4" s="25" t="s">
+      <c r="AE4" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="AG4" s="25" t="s">
+      <c r="AG4" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="AH4" s="22" t="n">
+      <c r="AH4" s="23" t="n">
         <v>44353</v>
       </c>
-      <c r="AI4" s="22" t="n">
+      <c r="AI4" s="23" t="n">
         <v>44360</v>
       </c>
-      <c r="AJ4" s="22" t="n">
+      <c r="AJ4" s="23" t="n">
         <v>44367</v>
       </c>
-    </row>
-    <row r="5" s="37" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AK4" s="23" t="n">
+        <v>44374</v>
+      </c>
+      <c r="AL4" s="23" t="n">
+        <v>44383</v>
+      </c>
+    </row>
+    <row r="5" s="38" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="40"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="40"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="40"/>
-      <c r="X5" s="40"/>
-      <c r="Y5" s="40"/>
-      <c r="Z5" s="41"/>
-      <c r="AA5" s="41"/>
-      <c r="AB5" s="41"/>
-      <c r="AC5" s="28" t="n">
+        <v>73</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="42"/>
+      <c r="V5" s="42"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="42"/>
+      <c r="AA5" s="42"/>
+      <c r="AB5" s="42"/>
+      <c r="AC5" s="6" t="n">
         <v>272.20742</v>
       </c>
       <c r="AD5" s="0" t="n">
@@ -7453,16 +7690,22 @@
       <c r="AJ5" s="0" t="n">
         <v>257.4753</v>
       </c>
-    </row>
-    <row r="6" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AK5" s="0" t="n">
+        <v>245.67225</v>
+      </c>
+      <c r="AL5" s="0" t="n">
+        <v>242.65954</v>
+      </c>
+    </row>
+    <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="28" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>125.35355</v>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="D6" s="9" t="n">
         <v>144.04571</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -7557,6 +7800,12 @@
       </c>
       <c r="AJ6" s="0" t="n">
         <v>202.62068</v>
+      </c>
+      <c r="AK6" s="0" t="n">
+        <v>201.36892</v>
+      </c>
+      <c r="AL6" s="0" t="n">
+        <v>201.08922</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7662,6 +7911,12 @@
       <c r="AJ7" s="0" t="n">
         <v>84.56981</v>
       </c>
+      <c r="AK7" s="0" t="n">
+        <v>85.02801</v>
+      </c>
+      <c r="AL7" s="0" t="n">
+        <v>85.80095</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="29" t="s">
@@ -7754,9 +8009,15 @@
       <c r="AJ8" s="0" t="n">
         <v>82.23518</v>
       </c>
+      <c r="AK8" s="0" t="n">
+        <v>85.47151</v>
+      </c>
+      <c r="AL8" s="0" t="n">
+        <v>89.23264</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -7857,6 +8118,12 @@
       </c>
       <c r="AJ9" s="0" t="n">
         <v>367.02511</v>
+      </c>
+      <c r="AK9" s="0" t="n">
+        <v>378.24715</v>
+      </c>
+      <c r="AL9" s="0" t="n">
+        <v>394.37914</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7962,10 +8229,16 @@
       <c r="AJ10" s="0" t="n">
         <v>46.60427</v>
       </c>
+      <c r="AK10" s="0" t="n">
+        <v>48.05456</v>
+      </c>
+      <c r="AL10" s="0" t="n">
+        <v>49.68901</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>90.30445</v>
@@ -8066,10 +8339,16 @@
       <c r="AJ11" s="0" t="n">
         <v>134.45877</v>
       </c>
+      <c r="AK11" s="0" t="n">
+        <v>132.9687</v>
+      </c>
+      <c r="AL11" s="0" t="n">
+        <v>149.73393</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>33.5291</v>
@@ -8143,10 +8422,16 @@
       <c r="AJ12" s="0" t="n">
         <v>44.2461</v>
       </c>
+      <c r="AK12" s="0" t="n">
+        <v>42.7937</v>
+      </c>
+      <c r="AL12" s="0" t="n">
+        <v>46.49996</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>134.91832</v>
@@ -8208,10 +8493,16 @@
       <c r="AJ13" s="0" t="n">
         <v>156.91935</v>
       </c>
+      <c r="AK13" s="0" t="n">
+        <v>152.0348</v>
+      </c>
+      <c r="AL13" s="0" t="n">
+        <v>165.68603</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="27" t="s">
-        <v>15</v>
+      <c r="B14" s="28" t="s">
+        <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>74.7034</v>
@@ -8312,10 +8603,16 @@
       <c r="AJ14" s="0" t="n">
         <v>122.50085</v>
       </c>
+      <c r="AK14" s="0" t="n">
+        <v>115.88999</v>
+      </c>
+      <c r="AL14" s="0" t="n">
+        <v>126.72426</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="27" t="s">
-        <v>16</v>
+      <c r="B15" s="28" t="s">
+        <v>15</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>101.31368</v>
@@ -8341,7 +8638,7 @@
       <c r="J15" s="0" t="n">
         <v>106.81782</v>
       </c>
-      <c r="K15" s="10" t="n">
+      <c r="K15" s="11" t="n">
         <v>111.0613</v>
       </c>
       <c r="L15" s="0" t="n">
@@ -8416,10 +8713,16 @@
       <c r="AJ15" s="0" t="n">
         <v>133.83578</v>
       </c>
+      <c r="AK15" s="0" t="n">
+        <v>133.21585</v>
+      </c>
+      <c r="AL15" s="0" t="n">
+        <v>146.36531</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="27" t="s">
-        <v>17</v>
+      <c r="B16" s="28" t="s">
+        <v>16</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>523.34115</v>
@@ -8520,9 +8823,17 @@
       <c r="AJ16" s="0" t="n">
         <v>647.08731</v>
       </c>
+      <c r="AK16" s="0" t="n">
+        <v>658.48807</v>
+      </c>
+      <c r="AL16" s="0" t="n">
+        <v>706.35853</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="27"/>
+      <c r="B17" s="28" t="s">
+        <v>17</v>
+      </c>
       <c r="AD17" s="0" t="n">
         <v>53.44944</v>
       </c>
@@ -8541,10 +8852,16 @@
       <c r="AJ17" s="0" t="n">
         <v>56.3747</v>
       </c>
+      <c r="AK17" s="0" t="n">
+        <v>54.36942</v>
+      </c>
+      <c r="AL17" s="0" t="n">
+        <v>15.64652</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="27" t="s">
-        <v>19</v>
+      <c r="B18" s="28" t="s">
+        <v>18</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>136.269</v>
@@ -8645,10 +8962,16 @@
       <c r="AJ18" s="0" t="n">
         <v>187.68721</v>
       </c>
+      <c r="AK18" s="0" t="n">
+        <v>187.51806</v>
+      </c>
+      <c r="AL18" s="0" t="n">
+        <v>201.24464</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="27" t="s">
-        <v>20</v>
+      <c r="B19" s="28" t="s">
+        <v>19</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>165.00564</v>
@@ -8749,10 +9072,16 @@
       <c r="AJ19" s="0" t="n">
         <v>222.75538</v>
       </c>
+      <c r="AK19" s="0" t="n">
+        <v>219.66025</v>
+      </c>
+      <c r="AL19" s="0" t="n">
+        <v>233.38656</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="27" t="s">
-        <v>21</v>
+      <c r="B20" s="28" t="s">
+        <v>20</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>43.42474</v>
@@ -8853,10 +9182,16 @@
       <c r="AJ20" s="0" t="n">
         <v>55.86961</v>
       </c>
+      <c r="AK20" s="0" t="n">
+        <v>53.58778</v>
+      </c>
+      <c r="AL20" s="0" t="n">
+        <v>57.87874</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="27" t="s">
-        <v>22</v>
+      <c r="B21" s="28" t="s">
+        <v>21</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>109.78636</v>
@@ -8957,10 +9292,16 @@
       <c r="AJ21" s="0" t="n">
         <v>148.24599</v>
       </c>
+      <c r="AK21" s="0" t="n">
+        <v>148.00328</v>
+      </c>
+      <c r="AL21" s="0" t="n">
+        <v>158.57442</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="27" t="s">
-        <v>23</v>
+      <c r="B22" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>93.06885</v>
@@ -9037,7 +9378,7 @@
       <c r="AA22" s="0" t="n">
         <v>113.63319</v>
       </c>
-      <c r="AB22" s="10" t="n">
+      <c r="AB22" s="11" t="n">
         <v>114.35779</v>
       </c>
       <c r="AC22" s="0" t="n">
@@ -9061,10 +9402,16 @@
       <c r="AJ22" s="0" t="n">
         <v>132.70001</v>
       </c>
+      <c r="AK22" s="0" t="n">
+        <v>127.0985</v>
+      </c>
+      <c r="AL22" s="0" t="n">
+        <v>137.82394</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="27" t="s">
-        <v>24</v>
+      <c r="B23" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>66.16259</v>
@@ -9165,10 +9512,16 @@
       <c r="AJ23" s="0" t="n">
         <v>95.84901</v>
       </c>
+      <c r="AK23" s="0" t="n">
+        <v>93.42322</v>
+      </c>
+      <c r="AL23" s="0" t="n">
+        <v>100.28026</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="27" t="s">
-        <v>25</v>
+      <c r="B24" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>66.85539</v>
@@ -9269,10 +9622,16 @@
       <c r="AJ24" s="0" t="n">
         <v>87.66823</v>
       </c>
+      <c r="AK24" s="0" t="n">
+        <v>85.87711</v>
+      </c>
+      <c r="AL24" s="0" t="n">
+        <v>93.20633</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="27" t="s">
-        <v>26</v>
+      <c r="B25" s="28" t="s">
+        <v>25</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>64.77227</v>
@@ -9373,10 +9732,16 @@
       <c r="AJ25" s="0" t="n">
         <v>95.01073</v>
       </c>
+      <c r="AK25" s="0" t="n">
+        <v>93.98365</v>
+      </c>
+      <c r="AL25" s="0" t="n">
+        <v>102.98585</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>170.8217</v>
@@ -9477,10 +9842,16 @@
       <c r="AJ26" s="0" t="n">
         <v>240.82268</v>
       </c>
+      <c r="AK26" s="0" t="n">
+        <v>239.60832</v>
+      </c>
+      <c r="AL26" s="0" t="n">
+        <v>259.49712</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="27" t="s">
-        <v>28</v>
+      <c r="B27" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>34.37503</v>
@@ -9581,10 +9952,16 @@
       <c r="AJ27" s="0" t="n">
         <v>52.09334</v>
       </c>
+      <c r="AK27" s="0" t="n">
+        <v>51.43692</v>
+      </c>
+      <c r="AL27" s="0" t="n">
+        <v>53.681</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="27" t="s">
-        <v>29</v>
+      <c r="B28" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="U28" s="0" t="n">
         <v>70.84659</v>
@@ -9631,10 +10008,16 @@
       <c r="AJ28" s="0" t="n">
         <v>123.55108</v>
       </c>
+      <c r="AK28" s="0" t="n">
+        <v>123.13846</v>
+      </c>
+      <c r="AL28" s="0" t="n">
+        <v>131.4421</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="27" t="s">
-        <v>30</v>
+      <c r="B29" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>338.33972</v>
@@ -9735,10 +10118,16 @@
       <c r="AJ29" s="0" t="n">
         <v>455.05082</v>
       </c>
+      <c r="AK29" s="0" t="n">
+        <v>455.04092</v>
+      </c>
+      <c r="AL29" s="0" t="n">
+        <v>473.3997</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="27" t="s">
-        <v>31</v>
+      <c r="B30" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>14.4627</v>
@@ -9839,10 +10228,16 @@
       <c r="AJ30" s="0" t="n">
         <v>22.31878</v>
       </c>
+      <c r="AK30" s="0" t="n">
+        <v>20.91764</v>
+      </c>
+      <c r="AL30" s="0" t="n">
+        <v>23.57155</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>6.41945</v>
@@ -9943,10 +10338,16 @@
       <c r="AJ31" s="0" t="n">
         <v>26.58519</v>
       </c>
+      <c r="AK31" s="0" t="n">
+        <v>23.93915</v>
+      </c>
+      <c r="AL31" s="0" t="n">
+        <v>25.34196</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>45.24003</v>
@@ -10047,289 +10448,316 @@
       <c r="AJ32" s="0" t="n">
         <v>60.24165</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="0" t="n">
+      <c r="AK32" s="0" t="n">
+        <v>56.79092</v>
+      </c>
+      <c r="AL32" s="0" t="n">
+        <v>62.46432</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
         <v>2612.46243</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D35" s="0" t="n">
         <f aca="false">SUM(D$6:D$32)</f>
         <v>3028.77253</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E35" s="0" t="n">
         <f aca="false">SUM(E$6:E$32)</f>
         <v>2647.14944</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F35" s="0" t="n">
         <f aca="false">SUM(F$6:F$32)</f>
         <v>2769.76382</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G35" s="0" t="n">
         <f aca="false">SUM(G$6:G$32)</f>
         <v>3016.57278</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H35" s="0" t="n">
         <f aca="false">SUM(H$6:H$32)</f>
         <v>3124.03663</v>
       </c>
-      <c r="I34" s="0" t="n">
+      <c r="I35" s="0" t="n">
         <f aca="false">SUM(I$6:I$32)</f>
         <v>3056.50511</v>
       </c>
-      <c r="J34" s="0" t="n">
+      <c r="J35" s="0" t="n">
         <f aca="false">SUM(J$6:J$32)</f>
         <v>3042.05414</v>
       </c>
-      <c r="K34" s="0" t="n">
+      <c r="K35" s="0" t="n">
         <f aca="false">SUM(K$6:K$32)</f>
         <v>3174.05903</v>
       </c>
-      <c r="L34" s="0" t="n">
+      <c r="L35" s="0" t="n">
         <f aca="false">SUM(L$6:L$32)</f>
         <v>3199.32619</v>
       </c>
-      <c r="M34" s="0" t="n">
+      <c r="M35" s="0" t="n">
         <f aca="false">SUM(M$6:M$32)</f>
         <v>3319.87056</v>
       </c>
-      <c r="N34" s="0" t="n">
+      <c r="N35" s="0" t="n">
         <f aca="false">SUM(N$6:N$32)</f>
         <v>3334.27172</v>
       </c>
-      <c r="O34" s="0" t="n">
+      <c r="O35" s="0" t="n">
         <f aca="false">SUM(O$6:O$32)</f>
         <v>3717.01054</v>
       </c>
-      <c r="P34" s="0" t="n">
+      <c r="P35" s="0" t="n">
         <f aca="false">SUM(P$6:P$32)</f>
         <v>3644.57944</v>
       </c>
-      <c r="Q34" s="0" t="n">
+      <c r="Q35" s="0" t="n">
         <f aca="false">SUM(Q$6:Q$32)</f>
         <v>3614.8949</v>
       </c>
-      <c r="R34" s="0" t="n">
+      <c r="R35" s="0" t="n">
         <f aca="false">SUM(R$6:R$32)</f>
         <v>3489.23673</v>
       </c>
-      <c r="S34" s="0" t="n">
+      <c r="S35" s="0" t="n">
         <f aca="false">SUM(S$6:S$32)</f>
         <v>3668.1901</v>
       </c>
-      <c r="T34" s="0" t="n">
+      <c r="T35" s="0" t="n">
         <f aca="false">SUM(T$6:T$32)</f>
         <v>3607.45241</v>
       </c>
-      <c r="U34" s="0" t="n">
+      <c r="U35" s="0" t="n">
         <f aca="false">SUM(U$6:U$32)</f>
         <v>3882.99563</v>
       </c>
-      <c r="V34" s="0" t="n">
+      <c r="V35" s="0" t="n">
         <f aca="false">SUM(V$6:V$32)</f>
         <v>3811.71968</v>
       </c>
-      <c r="W34" s="0" t="n">
+      <c r="W35" s="0" t="n">
         <f aca="false">SUM(W$6:W$32)</f>
         <v>3822.09531</v>
       </c>
-      <c r="X34" s="0" t="n">
+      <c r="X35" s="0" t="n">
         <f aca="false">SUM(X$6:X$32)</f>
         <v>3229.64777</v>
       </c>
-      <c r="Y34" s="0" t="n">
+      <c r="Y35" s="0" t="n">
         <f aca="false">SUM(Y$6:Y$32)</f>
         <v>3630.30786</v>
       </c>
-      <c r="Z34" s="0" t="n">
+      <c r="Z35" s="0" t="n">
         <f aca="false">SUM(Z$6:Z$32)</f>
         <v>3590.40803</v>
       </c>
-      <c r="AA34" s="0" t="n">
+      <c r="AA35" s="0" t="n">
         <f aca="false">SUM(AA$6:AA$32)</f>
         <v>3640.36933</v>
       </c>
-      <c r="AB34" s="0" t="n">
+      <c r="AB35" s="0" t="n">
         <f aca="false">SUM(AB$6:AB$32)</f>
         <v>3725.42452</v>
       </c>
-      <c r="AC34" s="0" t="n">
+      <c r="AC35" s="0" t="n">
         <f aca="false">SUM(AC$5:AC$32)</f>
         <v>3949.74629</v>
       </c>
-      <c r="AD34" s="0" t="n">
+      <c r="AD35" s="0" t="n">
         <f aca="false">SUM(AD$5:AD$32)</f>
         <v>4160.19797</v>
       </c>
-      <c r="AE34" s="0" t="n">
+      <c r="AE35" s="0" t="n">
         <f aca="false">SUM(AE$5:AE$32)</f>
         <v>4297.3518</v>
       </c>
-      <c r="AG34" s="0" t="n">
+      <c r="AG35" s="0" t="n">
         <f aca="false">SUM(AG$5:AG$32)</f>
         <v>4472.39476</v>
       </c>
-      <c r="AH34" s="0" t="n">
+      <c r="AH35" s="0" t="n">
         <f aca="false">SUM(AH$5:AH$32)</f>
         <v>4087.71284</v>
       </c>
-      <c r="AI34" s="0" t="n">
+      <c r="AI35" s="0" t="n">
         <f aca="false">SUM(AI$5:AI$32)</f>
         <v>4223.42963</v>
       </c>
-      <c r="AJ34" s="0" t="n">
+      <c r="AJ35" s="0" t="n">
         <f aca="false">SUM(AJ$5:AJ$32)</f>
         <v>4342.40292</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="42" t="n">
-        <f aca="false">1/(C34/Regular_Timings!C34)</f>
+      <c r="AK35" s="0" t="n">
+        <f aca="false">SUM(AK$5:AK$32)</f>
+        <v>4313.62711</v>
+      </c>
+      <c r="AL35" s="0" t="n">
+        <f aca="false">SUM(AL$5:AL$32)</f>
+        <v>4534.64353</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="43" t="n">
+        <f aca="false">1/(C35/Regular_Timings!C35)</f>
         <v>3.74749121272531</v>
       </c>
-      <c r="D35" s="42" t="n">
-        <f aca="false">1/(D34/Regular_Timings!D34)</f>
+      <c r="D36" s="43" t="n">
+        <f aca="false">1/(D35/Regular_Timings!D35)</f>
         <v>3.41302620041922</v>
       </c>
-      <c r="E35" s="42" t="n">
-        <f aca="false">1/(E34/Regular_Timings!E34)</f>
+      <c r="E36" s="43" t="n">
+        <f aca="false">1/(E35/Regular_Timings!E35)</f>
         <v>3.58035321194409</v>
       </c>
-      <c r="F35" s="42" t="n">
-        <f aca="false">1/(F34/Regular_Timings!F34)</f>
+      <c r="F36" s="43" t="n">
+        <f aca="false">1/(F35/Regular_Timings!F35)</f>
         <v>3.77604759094586</v>
       </c>
-      <c r="G35" s="42" t="n">
-        <f aca="false">1/(G34/Regular_Timings!G34)</f>
+      <c r="G36" s="43" t="n">
+        <f aca="false">1/(G35/Regular_Timings!G35)</f>
         <v>3.60534646208669</v>
       </c>
-      <c r="H35" s="42" t="n">
-        <f aca="false">1/(H34/Regular_Timings!H34)</f>
+      <c r="H36" s="43" t="n">
+        <f aca="false">1/(H35/Regular_Timings!H35)</f>
         <v>3.71338155532446</v>
       </c>
-      <c r="I35" s="42" t="n">
-        <f aca="false">1/(I34/Regular_Timings!I34)</f>
+      <c r="I36" s="43" t="n">
+        <f aca="false">1/(I35/Regular_Timings!I35)</f>
         <v>3.87995098100785</v>
       </c>
-      <c r="J35" s="42" t="n">
-        <f aca="false">1/(J34/Regular_Timings!J34)</f>
+      <c r="J36" s="43" t="n">
+        <f aca="false">1/(J35/Regular_Timings!J35)</f>
         <v>3.77692817787917</v>
       </c>
-      <c r="K35" s="42" t="n">
-        <f aca="false">1/(K34/Regular_Timings!K34)</f>
+      <c r="K36" s="43" t="n">
+        <f aca="false">1/(K35/Regular_Timings!K35)</f>
         <v>3.64724155744514</v>
       </c>
-      <c r="L35" s="42" t="n">
-        <f aca="false">1/(L34/Regular_Timings!L34)</f>
+      <c r="L36" s="43" t="n">
+        <f aca="false">1/(L35/Regular_Timings!L35)</f>
         <v>3.74020943453721</v>
       </c>
-      <c r="M35" s="42" t="n">
-        <f aca="false">1/(M34/Regular_Timings!M34)</f>
+      <c r="M36" s="43" t="n">
+        <f aca="false">1/(M35/Regular_Timings!M35)</f>
         <v>3.50672105722098</v>
       </c>
-      <c r="N35" s="42" t="n">
-        <f aca="false">1/(N34/Regular_Timings!N34)</f>
+      <c r="N36" s="43" t="n">
+        <f aca="false">1/(N35/Regular_Timings!N35)</f>
         <v>3.73405080495359</v>
       </c>
-      <c r="O35" s="42" t="n">
-        <f aca="false">1/(O34/Regular_Timings!O34)</f>
+      <c r="O36" s="43" t="n">
+        <f aca="false">1/(O35/Regular_Timings!O35)</f>
         <v>3.48066002524706</v>
       </c>
-      <c r="P35" s="42" t="n">
-        <f aca="false">1/(P34/Regular_Timings!P34)</f>
+      <c r="P36" s="43" t="n">
+        <f aca="false">1/(P35/Regular_Timings!P35)</f>
         <v>3.64532320360124</v>
       </c>
-      <c r="Q35" s="42" t="n">
-        <f aca="false">1/(Q34/Regular_Timings!Q34)</f>
+      <c r="Q36" s="43" t="n">
+        <f aca="false">1/(Q35/Regular_Timings!Q35)</f>
         <v>3.69283488712217</v>
       </c>
-      <c r="R35" s="42" t="n">
-        <f aca="false">1/(R34/Regular_Timings!R34)</f>
+      <c r="R36" s="43" t="n">
+        <f aca="false">1/(R35/Regular_Timings!R35)</f>
         <v>3.91914079157363</v>
       </c>
-      <c r="S35" s="42" t="n">
-        <f aca="false">1/(S34/Regular_Timings!S34)</f>
+      <c r="S36" s="43" t="n">
+        <f aca="false">1/(S35/Regular_Timings!S35)</f>
         <v>3.70850736443567</v>
       </c>
-      <c r="T35" s="42" t="n">
-        <f aca="false">1/(T34/Regular_Timings!T34)</f>
+      <c r="T36" s="43" t="n">
+        <f aca="false">1/(T35/Regular_Timings!T35)</f>
         <v>3.75420891553771</v>
       </c>
-      <c r="U35" s="42" t="n">
-        <f aca="false">1/(U34/Regular_Timings!U34)</f>
+      <c r="U36" s="43" t="n">
+        <f aca="false">1/(U35/Regular_Timings!U35)</f>
         <v>3.84853896938329</v>
       </c>
-      <c r="V35" s="42" t="n">
-        <f aca="false">Regular_Timings!V34/V34</f>
+      <c r="V36" s="43" t="n">
+        <f aca="false">Regular_Timings!V35/V35</f>
         <v>3.72104488019434</v>
       </c>
-      <c r="W35" s="42" t="n">
-        <f aca="false">Regular_Timings!W34/W34</f>
+      <c r="W36" s="43" t="n">
+        <f aca="false">Regular_Timings!W35/W35</f>
         <v>3.67572728059469</v>
       </c>
-      <c r="X35" s="42" t="n">
-        <f aca="false">Regular_Timings!X34/X34</f>
+      <c r="X36" s="43" t="n">
+        <f aca="false">Regular_Timings!X35/X35</f>
         <v>4.19080065811635</v>
       </c>
-      <c r="Y35" s="42" t="n">
-        <f aca="false">Regular_Timings!Y34/Y34</f>
+      <c r="Y36" s="43" t="n">
+        <f aca="false">Regular_Timings!Y35/Y35</f>
         <v>3.89406092958739</v>
       </c>
-      <c r="Z35" s="42" t="n">
-        <f aca="false">Regular_Timings!Z34/Z34</f>
+      <c r="Z36" s="43" t="n">
+        <f aca="false">Regular_Timings!Z35/Z35</f>
         <v>3.55407794695691</v>
       </c>
-      <c r="AA35" s="42" t="n">
-        <f aca="false">Regular_Timings!AA34/AA34</f>
+      <c r="AA36" s="43" t="n">
+        <f aca="false">Regular_Timings!AA35/AA35</f>
         <v>4.00488485600993</v>
       </c>
-      <c r="AB35" s="42" t="n">
-        <f aca="false">Regular_Timings!AB34/AB34</f>
+      <c r="AB36" s="43" t="n">
+        <f aca="false">Regular_Timings!AB35/AB35</f>
         <v>3.66631773819967</v>
       </c>
-      <c r="AC35" s="42" t="n">
-        <f aca="false">Regular_Timings!AC34/AC34</f>
+      <c r="AC36" s="43" t="n">
+        <f aca="false">Regular_Timings!AC35/AC35</f>
         <v>3.56831780200242</v>
       </c>
-      <c r="AD35" s="42" t="n">
-        <f aca="false">Regular_Timings!AD34/AD34</f>
+      <c r="AD36" s="43" t="n">
+        <f aca="false">Regular_Timings!AD35/AD35</f>
         <v>3.7717099313906</v>
       </c>
-      <c r="AE35" s="42" t="n">
-        <f aca="false">Regular_Timings!AE34/AE34</f>
+      <c r="AE36" s="43" t="n">
+        <f aca="false">Regular_Timings!AE35/AE35</f>
         <v>3.65797605865082</v>
       </c>
-      <c r="AG35" s="42" t="n">
-        <f aca="false">Regular_Timings!AG34/AG34</f>
+      <c r="AG36" s="43" t="n">
+        <f aca="false">Regular_Timings!AG35/AG35</f>
         <v>3.6639766566581</v>
       </c>
-      <c r="AH35" s="42" t="n">
-        <f aca="false">Regular_Timings!AH34/AH34</f>
+      <c r="AH36" s="43" t="n">
+        <f aca="false">Regular_Timings!AH35/AH35</f>
         <v>3.88981824858324</v>
       </c>
-      <c r="AI35" s="42" t="n">
-        <f aca="false">Regular_Timings!AI34/AI34</f>
+      <c r="AI36" s="43" t="n">
+        <f aca="false">Regular_Timings!AI35/AI35</f>
         <v>3.95034639182564</v>
       </c>
-      <c r="AJ35" s="42" t="n">
-        <f aca="false">Regular_Timings!AJ34/AJ34</f>
+      <c r="AJ36" s="43" t="n">
+        <f aca="false">Regular_Timings!AJ35/AJ35</f>
         <v>3.61276930976272</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="AC36" s="33"/>
+      <c r="AK36" s="43" t="n">
+        <f aca="false">Regular_Timings!AK35/AK35</f>
+        <v>3.47176276903545</v>
+      </c>
+      <c r="AL36" s="43" t="n">
+        <f aca="false">Regular_Timings!AL35/AL35</f>
+        <v>3.42704556536553</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AC37" s="43" t="s">
-        <v>85</v>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="AC37" s="33"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC38" s="44" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -10348,17 +10776,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF29"/>
+  <dimension ref="A1:AF97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="10" style="0" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10366,209 +10796,241 @@
         <v>50</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>38</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q3" s="44" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+      <c r="Q3" s="45" t="s">
+        <v>93</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>107</v>
+        <v>108</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>128</v>
-      </c>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J85" s="4"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J86" s="4"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J87" s="12"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J88" s="4"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J89" s="4"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J94" s="4"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J95" s="4"/>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J96" s="4"/>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J97" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
- Updated performance and milestone tracking
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="132">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">Sheet</t>
   </si>
   <si>
-    <t xml:space="preserve">VisualGrammar</t>
+    <t xml:space="preserve">VisualGrammar </t>
   </si>
   <si>
     <t xml:space="preserve">CoreTemps</t>
@@ -435,6 +435,28 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">07/11/2021
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">(run on  7/12/21)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">ICal</t>
   </si>
   <si>
@@ -468,9 +490,6 @@
   </si>
   <si>
     <t xml:space="preserve">GtkBuilder Added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Parallel</t>
   </si>
   <si>
     <t xml:space="preserve">CardDeck</t>
@@ -1280,15 +1299,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>15120</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>694080</xdr:colOff>
+      <xdr:colOff>694800</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1301,7 +1320,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2225160" y="11673360"/>
+          <a:off x="2225880" y="11674080"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1317,13 +1336,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>15120</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>659520</xdr:colOff>
+      <xdr:colOff>660240</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
@@ -1338,7 +1357,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2225160" y="14281200"/>
+          <a:off x="2225880" y="14281200"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1354,13 +1373,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>15120</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>502200</xdr:colOff>
+      <xdr:colOff>502920</xdr:colOff>
       <xdr:row>110</xdr:row>
       <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
@@ -1375,7 +1394,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2225160" y="16576920"/>
+          <a:off x="2225880" y="16576920"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1391,13 +1410,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>14040</xdr:colOff>
+      <xdr:colOff>14760</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>455400</xdr:colOff>
+      <xdr:colOff>456120</xdr:colOff>
       <xdr:row>126</xdr:row>
       <xdr:rowOff>75960</xdr:rowOff>
     </xdr:to>
@@ -1412,7 +1431,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2224800" y="19731600"/>
+          <a:off x="2225520" y="19731600"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1428,15 +1447,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>43560</xdr:colOff>
+      <xdr:colOff>44280</xdr:colOff>
       <xdr:row>129</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>480240</xdr:colOff>
+      <xdr:colOff>480960</xdr:colOff>
       <xdr:row>141</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1449,7 +1468,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2254320" y="22516920"/>
+          <a:off x="2255040" y="22517640"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1465,13 +1484,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>11520</xdr:colOff>
+      <xdr:colOff>12240</xdr:colOff>
       <xdr:row>143</xdr:row>
       <xdr:rowOff>24480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>887400</xdr:colOff>
+      <xdr:colOff>888120</xdr:colOff>
       <xdr:row>155</xdr:row>
       <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
@@ -1486,7 +1505,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2222280" y="24989400"/>
+          <a:off x="2223000" y="24989400"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1541,13 +1560,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>360360</xdr:colOff>
       <xdr:row>158</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>910440</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1560,7 +1579,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3210120" y="27605520"/>
+          <a:off x="3210120" y="27606240"/>
           <a:ext cx="8718120" cy="1964880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1578,13 +1597,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>209880</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>168840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>619920</xdr:colOff>
       <xdr:row>200</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1597,7 +1616,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3059640" y="32844240"/>
+          <a:off x="3059640" y="32844960"/>
           <a:ext cx="9787680" cy="2191320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1615,13 +1634,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>306720</xdr:colOff>
       <xdr:row>201</xdr:row>
-      <xdr:rowOff>113040</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>410040</xdr:colOff>
       <xdr:row>213</xdr:row>
-      <xdr:rowOff>119520</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1634,7 +1653,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3156480" y="35242920"/>
+          <a:off x="3156480" y="35243640"/>
           <a:ext cx="9480960" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2730,8 +2749,8 @@
   </sheetPr>
   <dimension ref="A1:W603"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2795,11 +2814,11 @@
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>721.09</v>
+        <v>763.4</v>
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>201.08922</v>
+        <v>224.0093</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2811,11 +2830,11 @@
       </c>
       <c r="O6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>207.11</v>
+        <v>218.1</v>
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>85.80095</v>
+        <v>96.1126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2827,11 +2846,11 @@
       </c>
       <c r="O7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>283.49</v>
+        <v>299.26</v>
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>89.23264</v>
+        <v>93.94092</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2848,11 +2867,11 @@
       </c>
       <c r="O8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1549.65</v>
+        <v>1634.58</v>
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>394.37914</v>
+        <v>397.38036</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2865,11 +2884,11 @@
       <c r="N9" s="3"/>
       <c r="O9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>153.26</v>
+        <v>162.82</v>
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>49.68901</v>
+        <v>49.86798</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2882,11 +2901,11 @@
       <c r="N10" s="3"/>
       <c r="O10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>149.73393</v>
+        <v>138.60975</v>
       </c>
       <c r="P10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>149.73393</v>
+        <v>138.60975</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2899,11 +2918,11 @@
       <c r="N11" s="3"/>
       <c r="O11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>108.67</v>
+        <v>114.75</v>
       </c>
       <c r="P11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>46.49996</v>
+        <v>44.00051</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2916,11 +2935,11 @@
       <c r="N12" s="3"/>
       <c r="O12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>585.16</v>
+        <v>617.09</v>
       </c>
       <c r="P12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>165.68603</v>
+        <v>158.05704</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2937,11 +2956,11 @@
       </c>
       <c r="O13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>334.56</v>
+        <v>354.04</v>
       </c>
       <c r="P13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>126.72426</v>
+        <v>119.37928</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2954,11 +2973,11 @@
       </c>
       <c r="O14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>410.34</v>
+        <v>436.89</v>
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>146.36531</v>
+        <v>138.64966</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,11 +2993,11 @@
       </c>
       <c r="O15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>2668.12</v>
+        <v>2812.44</v>
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>706.35853</v>
+        <v>699.5017</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2990,7 +3009,7 @@
       </c>
       <c r="O16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>229.12</v>
+        <v>237.57</v>
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
@@ -3006,11 +3025,11 @@
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>666.57</v>
+        <v>702.06</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>201.24464</v>
+        <v>198.0559</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3026,11 +3045,11 @@
       </c>
       <c r="O18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>815.33</v>
+        <v>855.38</v>
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>233.38656</v>
+        <v>232.20613</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3042,11 +3061,11 @@
       </c>
       <c r="O19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>135.95</v>
+        <v>140.71</v>
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>57.87874</v>
+        <v>56.22573</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,11 +3077,11 @@
       </c>
       <c r="O20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>456.1</v>
+        <v>476.98</v>
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>158.57442</v>
+        <v>157.33707</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3074,11 +3093,11 @@
       </c>
       <c r="O21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>412.46</v>
+        <v>436.46</v>
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>137.82394</v>
+        <v>136.05224</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3090,11 +3109,11 @@
       </c>
       <c r="O22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>258.54</v>
+        <v>272.59</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>100.28026</v>
+        <v>98.81968</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3106,11 +3125,11 @@
       </c>
       <c r="O23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>279.62</v>
+        <v>294.42</v>
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>93.20633</v>
+        <v>89.23575</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,11 +3142,11 @@
       <c r="N24" s="1"/>
       <c r="O24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>333.04</v>
+        <v>347.88</v>
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>102.98585</v>
+        <v>96.99919</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,11 +3158,11 @@
       </c>
       <c r="O25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>805.76</v>
+        <v>845.61</v>
       </c>
       <c r="P25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>259.49712</v>
+        <v>247.10647</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3155,11 +3174,11 @@
       </c>
       <c r="O26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>179.86</v>
+        <v>187.19</v>
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>53.681</v>
+        <v>53.34275</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3171,11 +3190,11 @@
       </c>
       <c r="O27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>421.24</v>
+        <v>442.08</v>
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>131.4421</v>
+        <v>127.00975</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3191,11 +3210,11 @@
       </c>
       <c r="O28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1704.92</v>
+        <v>1800.39</v>
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>473.3997</v>
+        <v>479.86395</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3207,11 +3226,11 @@
       </c>
       <c r="O29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>44.53</v>
+        <v>46.47</v>
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>23.57155</v>
+        <v>21.87859</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3223,11 +3242,11 @@
       </c>
       <c r="O30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>31.58</v>
+        <v>33.34</v>
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>25.34196</v>
+        <v>28.39049</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3239,11 +3258,11 @@
       </c>
       <c r="O31" s="9" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>163.64</v>
+        <v>171.26</v>
       </c>
       <c r="P31" s="9" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>62.46432</v>
+        <v>62.95408</v>
       </c>
       <c r="Q31" s="9"/>
     </row>
@@ -3392,11 +3411,11 @@
       </c>
       <c r="O47" s="0" t="n">
         <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
-        <v>15540.43</v>
+        <v>16354.44</v>
       </c>
       <c r="P47" s="0" t="n">
         <f aca="false">INDEX(Parallel_Timings!35:35,COUNT(Parallel_Timings!35:35,1,1))</f>
-        <v>4313.62711</v>
+        <v>4534.64353</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,7 +3430,7 @@
       </c>
       <c r="P48" s="17" t="n">
         <f aca="false">O47/P47</f>
-        <v>3.60263639014453</v>
+        <v>3.60655471412546</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3668,12 +3687,12 @@
   </sheetPr>
   <dimension ref="A2:BK109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="T5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AL4" activeCellId="0" sqref="AL4"/>
+      <selection pane="bottomRight" activeCell="AA45" activeCellId="0" sqref="AA45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3806,10 +3825,13 @@
       <c r="AL4" s="26" t="s">
         <v>72</v>
       </c>
+      <c r="AM4" s="26" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" s="19" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="27" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="21"/>
@@ -3867,6 +3889,9 @@
       <c r="AL5" s="0" t="n">
         <v>1121.77</v>
       </c>
+      <c r="AM5" s="0" t="n">
+        <v>1165.64</v>
+      </c>
     </row>
     <row r="6" s="11" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
@@ -3979,6 +4004,9 @@
       <c r="AL6" s="0" t="n">
         <v>721.09</v>
       </c>
+      <c r="AM6" s="0" t="n">
+        <v>763.4</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
@@ -4092,6 +4120,9 @@
       <c r="AL7" s="0" t="n">
         <v>207.11</v>
       </c>
+      <c r="AM7" s="0" t="n">
+        <v>218.1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
@@ -4193,6 +4224,9 @@
       <c r="AL8" s="0" t="n">
         <v>283.49</v>
       </c>
+      <c r="AM8" s="0" t="n">
+        <v>299.26</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="28" t="s">
@@ -4306,6 +4340,9 @@
       <c r="AL9" s="0" t="n">
         <v>1549.65</v>
       </c>
+      <c r="AM9" s="0" t="n">
+        <v>1634.58</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
@@ -4419,6 +4456,9 @@
       <c r="AL10" s="0" t="n">
         <v>153.26</v>
       </c>
+      <c r="AM10" s="0" t="n">
+        <v>162.82</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
@@ -4532,6 +4572,9 @@
       <c r="AL11" s="0" t="n">
         <v>458.95</v>
       </c>
+      <c r="AM11" s="0" t="n">
+        <v>485.04</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
@@ -4618,6 +4661,9 @@
       <c r="AL12" s="0" t="n">
         <v>108.67</v>
       </c>
+      <c r="AM12" s="0" t="n">
+        <v>114.75</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
@@ -4692,6 +4738,9 @@
       <c r="AL13" s="0" t="n">
         <v>585.16</v>
       </c>
+      <c r="AM13" s="0" t="n">
+        <v>617.09</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="28" t="s">
@@ -4805,6 +4854,9 @@
       <c r="AL14" s="0" t="n">
         <v>334.56</v>
       </c>
+      <c r="AM14" s="0" t="n">
+        <v>354.04</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="28" t="s">
@@ -4918,6 +4970,9 @@
       <c r="AL15" s="0" t="n">
         <v>410.34</v>
       </c>
+      <c r="AM15" s="0" t="n">
+        <v>436.89</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
@@ -5031,6 +5086,9 @@
       <c r="AL16" s="0" t="n">
         <v>2668.12</v>
       </c>
+      <c r="AM16" s="0" t="n">
+        <v>2812.44</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
@@ -5063,6 +5121,9 @@
       <c r="AL17" s="0" t="n">
         <v>229.12</v>
       </c>
+      <c r="AM17" s="0" t="n">
+        <v>237.57</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28" t="s">
@@ -5176,6 +5237,9 @@
       <c r="AL18" s="0" t="n">
         <v>666.57</v>
       </c>
+      <c r="AM18" s="0" t="n">
+        <v>702.06</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="s">
@@ -5289,6 +5353,9 @@
       <c r="AL19" s="0" t="n">
         <v>815.33</v>
       </c>
+      <c r="AM19" s="0" t="n">
+        <v>855.38</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
@@ -5402,6 +5469,9 @@
       <c r="AL20" s="0" t="n">
         <v>135.95</v>
       </c>
+      <c r="AM20" s="0" t="n">
+        <v>140.71</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
@@ -5515,6 +5585,9 @@
       <c r="AL21" s="0" t="n">
         <v>456.1</v>
       </c>
+      <c r="AM21" s="0" t="n">
+        <v>476.98</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="s">
@@ -5628,6 +5701,9 @@
       <c r="AL22" s="0" t="n">
         <v>412.46</v>
       </c>
+      <c r="AM22" s="0" t="n">
+        <v>436.46</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="28" t="s">
@@ -5741,6 +5817,9 @@
       <c r="AL23" s="0" t="n">
         <v>258.54</v>
       </c>
+      <c r="AM23" s="0" t="n">
+        <v>272.59</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="28" t="s">
@@ -5854,6 +5933,9 @@
       <c r="AL24" s="0" t="n">
         <v>279.62</v>
       </c>
+      <c r="AM24" s="0" t="n">
+        <v>294.42</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
@@ -5967,6 +6049,9 @@
       <c r="AL25" s="0" t="n">
         <v>333.04</v>
       </c>
+      <c r="AM25" s="0" t="n">
+        <v>347.88</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="s">
@@ -6080,6 +6165,9 @@
       <c r="AL26" s="0" t="n">
         <v>805.76</v>
       </c>
+      <c r="AM26" s="0" t="n">
+        <v>845.61</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
@@ -6193,6 +6281,9 @@
       <c r="AL27" s="0" t="n">
         <v>179.86</v>
       </c>
+      <c r="AM27" s="0" t="n">
+        <v>187.19</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
@@ -6252,6 +6343,9 @@
       <c r="AL28" s="0" t="n">
         <v>421.24</v>
       </c>
+      <c r="AM28" s="0" t="n">
+        <v>442.08</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
@@ -6365,6 +6459,9 @@
       <c r="AL29" s="0" t="n">
         <v>1704.92</v>
       </c>
+      <c r="AM29" s="0" t="n">
+        <v>1800.39</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
@@ -6478,6 +6575,9 @@
       <c r="AL30" s="0" t="n">
         <v>44.53</v>
       </c>
+      <c r="AM30" s="0" t="n">
+        <v>46.47</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="29" t="s">
@@ -6591,6 +6691,9 @@
       <c r="AL31" s="0" t="n">
         <v>31.58</v>
       </c>
+      <c r="AM31" s="0" t="n">
+        <v>33.34</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
@@ -6704,6 +6807,9 @@
       <c r="AL32" s="0" t="n">
         <v>163.64</v>
       </c>
+      <c r="AM32" s="0" t="n">
+        <v>171.26</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="29" t="s">
@@ -6712,7 +6818,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -6858,10 +6964,14 @@
         <f aca="false">SUM(AL$5:AL$32)</f>
         <v>15540.43</v>
       </c>
+      <c r="AM35" s="0" t="n">
+        <f aca="false">SUM(AM$5:AM$32)</f>
+        <v>16354.44</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="31" t="n">
@@ -7004,10 +7114,14 @@
         <f aca="false">AL35/AK35</f>
         <v>1.03769659098725</v>
       </c>
+      <c r="AM36" s="31" t="n">
+        <f aca="false">AM35/AL35</f>
+        <v>1.0523801464953</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
@@ -7015,179 +7129,31 @@
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
       <c r="H38" s="32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L38" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O38" s="34" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P38" s="33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="U38" s="33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AC38" s="33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AD38" s="33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AL38" s="35"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AB45" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC45" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA46" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA47" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA48" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA49" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA50" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA51" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA52" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA53" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA54" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA55" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA56" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA57" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA58" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA59" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA60" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA61" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA62" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA63" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA64" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA65" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA66" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA67" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA68" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA69" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA70" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA71" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA72" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AA73" s="0" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI82" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BJ82" s="0" t="n">
         <v>636.13</v>
@@ -7500,14 +7466,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AL38"/>
+  <dimension ref="A2:AM38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AD53" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AK36" activeCellId="0" sqref="AK36"/>
+      <selection pane="topRight" activeCell="AD1" activeCellId="0" sqref="AD1"/>
+      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="bottomRight" activeCell="AM17" activeCellId="0" sqref="AM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7641,7 +7607,7 @@
     <row r="5" s="38" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="40"/>
@@ -7696,6 +7662,9 @@
       <c r="AL5" s="0" t="n">
         <v>242.65954</v>
       </c>
+      <c r="AM5" s="0" t="n">
+        <v>271.32528</v>
+      </c>
     </row>
     <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -7807,6 +7776,9 @@
       <c r="AL6" s="0" t="n">
         <v>201.08922</v>
       </c>
+      <c r="AM6" s="0" t="n">
+        <v>224.0093</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="29" t="s">
@@ -7917,6 +7889,9 @@
       <c r="AL7" s="0" t="n">
         <v>85.80095</v>
       </c>
+      <c r="AM7" s="0" t="n">
+        <v>96.1126</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="29" t="s">
@@ -8015,6 +7990,9 @@
       <c r="AL8" s="0" t="n">
         <v>89.23264</v>
       </c>
+      <c r="AM8" s="0" t="n">
+        <v>93.94092</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="28" t="s">
@@ -8125,6 +8103,9 @@
       <c r="AL9" s="0" t="n">
         <v>394.37914</v>
       </c>
+      <c r="AM9" s="0" t="n">
+        <v>397.38036</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="29" t="s">
@@ -8235,6 +8216,9 @@
       <c r="AL10" s="0" t="n">
         <v>49.68901</v>
       </c>
+      <c r="AM10" s="0" t="n">
+        <v>49.86798</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="29" t="s">
@@ -8345,6 +8329,9 @@
       <c r="AL11" s="0" t="n">
         <v>149.73393</v>
       </c>
+      <c r="AM11" s="0" t="n">
+        <v>138.60975</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="29" t="s">
@@ -8428,6 +8415,9 @@
       <c r="AL12" s="0" t="n">
         <v>46.49996</v>
       </c>
+      <c r="AM12" s="0" t="n">
+        <v>44.00051</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="29" t="s">
@@ -8499,6 +8489,9 @@
       <c r="AL13" s="0" t="n">
         <v>165.68603</v>
       </c>
+      <c r="AM13" s="0" t="n">
+        <v>158.05704</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="28" t="s">
@@ -8609,6 +8602,9 @@
       <c r="AL14" s="0" t="n">
         <v>126.72426</v>
       </c>
+      <c r="AM14" s="0" t="n">
+        <v>119.37928</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="28" t="s">
@@ -8719,6 +8715,9 @@
       <c r="AL15" s="0" t="n">
         <v>146.36531</v>
       </c>
+      <c r="AM15" s="0" t="n">
+        <v>138.64966</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="28" t="s">
@@ -8829,6 +8828,9 @@
       <c r="AL16" s="0" t="n">
         <v>706.35853</v>
       </c>
+      <c r="AM16" s="0" t="n">
+        <v>699.5017</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="28" t="s">
@@ -8968,6 +8970,9 @@
       <c r="AL18" s="0" t="n">
         <v>201.24464</v>
       </c>
+      <c r="AM18" s="0" t="n">
+        <v>198.0559</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="28" t="s">
@@ -9078,6 +9083,9 @@
       <c r="AL19" s="0" t="n">
         <v>233.38656</v>
       </c>
+      <c r="AM19" s="0" t="n">
+        <v>232.20613</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="28" t="s">
@@ -9188,6 +9196,9 @@
       <c r="AL20" s="0" t="n">
         <v>57.87874</v>
       </c>
+      <c r="AM20" s="0" t="n">
+        <v>56.22573</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="28" t="s">
@@ -9298,6 +9309,9 @@
       <c r="AL21" s="0" t="n">
         <v>158.57442</v>
       </c>
+      <c r="AM21" s="0" t="n">
+        <v>157.33707</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="28" t="s">
@@ -9408,6 +9422,9 @@
       <c r="AL22" s="0" t="n">
         <v>137.82394</v>
       </c>
+      <c r="AM22" s="0" t="n">
+        <v>136.05224</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="28" t="s">
@@ -9518,6 +9535,9 @@
       <c r="AL23" s="0" t="n">
         <v>100.28026</v>
       </c>
+      <c r="AM23" s="0" t="n">
+        <v>98.81968</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="28" t="s">
@@ -9628,6 +9648,9 @@
       <c r="AL24" s="0" t="n">
         <v>93.20633</v>
       </c>
+      <c r="AM24" s="0" t="n">
+        <v>89.23575</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="28" t="s">
@@ -9738,6 +9761,9 @@
       <c r="AL25" s="0" t="n">
         <v>102.98585</v>
       </c>
+      <c r="AM25" s="0" t="n">
+        <v>96.99919</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
@@ -9848,6 +9874,9 @@
       <c r="AL26" s="0" t="n">
         <v>259.49712</v>
       </c>
+      <c r="AM26" s="0" t="n">
+        <v>247.10647</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="28" t="s">
@@ -9958,6 +9987,9 @@
       <c r="AL27" s="0" t="n">
         <v>53.681</v>
       </c>
+      <c r="AM27" s="0" t="n">
+        <v>53.34275</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="28" t="s">
@@ -10014,6 +10046,9 @@
       <c r="AL28" s="0" t="n">
         <v>131.4421</v>
       </c>
+      <c r="AM28" s="0" t="n">
+        <v>127.00975</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="28" t="s">
@@ -10124,6 +10159,9 @@
       <c r="AL29" s="0" t="n">
         <v>473.3997</v>
       </c>
+      <c r="AM29" s="0" t="n">
+        <v>479.86395</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="28" t="s">
@@ -10234,6 +10272,9 @@
       <c r="AL30" s="0" t="n">
         <v>23.57155</v>
       </c>
+      <c r="AM30" s="0" t="n">
+        <v>21.87859</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="29" t="s">
@@ -10344,6 +10385,9 @@
       <c r="AL31" s="0" t="n">
         <v>25.34196</v>
       </c>
+      <c r="AM31" s="0" t="n">
+        <v>28.39049</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="29" t="s">
@@ -10454,6 +10498,9 @@
       <c r="AL32" s="0" t="n">
         <v>62.46432</v>
       </c>
+      <c r="AM32" s="0" t="n">
+        <v>62.95408</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="29" t="s">
@@ -10462,7 +10509,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -10604,6 +10651,10 @@
         <f aca="false">SUM(AL$5:AL$32)</f>
         <v>4534.64353</v>
       </c>
+      <c r="AM35" s="0" t="n">
+        <f aca="false">SUM(AM$5:AM$32)</f>
+        <v>4516.31215</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
@@ -10748,6 +10799,10 @@
       <c r="AL36" s="43" t="n">
         <f aca="false">Regular_Timings!AL35/AL35</f>
         <v>3.42704556536553</v>
+      </c>
+      <c r="AM36" s="43" t="n">
+        <f aca="false">Regular_Timings!AM35/AM35</f>
+        <v>3.62119345537265</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
- Updated progress tracking data
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="135">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">EDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X11</t>
   </si>
   <si>
     <t xml:space="preserve">Sheet</t>
@@ -531,6 +534,9 @@
     <t xml:space="preserve">Crossed 20,000 lines on 04/21/21</t>
   </si>
   <si>
+    <t xml:space="preserve">Crossed 10,000 lines on 07/12/21</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crossed 280,000 on 9/13/2019</t>
   </si>
   <si>
@@ -631,6 +637,9 @@
   </si>
   <si>
     <t xml:space="preserve">Crossed 580,000 on 07/08/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crossed 590,000 on 07/12/21</t>
   </si>
 </sst>
 </file>
@@ -983,7 +992,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1060,7 +1069,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1068,15 +1077,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1096,11 +1097,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1132,11 +1165,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1148,11 +1177,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1263,14 +1288,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>738360</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>186480</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>150480</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1283,7 +1308,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="738360" y="9216000"/>
+          <a:off x="738360" y="9379080"/>
           <a:ext cx="9703800" cy="2053800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1299,14 +1324,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:colOff>18360</xdr:colOff>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>694800</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:colOff>698040</xdr:colOff>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1320,7 +1345,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2225880" y="11674080"/>
+          <a:off x="2229120" y="11834280"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1336,15 +1361,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:colOff>18360</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>660240</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:colOff>663480</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1357,7 +1382,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2225880" y="14281200"/>
+          <a:off x="2229120" y="14444280"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1373,15 +1398,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:colOff>18360</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:colOff>506160</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1394,7 +1419,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2225880" y="16576920"/>
+          <a:off x="2229120" y="16740000"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1410,15 +1435,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>14760</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:colOff>18000</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>456120</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:colOff>459360</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1431,7 +1456,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2225520" y="19731600"/>
+          <a:off x="2228760" y="19894680"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1447,14 +1472,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>44280</xdr:colOff>
-      <xdr:row>129</xdr:row>
+      <xdr:colOff>47520</xdr:colOff>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>480960</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:colOff>484200</xdr:colOff>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1468,7 +1493,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2255040" y="22517640"/>
+          <a:off x="2258280" y="22677840"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1484,15 +1509,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>12240</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:colOff>15480</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>888120</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:colOff>891360</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1505,7 +1530,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2223000" y="24989400"/>
+          <a:off x="2226240" y="25152480"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1522,14 +1547,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
-      <xdr:row>173</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>595800</xdr:colOff>
-      <xdr:row>185</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1542,7 +1567,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3115080" y="30253320"/>
+          <a:off x="3115080" y="30416400"/>
           <a:ext cx="9708120" cy="2138400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1559,13 +1584,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>360360</xdr:colOff>
-      <xdr:row>158</xdr:row>
+      <xdr:row>159</xdr:row>
       <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>910440</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>170</xdr:row>
       <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1579,7 +1604,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3210120" y="27606240"/>
+          <a:off x="3210120" y="27766440"/>
           <a:ext cx="8718120" cy="1964880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1596,13 +1621,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>209880</xdr:colOff>
-      <xdr:row>187</xdr:row>
+      <xdr:row>188</xdr:row>
       <xdr:rowOff>168840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>619920</xdr:colOff>
-      <xdr:row>200</xdr:row>
+      <xdr:row>201</xdr:row>
       <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1616,7 +1641,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3059640" y="32844960"/>
+          <a:off x="3059640" y="33005160"/>
           <a:ext cx="9787680" cy="2191320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1633,13 +1658,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>306720</xdr:colOff>
-      <xdr:row>201</xdr:row>
+      <xdr:row>202</xdr:row>
       <xdr:rowOff>113760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>410040</xdr:colOff>
-      <xdr:row>213</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1653,7 +1678,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3156480" y="35243640"/>
+          <a:off x="3156480" y="35403840"/>
           <a:ext cx="9480960" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1670,14 +1695,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>275040</xdr:colOff>
-      <xdr:row>214</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>58680</xdr:colOff>
-      <xdr:row>225</xdr:row>
-      <xdr:rowOff>147600</xdr:rowOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1690,7 +1715,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3124800" y="37438920"/>
+          <a:off x="3124800" y="37602000"/>
           <a:ext cx="9161280" cy="2044800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1707,14 +1732,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>382680</xdr:colOff>
-      <xdr:row>228</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:row>229</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>9000</xdr:colOff>
       <xdr:row>241</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1744,14 +1769,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>400680</xdr:colOff>
-      <xdr:row>242</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:row>243</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>2880</xdr:colOff>
       <xdr:row>254</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1781,14 +1806,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>373320</xdr:colOff>
-      <xdr:row>255</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:row>256</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1171800</xdr:colOff>
       <xdr:row>268</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1819,13 +1844,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>346320</xdr:colOff>
       <xdr:row>269</xdr:row>
-      <xdr:rowOff>14400</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1201680</xdr:colOff>
-      <xdr:row>280</xdr:row>
-      <xdr:rowOff>171360</xdr:rowOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1855,14 +1880,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>602280</xdr:colOff>
-      <xdr:row>282</xdr:row>
-      <xdr:rowOff>164520</xdr:rowOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1191240</xdr:colOff>
       <xdr:row>294</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1892,14 +1917,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>553680</xdr:colOff>
-      <xdr:row>295</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:row>296</xdr:row>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1180440</xdr:colOff>
       <xdr:row>306</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1930,13 +1955,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>428400</xdr:colOff>
       <xdr:row>307</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1186920</xdr:colOff>
       <xdr:row>319</xdr:row>
-      <xdr:rowOff>141120</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1966,14 +1991,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>550440</xdr:colOff>
-      <xdr:row>319</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:row>320</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1206000</xdr:colOff>
-      <xdr:row>331</xdr:row>
-      <xdr:rowOff>165240</xdr:rowOff>
+      <xdr:row>332</xdr:row>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2004,13 +2029,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>495000</xdr:colOff>
       <xdr:row>332</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>344</xdr:row>
-      <xdr:rowOff>36360</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2040,14 +2065,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>471960</xdr:colOff>
-      <xdr:row>345</xdr:row>
-      <xdr:rowOff>165600</xdr:rowOff>
+      <xdr:row>346</xdr:row>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1194120</xdr:colOff>
       <xdr:row>358</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2078,13 +2103,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>480240</xdr:colOff>
       <xdr:row>360</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1202400</xdr:colOff>
       <xdr:row>373</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2115,13 +2140,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>311040</xdr:colOff>
       <xdr:row>375</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1176120</xdr:colOff>
       <xdr:row>386</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2152,13 +2177,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>465840</xdr:colOff>
       <xdr:row>389</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1188000</xdr:colOff>
-      <xdr:row>400</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:row>401</xdr:row>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2189,13 +2214,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>509040</xdr:colOff>
       <xdr:row>402</xdr:row>
-      <xdr:rowOff>1800</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1190160</xdr:colOff>
       <xdr:row>413</xdr:row>
-      <xdr:rowOff>89640</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2226,13 +2251,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>495000</xdr:colOff>
       <xdr:row>415</xdr:row>
-      <xdr:rowOff>157680</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1207800</xdr:colOff>
       <xdr:row>427</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2263,13 +2288,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>517680</xdr:colOff>
       <xdr:row>428</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1206720</xdr:colOff>
       <xdr:row>440</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:rowOff>65880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2299,14 +2324,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>368640</xdr:colOff>
-      <xdr:row>440</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:row>441</xdr:row>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1195560</xdr:colOff>
       <xdr:row>452</xdr:row>
-      <xdr:rowOff>110160</xdr:rowOff>
+      <xdr:rowOff>125280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2337,13 +2362,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>362880</xdr:colOff>
       <xdr:row>456</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1191960</xdr:colOff>
       <xdr:row>467</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2374,13 +2399,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>313200</xdr:colOff>
       <xdr:row>468</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>23400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>11880</xdr:colOff>
       <xdr:row>479</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2411,13 +2436,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>178920</xdr:colOff>
       <xdr:row>481</xdr:row>
-      <xdr:rowOff>10800</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1193760</xdr:colOff>
       <xdr:row>493</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2448,13 +2473,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>123840</xdr:colOff>
       <xdr:row>494</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1175040</xdr:colOff>
-      <xdr:row>506</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:row>507</xdr:row>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2485,13 +2510,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>143640</xdr:colOff>
       <xdr:row>508</xdr:row>
-      <xdr:rowOff>11160</xdr:rowOff>
+      <xdr:rowOff>26280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1189440</xdr:colOff>
       <xdr:row>520</xdr:row>
-      <xdr:rowOff>145080</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2522,13 +2547,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>55080</xdr:colOff>
       <xdr:row>523</xdr:row>
-      <xdr:rowOff>54720</xdr:rowOff>
+      <xdr:rowOff>69840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1180440</xdr:colOff>
       <xdr:row>537</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2559,13 +2584,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>5760</xdr:colOff>
       <xdr:row>538</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1171080</xdr:colOff>
       <xdr:row>551</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2596,13 +2621,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>552</xdr:row>
-      <xdr:rowOff>93240</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1171800</xdr:colOff>
       <xdr:row>566</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>54360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2633,13 +2658,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1308600</xdr:colOff>
       <xdr:row>566</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1155600</xdr:colOff>
       <xdr:row>581</xdr:row>
-      <xdr:rowOff>14400</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2670,13 +2695,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>8280</xdr:colOff>
       <xdr:row>585</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1190160</xdr:colOff>
       <xdr:row>598</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2707,13 +2732,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>601</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>41760</xdr:colOff>
-      <xdr:row>615</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:row>616</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2747,10 +2772,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W603"/>
+  <dimension ref="A1:W604"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2814,11 +2839,11 @@
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>763.4</v>
+        <v>736.16</v>
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>224.0093</v>
+        <v>210.30995</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2830,11 +2855,11 @@
       </c>
       <c r="O6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>218.1</v>
+        <v>207.61</v>
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>96.1126</v>
+        <v>89.14734</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2846,11 +2871,11 @@
       </c>
       <c r="O7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>299.26</v>
+        <v>285.33</v>
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>93.94092</v>
+        <v>89.44785</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2867,11 +2892,11 @@
       </c>
       <c r="O8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1634.58</v>
+        <v>1548.6</v>
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>397.38036</v>
+        <v>395.9805</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2884,11 +2909,11 @@
       <c r="N9" s="3"/>
       <c r="O9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>162.82</v>
+        <v>153.45</v>
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>49.86798</v>
+        <v>50.28011</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2901,11 +2926,11 @@
       <c r="N10" s="3"/>
       <c r="O10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>138.60975</v>
+        <v>140.02589</v>
       </c>
       <c r="P10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>138.60975</v>
+        <v>140.02589</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2918,11 +2943,11 @@
       <c r="N11" s="3"/>
       <c r="O11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>114.75</v>
+        <v>108.81</v>
       </c>
       <c r="P11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>44.00051</v>
+        <v>44.94206</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2935,11 +2960,11 @@
       <c r="N12" s="3"/>
       <c r="O12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>617.09</v>
+        <v>589.14</v>
       </c>
       <c r="P12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>158.05704</v>
+        <v>160.42696</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,11 +2981,11 @@
       </c>
       <c r="O13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>354.04</v>
+        <v>335.68</v>
       </c>
       <c r="P13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>119.37928</v>
+        <v>121.16786</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2973,11 +2998,11 @@
       </c>
       <c r="O14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>436.89</v>
+        <v>411.26</v>
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>138.64966</v>
+        <v>140.04936</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2993,11 +3018,11 @@
       </c>
       <c r="O15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>2812.44</v>
+        <v>2718.77</v>
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>699.5017</v>
+        <v>697.39256</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3009,11 +3034,11 @@
       </c>
       <c r="O16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>237.57</v>
+        <v>242.28</v>
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
-        <v>15.64652</v>
+        <v>58.14421</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3025,11 +3050,11 @@
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>702.06</v>
+        <v>667.02</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>198.0559</v>
+        <v>198.52091</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,11 +3070,11 @@
       </c>
       <c r="O18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>855.38</v>
+        <v>814.21</v>
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>232.20613</v>
+        <v>230.24696</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3061,11 +3086,11 @@
       </c>
       <c r="O19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>140.71</v>
+        <v>133.93</v>
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>56.22573</v>
+        <v>56.11644</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3077,11 +3102,11 @@
       </c>
       <c r="O20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>476.98</v>
+        <v>452.39</v>
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>157.33707</v>
+        <v>155.56309</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3093,11 +3118,11 @@
       </c>
       <c r="O21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>436.46</v>
+        <v>409.92</v>
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>136.05224</v>
+        <v>134.11112</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3109,11 +3134,11 @@
       </c>
       <c r="O22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>272.59</v>
+        <v>256.29</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>98.81968</v>
+        <v>98.33153</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,11 +3150,11 @@
       </c>
       <c r="O23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>294.42</v>
+        <v>276.76</v>
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>89.23575</v>
+        <v>89.59884</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3142,11 +3167,11 @@
       <c r="N24" s="1"/>
       <c r="O24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>347.88</v>
+        <v>327.61</v>
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>96.99919</v>
+        <v>99.0768</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3158,11 +3183,11 @@
       </c>
       <c r="O25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>845.61</v>
+        <v>799.21</v>
       </c>
       <c r="P25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>247.10647</v>
+        <v>252.55173</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3174,11 +3199,11 @@
       </c>
       <c r="O26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>187.19</v>
+        <v>177.5</v>
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>53.34275</v>
+        <v>53.86057</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3190,11 +3215,11 @@
       </c>
       <c r="O27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>442.08</v>
+        <v>417.1</v>
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>127.00975</v>
+        <v>128.04221</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3210,11 +3235,11 @@
       </c>
       <c r="O28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1800.39</v>
+        <v>1701.77</v>
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>479.86395</v>
+        <v>473.46779</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3226,11 +3251,11 @@
       </c>
       <c r="O29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>46.47</v>
+        <v>43.79</v>
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>21.87859</v>
+        <v>21.88631</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,11 +3267,11 @@
       </c>
       <c r="O30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>33.34</v>
+        <v>31.74</v>
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>28.39049</v>
+        <v>24.85855</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3258,11 +3283,11 @@
       </c>
       <c r="O31" s="9" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>171.26</v>
+        <v>162.32</v>
       </c>
       <c r="P31" s="9" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>62.95408</v>
+        <v>59.76464</v>
       </c>
       <c r="Q31" s="9"/>
     </row>
@@ -3271,7 +3296,7 @@
         <v>33</v>
       </c>
       <c r="C32" s="4" t="n">
-        <v>17108</v>
+        <v>18796</v>
       </c>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
@@ -3290,49 +3315,54 @@
       </c>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="11" t="s">
+    <row r="34" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="12" t="n">
+      <c r="C34" s="4" t="n">
+        <v>16242</v>
+      </c>
+      <c r="E34" s="0" t="str">
+        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!AJ:AJ)), Miletone_Tracking!AJ:AJ )</f>
+        <v>Crossed 10,000 lines on 07/12/21</v>
+      </c>
+      <c r="N34" s="3"/>
+    </row>
+    <row r="35" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="12" t="n">
         <v>5260</v>
       </c>
-      <c r="O34" s="0"/>
-      <c r="P34" s="0"/>
-      <c r="Q34" s="0"/>
-      <c r="V34" s="0"/>
-      <c r="W34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>878</v>
-      </c>
+      <c r="O35" s="0"/>
+      <c r="P35" s="0"/>
+      <c r="Q35" s="0"/>
+      <c r="V35" s="0"/>
+      <c r="W35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="4" t="n">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="4" t="n">
         <v>190</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="4" t="n">
-        <v>22184</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
         <v>39</v>
       </c>
       <c r="C39" s="4" t="n">
-        <v>825</v>
+        <v>22184</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3340,191 +3370,196 @@
         <v>40</v>
       </c>
       <c r="C40" s="4" t="n">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="4" t="n">
         <v>21021</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="0" t="s">
+    <row r="42" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="B43" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="0" t="n">
         <f aca="false">4650-865</f>
         <v>3785</v>
       </c>
-      <c r="I42" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14" t="s">
+      <c r="I43" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="0" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="B44" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="0" t="n">
         <f aca="false">10319-580</f>
         <v>9739</v>
       </c>
-      <c r="I43" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+      <c r="I44" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="0" t="n">
-        <v>23768</v>
-      </c>
-      <c r="E44" s="16"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="0" t="n">
+        <v>23768</v>
+      </c>
+      <c r="E45" s="16"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="0" t="n">
         <v>3357</v>
       </c>
-      <c r="E45" s="16"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="4" t="n">
-        <f aca="false">SUM(C4:C45)</f>
-        <v>581502</v>
-      </c>
-      <c r="E47" s="0" t="str">
-        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!A:A)), Miletone_Tracking!A:A)</f>
-        <v>Crossed 580,000 on 07/08/21</v>
-      </c>
-      <c r="N47" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="O47" s="0" t="n">
-        <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
-        <v>16354.44</v>
-      </c>
-      <c r="P47" s="0" t="n">
-        <f aca="false">INDEX(Parallel_Timings!35:35,COUNT(Parallel_Timings!35:35,1,1))</f>
-        <v>4534.64353</v>
-      </c>
+      <c r="E46" s="16"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="4" t="n">
+        <f aca="false">SUM(C4:C46)</f>
+        <v>599432</v>
+      </c>
+      <c r="E48" s="0" t="str">
+        <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!A:A)), Miletone_Tracking!A:A)</f>
+        <v>Crossed 590,000 on 07/12/21</v>
+      </c>
+      <c r="N48" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="4" t="n">
+      <c r="O48" s="0" t="n">
+        <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
+        <v>15647.65</v>
+      </c>
+      <c r="P48" s="0" t="n">
+        <f aca="false">INDEX(Parallel_Timings!35:35,COUNT(Parallel_Timings!35:35,1,1))</f>
+        <v>4516.31215</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="N48" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="P48" s="17" t="n">
-        <f aca="false">O47/P47</f>
-        <v>3.60655471412546</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+      <c r="N49" s="0" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R55" s="0" t="s">
+      <c r="P49" s="17" t="n">
+        <f aca="false">O48/P48</f>
+        <v>3.46469630094102</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="0" t="s">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R56" s="0" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="0" t="s">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="0" t="s">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="0" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C105" s="0" t="s">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C90" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="0" t="s">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C106" s="0" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S145" s="18" t="n">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C121" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S146" s="18" t="n">
         <v>43729</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C157" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S161" s="18" t="n">
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C158" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S162" s="18" t="n">
         <v>43780</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S174" s="18" t="n">
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C173" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S175" s="18" t="n">
         <v>43765</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S189" s="18" t="n">
+    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S190" s="18" t="n">
         <v>43799</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S203" s="18" t="n">
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S204" s="18" t="n">
         <v>43814</v>
       </c>
     </row>
-    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S215" s="18" t="n">
+    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S216" s="18" t="n">
         <v>43827</v>
       </c>
     </row>
-    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S230" s="18" t="n">
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S231" s="18" t="n">
         <v>43930</v>
       </c>
     </row>
-    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S244" s="18" t="n">
+    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S245" s="18" t="n">
         <v>43939</v>
       </c>
     </row>
-    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S257" s="18" t="n">
+    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S258" s="18" t="n">
         <v>43955</v>
       </c>
-    </row>
-    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S265" s="18"/>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="S266" s="18"/>
@@ -3539,132 +3574,135 @@
       <c r="S269" s="18"/>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S270" s="18" t="n">
+      <c r="S270" s="18"/>
+    </row>
+    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S271" s="18" t="n">
         <v>43968</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S284" s="18" t="n">
+    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S285" s="18" t="n">
         <v>44025</v>
       </c>
     </row>
-    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S297" s="18" t="n">
+    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S298" s="18" t="n">
         <v>44031</v>
       </c>
     </row>
-    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S309" s="18" t="n">
+    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S310" s="18" t="n">
         <v>44050</v>
       </c>
     </row>
-    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S323" s="18" t="n">
+    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S324" s="18" t="n">
         <v>44053</v>
       </c>
     </row>
-    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S336" s="18" t="n">
+    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S337" s="18" t="n">
         <v>44072</v>
       </c>
     </row>
-    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S349" s="18" t="n">
+    <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S350" s="18" t="n">
         <v>44094</v>
       </c>
     </row>
-    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S364" s="18" t="n">
+    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S365" s="18" t="n">
         <v>44101</v>
       </c>
     </row>
-    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S378" s="18" t="n">
+    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S379" s="18" t="n">
         <v>44125</v>
       </c>
     </row>
-    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S392" s="18" t="n">
+    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S393" s="18" t="n">
         <v>44130</v>
       </c>
     </row>
-    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S405" s="18" t="n">
+    <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S406" s="18" t="n">
         <v>44136</v>
       </c>
     </row>
-    <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S419" s="18" t="n">
+    <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S420" s="18" t="n">
         <v>44157</v>
       </c>
     </row>
-    <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S432" s="18" t="n">
+    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S433" s="18" t="n">
         <v>44164</v>
       </c>
     </row>
-    <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S444" s="18" t="n">
+    <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S445" s="18" t="n">
         <v>44171</v>
       </c>
     </row>
-    <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S459" s="18" t="n">
+    <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S460" s="18" t="n">
         <v>44199</v>
       </c>
     </row>
-    <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S471" s="18" t="n">
+    <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S472" s="18" t="n">
         <v>44218</v>
       </c>
     </row>
-    <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S484" s="18" t="n">
+    <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S485" s="18" t="n">
         <v>44220</v>
       </c>
     </row>
-    <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S498" s="18" t="n">
+    <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S499" s="18" t="n">
         <v>44241</v>
       </c>
     </row>
-    <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S511" s="18" t="n">
+    <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S512" s="18" t="n">
         <v>44241</v>
       </c>
     </row>
-    <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S527" s="18" t="n">
+    <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S528" s="18" t="n">
         <v>44284</v>
       </c>
     </row>
-    <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J540" s="0" t="n">
+    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J541" s="0" t="n">
         <v>44</v>
       </c>
     </row>
-    <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S541" s="18" t="n">
+    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S542" s="18" t="n">
         <v>44290</v>
       </c>
     </row>
-    <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S556" s="18" t="n">
+    <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S557" s="18" t="n">
         <v>44318</v>
       </c>
     </row>
-    <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S570" s="18" t="n">
+    <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S571" s="18" t="n">
         <v>44325</v>
       </c>
     </row>
-    <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S587" s="18" t="n">
+    <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S588" s="18" t="n">
         <v>44367</v>
       </c>
     </row>
-    <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S603" s="18" t="n">
+    <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S604" s="18" t="n">
         <v>44370</v>
       </c>
     </row>
@@ -3688,11 +3726,11 @@
   <dimension ref="A2:BK109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="T5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="AF5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="topRight" activeCell="AF1" activeCellId="0" sqref="AF1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AA45" activeCellId="0" sqref="AA45"/>
+      <selection pane="bottomRight" activeCell="AM17" activeCellId="0" sqref="AM17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3713,152 +3751,155 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" s="19" customFormat="true" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="20" t="n">
         <v>44136</v>
       </c>
-      <c r="D4" s="21" t="n">
+      <c r="D4" s="20" t="n">
         <v>44143</v>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="E4" s="21" t="n">
         <v>44151</v>
       </c>
-      <c r="F4" s="22" t="n">
+      <c r="F4" s="21" t="n">
         <v>44157</v>
       </c>
       <c r="G4" s="20" t="n">
         <v>44164</v>
       </c>
-      <c r="H4" s="23" t="n">
+      <c r="H4" s="21" t="n">
         <v>44171</v>
       </c>
-      <c r="I4" s="23" t="n">
+      <c r="I4" s="21" t="n">
         <v>44178</v>
       </c>
-      <c r="J4" s="22" t="n">
+      <c r="J4" s="21" t="n">
         <v>44185</v>
       </c>
-      <c r="K4" s="22" t="n">
+      <c r="K4" s="21" t="n">
         <v>44192</v>
       </c>
-      <c r="L4" s="22" t="n">
+      <c r="L4" s="21" t="n">
         <v>43833</v>
       </c>
-      <c r="M4" s="22" t="n">
+      <c r="M4" s="21" t="n">
         <v>44206</v>
       </c>
-      <c r="N4" s="22" t="n">
+      <c r="N4" s="21" t="n">
         <v>44213</v>
       </c>
-      <c r="O4" s="22" t="n">
+      <c r="O4" s="21" t="n">
         <v>44220</v>
       </c>
-      <c r="P4" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q4" s="24" t="s">
+      <c r="P4" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="R4" s="22" t="n">
+      <c r="Q4" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="21" t="n">
         <v>44241</v>
       </c>
-      <c r="S4" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="T4" s="22" t="n">
+      <c r="S4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="T4" s="21" t="n">
         <v>44255</v>
       </c>
-      <c r="U4" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="V4" s="24" t="s">
+      <c r="U4" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="25" t="n">
+      <c r="V4" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="W4" s="23" t="n">
         <v>44276</v>
       </c>
-      <c r="X4" s="25" t="n">
+      <c r="X4" s="23" t="n">
         <v>44283</v>
       </c>
-      <c r="Y4" s="25" t="n">
+      <c r="Y4" s="23" t="n">
         <v>44290</v>
       </c>
-      <c r="Z4" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA4" s="24" t="s">
+      <c r="Z4" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="22" t="n">
+      <c r="AA4" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB4" s="21" t="n">
         <v>44311</v>
       </c>
-      <c r="AC4" s="23" t="n">
+      <c r="AC4" s="21" t="n">
         <v>44318</v>
       </c>
-      <c r="AD4" s="23" t="n">
+      <c r="AD4" s="21" t="n">
         <v>44325</v>
       </c>
-      <c r="AE4" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF4" s="23" t="n">
+      <c r="AE4" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF4" s="21" t="n">
         <v>44339</v>
       </c>
-      <c r="AG4" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH4" s="23" t="n">
+      <c r="AG4" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH4" s="21" t="n">
         <v>44353</v>
       </c>
-      <c r="AI4" s="23" t="n">
+      <c r="AI4" s="21" t="n">
         <v>44360</v>
       </c>
-      <c r="AJ4" s="23" t="n">
+      <c r="AJ4" s="21" t="n">
         <v>44367</v>
       </c>
-      <c r="AK4" s="23" t="n">
+      <c r="AK4" s="21" t="n">
         <v>44374</v>
       </c>
-      <c r="AL4" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM4" s="26" t="s">
+      <c r="AL4" s="24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" s="19" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+      <c r="AM4" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="22"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="22"/>
-      <c r="AA5" s="22"/>
-      <c r="AB5" s="22"/>
+      <c r="AN4" s="21" t="n">
+        <v>44395</v>
+      </c>
+    </row>
+    <row r="5" s="26" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
       <c r="AC5" s="0" t="n">
         <v>636.13</v>
       </c>
@@ -3892,16 +3933,19 @@
       <c r="AM5" s="0" t="n">
         <v>1165.64</v>
       </c>
-    </row>
-    <row r="6" s="11" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="28" t="s">
+      <c r="AN5" s="0" t="n">
+        <v>1179.7</v>
+      </c>
+    </row>
+    <row r="6" s="33" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="32" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0" t="n">
         <v>509.17</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="33" t="n">
         <v>561.22</v>
       </c>
       <c r="E6" s="0"/>
@@ -4007,9 +4051,12 @@
       <c r="AM6" s="0" t="n">
         <v>763.4</v>
       </c>
+      <c r="AN6" s="0" t="n">
+        <v>736.16</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -4123,9 +4170,12 @@
       <c r="AM7" s="0" t="n">
         <v>218.1</v>
       </c>
+      <c r="AN7" s="0" t="n">
+        <v>207.61</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -4227,9 +4277,12 @@
       <c r="AM8" s="0" t="n">
         <v>299.26</v>
       </c>
+      <c r="AN8" s="0" t="n">
+        <v>285.33</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -4343,9 +4396,12 @@
       <c r="AM9" s="0" t="n">
         <v>1634.58</v>
       </c>
+      <c r="AN9" s="0" t="n">
+        <v>1548.6</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -4459,9 +4515,12 @@
       <c r="AM10" s="0" t="n">
         <v>162.82</v>
       </c>
+      <c r="AN10" s="0" t="n">
+        <v>153.45</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -4575,9 +4634,12 @@
       <c r="AM11" s="0" t="n">
         <v>485.04</v>
       </c>
+      <c r="AN11" s="0" t="n">
+        <v>459.3</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="34" t="s">
         <v>12</v>
       </c>
       <c r="L12" s="0" t="n">
@@ -4664,9 +4726,12 @@
       <c r="AM12" s="0" t="n">
         <v>114.75</v>
       </c>
+      <c r="AN12" s="0" t="n">
+        <v>108.81</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="34" t="s">
         <v>13</v>
       </c>
       <c r="P13" s="0" t="n">
@@ -4741,9 +4806,12 @@
       <c r="AM13" s="0" t="n">
         <v>617.09</v>
       </c>
+      <c r="AN13" s="0" t="n">
+        <v>589.14</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -4857,9 +4925,12 @@
       <c r="AM14" s="0" t="n">
         <v>354.04</v>
       </c>
+      <c r="AN14" s="0" t="n">
+        <v>335.68</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="35" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -4973,9 +5044,12 @@
       <c r="AM15" s="0" t="n">
         <v>436.89</v>
       </c>
+      <c r="AN15" s="0" t="n">
+        <v>411.26</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -5089,9 +5163,12 @@
       <c r="AM16" s="0" t="n">
         <v>2812.44</v>
       </c>
+      <c r="AN16" s="0" t="n">
+        <v>2718.77</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="35" t="s">
         <v>17</v>
       </c>
       <c r="AD17" s="0" t="n">
@@ -5124,9 +5201,12 @@
       <c r="AM17" s="0" t="n">
         <v>237.57</v>
       </c>
+      <c r="AN17" s="0" t="n">
+        <v>242.28</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -5240,9 +5320,12 @@
       <c r="AM18" s="0" t="n">
         <v>702.06</v>
       </c>
+      <c r="AN18" s="0" t="n">
+        <v>667.02</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="35" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -5356,9 +5439,12 @@
       <c r="AM19" s="0" t="n">
         <v>855.38</v>
       </c>
+      <c r="AN19" s="0" t="n">
+        <v>814.21</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="35" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -5472,9 +5558,12 @@
       <c r="AM20" s="0" t="n">
         <v>140.71</v>
       </c>
+      <c r="AN20" s="0" t="n">
+        <v>133.93</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -5588,9 +5677,12 @@
       <c r="AM21" s="0" t="n">
         <v>476.98</v>
       </c>
+      <c r="AN21" s="0" t="n">
+        <v>452.39</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="35" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -5704,9 +5796,12 @@
       <c r="AM22" s="0" t="n">
         <v>436.46</v>
       </c>
+      <c r="AN22" s="0" t="n">
+        <v>409.92</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="35" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -5820,9 +5915,12 @@
       <c r="AM23" s="0" t="n">
         <v>272.59</v>
       </c>
+      <c r="AN23" s="0" t="n">
+        <v>256.29</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -5936,9 +6034,12 @@
       <c r="AM24" s="0" t="n">
         <v>294.42</v>
       </c>
+      <c r="AN24" s="0" t="n">
+        <v>276.76</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="35" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -6052,9 +6153,12 @@
       <c r="AM25" s="0" t="n">
         <v>347.88</v>
       </c>
+      <c r="AN25" s="0" t="n">
+        <v>327.61</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -6168,9 +6272,12 @@
       <c r="AM26" s="0" t="n">
         <v>845.61</v>
       </c>
+      <c r="AN26" s="0" t="n">
+        <v>799.21</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -6284,9 +6391,12 @@
       <c r="AM27" s="0" t="n">
         <v>187.19</v>
       </c>
+      <c r="AN27" s="0" t="n">
+        <v>177.5</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="35" t="s">
         <v>28</v>
       </c>
       <c r="U28" s="0" t="n">
@@ -6346,9 +6456,12 @@
       <c r="AM28" s="0" t="n">
         <v>442.08</v>
       </c>
+      <c r="AN28" s="0" t="n">
+        <v>417.1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -6462,9 +6575,12 @@
       <c r="AM29" s="0" t="n">
         <v>1800.39</v>
       </c>
+      <c r="AN29" s="0" t="n">
+        <v>1701.77</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="35" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -6578,9 +6694,12 @@
       <c r="AM30" s="0" t="n">
         <v>46.47</v>
       </c>
+      <c r="AN30" s="0" t="n">
+        <v>43.79</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="34" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -6694,9 +6813,12 @@
       <c r="AM31" s="0" t="n">
         <v>33.34</v>
       </c>
+      <c r="AN31" s="0" t="n">
+        <v>31.74</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -6810,15 +6932,18 @@
       <c r="AM32" s="0" t="n">
         <v>171.26</v>
       </c>
+      <c r="AN32" s="0" t="n">
+        <v>162.32</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -6968,192 +7093,200 @@
         <f aca="false">SUM(AM$5:AM$32)</f>
         <v>16354.44</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AN35" s="0" t="n">
+        <f aca="false">SUM(AN$5:AN$32)</f>
+        <v>15647.65</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31" t="n">
+        <v>77</v>
+      </c>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37" t="n">
         <f aca="false">D35/C35</f>
         <v>1.0558825271854</v>
       </c>
-      <c r="E36" s="31" t="n">
+      <c r="E36" s="37" t="n">
         <f aca="false">E35/D35</f>
         <v>0.916849500061912</v>
       </c>
-      <c r="F36" s="31" t="n">
+      <c r="F36" s="37" t="n">
         <f aca="false">F35/E35</f>
         <v>1.10350896258914</v>
       </c>
-      <c r="G36" s="31" t="n">
+      <c r="G36" s="37" t="n">
         <f aca="false">G35/F35</f>
         <v>1.03987375176407</v>
       </c>
-      <c r="H36" s="31" t="n">
+      <c r="H36" s="37" t="n">
         <f aca="false">H35/G35</f>
         <v>1.06665722673939</v>
       </c>
-      <c r="I36" s="31" t="n">
+      <c r="I36" s="37" t="n">
         <f aca="false">I35/H35</f>
         <v>1.02227013104336</v>
       </c>
-      <c r="J36" s="31" t="n">
+      <c r="J36" s="37" t="n">
         <f aca="false">J35/I35</f>
         <v>0.968844995695285</v>
       </c>
-      <c r="K36" s="31" t="n">
+      <c r="K36" s="37" t="n">
         <f aca="false">K35/J35</f>
         <v>1.00756682988645</v>
       </c>
-      <c r="L36" s="31" t="n">
+      <c r="L36" s="37" t="n">
         <f aca="false">L35/K35</f>
         <v>1.03365334779935</v>
       </c>
-      <c r="M36" s="31" t="n">
+      <c r="M36" s="37" t="n">
         <f aca="false">M35/L35</f>
         <v>0.972899387020888</v>
       </c>
-      <c r="N36" s="31" t="n">
+      <c r="N36" s="37" t="n">
         <f aca="false">N35/M35</f>
         <v>1.06944594764067</v>
       </c>
-      <c r="O36" s="31" t="n">
+      <c r="O36" s="37" t="n">
         <f aca="false">O35/N35</f>
         <v>1.03914029657021</v>
       </c>
-      <c r="P36" s="31" t="n">
+      <c r="P36" s="37" t="n">
         <f aca="false">P35/O35</f>
         <v>1.0268997847368</v>
       </c>
-      <c r="Q36" s="31" t="n">
+      <c r="Q36" s="37" t="n">
         <f aca="false">Q35/P35</f>
         <v>1.00478259658715</v>
       </c>
-      <c r="R36" s="31" t="n">
+      <c r="R36" s="37" t="n">
         <f aca="false">R35/Q35</f>
         <v>1.02439095646859</v>
       </c>
-      <c r="S36" s="31" t="n">
+      <c r="S36" s="37" t="n">
         <f aca="false">S35/R35</f>
         <v>0.994786033590229</v>
       </c>
-      <c r="T36" s="31" t="n">
+      <c r="T36" s="37" t="n">
         <f aca="false">T35/S35</f>
         <v>0.995561439657853</v>
       </c>
-      <c r="U36" s="31" t="n">
+      <c r="U36" s="37" t="n">
         <f aca="false">U35/T35</f>
         <v>1.10342734655874</v>
       </c>
-      <c r="V36" s="31" t="n">
+      <c r="V36" s="37" t="n">
         <f aca="false">V35/U35</f>
         <v>0.949124255714387</v>
       </c>
-      <c r="W36" s="31" t="n">
+      <c r="W36" s="37" t="n">
         <f aca="false">W35/V35</f>
         <v>0.990510153289931</v>
       </c>
-      <c r="X36" s="31" t="n">
+      <c r="X36" s="37" t="n">
         <f aca="false">X35/W35</f>
         <v>0.963401613497919</v>
       </c>
-      <c r="Y36" s="31" t="n">
+      <c r="Y36" s="37" t="n">
         <f aca="false">Y35/X35</f>
         <v>1.04446534528375</v>
       </c>
-      <c r="Z36" s="31" t="n">
+      <c r="Z36" s="37" t="n">
         <f aca="false">Z35/Y35</f>
         <v>0.902660745410508</v>
       </c>
-      <c r="AA36" s="31" t="n">
+      <c r="AA36" s="37" t="n">
         <f aca="false">AA35/Z35</f>
         <v>1.14252240687931</v>
       </c>
-      <c r="AB36" s="31" t="n">
+      <c r="AB36" s="37" t="n">
         <f aca="false">AB35/AA35</f>
         <v>0.936850704356737</v>
       </c>
-      <c r="AC36" s="31" t="n">
+      <c r="AC36" s="37" t="n">
         <f aca="false">AC35/AB35</f>
         <v>1.03187444677672</v>
       </c>
-      <c r="AD36" s="31" t="n">
+      <c r="AD36" s="37" t="n">
         <f aca="false">AD35/AC35</f>
         <v>1.11331883538682</v>
       </c>
-      <c r="AE36" s="31" t="n">
+      <c r="AE36" s="37" t="n">
         <f aca="false">AE35/AD35</f>
         <v>1.00181950741378</v>
       </c>
-      <c r="AF36" s="31" t="n">
+      <c r="AF36" s="37" t="n">
         <f aca="false">AF35/AE35</f>
         <v>1.03424321595765</v>
       </c>
-      <c r="AG36" s="31" t="n">
+      <c r="AG36" s="37" t="n">
         <f aca="false">AG35/AF35</f>
         <v>1.00792537781632</v>
       </c>
-      <c r="AH36" s="31" t="n">
+      <c r="AH36" s="37" t="n">
         <f aca="false">AH35/AG35</f>
         <v>0.970324194852549</v>
       </c>
-      <c r="AI36" s="31" t="n">
+      <c r="AI36" s="37" t="n">
         <f aca="false">AI35/AH35</f>
         <v>1.04927844854803</v>
       </c>
-      <c r="AJ36" s="31" t="n">
+      <c r="AJ36" s="37" t="n">
         <f aca="false">AJ35/AI35</f>
         <v>0.940307515998851</v>
       </c>
-      <c r="AK36" s="31" t="n">
+      <c r="AK36" s="37" t="n">
         <f aca="false">AK35/AJ35</f>
         <v>0.954601895704387</v>
       </c>
-      <c r="AL36" s="31" t="n">
+      <c r="AL36" s="37" t="n">
         <f aca="false">AL35/AK35</f>
         <v>1.03769659098725</v>
       </c>
-      <c r="AM36" s="31" t="n">
+      <c r="AM36" s="37" t="n">
         <f aca="false">AM35/AL35</f>
         <v>1.0523801464953</v>
       </c>
+      <c r="AN36" s="37" t="n">
+        <f aca="false">AN35/AM35</f>
+        <v>0.956782989818056</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
-      <c r="H38" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="L38" s="33" t="s">
+      <c r="H38" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="O38" s="34" t="s">
+      <c r="L38" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="P38" s="33" t="s">
+      <c r="O38" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="U38" s="33" t="s">
+      <c r="P38" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="AC38" s="33" t="s">
+      <c r="U38" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="AD38" s="33" t="s">
+      <c r="AC38" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="AL38" s="35"/>
+      <c r="AD38" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL38" s="41"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI82" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BJ82" s="0" t="n">
         <v>636.13</v>
@@ -7430,7 +7563,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI108" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="BJ108" s="0" t="n">
         <v>27.54</v>
@@ -7466,14 +7599,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AM38"/>
+  <dimension ref="A2:AN38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AD53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AD11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="AD1" activeCellId="0" sqref="AD1"/>
-      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
-      <selection pane="bottomRight" activeCell="AM17" activeCellId="0" sqref="AM17"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="AD18" activeCellId="0" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7492,149 +7625,155 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" s="38" customFormat="true" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0"/>
-      <c r="B4" s="0"/>
-      <c r="C4" s="36" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" s="43" customFormat="true" ht="42.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="42" t="n">
         <v>44136</v>
       </c>
-      <c r="D4" s="37" t="n">
+      <c r="D4" s="42" t="n">
         <v>44144</v>
       </c>
-      <c r="E4" s="36" t="n">
+      <c r="E4" s="42" t="n">
         <v>44151</v>
       </c>
-      <c r="F4" s="36" t="n">
+      <c r="F4" s="42" t="n">
         <v>44157</v>
       </c>
-      <c r="G4" s="36" t="n">
+      <c r="G4" s="42" t="n">
         <v>44164</v>
       </c>
-      <c r="H4" s="36" t="n">
+      <c r="H4" s="42" t="n">
         <v>44171</v>
       </c>
-      <c r="I4" s="36" t="n">
+      <c r="I4" s="42" t="n">
         <v>44178</v>
       </c>
-      <c r="J4" s="36" t="n">
+      <c r="J4" s="42" t="n">
         <v>44185</v>
       </c>
-      <c r="K4" s="36" t="n">
+      <c r="K4" s="42" t="n">
         <v>44192</v>
       </c>
-      <c r="L4" s="36" t="n">
+      <c r="L4" s="42" t="n">
         <v>43833</v>
       </c>
-      <c r="M4" s="36" t="n">
+      <c r="M4" s="42" t="n">
         <v>44206</v>
       </c>
-      <c r="N4" s="36" t="n">
+      <c r="N4" s="42" t="n">
         <v>44213</v>
       </c>
-      <c r="O4" s="36" t="n">
+      <c r="O4" s="42" t="n">
         <v>44220</v>
       </c>
-      <c r="P4" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q4" s="24" t="s">
+      <c r="P4" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="R4" s="25" t="n">
+      <c r="Q4" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="23" t="n">
         <v>44241</v>
       </c>
-      <c r="S4" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="T4" s="25" t="n">
+      <c r="S4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="T4" s="23" t="n">
         <v>44255</v>
       </c>
-      <c r="U4" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="V4" s="24" t="s">
+      <c r="U4" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="25" t="n">
+      <c r="V4" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="W4" s="23" t="n">
         <v>44276</v>
       </c>
-      <c r="X4" s="25" t="n">
+      <c r="X4" s="23" t="n">
         <v>44276</v>
       </c>
-      <c r="Y4" s="25" t="n">
+      <c r="Y4" s="23" t="n">
         <v>44290</v>
       </c>
-      <c r="Z4" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA4" s="24" t="s">
+      <c r="Z4" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="22" t="n">
+      <c r="AA4" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB4" s="21" t="n">
         <v>44311</v>
       </c>
-      <c r="AC4" s="22" t="n">
+      <c r="AC4" s="21" t="n">
         <v>44318</v>
       </c>
-      <c r="AD4" s="36" t="n">
+      <c r="AD4" s="42" t="n">
         <v>44325</v>
       </c>
-      <c r="AE4" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG4" s="26" t="s">
+      <c r="AE4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AH4" s="23" t="n">
+      <c r="AG4" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH4" s="21" t="n">
         <v>44353</v>
       </c>
-      <c r="AI4" s="23" t="n">
+      <c r="AI4" s="21" t="n">
         <v>44360</v>
       </c>
-      <c r="AJ4" s="23" t="n">
+      <c r="AJ4" s="21" t="n">
         <v>44367</v>
       </c>
-      <c r="AK4" s="23" t="n">
+      <c r="AK4" s="21" t="n">
         <v>44374</v>
       </c>
-      <c r="AL4" s="23" t="n">
+      <c r="AL4" s="21" t="n">
         <v>44383</v>
       </c>
-    </row>
-    <row r="5" s="38" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AM4" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN4" s="21" t="n">
+        <v>44395</v>
+      </c>
+    </row>
+    <row r="5" s="46" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="42"/>
-      <c r="AA5" s="42"/>
-      <c r="AB5" s="42"/>
+        <v>75</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
       <c r="AC5" s="6" t="n">
         <v>272.20742</v>
       </c>
@@ -7665,10 +7804,13 @@
       <c r="AM5" s="0" t="n">
         <v>271.32528</v>
       </c>
-    </row>
-    <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AN5" s="0" t="n">
+        <v>252.32084</v>
+      </c>
+    </row>
+    <row r="6" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -7779,9 +7921,12 @@
       <c r="AM6" s="0" t="n">
         <v>224.0093</v>
       </c>
+      <c r="AN6" s="0" t="n">
+        <v>210.30995</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -7892,9 +8037,12 @@
       <c r="AM7" s="0" t="n">
         <v>96.1126</v>
       </c>
+      <c r="AN7" s="0" t="n">
+        <v>89.14734</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="34" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -7993,9 +8141,12 @@
       <c r="AM8" s="0" t="n">
         <v>93.94092</v>
       </c>
+      <c r="AN8" s="0" t="n">
+        <v>89.44785</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -8106,9 +8257,12 @@
       <c r="AM9" s="0" t="n">
         <v>397.38036</v>
       </c>
+      <c r="AN9" s="0" t="n">
+        <v>395.9805</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -8219,9 +8373,12 @@
       <c r="AM10" s="0" t="n">
         <v>49.86798</v>
       </c>
+      <c r="AN10" s="0" t="n">
+        <v>50.28011</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -8332,9 +8489,12 @@
       <c r="AM11" s="0" t="n">
         <v>138.60975</v>
       </c>
+      <c r="AN11" s="0" t="n">
+        <v>140.02589</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="34" t="s">
         <v>12</v>
       </c>
       <c r="L12" s="0" t="n">
@@ -8418,9 +8578,12 @@
       <c r="AM12" s="0" t="n">
         <v>44.00051</v>
       </c>
+      <c r="AN12" s="0" t="n">
+        <v>44.94206</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="34" t="s">
         <v>13</v>
       </c>
       <c r="P13" s="0" t="n">
@@ -8492,9 +8655,12 @@
       <c r="AM13" s="0" t="n">
         <v>158.05704</v>
       </c>
+      <c r="AN13" s="0" t="n">
+        <v>160.42696</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -8605,9 +8771,12 @@
       <c r="AM14" s="0" t="n">
         <v>119.37928</v>
       </c>
+      <c r="AN14" s="0" t="n">
+        <v>121.16786</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="35" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -8718,9 +8887,12 @@
       <c r="AM15" s="0" t="n">
         <v>138.64966</v>
       </c>
+      <c r="AN15" s="0" t="n">
+        <v>140.04936</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -8831,9 +9003,12 @@
       <c r="AM16" s="0" t="n">
         <v>699.5017</v>
       </c>
+      <c r="AN16" s="0" t="n">
+        <v>697.39256</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="35" t="s">
         <v>17</v>
       </c>
       <c r="AD17" s="0" t="n">
@@ -8860,9 +9035,12 @@
       <c r="AL17" s="0" t="n">
         <v>15.64652</v>
       </c>
+      <c r="AN17" s="0" t="n">
+        <v>58.14421</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -8973,9 +9151,12 @@
       <c r="AM18" s="0" t="n">
         <v>198.0559</v>
       </c>
+      <c r="AN18" s="0" t="n">
+        <v>198.52091</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="35" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -9086,9 +9267,12 @@
       <c r="AM19" s="0" t="n">
         <v>232.20613</v>
       </c>
+      <c r="AN19" s="0" t="n">
+        <v>230.24696</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="35" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -9199,9 +9383,12 @@
       <c r="AM20" s="0" t="n">
         <v>56.22573</v>
       </c>
+      <c r="AN20" s="0" t="n">
+        <v>56.11644</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -9312,9 +9499,12 @@
       <c r="AM21" s="0" t="n">
         <v>157.33707</v>
       </c>
+      <c r="AN21" s="0" t="n">
+        <v>155.56309</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="35" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -9425,9 +9615,12 @@
       <c r="AM22" s="0" t="n">
         <v>136.05224</v>
       </c>
+      <c r="AN22" s="0" t="n">
+        <v>134.11112</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="35" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -9538,9 +9731,12 @@
       <c r="AM23" s="0" t="n">
         <v>98.81968</v>
       </c>
+      <c r="AN23" s="0" t="n">
+        <v>98.33153</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -9651,9 +9847,12 @@
       <c r="AM24" s="0" t="n">
         <v>89.23575</v>
       </c>
+      <c r="AN24" s="0" t="n">
+        <v>89.59884</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="35" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -9764,9 +9963,12 @@
       <c r="AM25" s="0" t="n">
         <v>96.99919</v>
       </c>
+      <c r="AN25" s="0" t="n">
+        <v>99.0768</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -9877,9 +10079,12 @@
       <c r="AM26" s="0" t="n">
         <v>247.10647</v>
       </c>
+      <c r="AN26" s="0" t="n">
+        <v>252.55173</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -9990,9 +10195,12 @@
       <c r="AM27" s="0" t="n">
         <v>53.34275</v>
       </c>
+      <c r="AN27" s="0" t="n">
+        <v>53.86057</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="35" t="s">
         <v>28</v>
       </c>
       <c r="U28" s="0" t="n">
@@ -10049,9 +10257,12 @@
       <c r="AM28" s="0" t="n">
         <v>127.00975</v>
       </c>
+      <c r="AN28" s="0" t="n">
+        <v>128.04221</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -10162,9 +10373,12 @@
       <c r="AM29" s="0" t="n">
         <v>479.86395</v>
       </c>
+      <c r="AN29" s="0" t="n">
+        <v>473.46779</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="35" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -10275,9 +10489,12 @@
       <c r="AM30" s="0" t="n">
         <v>21.87859</v>
       </c>
+      <c r="AN30" s="0" t="n">
+        <v>21.88631</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="34" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -10388,9 +10605,12 @@
       <c r="AM31" s="0" t="n">
         <v>28.39049</v>
       </c>
+      <c r="AN31" s="0" t="n">
+        <v>24.85855</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -10501,15 +10721,18 @@
       <c r="AM32" s="0" t="n">
         <v>62.95408</v>
       </c>
+      <c r="AN32" s="0" t="n">
+        <v>59.76464</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -10655,164 +10878,172 @@
         <f aca="false">SUM(AM$5:AM$32)</f>
         <v>4516.31215</v>
       </c>
+      <c r="AN35" s="0" t="n">
+        <f aca="false">SUM(AN$5:AN$32)</f>
+        <v>4525.63298</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="43" t="n">
+        <v>87</v>
+      </c>
+      <c r="C36" s="47" t="n">
         <f aca="false">1/(C35/Regular_Timings!C35)</f>
         <v>3.74749121272531</v>
       </c>
-      <c r="D36" s="43" t="n">
+      <c r="D36" s="47" t="n">
         <f aca="false">1/(D35/Regular_Timings!D35)</f>
         <v>3.41302620041922</v>
       </c>
-      <c r="E36" s="43" t="n">
+      <c r="E36" s="47" t="n">
         <f aca="false">1/(E35/Regular_Timings!E35)</f>
         <v>3.58035321194409</v>
       </c>
-      <c r="F36" s="43" t="n">
+      <c r="F36" s="47" t="n">
         <f aca="false">1/(F35/Regular_Timings!F35)</f>
         <v>3.77604759094586</v>
       </c>
-      <c r="G36" s="43" t="n">
+      <c r="G36" s="47" t="n">
         <f aca="false">1/(G35/Regular_Timings!G35)</f>
         <v>3.60534646208669</v>
       </c>
-      <c r="H36" s="43" t="n">
+      <c r="H36" s="47" t="n">
         <f aca="false">1/(H35/Regular_Timings!H35)</f>
         <v>3.71338155532446</v>
       </c>
-      <c r="I36" s="43" t="n">
+      <c r="I36" s="47" t="n">
         <f aca="false">1/(I35/Regular_Timings!I35)</f>
         <v>3.87995098100785</v>
       </c>
-      <c r="J36" s="43" t="n">
+      <c r="J36" s="47" t="n">
         <f aca="false">1/(J35/Regular_Timings!J35)</f>
         <v>3.77692817787917</v>
       </c>
-      <c r="K36" s="43" t="n">
+      <c r="K36" s="47" t="n">
         <f aca="false">1/(K35/Regular_Timings!K35)</f>
         <v>3.64724155744514</v>
       </c>
-      <c r="L36" s="43" t="n">
+      <c r="L36" s="47" t="n">
         <f aca="false">1/(L35/Regular_Timings!L35)</f>
         <v>3.74020943453721</v>
       </c>
-      <c r="M36" s="43" t="n">
+      <c r="M36" s="47" t="n">
         <f aca="false">1/(M35/Regular_Timings!M35)</f>
         <v>3.50672105722098</v>
       </c>
-      <c r="N36" s="43" t="n">
+      <c r="N36" s="47" t="n">
         <f aca="false">1/(N35/Regular_Timings!N35)</f>
         <v>3.73405080495359</v>
       </c>
-      <c r="O36" s="43" t="n">
+      <c r="O36" s="47" t="n">
         <f aca="false">1/(O35/Regular_Timings!O35)</f>
         <v>3.48066002524706</v>
       </c>
-      <c r="P36" s="43" t="n">
+      <c r="P36" s="47" t="n">
         <f aca="false">1/(P35/Regular_Timings!P35)</f>
         <v>3.64532320360124</v>
       </c>
-      <c r="Q36" s="43" t="n">
+      <c r="Q36" s="47" t="n">
         <f aca="false">1/(Q35/Regular_Timings!Q35)</f>
         <v>3.69283488712217</v>
       </c>
-      <c r="R36" s="43" t="n">
+      <c r="R36" s="47" t="n">
         <f aca="false">1/(R35/Regular_Timings!R35)</f>
         <v>3.91914079157363</v>
       </c>
-      <c r="S36" s="43" t="n">
+      <c r="S36" s="47" t="n">
         <f aca="false">1/(S35/Regular_Timings!S35)</f>
         <v>3.70850736443567</v>
       </c>
-      <c r="T36" s="43" t="n">
+      <c r="T36" s="47" t="n">
         <f aca="false">1/(T35/Regular_Timings!T35)</f>
         <v>3.75420891553771</v>
       </c>
-      <c r="U36" s="43" t="n">
+      <c r="U36" s="47" t="n">
         <f aca="false">1/(U35/Regular_Timings!U35)</f>
         <v>3.84853896938329</v>
       </c>
-      <c r="V36" s="43" t="n">
+      <c r="V36" s="47" t="n">
         <f aca="false">Regular_Timings!V35/V35</f>
         <v>3.72104488019434</v>
       </c>
-      <c r="W36" s="43" t="n">
+      <c r="W36" s="47" t="n">
         <f aca="false">Regular_Timings!W35/W35</f>
         <v>3.67572728059469</v>
       </c>
-      <c r="X36" s="43" t="n">
+      <c r="X36" s="47" t="n">
         <f aca="false">Regular_Timings!X35/X35</f>
         <v>4.19080065811635</v>
       </c>
-      <c r="Y36" s="43" t="n">
+      <c r="Y36" s="47" t="n">
         <f aca="false">Regular_Timings!Y35/Y35</f>
         <v>3.89406092958739</v>
       </c>
-      <c r="Z36" s="43" t="n">
+      <c r="Z36" s="47" t="n">
         <f aca="false">Regular_Timings!Z35/Z35</f>
         <v>3.55407794695691</v>
       </c>
-      <c r="AA36" s="43" t="n">
+      <c r="AA36" s="47" t="n">
         <f aca="false">Regular_Timings!AA35/AA35</f>
         <v>4.00488485600993</v>
       </c>
-      <c r="AB36" s="43" t="n">
+      <c r="AB36" s="47" t="n">
         <f aca="false">Regular_Timings!AB35/AB35</f>
         <v>3.66631773819967</v>
       </c>
-      <c r="AC36" s="43" t="n">
+      <c r="AC36" s="47" t="n">
         <f aca="false">Regular_Timings!AC35/AC35</f>
         <v>3.56831780200242</v>
       </c>
-      <c r="AD36" s="43" t="n">
+      <c r="AD36" s="47" t="n">
         <f aca="false">Regular_Timings!AD35/AD35</f>
         <v>3.7717099313906</v>
       </c>
-      <c r="AE36" s="43" t="n">
+      <c r="AE36" s="47" t="n">
         <f aca="false">Regular_Timings!AE35/AE35</f>
         <v>3.65797605865082</v>
       </c>
-      <c r="AG36" s="43" t="n">
+      <c r="AG36" s="47" t="n">
         <f aca="false">Regular_Timings!AG35/AG35</f>
         <v>3.6639766566581</v>
       </c>
-      <c r="AH36" s="43" t="n">
+      <c r="AH36" s="47" t="n">
         <f aca="false">Regular_Timings!AH35/AH35</f>
         <v>3.88981824858324</v>
       </c>
-      <c r="AI36" s="43" t="n">
+      <c r="AI36" s="47" t="n">
         <f aca="false">Regular_Timings!AI35/AI35</f>
         <v>3.95034639182564</v>
       </c>
-      <c r="AJ36" s="43" t="n">
+      <c r="AJ36" s="47" t="n">
         <f aca="false">Regular_Timings!AJ35/AJ35</f>
         <v>3.61276930976272</v>
       </c>
-      <c r="AK36" s="43" t="n">
+      <c r="AK36" s="47" t="n">
         <f aca="false">Regular_Timings!AK35/AK35</f>
         <v>3.47176276903545</v>
       </c>
-      <c r="AL36" s="43" t="n">
+      <c r="AL36" s="47" t="n">
         <f aca="false">Regular_Timings!AL35/AL35</f>
         <v>3.42704556536553</v>
       </c>
-      <c r="AM36" s="43" t="n">
+      <c r="AM36" s="47" t="n">
         <f aca="false">Regular_Timings!AM35/AM35</f>
         <v>3.62119345537265</v>
+      </c>
+      <c r="AN36" s="47" t="n">
+        <f aca="false">Regular_Timings!AN35/AN35</f>
+        <v>3.45756053775267</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="AC37" s="33"/>
+      <c r="AC37" s="39"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AC38" s="44" t="s">
-        <v>87</v>
+      <c r="AC38" s="48" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -10831,10 +11062,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF97"/>
+  <dimension ref="A1:AJ97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ2" activeCellId="0" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10848,13 +11079,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>14</v>
@@ -10874,190 +11105,201 @@
       <c r="AF1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q3" s="45" t="s">
         <v>93</v>
       </c>
+      <c r="Q3" s="49" t="s">
+        <v>94</v>
+      </c>
       <c r="T3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="45" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
- Updates milestone and timing tracking updates in both spreadsheet formats
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="137">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">Properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">As of June 3, 2019</t>
@@ -640,6 +643,9 @@
   </si>
   <si>
     <t xml:space="preserve">Crossed 590,000 on 07/12/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crossed 600,000 on 7/19/21</t>
   </si>
 </sst>
 </file>
@@ -992,7 +998,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1030,6 +1036,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1093,6 +1103,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1122,10 +1136,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1289,13 +1299,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>738360</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>186480</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1308,7 +1318,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="738360" y="9379080"/>
+          <a:off x="738360" y="9381240"/>
           <a:ext cx="9703800" cy="2053800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1324,13 +1334,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>18360</xdr:colOff>
+      <xdr:colOff>20520</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>698040</xdr:colOff>
+      <xdr:colOff>700200</xdr:colOff>
       <xdr:row>80</xdr:row>
       <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
@@ -1345,7 +1355,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2229120" y="11834280"/>
+          <a:off x="2231280" y="11834280"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1361,15 +1371,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>18360</xdr:colOff>
+      <xdr:colOff>20520</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>663480</xdr:colOff>
+      <xdr:colOff>665640</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1382,7 +1392,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2229120" y="14444280"/>
+          <a:off x="2231280" y="14446440"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1398,15 +1408,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>18360</xdr:colOff>
+      <xdr:colOff>20520</xdr:colOff>
       <xdr:row>96</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>506160</xdr:colOff>
+      <xdr:colOff>508320</xdr:colOff>
       <xdr:row>111</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1419,7 +1429,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2229120" y="16740000"/>
+          <a:off x="2231280" y="16742160"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1435,15 +1445,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>18000</xdr:colOff>
+      <xdr:colOff>20160</xdr:colOff>
       <xdr:row>114</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>459360</xdr:colOff>
+      <xdr:colOff>461520</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1456,7 +1466,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2228760" y="19894680"/>
+          <a:off x="2230920" y="19896840"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1472,13 +1482,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>47520</xdr:colOff>
+      <xdr:colOff>49680</xdr:colOff>
       <xdr:row>130</xdr:row>
       <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>484200</xdr:colOff>
+      <xdr:colOff>486360</xdr:colOff>
       <xdr:row>142</xdr:row>
       <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
@@ -1493,7 +1503,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2258280" y="22677840"/>
+          <a:off x="2260440" y="22677840"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1509,15 +1519,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>15480</xdr:colOff>
+      <xdr:colOff>17640</xdr:colOff>
       <xdr:row>144</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>891360</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1530,7 +1540,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2226240" y="25152480"/>
+          <a:off x="2228400" y="25154640"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1548,13 +1558,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
       <xdr:row>174</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>595800</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>309600</xdr:colOff>
       <xdr:row>186</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>71280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1567,7 +1577,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3115080" y="30416400"/>
+          <a:off x="3115080" y="30418560"/>
           <a:ext cx="9708120" cy="2138400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1588,8 +1598,8 @@
       <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>910440</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>53280</xdr:colOff>
       <xdr:row>170</xdr:row>
       <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
@@ -1625,8 +1635,8 @@
       <xdr:rowOff>168840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>619920</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333720</xdr:colOff>
       <xdr:row>201</xdr:row>
       <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
@@ -1662,8 +1672,8 @@
       <xdr:rowOff>113760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>410040</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>123840</xdr:colOff>
       <xdr:row>214</xdr:row>
       <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
@@ -1696,13 +1706,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>275040</xdr:colOff>
       <xdr:row>215</xdr:row>
-      <xdr:rowOff>33840</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>58680</xdr:colOff>
+      <xdr:colOff>411120</xdr:colOff>
       <xdr:row>226</xdr:row>
-      <xdr:rowOff>150480</xdr:rowOff>
+      <xdr:rowOff>152640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1715,7 +1725,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3124800" y="37602000"/>
+          <a:off x="3124800" y="37604160"/>
           <a:ext cx="9161280" cy="2044800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1737,7 +1747,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>361440</xdr:colOff>
       <xdr:row>241</xdr:row>
       <xdr:rowOff>73440</xdr:rowOff>
     </xdr:to>
@@ -1774,7 +1784,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
+      <xdr:colOff>355320</xdr:colOff>
       <xdr:row>254</xdr:row>
       <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
@@ -1810,8 +1820,8 @@
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1171800</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314640</xdr:colOff>
       <xdr:row>268</xdr:row>
       <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
@@ -1847,8 +1857,8 @@
       <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1201680</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>344520</xdr:colOff>
       <xdr:row>281</xdr:row>
       <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
@@ -1884,8 +1894,8 @@
       <xdr:rowOff>4680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1191240</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>334080</xdr:colOff>
       <xdr:row>294</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
@@ -1921,8 +1931,8 @@
       <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1180440</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323280</xdr:colOff>
       <xdr:row>306</xdr:row>
       <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
@@ -1958,8 +1968,8 @@
       <xdr:rowOff>165960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1186920</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>329760</xdr:colOff>
       <xdr:row>319</xdr:row>
       <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
@@ -1995,8 +2005,8 @@
       <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1206000</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>348840</xdr:colOff>
       <xdr:row>332</xdr:row>
       <xdr:rowOff>5040</xdr:rowOff>
     </xdr:to>
@@ -2032,8 +2042,8 @@
       <xdr:rowOff>174600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1179000</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>321840</xdr:colOff>
       <xdr:row>344</xdr:row>
       <xdr:rowOff>51480</xdr:rowOff>
     </xdr:to>
@@ -2069,8 +2079,8 @@
       <xdr:rowOff>5400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1194120</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>336960</xdr:colOff>
       <xdr:row>358</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -2106,8 +2116,8 @@
       <xdr:rowOff>169560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1202400</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>345240</xdr:colOff>
       <xdr:row>373</xdr:row>
       <xdr:rowOff>109440</xdr:rowOff>
     </xdr:to>
@@ -2143,8 +2153,8 @@
       <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1176120</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>318960</xdr:colOff>
       <xdr:row>386</xdr:row>
       <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
@@ -2180,8 +2190,8 @@
       <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1188000</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>330840</xdr:colOff>
       <xdr:row>401</xdr:row>
       <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
@@ -2217,8 +2227,8 @@
       <xdr:rowOff>17280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1190160</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>333000</xdr:colOff>
       <xdr:row>413</xdr:row>
       <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
@@ -2254,8 +2264,8 @@
       <xdr:rowOff>172800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1207800</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>350640</xdr:colOff>
       <xdr:row>427</xdr:row>
       <xdr:rowOff>97200</xdr:rowOff>
     </xdr:to>
@@ -2291,8 +2301,8 @@
       <xdr:rowOff>169920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1206720</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>349560</xdr:colOff>
       <xdr:row>440</xdr:row>
       <xdr:rowOff>65880</xdr:rowOff>
     </xdr:to>
@@ -2328,8 +2338,8 @@
       <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1195560</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>338400</xdr:colOff>
       <xdr:row>452</xdr:row>
       <xdr:rowOff>125280</xdr:rowOff>
     </xdr:to>
@@ -2365,8 +2375,8 @@
       <xdr:rowOff>31320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1191960</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>334800</xdr:colOff>
       <xdr:row>467</xdr:row>
       <xdr:rowOff>127800</xdr:rowOff>
     </xdr:to>
@@ -2403,7 +2413,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>11880</xdr:colOff>
+      <xdr:colOff>364320</xdr:colOff>
       <xdr:row>479</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
@@ -2439,8 +2449,8 @@
       <xdr:rowOff>25920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1193760</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>336600</xdr:colOff>
       <xdr:row>493</xdr:row>
       <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
@@ -2476,8 +2486,8 @@
       <xdr:rowOff>159120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1175040</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>317880</xdr:colOff>
       <xdr:row>507</xdr:row>
       <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
@@ -2513,8 +2523,8 @@
       <xdr:rowOff>26280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1189440</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>332280</xdr:colOff>
       <xdr:row>520</xdr:row>
       <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
@@ -2550,8 +2560,8 @@
       <xdr:rowOff>69840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1180440</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323280</xdr:colOff>
       <xdr:row>537</xdr:row>
       <xdr:rowOff>126000</xdr:rowOff>
     </xdr:to>
@@ -2587,8 +2597,8 @@
       <xdr:rowOff>24120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1171080</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>313920</xdr:colOff>
       <xdr:row>551</xdr:row>
       <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
@@ -2624,8 +2634,8 @@
       <xdr:rowOff>108720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1171800</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314640</xdr:colOff>
       <xdr:row>566</xdr:row>
       <xdr:rowOff>54360</xdr:rowOff>
     </xdr:to>
@@ -2661,8 +2671,8 @@
       <xdr:rowOff>163800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1155600</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>298440</xdr:colOff>
       <xdr:row>581</xdr:row>
       <xdr:rowOff>29880</xdr:rowOff>
     </xdr:to>
@@ -2698,8 +2708,8 @@
       <xdr:rowOff>24120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1190160</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>333000</xdr:colOff>
       <xdr:row>598</xdr:row>
       <xdr:rowOff>161640</xdr:rowOff>
     </xdr:to>
@@ -2736,7 +2746,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>41760</xdr:colOff>
+      <xdr:colOff>394200</xdr:colOff>
       <xdr:row>616</xdr:row>
       <xdr:rowOff>720</xdr:rowOff>
     </xdr:to>
@@ -2764,6 +2774,43 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1337040</xdr:colOff>
+      <xdr:row>617</xdr:row>
+      <xdr:rowOff>147960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>326880</xdr:colOff>
+      <xdr:row>631</xdr:row>
+      <xdr:rowOff>163440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Image 39" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId41"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2204280" y="108170640"/>
+          <a:ext cx="9997560" cy="2469240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2772,10 +2819,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W604"/>
+  <dimension ref="A1:W620"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2787,7 +2834,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="8" style="0" width="9.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="9.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="20" style="0" width="9.05"/>
@@ -2802,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="n">
-        <v>44385</v>
+        <v>44401</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>2</v>
@@ -2839,11 +2886,11 @@
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>736.16</v>
+        <v>721.55</v>
       </c>
       <c r="P5" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>210.30995</v>
+        <v>212.31225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2855,11 +2902,11 @@
       </c>
       <c r="O6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>207.61</v>
+        <v>206.73</v>
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>89.14734</v>
+        <v>90.82206</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2871,11 +2918,11 @@
       </c>
       <c r="O7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>285.33</v>
+        <v>280.21</v>
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>89.44785</v>
+        <v>90.75888</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2892,11 +2939,11 @@
       </c>
       <c r="O8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1548.6</v>
+        <v>1521.09</v>
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>395.9805</v>
+        <v>409.14567</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2909,11 +2956,11 @@
       <c r="N9" s="3"/>
       <c r="O9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>153.45</v>
+        <v>150.04</v>
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>50.28011</v>
+        <v>51.79205</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2926,11 +2973,11 @@
       <c r="N10" s="3"/>
       <c r="O10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>140.02589</v>
+        <v>144.53663</v>
       </c>
       <c r="P10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>140.02589</v>
+        <v>144.53663</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2943,11 +2990,11 @@
       <c r="N11" s="3"/>
       <c r="O11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>108.81</v>
+        <v>111.63</v>
       </c>
       <c r="P11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>44.94206</v>
+        <v>46.32702</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2960,11 +3007,11 @@
       <c r="N12" s="3"/>
       <c r="O12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>589.14</v>
+        <v>590.76</v>
       </c>
       <c r="P12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>160.42696</v>
+        <v>165.7346</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2981,11 +3028,11 @@
       </c>
       <c r="O13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>335.68</v>
+        <v>337.16</v>
       </c>
       <c r="P13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>121.16786</v>
+        <v>126.72064</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2998,11 +3045,11 @@
       </c>
       <c r="O14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>411.26</v>
+        <v>416.19</v>
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>140.04936</v>
+        <v>145.61946</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3018,11 +3065,11 @@
       </c>
       <c r="O15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>2718.77</v>
+        <v>2698.37</v>
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>697.39256</v>
+        <v>711.58348</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3034,11 +3081,11 @@
       </c>
       <c r="O16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>242.28</v>
+        <v>245.65</v>
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
-        <v>58.14421</v>
+        <v>58.99668</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3050,11 +3097,11 @@
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>667.02</v>
+        <v>673.81</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>198.52091</v>
+        <v>204.55998</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3070,11 +3117,11 @@
       </c>
       <c r="O18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>814.21</v>
+        <v>821.4</v>
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>230.24696</v>
+        <v>240.32241</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3086,11 +3133,11 @@
       </c>
       <c r="O19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>133.93</v>
+        <v>135.64</v>
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>56.11644</v>
+        <v>58.4548</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3102,11 +3149,11 @@
       </c>
       <c r="O20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>452.39</v>
+        <v>459.92</v>
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>155.56309</v>
+        <v>160.45979</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3118,11 +3165,11 @@
       </c>
       <c r="O21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>409.92</v>
+        <v>416.36</v>
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>134.11112</v>
+        <v>137.28949</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3134,11 +3181,11 @@
       </c>
       <c r="O22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>256.29</v>
+        <v>259.86</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>98.33153</v>
+        <v>100.64183</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3150,11 +3197,11 @@
       </c>
       <c r="O23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>276.76</v>
+        <v>281.98</v>
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>89.59884</v>
+        <v>91.96451</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,11 +3214,11 @@
       <c r="N24" s="1"/>
       <c r="O24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>327.61</v>
+        <v>333.8</v>
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>99.0768</v>
+        <v>101.06361</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3183,11 +3230,11 @@
       </c>
       <c r="O25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>799.21</v>
+        <v>815.28</v>
       </c>
       <c r="P25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>252.55173</v>
+        <v>255.82734</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3199,11 +3246,11 @@
       </c>
       <c r="O26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>177.5</v>
+        <v>180.75</v>
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>53.86057</v>
+        <v>55.17855</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3215,11 +3262,11 @@
       </c>
       <c r="O27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>417.1</v>
+        <v>425.18</v>
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>128.04221</v>
+        <v>132.08827</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3235,11 +3282,11 @@
       </c>
       <c r="O28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1701.77</v>
+        <v>1731.05</v>
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>473.46779</v>
+        <v>492.12186</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3251,11 +3298,11 @@
       </c>
       <c r="O29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>43.79</v>
+        <v>44.53</v>
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>21.88631</v>
+        <v>22.529</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3267,11 +3314,11 @@
       </c>
       <c r="O30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>31.74</v>
+        <v>32.14</v>
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>24.85855</v>
+        <v>25.98439</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3283,11 +3330,11 @@
       </c>
       <c r="O31" s="9" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>162.32</v>
+        <v>164.67</v>
       </c>
       <c r="P31" s="9" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>59.76464</v>
+        <v>61.74287</v>
       </c>
       <c r="Q31" s="9"/>
     </row>
@@ -3307,7 +3354,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="4" t="n">
-        <v>39105</v>
+        <v>39684</v>
       </c>
       <c r="E33" s="0" t="str">
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!AF:AF)), Miletone_Tracking!AF:AF)</f>
@@ -3320,19 +3367,22 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="n">
-        <v>16242</v>
+        <v>20272</v>
       </c>
       <c r="E34" s="0" t="str">
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!AJ:AJ)), Miletone_Tracking!AJ:AJ )</f>
         <v>Crossed 10,000 lines on 07/12/21</v>
       </c>
       <c r="N34" s="3"/>
-    </row>
-    <row r="35" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="11" t="s">
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+    </row>
+    <row r="35" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="12" t="n">
+      <c r="C35" s="13" t="n">
         <v>5260</v>
       </c>
       <c r="O35" s="0"/>
@@ -3395,12 +3445,12 @@
         <f aca="false">4650-865</f>
         <v>3785</v>
       </c>
-      <c r="I43" s="13" t="s">
+      <c r="I43" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B44" s="0" t="s">
@@ -3410,7 +3460,7 @@
         <f aca="false">10319-580</f>
         <v>9739</v>
       </c>
-      <c r="I44" s="15" t="s">
+      <c r="I44" s="16" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3421,7 +3471,7 @@
       <c r="C45" s="0" t="n">
         <v>23768</v>
       </c>
-      <c r="E45" s="16"/>
+      <c r="E45" s="17"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
@@ -3430,7 +3480,7 @@
       <c r="C46" s="0" t="n">
         <v>3357</v>
       </c>
-      <c r="E46" s="16"/>
+      <c r="E46" s="17"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="4" t="s">
@@ -3438,22 +3488,22 @@
       </c>
       <c r="C48" s="4" t="n">
         <f aca="false">SUM(C4:C46)</f>
-        <v>599432</v>
+        <v>604041</v>
       </c>
       <c r="E48" s="0" t="str">
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!A:A)), Miletone_Tracking!A:A)</f>
-        <v>Crossed 590,000 on 07/12/21</v>
+        <v>Crossed 600,000 on 7/19/21</v>
       </c>
       <c r="N48" s="0" t="s">
         <v>51</v>
       </c>
       <c r="O48" s="0" t="n">
         <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
-        <v>15647.65</v>
-      </c>
-      <c r="P48" s="0" t="n">
-        <f aca="false">INDEX(Parallel_Timings!35:35,COUNT(Parallel_Timings!35:35,1,1))</f>
-        <v>4516.31215</v>
+        <v>15779.82</v>
+      </c>
+      <c r="P48" s="9" t="n">
+        <f aca="false">LOOKUP(2,1/(Parallel_Timings!D35:ND35&lt;&gt;""),Parallel_Timings!D35:ND35)</f>
+        <v>4647.93053</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3466,213 +3516,216 @@
       <c r="N49" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="P49" s="17" t="n">
+      <c r="P49" s="18" t="n">
         <f aca="false">O48/P48</f>
-        <v>3.46469630094102</v>
+        <v>3.39502062222087</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="P52" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="R56" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C121" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S146" s="18" t="n">
+      <c r="S146" s="19" t="n">
         <v>43729</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C158" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S162" s="18" t="n">
+      <c r="S162" s="19" t="n">
         <v>43780</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C173" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S175" s="18" t="n">
+      <c r="S175" s="19" t="n">
         <v>43765</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S190" s="18" t="n">
+      <c r="S190" s="19" t="n">
         <v>43799</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S204" s="18" t="n">
+      <c r="S204" s="19" t="n">
         <v>43814</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S216" s="18" t="n">
+      <c r="S216" s="19" t="n">
         <v>43827</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S231" s="18" t="n">
+      <c r="S231" s="19" t="n">
         <v>43930</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S245" s="18" t="n">
+      <c r="S245" s="19" t="n">
         <v>43939</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S258" s="18" t="n">
+      <c r="S258" s="19" t="n">
         <v>43955</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S266" s="18"/>
+      <c r="S266" s="19"/>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S267" s="18"/>
+      <c r="S267" s="19"/>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S268" s="18"/>
+      <c r="S268" s="19"/>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S269" s="18"/>
+      <c r="S269" s="19"/>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S270" s="18"/>
+      <c r="S270" s="19"/>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S271" s="18" t="n">
+      <c r="S271" s="19" t="n">
         <v>43968</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S285" s="18" t="n">
+      <c r="S285" s="19" t="n">
         <v>44025</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S298" s="18" t="n">
+      <c r="S298" s="19" t="n">
         <v>44031</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S310" s="18" t="n">
+      <c r="S310" s="19" t="n">
         <v>44050</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S324" s="18" t="n">
+      <c r="S324" s="19" t="n">
         <v>44053</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S337" s="18" t="n">
+      <c r="S337" s="19" t="n">
         <v>44072</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S350" s="18" t="n">
+      <c r="S350" s="19" t="n">
         <v>44094</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S365" s="18" t="n">
+      <c r="S365" s="19" t="n">
         <v>44101</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S379" s="18" t="n">
+      <c r="S379" s="19" t="n">
         <v>44125</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S393" s="18" t="n">
+      <c r="S393" s="19" t="n">
         <v>44130</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S406" s="18" t="n">
+      <c r="S406" s="19" t="n">
         <v>44136</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S420" s="18" t="n">
+      <c r="S420" s="19" t="n">
         <v>44157</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S433" s="18" t="n">
+      <c r="S433" s="19" t="n">
         <v>44164</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S445" s="18" t="n">
+      <c r="S445" s="19" t="n">
         <v>44171</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S460" s="18" t="n">
+      <c r="S460" s="19" t="n">
         <v>44199</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S472" s="18" t="n">
+      <c r="S472" s="19" t="n">
         <v>44218</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S485" s="18" t="n">
+      <c r="S485" s="19" t="n">
         <v>44220</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S499" s="18" t="n">
+      <c r="S499" s="19" t="n">
         <v>44241</v>
       </c>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S512" s="18" t="n">
+      <c r="S512" s="19" t="n">
         <v>44241</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S528" s="18" t="n">
+      <c r="S528" s="19" t="n">
         <v>44284</v>
       </c>
     </row>
@@ -3682,28 +3735,33 @@
       </c>
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S542" s="18" t="n">
+      <c r="S542" s="19" t="n">
         <v>44290</v>
       </c>
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S557" s="18" t="n">
+      <c r="S557" s="19" t="n">
         <v>44318</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S571" s="18" t="n">
+      <c r="S571" s="19" t="n">
         <v>44325</v>
       </c>
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S588" s="18" t="n">
+      <c r="S588" s="19" t="n">
         <v>44367</v>
       </c>
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S604" s="18" t="n">
+      <c r="S604" s="19" t="n">
         <v>44370</v>
+      </c>
+    </row>
+    <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S620" s="19" t="n">
+        <v>44395</v>
       </c>
     </row>
   </sheetData>
@@ -3725,12 +3783,12 @@
   </sheetPr>
   <dimension ref="A2:BK109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="AF5" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AF1" activeCellId="0" sqref="AF1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AM17" activeCellId="0" sqref="AM17"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="AO35" activeCellId="1" sqref="I15 AO35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3751,155 +3809,158 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" s="19" customFormat="true" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="20" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" s="20" customFormat="true" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C4" s="21" t="n">
         <v>44136</v>
       </c>
-      <c r="D4" s="20" t="n">
+      <c r="D4" s="21" t="n">
         <v>44143</v>
       </c>
-      <c r="E4" s="21" t="n">
+      <c r="E4" s="22" t="n">
         <v>44151</v>
       </c>
-      <c r="F4" s="21" t="n">
+      <c r="F4" s="22" t="n">
         <v>44157</v>
       </c>
-      <c r="G4" s="20" t="n">
+      <c r="G4" s="21" t="n">
         <v>44164</v>
       </c>
-      <c r="H4" s="21" t="n">
+      <c r="H4" s="22" t="n">
         <v>44171</v>
       </c>
-      <c r="I4" s="21" t="n">
+      <c r="I4" s="22" t="n">
         <v>44178</v>
       </c>
-      <c r="J4" s="21" t="n">
+      <c r="J4" s="22" t="n">
         <v>44185</v>
       </c>
-      <c r="K4" s="21" t="n">
+      <c r="K4" s="22" t="n">
         <v>44192</v>
       </c>
-      <c r="L4" s="21" t="n">
+      <c r="L4" s="22" t="n">
         <v>43833</v>
       </c>
-      <c r="M4" s="21" t="n">
+      <c r="M4" s="22" t="n">
         <v>44206</v>
       </c>
-      <c r="N4" s="21" t="n">
+      <c r="N4" s="22" t="n">
         <v>44213</v>
       </c>
-      <c r="O4" s="21" t="n">
+      <c r="O4" s="22" t="n">
         <v>44220</v>
       </c>
-      <c r="P4" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="22" t="s">
+      <c r="P4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="R4" s="21" t="n">
+      <c r="Q4" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="22" t="n">
         <v>44241</v>
       </c>
-      <c r="S4" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="T4" s="21" t="n">
+      <c r="S4" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="T4" s="22" t="n">
         <v>44255</v>
       </c>
-      <c r="U4" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="V4" s="22" t="s">
+      <c r="U4" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="W4" s="23" t="n">
+      <c r="V4" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="W4" s="24" t="n">
         <v>44276</v>
       </c>
-      <c r="X4" s="23" t="n">
+      <c r="X4" s="24" t="n">
         <v>44283</v>
       </c>
-      <c r="Y4" s="23" t="n">
+      <c r="Y4" s="24" t="n">
         <v>44290</v>
       </c>
-      <c r="Z4" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA4" s="22" t="s">
+      <c r="Z4" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="AB4" s="21" t="n">
+      <c r="AA4" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB4" s="22" t="n">
         <v>44311</v>
       </c>
-      <c r="AC4" s="21" t="n">
+      <c r="AC4" s="22" t="n">
         <v>44318</v>
       </c>
-      <c r="AD4" s="21" t="n">
+      <c r="AD4" s="22" t="n">
         <v>44325</v>
       </c>
-      <c r="AE4" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF4" s="21" t="n">
+      <c r="AE4" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF4" s="22" t="n">
         <v>44339</v>
       </c>
-      <c r="AG4" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH4" s="21" t="n">
+      <c r="AG4" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH4" s="22" t="n">
         <v>44353</v>
       </c>
-      <c r="AI4" s="21" t="n">
+      <c r="AI4" s="22" t="n">
         <v>44360</v>
       </c>
-      <c r="AJ4" s="21" t="n">
+      <c r="AJ4" s="22" t="n">
         <v>44367</v>
       </c>
-      <c r="AK4" s="21" t="n">
+      <c r="AK4" s="22" t="n">
         <v>44374</v>
       </c>
-      <c r="AL4" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM4" s="24" t="s">
+      <c r="AL4" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="AN4" s="21" t="n">
+      <c r="AM4" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN4" s="22" t="n">
         <v>44395</v>
       </c>
-    </row>
-    <row r="5" s="26" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
+      <c r="AO4" s="26" t="n">
+        <v>44402</v>
+      </c>
+    </row>
+    <row r="5" s="28" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
       <c r="AC5" s="0" t="n">
         <v>636.13</v>
       </c>
@@ -3936,16 +3997,19 @@
       <c r="AN5" s="0" t="n">
         <v>1179.7</v>
       </c>
-    </row>
-    <row r="6" s="33" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="s">
+      <c r="AO5" s="0" t="n">
+        <v>1271.03</v>
+      </c>
+    </row>
+    <row r="6" s="10" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0" t="n">
         <v>509.17</v>
       </c>
-      <c r="D6" s="33" t="n">
+      <c r="D6" s="10" t="n">
         <v>561.22</v>
       </c>
       <c r="E6" s="0"/>
@@ -4054,9 +4118,12 @@
       <c r="AN6" s="0" t="n">
         <v>736.16</v>
       </c>
+      <c r="AO6" s="0" t="n">
+        <v>721.55</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -4173,9 +4240,12 @@
       <c r="AN7" s="0" t="n">
         <v>207.61</v>
       </c>
+      <c r="AO7" s="0" t="n">
+        <v>206.73</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="35" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -4280,9 +4350,12 @@
       <c r="AN8" s="0" t="n">
         <v>285.33</v>
       </c>
+      <c r="AO8" s="0" t="n">
+        <v>280.21</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -4399,9 +4472,12 @@
       <c r="AN9" s="0" t="n">
         <v>1548.6</v>
       </c>
+      <c r="AO9" s="0" t="n">
+        <v>1521.09</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -4518,9 +4594,12 @@
       <c r="AN10" s="0" t="n">
         <v>153.45</v>
       </c>
+      <c r="AO10" s="0" t="n">
+        <v>150.04</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -4637,9 +4716,12 @@
       <c r="AN11" s="0" t="n">
         <v>459.3</v>
       </c>
+      <c r="AO11" s="0" t="n">
+        <v>453.04</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>12</v>
       </c>
       <c r="L12" s="0" t="n">
@@ -4729,9 +4811,12 @@
       <c r="AN12" s="0" t="n">
         <v>108.81</v>
       </c>
+      <c r="AO12" s="0" t="n">
+        <v>111.63</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>13</v>
       </c>
       <c r="P13" s="0" t="n">
@@ -4809,9 +4894,12 @@
       <c r="AN13" s="0" t="n">
         <v>589.14</v>
       </c>
+      <c r="AO13" s="0" t="n">
+        <v>590.76</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="36" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -4928,9 +5016,12 @@
       <c r="AN14" s="0" t="n">
         <v>335.68</v>
       </c>
+      <c r="AO14" s="0" t="n">
+        <v>337.16</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -5047,9 +5138,12 @@
       <c r="AN15" s="0" t="n">
         <v>411.26</v>
       </c>
+      <c r="AO15" s="0" t="n">
+        <v>416.19</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -5166,9 +5260,12 @@
       <c r="AN16" s="0" t="n">
         <v>2718.77</v>
       </c>
+      <c r="AO16" s="0" t="n">
+        <v>2698.37</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>17</v>
       </c>
       <c r="AD17" s="0" t="n">
@@ -5204,9 +5301,12 @@
       <c r="AN17" s="0" t="n">
         <v>242.28</v>
       </c>
+      <c r="AO17" s="0" t="n">
+        <v>245.65</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -5323,9 +5423,12 @@
       <c r="AN18" s="0" t="n">
         <v>667.02</v>
       </c>
+      <c r="AO18" s="0" t="n">
+        <v>673.81</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -5442,9 +5545,12 @@
       <c r="AN19" s="0" t="n">
         <v>814.21</v>
       </c>
+      <c r="AO19" s="0" t="n">
+        <v>821.4</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="36" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -5561,9 +5667,12 @@
       <c r="AN20" s="0" t="n">
         <v>133.93</v>
       </c>
+      <c r="AO20" s="0" t="n">
+        <v>135.64</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="36" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -5680,9 +5789,12 @@
       <c r="AN21" s="0" t="n">
         <v>452.39</v>
       </c>
+      <c r="AO21" s="0" t="n">
+        <v>459.92</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="36" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -5760,7 +5872,7 @@
       <c r="AA22" s="0" t="n">
         <v>407.53</v>
       </c>
-      <c r="AB22" s="11" t="n">
+      <c r="AB22" s="12" t="n">
         <v>375.94</v>
       </c>
       <c r="AC22" s="0" t="n">
@@ -5799,9 +5911,12 @@
       <c r="AN22" s="0" t="n">
         <v>409.92</v>
       </c>
+      <c r="AO22" s="0" t="n">
+        <v>416.36</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="36" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -5918,9 +6033,12 @@
       <c r="AN23" s="0" t="n">
         <v>256.29</v>
       </c>
+      <c r="AO23" s="0" t="n">
+        <v>259.86</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="36" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -6037,9 +6155,12 @@
       <c r="AN24" s="0" t="n">
         <v>276.76</v>
       </c>
+      <c r="AO24" s="0" t="n">
+        <v>281.98</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -6156,9 +6277,12 @@
       <c r="AN25" s="0" t="n">
         <v>327.61</v>
       </c>
+      <c r="AO25" s="0" t="n">
+        <v>333.8</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -6275,9 +6399,12 @@
       <c r="AN26" s="0" t="n">
         <v>799.21</v>
       </c>
+      <c r="AO26" s="0" t="n">
+        <v>815.28</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -6394,9 +6521,12 @@
       <c r="AN27" s="0" t="n">
         <v>177.5</v>
       </c>
+      <c r="AO27" s="0" t="n">
+        <v>180.75</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>28</v>
       </c>
       <c r="U28" s="0" t="n">
@@ -6459,9 +6589,12 @@
       <c r="AN28" s="0" t="n">
         <v>417.1</v>
       </c>
+      <c r="AO28" s="0" t="n">
+        <v>425.18</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -6578,9 +6711,12 @@
       <c r="AN29" s="0" t="n">
         <v>1701.77</v>
       </c>
+      <c r="AO29" s="0" t="n">
+        <v>1731.05</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -6697,9 +6833,12 @@
       <c r="AN30" s="0" t="n">
         <v>43.79</v>
       </c>
+      <c r="AO30" s="0" t="n">
+        <v>44.53</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="35" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -6816,9 +6955,12 @@
       <c r="AN31" s="0" t="n">
         <v>31.74</v>
       </c>
+      <c r="AO31" s="0" t="n">
+        <v>32.14</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="35" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -6935,15 +7077,18 @@
       <c r="AN32" s="0" t="n">
         <v>162.32</v>
       </c>
+      <c r="AO32" s="0" t="n">
+        <v>164.67</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -7097,196 +7242,204 @@
         <f aca="false">SUM(AN$5:AN$32)</f>
         <v>15647.65</v>
       </c>
+      <c r="AO35" s="0" t="n">
+        <f aca="false">SUM(AO$5:AO$32)</f>
+        <v>15779.82</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37" t="n">
+        <v>78</v>
+      </c>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38" t="n">
         <f aca="false">D35/C35</f>
         <v>1.0558825271854</v>
       </c>
-      <c r="E36" s="37" t="n">
+      <c r="E36" s="38" t="n">
         <f aca="false">E35/D35</f>
         <v>0.916849500061912</v>
       </c>
-      <c r="F36" s="37" t="n">
+      <c r="F36" s="38" t="n">
         <f aca="false">F35/E35</f>
         <v>1.10350896258914</v>
       </c>
-      <c r="G36" s="37" t="n">
+      <c r="G36" s="38" t="n">
         <f aca="false">G35/F35</f>
         <v>1.03987375176407</v>
       </c>
-      <c r="H36" s="37" t="n">
+      <c r="H36" s="38" t="n">
         <f aca="false">H35/G35</f>
         <v>1.06665722673939</v>
       </c>
-      <c r="I36" s="37" t="n">
+      <c r="I36" s="38" t="n">
         <f aca="false">I35/H35</f>
         <v>1.02227013104336</v>
       </c>
-      <c r="J36" s="37" t="n">
+      <c r="J36" s="38" t="n">
         <f aca="false">J35/I35</f>
         <v>0.968844995695285</v>
       </c>
-      <c r="K36" s="37" t="n">
+      <c r="K36" s="38" t="n">
         <f aca="false">K35/J35</f>
         <v>1.00756682988645</v>
       </c>
-      <c r="L36" s="37" t="n">
+      <c r="L36" s="38" t="n">
         <f aca="false">L35/K35</f>
         <v>1.03365334779935</v>
       </c>
-      <c r="M36" s="37" t="n">
+      <c r="M36" s="38" t="n">
         <f aca="false">M35/L35</f>
         <v>0.972899387020888</v>
       </c>
-      <c r="N36" s="37" t="n">
+      <c r="N36" s="38" t="n">
         <f aca="false">N35/M35</f>
         <v>1.06944594764067</v>
       </c>
-      <c r="O36" s="37" t="n">
+      <c r="O36" s="38" t="n">
         <f aca="false">O35/N35</f>
         <v>1.03914029657021</v>
       </c>
-      <c r="P36" s="37" t="n">
+      <c r="P36" s="38" t="n">
         <f aca="false">P35/O35</f>
         <v>1.0268997847368</v>
       </c>
-      <c r="Q36" s="37" t="n">
+      <c r="Q36" s="38" t="n">
         <f aca="false">Q35/P35</f>
         <v>1.00478259658715</v>
       </c>
-      <c r="R36" s="37" t="n">
+      <c r="R36" s="38" t="n">
         <f aca="false">R35/Q35</f>
         <v>1.02439095646859</v>
       </c>
-      <c r="S36" s="37" t="n">
+      <c r="S36" s="38" t="n">
         <f aca="false">S35/R35</f>
         <v>0.994786033590229</v>
       </c>
-      <c r="T36" s="37" t="n">
+      <c r="T36" s="38" t="n">
         <f aca="false">T35/S35</f>
         <v>0.995561439657853</v>
       </c>
-      <c r="U36" s="37" t="n">
+      <c r="U36" s="38" t="n">
         <f aca="false">U35/T35</f>
         <v>1.10342734655874</v>
       </c>
-      <c r="V36" s="37" t="n">
+      <c r="V36" s="38" t="n">
         <f aca="false">V35/U35</f>
         <v>0.949124255714387</v>
       </c>
-      <c r="W36" s="37" t="n">
+      <c r="W36" s="38" t="n">
         <f aca="false">W35/V35</f>
         <v>0.990510153289931</v>
       </c>
-      <c r="X36" s="37" t="n">
+      <c r="X36" s="38" t="n">
         <f aca="false">X35/W35</f>
         <v>0.963401613497919</v>
       </c>
-      <c r="Y36" s="37" t="n">
+      <c r="Y36" s="38" t="n">
         <f aca="false">Y35/X35</f>
         <v>1.04446534528375</v>
       </c>
-      <c r="Z36" s="37" t="n">
+      <c r="Z36" s="38" t="n">
         <f aca="false">Z35/Y35</f>
         <v>0.902660745410508</v>
       </c>
-      <c r="AA36" s="37" t="n">
+      <c r="AA36" s="38" t="n">
         <f aca="false">AA35/Z35</f>
         <v>1.14252240687931</v>
       </c>
-      <c r="AB36" s="37" t="n">
+      <c r="AB36" s="38" t="n">
         <f aca="false">AB35/AA35</f>
         <v>0.936850704356737</v>
       </c>
-      <c r="AC36" s="37" t="n">
+      <c r="AC36" s="38" t="n">
         <f aca="false">AC35/AB35</f>
         <v>1.03187444677672</v>
       </c>
-      <c r="AD36" s="37" t="n">
+      <c r="AD36" s="38" t="n">
         <f aca="false">AD35/AC35</f>
         <v>1.11331883538682</v>
       </c>
-      <c r="AE36" s="37" t="n">
+      <c r="AE36" s="38" t="n">
         <f aca="false">AE35/AD35</f>
         <v>1.00181950741378</v>
       </c>
-      <c r="AF36" s="37" t="n">
+      <c r="AF36" s="38" t="n">
         <f aca="false">AF35/AE35</f>
         <v>1.03424321595765</v>
       </c>
-      <c r="AG36" s="37" t="n">
+      <c r="AG36" s="38" t="n">
         <f aca="false">AG35/AF35</f>
         <v>1.00792537781632</v>
       </c>
-      <c r="AH36" s="37" t="n">
+      <c r="AH36" s="38" t="n">
         <f aca="false">AH35/AG35</f>
         <v>0.970324194852549</v>
       </c>
-      <c r="AI36" s="37" t="n">
+      <c r="AI36" s="38" t="n">
         <f aca="false">AI35/AH35</f>
         <v>1.04927844854803</v>
       </c>
-      <c r="AJ36" s="37" t="n">
+      <c r="AJ36" s="38" t="n">
         <f aca="false">AJ35/AI35</f>
         <v>0.940307515998851</v>
       </c>
-      <c r="AK36" s="37" t="n">
+      <c r="AK36" s="38" t="n">
         <f aca="false">AK35/AJ35</f>
         <v>0.954601895704387</v>
       </c>
-      <c r="AL36" s="37" t="n">
+      <c r="AL36" s="38" t="n">
         <f aca="false">AL35/AK35</f>
         <v>1.03769659098725</v>
       </c>
-      <c r="AM36" s="37" t="n">
+      <c r="AM36" s="38" t="n">
         <f aca="false">AM35/AL35</f>
         <v>1.0523801464953</v>
       </c>
-      <c r="AN36" s="37" t="n">
+      <c r="AN36" s="38" t="n">
         <f aca="false">AN35/AM35</f>
         <v>0.956782989818056</v>
       </c>
+      <c r="AO36" s="38" t="n">
+        <f aca="false">AO35/AN35</f>
+        <v>1.00844663575681</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="L38" s="39" t="s">
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="O38" s="40" t="s">
+      <c r="L38" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="P38" s="39" t="s">
+      <c r="O38" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="U38" s="39" t="s">
+      <c r="P38" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="AC38" s="39" t="s">
+      <c r="U38" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="AD38" s="39" t="s">
+      <c r="AC38" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="AL38" s="41"/>
+      <c r="AD38" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL38" s="42"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI82" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BJ82" s="0" t="n">
         <v>636.13</v>
@@ -7563,7 +7716,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI108" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="BJ108" s="0" t="n">
         <v>27.54</v>
@@ -7599,14 +7752,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AN38"/>
+  <dimension ref="A2:AO38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AD11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AD1" activeCellId="0" sqref="AD1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="AD18" activeCellId="0" sqref="AD18"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AP35" activeCellId="1" sqref="I15 AP35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7625,155 +7778,158 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" s="43" customFormat="true" ht="42.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="42" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" s="44" customFormat="true" ht="42.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="43" t="n">
         <v>44136</v>
       </c>
-      <c r="D4" s="42" t="n">
+      <c r="D4" s="43" t="n">
         <v>44144</v>
       </c>
-      <c r="E4" s="42" t="n">
+      <c r="E4" s="43" t="n">
         <v>44151</v>
       </c>
-      <c r="F4" s="42" t="n">
+      <c r="F4" s="43" t="n">
         <v>44157</v>
       </c>
-      <c r="G4" s="42" t="n">
+      <c r="G4" s="43" t="n">
         <v>44164</v>
       </c>
-      <c r="H4" s="42" t="n">
+      <c r="H4" s="43" t="n">
         <v>44171</v>
       </c>
-      <c r="I4" s="42" t="n">
+      <c r="I4" s="43" t="n">
         <v>44178</v>
       </c>
-      <c r="J4" s="42" t="n">
+      <c r="J4" s="43" t="n">
         <v>44185</v>
       </c>
-      <c r="K4" s="42" t="n">
+      <c r="K4" s="43" t="n">
         <v>44192</v>
       </c>
-      <c r="L4" s="42" t="n">
+      <c r="L4" s="43" t="n">
         <v>43833</v>
       </c>
-      <c r="M4" s="42" t="n">
+      <c r="M4" s="43" t="n">
         <v>44206</v>
       </c>
-      <c r="N4" s="42" t="n">
+      <c r="N4" s="43" t="n">
         <v>44213</v>
       </c>
-      <c r="O4" s="42" t="n">
+      <c r="O4" s="43" t="n">
         <v>44220</v>
       </c>
-      <c r="P4" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="22" t="s">
+      <c r="P4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="R4" s="23" t="n">
+      <c r="Q4" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="R4" s="24" t="n">
         <v>44241</v>
       </c>
-      <c r="S4" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="T4" s="23" t="n">
+      <c r="S4" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="T4" s="24" t="n">
         <v>44255</v>
       </c>
-      <c r="U4" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="V4" s="22" t="s">
+      <c r="U4" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="W4" s="23" t="n">
+      <c r="V4" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="W4" s="24" t="n">
         <v>44276</v>
       </c>
-      <c r="X4" s="23" t="n">
+      <c r="X4" s="24" t="n">
         <v>44276</v>
       </c>
-      <c r="Y4" s="23" t="n">
+      <c r="Y4" s="24" t="n">
         <v>44290</v>
       </c>
-      <c r="Z4" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA4" s="22" t="s">
+      <c r="Z4" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="AB4" s="21" t="n">
+      <c r="AA4" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB4" s="22" t="n">
         <v>44311</v>
       </c>
-      <c r="AC4" s="21" t="n">
+      <c r="AC4" s="22" t="n">
         <v>44318</v>
       </c>
-      <c r="AD4" s="42" t="n">
+      <c r="AD4" s="43" t="n">
         <v>44325</v>
       </c>
-      <c r="AE4" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG4" s="24" t="s">
+      <c r="AE4" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AH4" s="21" t="n">
+      <c r="AG4" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH4" s="22" t="n">
         <v>44353</v>
       </c>
-      <c r="AI4" s="21" t="n">
+      <c r="AI4" s="22" t="n">
         <v>44360</v>
       </c>
-      <c r="AJ4" s="21" t="n">
+      <c r="AJ4" s="22" t="n">
         <v>44367</v>
       </c>
-      <c r="AK4" s="21" t="n">
+      <c r="AK4" s="22" t="n">
         <v>44374</v>
       </c>
-      <c r="AL4" s="21" t="n">
+      <c r="AL4" s="22" t="n">
         <v>44383</v>
       </c>
-      <c r="AM4" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="AN4" s="21" t="n">
+      <c r="AM4" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN4" s="22" t="n">
         <v>44395</v>
       </c>
-    </row>
-    <row r="5" s="46" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AO4" s="22" t="n">
+        <v>44402</v>
+      </c>
+    </row>
+    <row r="5" s="47" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
+        <v>76</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
       <c r="AC5" s="6" t="n">
         <v>272.20742</v>
       </c>
@@ -7807,10 +7963,13 @@
       <c r="AN5" s="0" t="n">
         <v>252.32084</v>
       </c>
-    </row>
-    <row r="6" s="33" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AO5" s="0" t="n">
+        <v>253.35241</v>
+      </c>
+    </row>
+    <row r="6" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -7924,9 +8083,12 @@
       <c r="AN6" s="0" t="n">
         <v>210.30995</v>
       </c>
+      <c r="AO6" s="0" t="n">
+        <v>212.31225</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="35" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -8040,9 +8202,12 @@
       <c r="AN7" s="0" t="n">
         <v>89.14734</v>
       </c>
+      <c r="AO7" s="0" t="n">
+        <v>90.82206</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="35" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -8144,9 +8309,12 @@
       <c r="AN8" s="0" t="n">
         <v>89.44785</v>
       </c>
+      <c r="AO8" s="0" t="n">
+        <v>90.75888</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -8260,9 +8428,12 @@
       <c r="AN9" s="0" t="n">
         <v>395.9805</v>
       </c>
+      <c r="AO9" s="0" t="n">
+        <v>409.14567</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -8376,9 +8547,12 @@
       <c r="AN10" s="0" t="n">
         <v>50.28011</v>
       </c>
+      <c r="AO10" s="0" t="n">
+        <v>51.79205</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -8492,9 +8666,12 @@
       <c r="AN11" s="0" t="n">
         <v>140.02589</v>
       </c>
+      <c r="AO11" s="0" t="n">
+        <v>144.53663</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="35" t="s">
         <v>12</v>
       </c>
       <c r="L12" s="0" t="n">
@@ -8581,9 +8758,12 @@
       <c r="AN12" s="0" t="n">
         <v>44.94206</v>
       </c>
+      <c r="AO12" s="0" t="n">
+        <v>46.32702</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="35" t="s">
         <v>13</v>
       </c>
       <c r="P13" s="0" t="n">
@@ -8658,9 +8838,12 @@
       <c r="AN13" s="0" t="n">
         <v>160.42696</v>
       </c>
+      <c r="AO13" s="0" t="n">
+        <v>165.7346</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="36" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="0" t="n">
@@ -8774,9 +8957,12 @@
       <c r="AN14" s="0" t="n">
         <v>121.16786</v>
       </c>
+      <c r="AO14" s="0" t="n">
+        <v>126.72064</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="36" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -8803,7 +8989,7 @@
       <c r="J15" s="0" t="n">
         <v>106.81782</v>
       </c>
-      <c r="K15" s="11" t="n">
+      <c r="K15" s="12" t="n">
         <v>111.0613</v>
       </c>
       <c r="L15" s="0" t="n">
@@ -8890,9 +9076,12 @@
       <c r="AN15" s="0" t="n">
         <v>140.04936</v>
       </c>
+      <c r="AO15" s="0" t="n">
+        <v>145.61946</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="0" t="n">
@@ -9006,9 +9195,12 @@
       <c r="AN16" s="0" t="n">
         <v>697.39256</v>
       </c>
+      <c r="AO16" s="0" t="n">
+        <v>711.58348</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="36" t="s">
         <v>17</v>
       </c>
       <c r="AD17" s="0" t="n">
@@ -9038,9 +9230,12 @@
       <c r="AN17" s="0" t="n">
         <v>58.14421</v>
       </c>
+      <c r="AO17" s="0" t="n">
+        <v>58.99668</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="0" t="n">
@@ -9154,9 +9349,12 @@
       <c r="AN18" s="0" t="n">
         <v>198.52091</v>
       </c>
+      <c r="AO18" s="0" t="n">
+        <v>204.55998</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="36" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="0" t="n">
@@ -9270,9 +9468,12 @@
       <c r="AN19" s="0" t="n">
         <v>230.24696</v>
       </c>
+      <c r="AO19" s="0" t="n">
+        <v>240.32241</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -9386,9 +9587,12 @@
       <c r="AN20" s="0" t="n">
         <v>56.11644</v>
       </c>
+      <c r="AO20" s="0" t="n">
+        <v>58.4548</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="36" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="0" t="n">
@@ -9502,9 +9706,12 @@
       <c r="AN21" s="0" t="n">
         <v>155.56309</v>
       </c>
+      <c r="AO21" s="0" t="n">
+        <v>160.45979</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="36" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="0" t="n">
@@ -9582,7 +9789,7 @@
       <c r="AA22" s="0" t="n">
         <v>113.63319</v>
       </c>
-      <c r="AB22" s="11" t="n">
+      <c r="AB22" s="12" t="n">
         <v>114.35779</v>
       </c>
       <c r="AC22" s="0" t="n">
@@ -9618,9 +9825,12 @@
       <c r="AN22" s="0" t="n">
         <v>134.11112</v>
       </c>
+      <c r="AO22" s="0" t="n">
+        <v>137.28949</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="36" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="0" t="n">
@@ -9734,9 +9944,12 @@
       <c r="AN23" s="0" t="n">
         <v>98.33153</v>
       </c>
+      <c r="AO23" s="0" t="n">
+        <v>100.64183</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="36" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="0" t="n">
@@ -9850,9 +10063,12 @@
       <c r="AN24" s="0" t="n">
         <v>89.59884</v>
       </c>
+      <c r="AO24" s="0" t="n">
+        <v>91.96451</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -9966,9 +10182,12 @@
       <c r="AN25" s="0" t="n">
         <v>99.0768</v>
       </c>
+      <c r="AO25" s="0" t="n">
+        <v>101.06361</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -10082,9 +10301,12 @@
       <c r="AN26" s="0" t="n">
         <v>252.55173</v>
       </c>
+      <c r="AO26" s="0" t="n">
+        <v>255.82734</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="0" t="n">
@@ -10198,9 +10420,12 @@
       <c r="AN27" s="0" t="n">
         <v>53.86057</v>
       </c>
+      <c r="AO27" s="0" t="n">
+        <v>55.17855</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="36" t="s">
         <v>28</v>
       </c>
       <c r="U28" s="0" t="n">
@@ -10260,9 +10485,12 @@
       <c r="AN28" s="0" t="n">
         <v>128.04221</v>
       </c>
+      <c r="AO28" s="0" t="n">
+        <v>132.08827</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C29" s="0" t="n">
@@ -10376,9 +10604,12 @@
       <c r="AN29" s="0" t="n">
         <v>473.46779</v>
       </c>
+      <c r="AO29" s="0" t="n">
+        <v>492.12186</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -10492,9 +10723,12 @@
       <c r="AN30" s="0" t="n">
         <v>21.88631</v>
       </c>
+      <c r="AO30" s="0" t="n">
+        <v>22.529</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="35" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="0" t="n">
@@ -10608,9 +10842,12 @@
       <c r="AN31" s="0" t="n">
         <v>24.85855</v>
       </c>
+      <c r="AO31" s="0" t="n">
+        <v>25.98439</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="35" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="0" t="n">
@@ -10724,15 +10961,18 @@
       <c r="AN32" s="0" t="n">
         <v>59.76464</v>
       </c>
+      <c r="AO32" s="0" t="n">
+        <v>61.74287</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -10882,168 +11122,176 @@
         <f aca="false">SUM(AN$5:AN$32)</f>
         <v>4525.63298</v>
       </c>
+      <c r="AO35" s="0" t="n">
+        <f aca="false">SUM(AO$5:AO$32)</f>
+        <v>4647.93053</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="47" t="n">
+        <v>88</v>
+      </c>
+      <c r="C36" s="48" t="n">
         <f aca="false">1/(C35/Regular_Timings!C35)</f>
         <v>3.74749121272531</v>
       </c>
-      <c r="D36" s="47" t="n">
+      <c r="D36" s="48" t="n">
         <f aca="false">1/(D35/Regular_Timings!D35)</f>
         <v>3.41302620041922</v>
       </c>
-      <c r="E36" s="47" t="n">
+      <c r="E36" s="48" t="n">
         <f aca="false">1/(E35/Regular_Timings!E35)</f>
         <v>3.58035321194409</v>
       </c>
-      <c r="F36" s="47" t="n">
+      <c r="F36" s="48" t="n">
         <f aca="false">1/(F35/Regular_Timings!F35)</f>
         <v>3.77604759094586</v>
       </c>
-      <c r="G36" s="47" t="n">
+      <c r="G36" s="48" t="n">
         <f aca="false">1/(G35/Regular_Timings!G35)</f>
         <v>3.60534646208669</v>
       </c>
-      <c r="H36" s="47" t="n">
+      <c r="H36" s="48" t="n">
         <f aca="false">1/(H35/Regular_Timings!H35)</f>
         <v>3.71338155532446</v>
       </c>
-      <c r="I36" s="47" t="n">
+      <c r="I36" s="48" t="n">
         <f aca="false">1/(I35/Regular_Timings!I35)</f>
         <v>3.87995098100785</v>
       </c>
-      <c r="J36" s="47" t="n">
+      <c r="J36" s="48" t="n">
         <f aca="false">1/(J35/Regular_Timings!J35)</f>
         <v>3.77692817787917</v>
       </c>
-      <c r="K36" s="47" t="n">
+      <c r="K36" s="48" t="n">
         <f aca="false">1/(K35/Regular_Timings!K35)</f>
         <v>3.64724155744514</v>
       </c>
-      <c r="L36" s="47" t="n">
+      <c r="L36" s="48" t="n">
         <f aca="false">1/(L35/Regular_Timings!L35)</f>
         <v>3.74020943453721</v>
       </c>
-      <c r="M36" s="47" t="n">
+      <c r="M36" s="48" t="n">
         <f aca="false">1/(M35/Regular_Timings!M35)</f>
         <v>3.50672105722098</v>
       </c>
-      <c r="N36" s="47" t="n">
+      <c r="N36" s="48" t="n">
         <f aca="false">1/(N35/Regular_Timings!N35)</f>
         <v>3.73405080495359</v>
       </c>
-      <c r="O36" s="47" t="n">
+      <c r="O36" s="48" t="n">
         <f aca="false">1/(O35/Regular_Timings!O35)</f>
         <v>3.48066002524706</v>
       </c>
-      <c r="P36" s="47" t="n">
+      <c r="P36" s="48" t="n">
         <f aca="false">1/(P35/Regular_Timings!P35)</f>
         <v>3.64532320360124</v>
       </c>
-      <c r="Q36" s="47" t="n">
+      <c r="Q36" s="48" t="n">
         <f aca="false">1/(Q35/Regular_Timings!Q35)</f>
         <v>3.69283488712217</v>
       </c>
-      <c r="R36" s="47" t="n">
+      <c r="R36" s="48" t="n">
         <f aca="false">1/(R35/Regular_Timings!R35)</f>
         <v>3.91914079157363</v>
       </c>
-      <c r="S36" s="47" t="n">
+      <c r="S36" s="48" t="n">
         <f aca="false">1/(S35/Regular_Timings!S35)</f>
         <v>3.70850736443567</v>
       </c>
-      <c r="T36" s="47" t="n">
+      <c r="T36" s="48" t="n">
         <f aca="false">1/(T35/Regular_Timings!T35)</f>
         <v>3.75420891553771</v>
       </c>
-      <c r="U36" s="47" t="n">
+      <c r="U36" s="48" t="n">
         <f aca="false">1/(U35/Regular_Timings!U35)</f>
         <v>3.84853896938329</v>
       </c>
-      <c r="V36" s="47" t="n">
+      <c r="V36" s="48" t="n">
         <f aca="false">Regular_Timings!V35/V35</f>
         <v>3.72104488019434</v>
       </c>
-      <c r="W36" s="47" t="n">
+      <c r="W36" s="48" t="n">
         <f aca="false">Regular_Timings!W35/W35</f>
         <v>3.67572728059469</v>
       </c>
-      <c r="X36" s="47" t="n">
+      <c r="X36" s="48" t="n">
         <f aca="false">Regular_Timings!X35/X35</f>
         <v>4.19080065811635</v>
       </c>
-      <c r="Y36" s="47" t="n">
+      <c r="Y36" s="48" t="n">
         <f aca="false">Regular_Timings!Y35/Y35</f>
         <v>3.89406092958739</v>
       </c>
-      <c r="Z36" s="47" t="n">
+      <c r="Z36" s="48" t="n">
         <f aca="false">Regular_Timings!Z35/Z35</f>
         <v>3.55407794695691</v>
       </c>
-      <c r="AA36" s="47" t="n">
+      <c r="AA36" s="48" t="n">
         <f aca="false">Regular_Timings!AA35/AA35</f>
         <v>4.00488485600993</v>
       </c>
-      <c r="AB36" s="47" t="n">
+      <c r="AB36" s="48" t="n">
         <f aca="false">Regular_Timings!AB35/AB35</f>
         <v>3.66631773819967</v>
       </c>
-      <c r="AC36" s="47" t="n">
+      <c r="AC36" s="48" t="n">
         <f aca="false">Regular_Timings!AC35/AC35</f>
         <v>3.56831780200242</v>
       </c>
-      <c r="AD36" s="47" t="n">
+      <c r="AD36" s="48" t="n">
         <f aca="false">Regular_Timings!AD35/AD35</f>
         <v>3.7717099313906</v>
       </c>
-      <c r="AE36" s="47" t="n">
+      <c r="AE36" s="48" t="n">
         <f aca="false">Regular_Timings!AE35/AE35</f>
         <v>3.65797605865082</v>
       </c>
-      <c r="AG36" s="47" t="n">
+      <c r="AG36" s="48" t="n">
         <f aca="false">Regular_Timings!AG35/AG35</f>
         <v>3.6639766566581</v>
       </c>
-      <c r="AH36" s="47" t="n">
+      <c r="AH36" s="48" t="n">
         <f aca="false">Regular_Timings!AH35/AH35</f>
         <v>3.88981824858324</v>
       </c>
-      <c r="AI36" s="47" t="n">
+      <c r="AI36" s="48" t="n">
         <f aca="false">Regular_Timings!AI35/AI35</f>
         <v>3.95034639182564</v>
       </c>
-      <c r="AJ36" s="47" t="n">
+      <c r="AJ36" s="48" t="n">
         <f aca="false">Regular_Timings!AJ35/AJ35</f>
         <v>3.61276930976272</v>
       </c>
-      <c r="AK36" s="47" t="n">
+      <c r="AK36" s="48" t="n">
         <f aca="false">Regular_Timings!AK35/AK35</f>
         <v>3.47176276903545</v>
       </c>
-      <c r="AL36" s="47" t="n">
+      <c r="AL36" s="48" t="n">
         <f aca="false">Regular_Timings!AL35/AL35</f>
         <v>3.42704556536553</v>
       </c>
-      <c r="AM36" s="47" t="n">
+      <c r="AM36" s="48" t="n">
         <f aca="false">Regular_Timings!AM35/AM35</f>
         <v>3.62119345537265</v>
       </c>
-      <c r="AN36" s="47" t="n">
+      <c r="AN36" s="48" t="n">
         <f aca="false">Regular_Timings!AN35/AN35</f>
         <v>3.45756053775267</v>
+      </c>
+      <c r="AO36" s="48" t="n">
+        <f aca="false">Regular_Timings!AO35/AO35</f>
+        <v>3.39502062222087</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="AC37" s="39"/>
+      <c r="AC37" s="40"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AC38" s="48" t="s">
-        <v>88</v>
+      <c r="AC38" s="49" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -11064,8 +11312,8 @@
   </sheetPr>
   <dimension ref="A1:AJ97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ2" activeCellId="0" sqref="AJ2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="I15 A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11082,7 +11330,7 @@
         <v>51</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>39</v>
@@ -11111,195 +11359,200 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q3" s="49" t="s">
         <v>94</v>
       </c>
+      <c r="Q3" s="50" t="s">
+        <v>95</v>
+      </c>
       <c r="T3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AJ3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" s="49" t="s">
         <v>111</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11309,7 +11562,7 @@
       <c r="J86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J87" s="12"/>
+      <c r="J87" s="13"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J88" s="4"/>

</xml_diff>

<commit_message>
- Updated milestone and line count statistics data
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="168">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -791,7 +791,7 @@
     <numFmt numFmtId="168" formatCode="0.00%"/>
     <numFmt numFmtId="169" formatCode="0.00"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -953,6 +953,14 @@
     </font>
     <font>
       <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -1129,7 +1137,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1318,6 +1326,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1438,13 +1450,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>738360</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>186480</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1457,7 +1469,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="738360" y="9558720"/>
+          <a:off x="738360" y="9559080"/>
           <a:ext cx="9703800" cy="2053800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1473,13 +1485,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>22680</xdr:colOff>
+      <xdr:colOff>23040</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>63720</xdr:colOff>
+      <xdr:colOff>64080</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
@@ -1494,7 +1506,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233440" y="12009600"/>
+          <a:off x="2233800" y="12009600"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1510,15 +1522,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>22680</xdr:colOff>
+      <xdr:colOff>23040</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>29160</xdr:colOff>
+      <xdr:colOff>29520</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>83160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1531,7 +1543,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233440" y="14623920"/>
+          <a:off x="2233800" y="14624280"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1547,15 +1559,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>22680</xdr:colOff>
+      <xdr:colOff>23040</xdr:colOff>
       <xdr:row>97</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>633600</xdr:colOff>
+      <xdr:colOff>633960</xdr:colOff>
       <xdr:row>112</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1568,7 +1580,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233440" y="16919640"/>
+          <a:off x="2233800" y="16920000"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1584,15 +1596,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>22320</xdr:colOff>
+      <xdr:colOff>22680</xdr:colOff>
       <xdr:row>115</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>586800</xdr:colOff>
+      <xdr:colOff>587160</xdr:colOff>
       <xdr:row>128</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1605,7 +1617,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233080" y="20074320"/>
+          <a:off x="2233440" y="20074680"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1621,15 +1633,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>51840</xdr:colOff>
+      <xdr:colOff>52200</xdr:colOff>
       <xdr:row>131</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>611640</xdr:colOff>
+      <xdr:colOff>612000</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1642,7 +1654,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2262600" y="22853880"/>
+          <a:off x="2262960" y="22854240"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1658,15 +1670,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
+      <xdr:colOff>20160</xdr:colOff>
       <xdr:row>145</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>257040</xdr:colOff>
+      <xdr:colOff>257400</xdr:colOff>
       <xdr:row>157</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1679,7 +1691,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2230560" y="25332120"/>
+          <a:off x="2230920" y="25332480"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1697,13 +1709,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
       <xdr:row>175</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>309600</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1716,7 +1728,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3115080" y="30596040"/>
+          <a:off x="3115080" y="30596400"/>
           <a:ext cx="9708120" cy="2138400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1808,13 +1820,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>306720</xdr:colOff>
       <xdr:row>203</xdr:row>
-      <xdr:rowOff>114840</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>123840</xdr:colOff>
       <xdr:row>215</xdr:row>
-      <xdr:rowOff>121320</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1827,7 +1839,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3156480" y="35579880"/>
+          <a:off x="3156480" y="35580240"/>
           <a:ext cx="9480960" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1845,13 +1857,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>275040</xdr:colOff>
       <xdr:row>216</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>629640</xdr:colOff>
       <xdr:row>227</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1864,7 +1876,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3124800" y="37781640"/>
+          <a:off x="3124800" y="37782000"/>
           <a:ext cx="9161280" cy="2044800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3045,11 +3057,11 @@
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>794.02</v>
+        <v>718.46</v>
       </c>
       <c r="Q6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>223.68851</v>
+        <v>208.05438</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3064,11 +3076,11 @@
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>227.04</v>
+        <v>206.34</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>94.30204</v>
+        <v>88.19253</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3083,11 +3095,11 @@
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>348.45</v>
+        <v>293.42</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>94.69443</v>
+        <v>88.95074</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3110,11 +3122,11 @@
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1692.44</v>
+        <v>1563.83</v>
       </c>
       <c r="Q9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>417.17874</v>
+        <v>402.22093</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3133,11 +3145,11 @@
       <c r="O10" s="4"/>
       <c r="P10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>167.94</v>
+        <v>160.46</v>
       </c>
       <c r="Q10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>52.72242</v>
+        <v>51.02656</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3156,11 +3168,11 @@
       <c r="O11" s="4"/>
       <c r="P11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>145.92355</v>
+        <v>141.90512</v>
       </c>
       <c r="Q11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>145.92355</v>
+        <v>141.90512</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3179,11 +3191,11 @@
       <c r="O12" s="4"/>
       <c r="P12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>115.41</v>
+        <v>110.49</v>
       </c>
       <c r="Q12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>46.94905</v>
+        <v>45.08509</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3202,11 +3214,11 @@
       <c r="O13" s="4"/>
       <c r="P13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>608.85</v>
+        <v>589.26</v>
       </c>
       <c r="Q13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>166.8921</v>
+        <v>160.43867</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3229,11 +3241,11 @@
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>381.37</v>
+        <v>334.27</v>
       </c>
       <c r="Q14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>125.92209</v>
+        <v>120.60729</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,11 +3264,11 @@
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>462.26</v>
+        <v>416.12</v>
       </c>
       <c r="Q15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>146.09033</v>
+        <v>140.40068</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3278,11 +3290,11 @@
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>2869.1</v>
+        <v>2766.77</v>
       </c>
       <c r="Q16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>708.86256</v>
+        <v>690.5803</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3300,11 +3312,11 @@
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>194.14</v>
+        <v>339.13</v>
       </c>
       <c r="Q17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
-        <v>58.72226</v>
+        <v>57.41775</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3322,11 +3334,11 @@
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>690.24</v>
+        <v>940.81</v>
       </c>
       <c r="Q18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>200.84803</v>
+        <v>198.75492</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3348,11 +3360,11 @@
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>819.99</v>
+        <v>888.46</v>
       </c>
       <c r="Q19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>237.8355</v>
+        <v>234.58123</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,11 +3382,11 @@
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>132.48</v>
+        <v>134.32</v>
       </c>
       <c r="Q20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>59.09289</v>
+        <v>56.79314</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3392,11 +3404,11 @@
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>452.53</v>
+        <v>458.41</v>
       </c>
       <c r="Q21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>162.27863</v>
+        <v>157.68583</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,11 +3426,11 @@
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>408.59</v>
+        <v>412.82</v>
       </c>
       <c r="Q22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>141.76978</v>
+        <v>135.29315</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3436,11 +3448,11 @@
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>254.97</v>
+        <v>257.81</v>
       </c>
       <c r="Q23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>105.04129</v>
+        <v>98.06408</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,11 +3470,11 @@
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>277.5</v>
+        <v>280.82</v>
       </c>
       <c r="Q24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>96.11108</v>
+        <v>90.14262</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3481,11 +3493,11 @@
       <c r="O25" s="1"/>
       <c r="P25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>327.1</v>
+        <v>331.41</v>
       </c>
       <c r="Q25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>105.36939</v>
+        <v>99.25307</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3503,11 +3515,11 @@
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>801.22</v>
+        <v>814.98</v>
       </c>
       <c r="Q26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>260.98396</v>
+        <v>251.39177</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3525,11 +3537,11 @@
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>176.97</v>
+        <v>189.39</v>
       </c>
       <c r="Q27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>53.77898</v>
+        <v>53.83953</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3547,11 +3559,11 @@
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>416.46</v>
+        <v>428.23</v>
       </c>
       <c r="Q28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>128.46179</v>
+        <v>128.0109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,11 +3585,11 @@
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1697.75</v>
+        <v>1727.58</v>
       </c>
       <c r="Q29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>471.05463</v>
+        <v>479.03154</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3595,11 +3607,11 @@
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>43.58</v>
+        <v>44.85</v>
       </c>
       <c r="Q30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>21.41855</v>
+        <v>22.08076</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3617,11 +3629,11 @@
       </c>
       <c r="P31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>31.45</v>
+        <v>32.61</v>
       </c>
       <c r="Q31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>24.87601</v>
+        <v>25.16425</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3639,11 +3651,11 @@
       </c>
       <c r="P32" s="11" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>161.45</v>
+        <v>167.46</v>
       </c>
       <c r="Q32" s="11" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>58.55777</v>
+        <v>60.31915</v>
       </c>
       <c r="R32" s="11"/>
     </row>
@@ -3818,11 +3830,11 @@
       </c>
       <c r="P49" s="0" t="n">
         <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
-        <v>16369.63</v>
+        <v>16188.34</v>
       </c>
       <c r="Q49" s="11" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D35:ND35&lt;&gt;""),Parallel_Timings!D35:ND35)</f>
-        <v>4682.64208</v>
+        <v>4536.31213</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3837,7 +3849,7 @@
       </c>
       <c r="Q50" s="19" t="n">
         <f aca="false">P49/Q49</f>
-        <v>3.49581063859572</v>
+        <v>3.56861246229986</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4103,11 +4115,11 @@
   <dimension ref="A2:BK109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="AF5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AF1" activeCellId="0" sqref="AF1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AR38" activeCellId="0" sqref="AR38"/>
+      <selection pane="bottomRight" activeCell="AP42" activeCellId="0" sqref="AP42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4258,6 +4270,9 @@
       </c>
       <c r="AR4" s="27" t="n">
         <v>44423</v>
+      </c>
+      <c r="AS4" s="27" t="n">
+        <v>44430</v>
       </c>
     </row>
     <row r="5" s="30" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4338,6 +4353,9 @@
       <c r="AR5" s="0" t="n">
         <v>1292.34</v>
       </c>
+      <c r="AS5" s="0" t="n">
+        <v>1117.64</v>
+      </c>
     </row>
     <row r="6" s="12" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="36" t="s">
@@ -4468,6 +4486,9 @@
       <c r="AR6" s="0" t="n">
         <v>794.02</v>
       </c>
+      <c r="AS6" s="0" t="n">
+        <v>718.46</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
@@ -4599,6 +4620,9 @@
       <c r="AR7" s="0" t="n">
         <v>227.04</v>
       </c>
+      <c r="AS7" s="0" t="n">
+        <v>206.34</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="37" t="s">
@@ -4718,6 +4742,9 @@
       <c r="AR8" s="0" t="n">
         <v>348.45</v>
       </c>
+      <c r="AS8" s="0" t="n">
+        <v>293.42</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
@@ -4849,6 +4876,9 @@
       <c r="AR9" s="0" t="n">
         <v>1692.44</v>
       </c>
+      <c r="AS9" s="0" t="n">
+        <v>1563.83</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
@@ -4980,6 +5010,9 @@
       <c r="AR10" s="0" t="n">
         <v>167.94</v>
       </c>
+      <c r="AS10" s="0" t="n">
+        <v>160.46</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
@@ -5111,6 +5144,9 @@
       <c r="AR11" s="0" t="n">
         <v>523.99</v>
       </c>
+      <c r="AS11" s="0" t="n">
+        <v>462.19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
@@ -5215,6 +5251,9 @@
       <c r="AR12" s="0" t="n">
         <v>115.41</v>
       </c>
+      <c r="AS12" s="0" t="n">
+        <v>110.49</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="37" t="s">
@@ -5307,6 +5346,9 @@
       <c r="AR13" s="0" t="n">
         <v>608.85</v>
       </c>
+      <c r="AS13" s="0" t="n">
+        <v>589.26</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
@@ -5438,6 +5480,9 @@
       <c r="AR14" s="0" t="n">
         <v>381.37</v>
       </c>
+      <c r="AS14" s="0" t="n">
+        <v>334.27</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38" t="s">
@@ -5569,6 +5614,9 @@
       <c r="AR15" s="0" t="n">
         <v>462.26</v>
       </c>
+      <c r="AS15" s="0" t="n">
+        <v>416.12</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38" t="s">
@@ -5700,6 +5748,9 @@
       <c r="AR16" s="0" t="n">
         <v>2869.1</v>
       </c>
+      <c r="AS16" s="0" t="n">
+        <v>2766.77</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38" t="s">
@@ -5750,6 +5801,9 @@
       <c r="AR17" s="0" t="n">
         <v>194.14</v>
       </c>
+      <c r="AS17" s="0" t="n">
+        <v>339.13</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38" t="s">
@@ -5881,6 +5935,9 @@
       <c r="AR18" s="0" t="n">
         <v>690.24</v>
       </c>
+      <c r="AS18" s="0" t="n">
+        <v>940.81</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38" t="s">
@@ -6012,6 +6069,9 @@
       <c r="AR19" s="0" t="n">
         <v>819.99</v>
       </c>
+      <c r="AS19" s="0" t="n">
+        <v>888.46</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38" t="s">
@@ -6143,6 +6203,9 @@
       <c r="AR20" s="0" t="n">
         <v>132.48</v>
       </c>
+      <c r="AS20" s="0" t="n">
+        <v>134.32</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38" t="s">
@@ -6274,6 +6337,9 @@
       <c r="AR21" s="0" t="n">
         <v>452.53</v>
       </c>
+      <c r="AS21" s="0" t="n">
+        <v>458.41</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38" t="s">
@@ -6405,6 +6471,9 @@
       <c r="AR22" s="0" t="n">
         <v>408.59</v>
       </c>
+      <c r="AS22" s="0" t="n">
+        <v>412.82</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38" t="s">
@@ -6536,6 +6605,9 @@
       <c r="AR23" s="0" t="n">
         <v>254.97</v>
       </c>
+      <c r="AS23" s="0" t="n">
+        <v>257.81</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38" t="s">
@@ -6667,6 +6739,9 @@
       <c r="AR24" s="0" t="n">
         <v>277.5</v>
       </c>
+      <c r="AS24" s="0" t="n">
+        <v>280.82</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38" t="s">
@@ -6798,6 +6873,9 @@
       <c r="AR25" s="0" t="n">
         <v>327.1</v>
       </c>
+      <c r="AS25" s="0" t="n">
+        <v>331.41</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39" t="s">
@@ -6929,6 +7007,9 @@
       <c r="AR26" s="0" t="n">
         <v>801.22</v>
       </c>
+      <c r="AS26" s="0" t="n">
+        <v>814.98</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="38" t="s">
@@ -7060,6 +7141,9 @@
       <c r="AR27" s="0" t="n">
         <v>176.97</v>
       </c>
+      <c r="AS27" s="0" t="n">
+        <v>189.39</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38" t="s">
@@ -7137,6 +7221,9 @@
       <c r="AR28" s="0" t="n">
         <v>416.46</v>
       </c>
+      <c r="AS28" s="0" t="n">
+        <v>428.23</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="38" t="s">
@@ -7268,6 +7355,9 @@
       <c r="AR29" s="0" t="n">
         <v>1697.75</v>
       </c>
+      <c r="AS29" s="0" t="n">
+        <v>1727.58</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38" t="s">
@@ -7399,6 +7489,9 @@
       <c r="AR30" s="0" t="n">
         <v>43.58</v>
       </c>
+      <c r="AS30" s="0" t="n">
+        <v>44.85</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="37" t="s">
@@ -7530,6 +7623,9 @@
       <c r="AR31" s="0" t="n">
         <v>31.45</v>
       </c>
+      <c r="AS31" s="0" t="n">
+        <v>32.61</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="37" t="s">
@@ -7661,6 +7757,9 @@
       <c r="AR32" s="0" t="n">
         <v>161.45</v>
       </c>
+      <c r="AS32" s="0" t="n">
+        <v>167.46</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="37" t="s">
@@ -7838,6 +7937,10 @@
       <c r="AR35" s="0" t="n">
         <f aca="false">SUM(AR$5:AR$32)</f>
         <v>16369.63</v>
+      </c>
+      <c r="AS35" s="0" t="n">
+        <f aca="false">SUM(AS$5:AS$32)</f>
+        <v>16188.34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8009,8 +8112,12 @@
         <f aca="false">AR35/AQ35</f>
         <v>1.04525807986157</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AS36" s="40" t="n">
+        <f aca="false">AS35/AR35</f>
+        <v>0.988925223111335</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="19.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>108</v>
       </c>
@@ -8042,6 +8149,9 @@
       </c>
       <c r="AL38" s="44"/>
       <c r="AR38" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS38" s="0" t="s">
         <v>116</v>
       </c>
     </row>
@@ -8360,14 +8470,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AR38"/>
+  <dimension ref="A2:AS38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AF5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="AH44" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AF1" activeCellId="0" sqref="AF1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AQ35" activeCellId="0" sqref="AQ35"/>
+      <selection pane="topRight" activeCell="AH1" activeCellId="0" sqref="AH1"/>
+      <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+      <selection pane="bottomRight" activeCell="AR39" activeCellId="0" sqref="AR39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8515,25 +8625,28 @@
       <c r="AR4" s="23" t="n">
         <v>44423</v>
       </c>
-    </row>
-    <row r="5" s="49" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AS4" s="47" t="n">
+        <v>44430</v>
+      </c>
+    </row>
+    <row r="5" s="50" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
       <c r="P5" s="35"/>
       <c r="Q5" s="33"/>
       <c r="R5" s="35"/>
@@ -8592,6 +8705,9 @@
       <c r="AR5" s="0" t="n">
         <v>273.21572</v>
       </c>
+      <c r="AS5" s="0" t="n">
+        <v>251.02615</v>
+      </c>
     </row>
     <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -8721,6 +8837,9 @@
       <c r="AR6" s="0" t="n">
         <v>223.68851</v>
       </c>
+      <c r="AS6" s="0" t="n">
+        <v>208.05438</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
@@ -8849,6 +8968,9 @@
       <c r="AR7" s="0" t="n">
         <v>94.30204</v>
       </c>
+      <c r="AS7" s="0" t="n">
+        <v>88.19253</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
@@ -8965,6 +9087,9 @@
       <c r="AR8" s="0" t="n">
         <v>94.69443</v>
       </c>
+      <c r="AS8" s="0" t="n">
+        <v>88.95074</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="38" t="s">
@@ -9093,6 +9218,9 @@
       <c r="AR9" s="0" t="n">
         <v>417.17874</v>
       </c>
+      <c r="AS9" s="0" t="n">
+        <v>402.22093</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="37" t="s">
@@ -9221,6 +9349,9 @@
       <c r="AR10" s="0" t="n">
         <v>52.72242</v>
       </c>
+      <c r="AS10" s="0" t="n">
+        <v>51.02656</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
@@ -9349,6 +9480,9 @@
       <c r="AR11" s="0" t="n">
         <v>145.92355</v>
       </c>
+      <c r="AS11" s="0" t="n">
+        <v>141.90512</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="37" t="s">
@@ -9450,6 +9584,9 @@
       <c r="AR12" s="0" t="n">
         <v>46.94905</v>
       </c>
+      <c r="AS12" s="0" t="n">
+        <v>45.08509</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
@@ -9539,6 +9676,9 @@
       <c r="AR13" s="0" t="n">
         <v>166.8921</v>
       </c>
+      <c r="AS13" s="0" t="n">
+        <v>160.43867</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="38" t="s">
@@ -9667,6 +9807,9 @@
       <c r="AR14" s="0" t="n">
         <v>125.92209</v>
       </c>
+      <c r="AS14" s="0" t="n">
+        <v>120.60729</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="38" t="s">
@@ -9795,6 +9938,9 @@
       <c r="AR15" s="0" t="n">
         <v>146.09033</v>
       </c>
+      <c r="AS15" s="0" t="n">
+        <v>140.40068</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="38" t="s">
@@ -9923,6 +10069,9 @@
       <c r="AR16" s="0" t="n">
         <v>708.86256</v>
       </c>
+      <c r="AS16" s="0" t="n">
+        <v>690.5803</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="38" t="s">
@@ -9967,6 +10116,9 @@
       <c r="AR17" s="0" t="n">
         <v>58.72226</v>
       </c>
+      <c r="AS17" s="0" t="n">
+        <v>57.41775</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="38" t="s">
@@ -10095,6 +10247,9 @@
       <c r="AR18" s="0" t="n">
         <v>200.84803</v>
       </c>
+      <c r="AS18" s="0" t="n">
+        <v>198.75492</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="38" t="s">
@@ -10223,6 +10378,9 @@
       <c r="AR19" s="0" t="n">
         <v>237.8355</v>
       </c>
+      <c r="AS19" s="0" t="n">
+        <v>234.58123</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="38" t="s">
@@ -10351,6 +10509,9 @@
       <c r="AR20" s="0" t="n">
         <v>59.09289</v>
       </c>
+      <c r="AS20" s="0" t="n">
+        <v>56.79314</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="38" t="s">
@@ -10479,6 +10640,9 @@
       <c r="AR21" s="0" t="n">
         <v>162.27863</v>
       </c>
+      <c r="AS21" s="0" t="n">
+        <v>157.68583</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="38" t="s">
@@ -10607,6 +10771,9 @@
       <c r="AR22" s="0" t="n">
         <v>141.76978</v>
       </c>
+      <c r="AS22" s="0" t="n">
+        <v>135.29315</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="38" t="s">
@@ -10735,6 +10902,9 @@
       <c r="AR23" s="0" t="n">
         <v>105.04129</v>
       </c>
+      <c r="AS23" s="0" t="n">
+        <v>98.06408</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="38" t="s">
@@ -10863,6 +11033,9 @@
       <c r="AR24" s="0" t="n">
         <v>96.11108</v>
       </c>
+      <c r="AS24" s="0" t="n">
+        <v>90.14262</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="38" t="s">
@@ -10991,6 +11164,9 @@
       <c r="AR25" s="0" t="n">
         <v>105.36939</v>
       </c>
+      <c r="AS25" s="0" t="n">
+        <v>99.25307</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="39" t="s">
@@ -11119,6 +11295,9 @@
       <c r="AR26" s="0" t="n">
         <v>260.98396</v>
       </c>
+      <c r="AS26" s="0" t="n">
+        <v>251.39177</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="38" t="s">
@@ -11247,6 +11426,9 @@
       <c r="AR27" s="0" t="n">
         <v>53.77898</v>
       </c>
+      <c r="AS27" s="0" t="n">
+        <v>53.83953</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="38" t="s">
@@ -11321,6 +11503,9 @@
       <c r="AR28" s="0" t="n">
         <v>128.46179</v>
       </c>
+      <c r="AS28" s="0" t="n">
+        <v>128.0109</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="38" t="s">
@@ -11449,6 +11634,9 @@
       <c r="AR29" s="0" t="n">
         <v>471.05463</v>
       </c>
+      <c r="AS29" s="0" t="n">
+        <v>479.03154</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="38" t="s">
@@ -11577,6 +11765,9 @@
       <c r="AR30" s="0" t="n">
         <v>21.41855</v>
       </c>
+      <c r="AS30" s="0" t="n">
+        <v>22.08076</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="37" t="s">
@@ -11705,8 +11896,11 @@
       <c r="AR31" s="0" t="n">
         <v>24.87601</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AS31" s="0" t="n">
+        <v>25.16425</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
         <v>58</v>
       </c>
@@ -11832,6 +12026,9 @@
       </c>
       <c r="AR32" s="0" t="n">
         <v>58.55777</v>
+      </c>
+      <c r="AS32" s="0" t="n">
+        <v>60.31915</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12007,174 +12204,182 @@
         <f aca="false">SUM(AR$5:AR$32)</f>
         <v>4682.64208</v>
       </c>
+      <c r="AS35" s="0" t="n">
+        <f aca="false">SUM(AS$5:AS$32)</f>
+        <v>4536.31213</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C36" s="50" t="n">
+      <c r="C36" s="51" t="n">
         <f aca="false">1/(C35/Regular_Timings!C35)</f>
         <v>3.74749121272531</v>
       </c>
-      <c r="D36" s="50" t="n">
+      <c r="D36" s="51" t="n">
         <f aca="false">1/(D35/Regular_Timings!D35)</f>
         <v>3.41302620041922</v>
       </c>
-      <c r="E36" s="50" t="n">
+      <c r="E36" s="51" t="n">
         <f aca="false">1/(E35/Regular_Timings!E35)</f>
         <v>3.58035321194409</v>
       </c>
-      <c r="F36" s="50" t="n">
+      <c r="F36" s="51" t="n">
         <f aca="false">1/(F35/Regular_Timings!F35)</f>
         <v>3.77604759094586</v>
       </c>
-      <c r="G36" s="50" t="n">
+      <c r="G36" s="51" t="n">
         <f aca="false">1/(G35/Regular_Timings!G35)</f>
         <v>3.60534646208669</v>
       </c>
-      <c r="H36" s="50" t="n">
+      <c r="H36" s="51" t="n">
         <f aca="false">1/(H35/Regular_Timings!H35)</f>
         <v>3.71338155532446</v>
       </c>
-      <c r="I36" s="50" t="n">
+      <c r="I36" s="51" t="n">
         <f aca="false">1/(I35/Regular_Timings!I35)</f>
         <v>3.87995098100785</v>
       </c>
-      <c r="J36" s="50" t="n">
+      <c r="J36" s="51" t="n">
         <f aca="false">1/(J35/Regular_Timings!J35)</f>
         <v>3.77692817787917</v>
       </c>
-      <c r="K36" s="50" t="n">
+      <c r="K36" s="51" t="n">
         <f aca="false">1/(K35/Regular_Timings!K35)</f>
         <v>3.64724155744514</v>
       </c>
-      <c r="L36" s="50" t="n">
+      <c r="L36" s="51" t="n">
         <f aca="false">1/(L35/Regular_Timings!L35)</f>
         <v>3.74020943453721</v>
       </c>
-      <c r="M36" s="50" t="n">
+      <c r="M36" s="51" t="n">
         <f aca="false">1/(M35/Regular_Timings!M35)</f>
         <v>3.50672105722098</v>
       </c>
-      <c r="N36" s="50" t="n">
+      <c r="N36" s="51" t="n">
         <f aca="false">1/(N35/Regular_Timings!N35)</f>
         <v>3.73405080495359</v>
       </c>
-      <c r="O36" s="50" t="n">
+      <c r="O36" s="51" t="n">
         <f aca="false">1/(O35/Regular_Timings!O35)</f>
         <v>3.48066002524706</v>
       </c>
-      <c r="P36" s="50" t="n">
+      <c r="P36" s="51" t="n">
         <f aca="false">1/(P35/Regular_Timings!P35)</f>
         <v>3.64532320360124</v>
       </c>
-      <c r="Q36" s="50" t="n">
+      <c r="Q36" s="51" t="n">
         <f aca="false">1/(Q35/Regular_Timings!Q35)</f>
         <v>3.69283488712217</v>
       </c>
-      <c r="R36" s="50" t="n">
+      <c r="R36" s="51" t="n">
         <f aca="false">1/(R35/Regular_Timings!R35)</f>
         <v>3.91914079157363</v>
       </c>
-      <c r="S36" s="50" t="n">
+      <c r="S36" s="51" t="n">
         <f aca="false">1/(S35/Regular_Timings!S35)</f>
         <v>3.70850736443567</v>
       </c>
-      <c r="T36" s="50" t="n">
+      <c r="T36" s="51" t="n">
         <f aca="false">1/(T35/Regular_Timings!T35)</f>
         <v>3.75420891553771</v>
       </c>
-      <c r="U36" s="50" t="n">
+      <c r="U36" s="51" t="n">
         <f aca="false">1/(U35/Regular_Timings!U35)</f>
         <v>3.84853896938329</v>
       </c>
-      <c r="V36" s="50" t="n">
+      <c r="V36" s="51" t="n">
         <f aca="false">Regular_Timings!V35/V35</f>
         <v>3.72104488019434</v>
       </c>
-      <c r="W36" s="50" t="n">
+      <c r="W36" s="51" t="n">
         <f aca="false">Regular_Timings!W35/W35</f>
         <v>3.67572728059469</v>
       </c>
-      <c r="X36" s="50" t="n">
+      <c r="X36" s="51" t="n">
         <f aca="false">Regular_Timings!X35/X35</f>
         <v>4.19080065811635</v>
       </c>
-      <c r="Y36" s="50" t="n">
+      <c r="Y36" s="51" t="n">
         <f aca="false">Regular_Timings!Y35/Y35</f>
         <v>3.89406092958739</v>
       </c>
-      <c r="Z36" s="50" t="n">
+      <c r="Z36" s="51" t="n">
         <f aca="false">Regular_Timings!Z35/Z35</f>
         <v>3.55407794695691</v>
       </c>
-      <c r="AA36" s="50" t="n">
+      <c r="AA36" s="51" t="n">
         <f aca="false">Regular_Timings!AA35/AA35</f>
         <v>4.00488485600993</v>
       </c>
-      <c r="AB36" s="50" t="n">
+      <c r="AB36" s="51" t="n">
         <f aca="false">Regular_Timings!AB35/AB35</f>
         <v>3.66631773819967</v>
       </c>
-      <c r="AC36" s="50" t="n">
+      <c r="AC36" s="51" t="n">
         <f aca="false">Regular_Timings!AC35/AC35</f>
         <v>3.56831780200242</v>
       </c>
-      <c r="AD36" s="50" t="n">
+      <c r="AD36" s="51" t="n">
         <f aca="false">Regular_Timings!AD35/AD35</f>
         <v>3.7717099313906</v>
       </c>
-      <c r="AE36" s="50" t="n">
+      <c r="AE36" s="51" t="n">
         <f aca="false">Regular_Timings!AE35/AE35</f>
         <v>3.65797605865082</v>
       </c>
-      <c r="AG36" s="50" t="n">
+      <c r="AG36" s="51" t="n">
         <f aca="false">Regular_Timings!AG35/AG35</f>
         <v>3.6639766566581</v>
       </c>
-      <c r="AH36" s="50" t="n">
+      <c r="AH36" s="51" t="n">
         <f aca="false">Regular_Timings!AH35/AH35</f>
         <v>3.88981824858324</v>
       </c>
-      <c r="AI36" s="50" t="n">
+      <c r="AI36" s="51" t="n">
         <f aca="false">Regular_Timings!AI35/AI35</f>
         <v>3.95034639182564</v>
       </c>
-      <c r="AJ36" s="50" t="n">
+      <c r="AJ36" s="51" t="n">
         <f aca="false">Regular_Timings!AJ35/AJ35</f>
         <v>3.61276930976272</v>
       </c>
-      <c r="AK36" s="50" t="n">
+      <c r="AK36" s="51" t="n">
         <f aca="false">Regular_Timings!AK35/AK35</f>
         <v>3.47176276903545</v>
       </c>
-      <c r="AL36" s="50" t="n">
+      <c r="AL36" s="51" t="n">
         <f aca="false">Regular_Timings!AL35/AL35</f>
         <v>3.42704556536553</v>
       </c>
-      <c r="AM36" s="50" t="n">
+      <c r="AM36" s="51" t="n">
         <f aca="false">Regular_Timings!AM35/AM35</f>
         <v>3.62119345537265</v>
       </c>
-      <c r="AN36" s="50" t="n">
+      <c r="AN36" s="51" t="n">
         <f aca="false">Regular_Timings!AN35/AN35</f>
         <v>3.45756053775267</v>
       </c>
-      <c r="AO36" s="50" t="n">
+      <c r="AO36" s="51" t="n">
         <f aca="false">Regular_Timings!AO35/AO35</f>
         <v>3.39502062222087</v>
       </c>
-      <c r="AP36" s="50" t="n">
+      <c r="AP36" s="51" t="n">
         <f aca="false">Regular_Timings!AP35/AP35</f>
         <v>3.44119135284858</v>
       </c>
-      <c r="AQ36" s="50" t="n">
+      <c r="AQ36" s="51" t="n">
         <f aca="false">Regular_Timings!AQ35/AQ35</f>
         <v>3.37549763471932</v>
       </c>
-      <c r="AR36" s="50" t="n">
+      <c r="AR36" s="51" t="n">
         <f aca="false">Regular_Timings!AR35/AR35</f>
         <v>3.49581063859572</v>
+      </c>
+      <c r="AS36" s="51" t="n">
+        <f aca="false">Regular_Timings!AS35/AS35</f>
+        <v>3.56861246229986</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12183,7 +12388,7 @@
       <c r="AC37" s="42"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AC38" s="51" t="s">
+      <c r="AC38" s="52" t="s">
         <v>120</v>
       </c>
     </row>
@@ -12263,7 +12468,7 @@
       <c r="M3" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="Q3" s="52" t="s">
+      <c r="Q3" s="53" t="s">
         <v>126</v>
       </c>
       <c r="T3" s="0" t="s">
@@ -12324,7 +12529,7 @@
       <c r="A8" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="53" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Updated milestone tracking and line counts.
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="168">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -1450,13 +1450,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>738360</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>186480</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1469,7 +1469,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="738360" y="9559080"/>
+          <a:off x="738360" y="9559440"/>
           <a:ext cx="9703800" cy="2053800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1485,13 +1485,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23040</xdr:colOff>
+      <xdr:colOff>23400</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>29160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>64080</xdr:colOff>
+      <xdr:colOff>64440</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
@@ -1506,7 +1506,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233800" y="12009600"/>
+          <a:off x="2234160" y="12009600"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1522,15 +1522,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23040</xdr:colOff>
+      <xdr:colOff>23400</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>29880</xdr:colOff>
       <xdr:row>95</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1543,7 +1543,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233800" y="14624280"/>
+          <a:off x="2234160" y="14624640"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1559,15 +1559,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23040</xdr:colOff>
+      <xdr:colOff>23400</xdr:colOff>
       <xdr:row>97</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>633960</xdr:colOff>
+      <xdr:colOff>634320</xdr:colOff>
       <xdr:row>112</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1580,7 +1580,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233800" y="16920000"/>
+          <a:off x="2234160" y="16920360"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1596,15 +1596,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>22680</xdr:colOff>
+      <xdr:colOff>23040</xdr:colOff>
       <xdr:row>115</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>587160</xdr:colOff>
+      <xdr:colOff>587520</xdr:colOff>
       <xdr:row>128</xdr:row>
-      <xdr:rowOff>83880</xdr:rowOff>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1617,7 +1617,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233440" y="20074680"/>
+          <a:off x="2233800" y="20075040"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1633,15 +1633,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>52200</xdr:colOff>
+      <xdr:colOff>52560</xdr:colOff>
       <xdr:row>131</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>612000</xdr:colOff>
+      <xdr:colOff>612360</xdr:colOff>
       <xdr:row>143</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1654,7 +1654,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2262960" y="22854240"/>
+          <a:off x="2263320" y="22854600"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1670,15 +1670,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>20160</xdr:colOff>
+      <xdr:colOff>20520</xdr:colOff>
       <xdr:row>145</xdr:row>
-      <xdr:rowOff>32400</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
+      <xdr:colOff>257760</xdr:colOff>
       <xdr:row>157</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>38880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1691,7 +1691,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2230920" y="25332480"/>
+          <a:off x="2231280" y="25332840"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1709,13 +1709,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
       <xdr:row>175</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>38880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>309600</xdr:colOff>
       <xdr:row>187</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>74160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1728,7 +1728,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3115080" y="30596400"/>
+          <a:off x="3115080" y="30596760"/>
           <a:ext cx="9708120" cy="2138400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1820,13 +1820,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>306720</xdr:colOff>
       <xdr:row>203</xdr:row>
-      <xdr:rowOff>115200</xdr:rowOff>
+      <xdr:rowOff>115560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>123840</xdr:colOff>
       <xdr:row>215</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1839,7 +1839,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3156480" y="35580240"/>
+          <a:off x="3156480" y="35580600"/>
           <a:ext cx="9480960" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1857,13 +1857,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>275040</xdr:colOff>
       <xdr:row>216</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>38880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>629640</xdr:colOff>
       <xdr:row>227</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1876,7 +1876,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3124800" y="37782000"/>
+          <a:off x="3124800" y="37782360"/>
           <a:ext cx="9161280" cy="2044800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2973,7 +2973,7 @@
   <dimension ref="A1:X621"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E48" activeCellId="0" sqref="E48"/>
+      <selection pane="topLeft" activeCell="E48" activeCellId="1" sqref="AM69:AM96 E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3057,11 +3057,11 @@
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>718.46</v>
+        <v>748.28</v>
       </c>
       <c r="Q6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>208.05438</v>
+        <v>210.2638</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3076,11 +3076,11 @@
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>206.34</v>
+        <v>214.7</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>88.19253</v>
+        <v>89.32501</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3095,11 +3095,11 @@
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>293.42</v>
+        <v>295.13</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>88.95074</v>
+        <v>89.27404</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3122,11 +3122,11 @@
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1563.83</v>
+        <v>1608.31</v>
       </c>
       <c r="Q9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>402.22093</v>
+        <v>402.9341</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3145,11 +3145,11 @@
       <c r="O10" s="4"/>
       <c r="P10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>160.46</v>
+        <v>160.19</v>
       </c>
       <c r="Q10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>51.02656</v>
+        <v>51.34159</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3168,11 +3168,11 @@
       <c r="O11" s="4"/>
       <c r="P11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>141.90512</v>
+        <v>141.63361</v>
       </c>
       <c r="Q11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>141.90512</v>
+        <v>141.63361</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3191,11 +3191,11 @@
       <c r="O12" s="4"/>
       <c r="P12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>110.49</v>
+        <v>113.14</v>
       </c>
       <c r="Q12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>45.08509</v>
+        <v>45.53721</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3214,11 +3214,11 @@
       <c r="O13" s="4"/>
       <c r="P13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>589.26</v>
+        <v>610.03</v>
       </c>
       <c r="Q13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>160.43867</v>
+        <v>164.25094</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3241,11 +3241,11 @@
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>334.27</v>
+        <v>347.14</v>
       </c>
       <c r="Q14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>120.60729</v>
+        <v>122.76784</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3264,11 +3264,11 @@
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>416.12</v>
+        <v>426.34</v>
       </c>
       <c r="Q15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>140.40068</v>
+        <v>142.33849</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3290,11 +3290,11 @@
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>2766.77</v>
+        <v>2779.73</v>
       </c>
       <c r="Q16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>690.5803</v>
+        <v>706.54516</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3312,11 +3312,11 @@
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>339.13</v>
+        <v>252.51</v>
       </c>
       <c r="Q17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
-        <v>57.41775</v>
+        <v>57.20562</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3334,11 +3334,11 @@
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>940.81</v>
+        <v>694.36</v>
       </c>
       <c r="Q18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>198.75492</v>
+        <v>197.45861</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3360,11 +3360,11 @@
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>888.46</v>
+        <v>847.06</v>
       </c>
       <c r="Q19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>234.58123</v>
+        <v>248.03044</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3382,11 +3382,11 @@
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>134.32</v>
+        <v>138.82</v>
       </c>
       <c r="Q20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>56.79314</v>
+        <v>57.76155</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3404,11 +3404,11 @@
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>458.41</v>
+        <v>473.33</v>
       </c>
       <c r="Q21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>157.68583</v>
+        <v>161.27427</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3426,11 +3426,11 @@
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>412.82</v>
+        <v>428.78</v>
       </c>
       <c r="Q22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>135.29315</v>
+        <v>137.73073</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3448,11 +3448,11 @@
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>257.81</v>
+        <v>267.23</v>
       </c>
       <c r="Q23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>98.06408</v>
+        <v>103.11229</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3470,11 +3470,11 @@
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>280.82</v>
+        <v>289.86</v>
       </c>
       <c r="Q24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>90.14262</v>
+        <v>92.93745</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3493,11 +3493,11 @@
       <c r="O25" s="1"/>
       <c r="P25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>331.41</v>
+        <v>342.92</v>
       </c>
       <c r="Q25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>99.25307</v>
+        <v>102.59401</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3515,11 +3515,11 @@
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>814.98</v>
+        <v>839.5</v>
       </c>
       <c r="Q26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>251.39177</v>
+        <v>255.02598</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3537,11 +3537,11 @@
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>189.39</v>
+        <v>186.46</v>
       </c>
       <c r="Q27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>53.83953</v>
+        <v>58.78364</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3559,11 +3559,11 @@
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>428.23</v>
+        <v>438.13</v>
       </c>
       <c r="Q28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>128.0109</v>
+        <v>144.56536</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,11 +3585,11 @@
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1727.58</v>
+        <v>1780.01</v>
       </c>
       <c r="Q29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>479.03154</v>
+        <v>487.48703</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3607,11 +3607,11 @@
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>44.85</v>
+        <v>46.13</v>
       </c>
       <c r="Q30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>22.08076</v>
+        <v>22.11175</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3629,11 +3629,11 @@
       </c>
       <c r="P31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>32.61</v>
+        <v>33.2</v>
       </c>
       <c r="Q31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>25.16425</v>
+        <v>25.2621</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3651,11 +3651,11 @@
       </c>
       <c r="P32" s="11" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>167.46</v>
+        <v>170.28</v>
       </c>
       <c r="Q32" s="11" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>60.31915</v>
+        <v>61.16896</v>
       </c>
       <c r="R32" s="11"/>
     </row>
@@ -3830,11 +3830,11 @@
       </c>
       <c r="P49" s="0" t="n">
         <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
-        <v>16188.34</v>
+        <v>16169.85</v>
       </c>
       <c r="Q49" s="11" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D35:ND35&lt;&gt;""),Parallel_Timings!D35:ND35)</f>
-        <v>4536.31213</v>
+        <v>4631.61889</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="Q50" s="19" t="n">
         <f aca="false">P49/Q49</f>
-        <v>3.56861246229986</v>
+        <v>3.49118750571466</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4115,11 +4115,11 @@
   <dimension ref="A2:BK109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="AI17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AP42" activeCellId="0" sqref="AP42"/>
+      <selection pane="topRight" activeCell="AI1" activeCellId="0" sqref="AI1"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="AM96" activeCellId="0" sqref="AM69:AM96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4273,6 +4273,9 @@
       </c>
       <c r="AS4" s="27" t="n">
         <v>44430</v>
+      </c>
+      <c r="AT4" s="27" t="n">
+        <v>44437</v>
       </c>
     </row>
     <row r="5" s="30" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4356,6 +4359,9 @@
       <c r="AS5" s="0" t="n">
         <v>1117.64</v>
       </c>
+      <c r="AT5" s="0" t="n">
+        <v>1160.42</v>
+      </c>
     </row>
     <row r="6" s="12" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="36" t="s">
@@ -4489,6 +4495,9 @@
       <c r="AS6" s="0" t="n">
         <v>718.46</v>
       </c>
+      <c r="AT6" s="0" t="n">
+        <v>748.28</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
@@ -4623,6 +4632,9 @@
       <c r="AS7" s="0" t="n">
         <v>206.34</v>
       </c>
+      <c r="AT7" s="0" t="n">
+        <v>214.7</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="37" t="s">
@@ -4745,6 +4757,9 @@
       <c r="AS8" s="0" t="n">
         <v>293.42</v>
       </c>
+      <c r="AT8" s="0" t="n">
+        <v>295.13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
@@ -4879,6 +4894,9 @@
       <c r="AS9" s="0" t="n">
         <v>1563.83</v>
       </c>
+      <c r="AT9" s="0" t="n">
+        <v>1608.31</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
@@ -5013,6 +5031,9 @@
       <c r="AS10" s="0" t="n">
         <v>160.46</v>
       </c>
+      <c r="AT10" s="0" t="n">
+        <v>160.19</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
@@ -5147,6 +5168,9 @@
       <c r="AS11" s="0" t="n">
         <v>462.19</v>
       </c>
+      <c r="AT11" s="0" t="n">
+        <v>477.86</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
@@ -5254,6 +5278,9 @@
       <c r="AS12" s="0" t="n">
         <v>110.49</v>
       </c>
+      <c r="AT12" s="0" t="n">
+        <v>113.14</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="37" t="s">
@@ -5349,6 +5376,9 @@
       <c r="AS13" s="0" t="n">
         <v>589.26</v>
       </c>
+      <c r="AT13" s="0" t="n">
+        <v>610.03</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
@@ -5483,6 +5513,9 @@
       <c r="AS14" s="0" t="n">
         <v>334.27</v>
       </c>
+      <c r="AT14" s="0" t="n">
+        <v>347.14</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38" t="s">
@@ -5617,6 +5650,9 @@
       <c r="AS15" s="0" t="n">
         <v>416.12</v>
       </c>
+      <c r="AT15" s="0" t="n">
+        <v>426.34</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38" t="s">
@@ -5751,6 +5787,9 @@
       <c r="AS16" s="0" t="n">
         <v>2766.77</v>
       </c>
+      <c r="AT16" s="0" t="n">
+        <v>2779.73</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38" t="s">
@@ -5804,6 +5843,9 @@
       <c r="AS17" s="0" t="n">
         <v>339.13</v>
       </c>
+      <c r="AT17" s="0" t="n">
+        <v>252.51</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38" t="s">
@@ -5938,6 +5980,9 @@
       <c r="AS18" s="0" t="n">
         <v>940.81</v>
       </c>
+      <c r="AT18" s="0" t="n">
+        <v>694.36</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38" t="s">
@@ -6072,6 +6117,9 @@
       <c r="AS19" s="0" t="n">
         <v>888.46</v>
       </c>
+      <c r="AT19" s="0" t="n">
+        <v>847.06</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38" t="s">
@@ -6206,6 +6254,9 @@
       <c r="AS20" s="0" t="n">
         <v>134.32</v>
       </c>
+      <c r="AT20" s="0" t="n">
+        <v>138.82</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38" t="s">
@@ -6340,6 +6391,9 @@
       <c r="AS21" s="0" t="n">
         <v>458.41</v>
       </c>
+      <c r="AT21" s="0" t="n">
+        <v>473.33</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38" t="s">
@@ -6474,6 +6528,9 @@
       <c r="AS22" s="0" t="n">
         <v>412.82</v>
       </c>
+      <c r="AT22" s="0" t="n">
+        <v>428.78</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38" t="s">
@@ -6608,6 +6665,9 @@
       <c r="AS23" s="0" t="n">
         <v>257.81</v>
       </c>
+      <c r="AT23" s="0" t="n">
+        <v>267.23</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38" t="s">
@@ -6742,6 +6802,9 @@
       <c r="AS24" s="0" t="n">
         <v>280.82</v>
       </c>
+      <c r="AT24" s="0" t="n">
+        <v>289.86</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38" t="s">
@@ -6876,6 +6939,9 @@
       <c r="AS25" s="0" t="n">
         <v>331.41</v>
       </c>
+      <c r="AT25" s="0" t="n">
+        <v>342.92</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="39" t="s">
@@ -7010,6 +7076,9 @@
       <c r="AS26" s="0" t="n">
         <v>814.98</v>
       </c>
+      <c r="AT26" s="0" t="n">
+        <v>839.5</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="38" t="s">
@@ -7144,6 +7213,9 @@
       <c r="AS27" s="0" t="n">
         <v>189.39</v>
       </c>
+      <c r="AT27" s="0" t="n">
+        <v>186.46</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38" t="s">
@@ -7224,6 +7296,9 @@
       <c r="AS28" s="0" t="n">
         <v>428.23</v>
       </c>
+      <c r="AT28" s="0" t="n">
+        <v>438.13</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="38" t="s">
@@ -7358,6 +7433,9 @@
       <c r="AS29" s="0" t="n">
         <v>1727.58</v>
       </c>
+      <c r="AT29" s="0" t="n">
+        <v>1780.01</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38" t="s">
@@ -7492,6 +7570,9 @@
       <c r="AS30" s="0" t="n">
         <v>44.85</v>
       </c>
+      <c r="AT30" s="0" t="n">
+        <v>46.13</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="37" t="s">
@@ -7626,6 +7707,9 @@
       <c r="AS31" s="0" t="n">
         <v>32.61</v>
       </c>
+      <c r="AT31" s="0" t="n">
+        <v>33.2</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="37" t="s">
@@ -7760,6 +7844,9 @@
       <c r="AS32" s="0" t="n">
         <v>167.46</v>
       </c>
+      <c r="AT32" s="0" t="n">
+        <v>170.28</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="37" t="s">
@@ -7941,6 +8028,10 @@
       <c r="AS35" s="0" t="n">
         <f aca="false">SUM(AS$5:AS$32)</f>
         <v>16188.34</v>
+      </c>
+      <c r="AT35" s="0" t="n">
+        <f aca="false">SUM(AT$5:AT$32)</f>
+        <v>16169.85</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8116,8 +8207,12 @@
         <f aca="false">AS35/AR35</f>
         <v>0.988925223111335</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="19.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AT36" s="40" t="n">
+        <f aca="false">AT35/AS35</f>
+        <v>0.998857819887648</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>108</v>
       </c>
@@ -8149,9 +8244,6 @@
       </c>
       <c r="AL38" s="44"/>
       <c r="AR38" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="AS38" s="0" t="s">
         <v>116</v>
       </c>
     </row>
@@ -8470,14 +8562,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AS38"/>
+  <dimension ref="A2:AT38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="AH44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AH1" activeCellId="0" sqref="AH1"/>
-      <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
-      <selection pane="bottomRight" activeCell="AR39" activeCellId="0" sqref="AR39"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="bottomRight" activeCell="AT4" activeCellId="1" sqref="AM69:AM96 AT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8627,6 +8719,9 @@
       </c>
       <c r="AS4" s="47" t="n">
         <v>44430</v>
+      </c>
+      <c r="AT4" s="47" t="n">
+        <v>44437</v>
       </c>
     </row>
     <row r="5" s="50" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8708,6 +8803,9 @@
       <c r="AS5" s="0" t="n">
         <v>251.02615</v>
       </c>
+      <c r="AT5" s="0" t="n">
+        <v>252.89731</v>
+      </c>
     </row>
     <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -8840,6 +8938,9 @@
       <c r="AS6" s="0" t="n">
         <v>208.05438</v>
       </c>
+      <c r="AT6" s="0" t="n">
+        <v>210.2638</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
@@ -8971,6 +9072,9 @@
       <c r="AS7" s="0" t="n">
         <v>88.19253</v>
       </c>
+      <c r="AT7" s="0" t="n">
+        <v>89.32501</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
@@ -9090,6 +9194,9 @@
       <c r="AS8" s="0" t="n">
         <v>88.95074</v>
       </c>
+      <c r="AT8" s="0" t="n">
+        <v>89.27404</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="38" t="s">
@@ -9221,6 +9328,9 @@
       <c r="AS9" s="0" t="n">
         <v>402.22093</v>
       </c>
+      <c r="AT9" s="0" t="n">
+        <v>402.9341</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="37" t="s">
@@ -9352,6 +9462,9 @@
       <c r="AS10" s="0" t="n">
         <v>51.02656</v>
       </c>
+      <c r="AT10" s="0" t="n">
+        <v>51.34159</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
@@ -9483,6 +9596,9 @@
       <c r="AS11" s="0" t="n">
         <v>141.90512</v>
       </c>
+      <c r="AT11" s="0" t="n">
+        <v>141.63361</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="37" t="s">
@@ -9587,6 +9703,9 @@
       <c r="AS12" s="0" t="n">
         <v>45.08509</v>
       </c>
+      <c r="AT12" s="0" t="n">
+        <v>45.53721</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
@@ -9679,6 +9798,9 @@
       <c r="AS13" s="0" t="n">
         <v>160.43867</v>
       </c>
+      <c r="AT13" s="0" t="n">
+        <v>164.25094</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="38" t="s">
@@ -9810,6 +9932,9 @@
       <c r="AS14" s="0" t="n">
         <v>120.60729</v>
       </c>
+      <c r="AT14" s="0" t="n">
+        <v>122.76784</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="38" t="s">
@@ -9941,6 +10066,9 @@
       <c r="AS15" s="0" t="n">
         <v>140.40068</v>
       </c>
+      <c r="AT15" s="0" t="n">
+        <v>142.33849</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="38" t="s">
@@ -10072,6 +10200,9 @@
       <c r="AS16" s="0" t="n">
         <v>690.5803</v>
       </c>
+      <c r="AT16" s="0" t="n">
+        <v>706.54516</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="38" t="s">
@@ -10119,6 +10250,9 @@
       <c r="AS17" s="0" t="n">
         <v>57.41775</v>
       </c>
+      <c r="AT17" s="0" t="n">
+        <v>57.20562</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="38" t="s">
@@ -10250,6 +10384,9 @@
       <c r="AS18" s="0" t="n">
         <v>198.75492</v>
       </c>
+      <c r="AT18" s="0" t="n">
+        <v>197.45861</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="38" t="s">
@@ -10381,6 +10518,9 @@
       <c r="AS19" s="0" t="n">
         <v>234.58123</v>
       </c>
+      <c r="AT19" s="0" t="n">
+        <v>248.03044</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="38" t="s">
@@ -10512,6 +10652,9 @@
       <c r="AS20" s="0" t="n">
         <v>56.79314</v>
       </c>
+      <c r="AT20" s="0" t="n">
+        <v>57.76155</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="38" t="s">
@@ -10643,6 +10786,9 @@
       <c r="AS21" s="0" t="n">
         <v>157.68583</v>
       </c>
+      <c r="AT21" s="0" t="n">
+        <v>161.27427</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="38" t="s">
@@ -10774,6 +10920,9 @@
       <c r="AS22" s="0" t="n">
         <v>135.29315</v>
       </c>
+      <c r="AT22" s="0" t="n">
+        <v>137.73073</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="38" t="s">
@@ -10905,6 +11054,9 @@
       <c r="AS23" s="0" t="n">
         <v>98.06408</v>
       </c>
+      <c r="AT23" s="0" t="n">
+        <v>103.11229</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="38" t="s">
@@ -11036,6 +11188,9 @@
       <c r="AS24" s="0" t="n">
         <v>90.14262</v>
       </c>
+      <c r="AT24" s="0" t="n">
+        <v>92.93745</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="38" t="s">
@@ -11167,6 +11322,9 @@
       <c r="AS25" s="0" t="n">
         <v>99.25307</v>
       </c>
+      <c r="AT25" s="0" t="n">
+        <v>102.59401</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="39" t="s">
@@ -11298,6 +11456,9 @@
       <c r="AS26" s="0" t="n">
         <v>251.39177</v>
       </c>
+      <c r="AT26" s="0" t="n">
+        <v>255.02598</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="38" t="s">
@@ -11429,6 +11590,9 @@
       <c r="AS27" s="0" t="n">
         <v>53.83953</v>
       </c>
+      <c r="AT27" s="0" t="n">
+        <v>58.78364</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="38" t="s">
@@ -11506,6 +11670,9 @@
       <c r="AS28" s="0" t="n">
         <v>128.0109</v>
       </c>
+      <c r="AT28" s="0" t="n">
+        <v>144.56536</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="38" t="s">
@@ -11637,6 +11804,9 @@
       <c r="AS29" s="0" t="n">
         <v>479.03154</v>
       </c>
+      <c r="AT29" s="0" t="n">
+        <v>487.48703</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="38" t="s">
@@ -11768,6 +11938,9 @@
       <c r="AS30" s="0" t="n">
         <v>22.08076</v>
       </c>
+      <c r="AT30" s="0" t="n">
+        <v>22.11175</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="37" t="s">
@@ -11899,8 +12072,11 @@
       <c r="AS31" s="0" t="n">
         <v>25.16425</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AT31" s="0" t="n">
+        <v>25.2621</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
         <v>58</v>
       </c>
@@ -12029,6 +12205,9 @@
       </c>
       <c r="AS32" s="0" t="n">
         <v>60.31915</v>
+      </c>
+      <c r="AT32" s="0" t="n">
+        <v>61.16896</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12208,6 +12387,10 @@
         <f aca="false">SUM(AS$5:AS$32)</f>
         <v>4536.31213</v>
       </c>
+      <c r="AT35" s="0" t="n">
+        <f aca="false">SUM(AT$5:AT$32)</f>
+        <v>4631.61889</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
@@ -12380,6 +12563,10 @@
       <c r="AS36" s="51" t="n">
         <f aca="false">Regular_Timings!AS35/AS35</f>
         <v>3.56861246229986</v>
+      </c>
+      <c r="AT36" s="51" t="n">
+        <f aca="false">Regular_Timings!AT35/AT35</f>
+        <v>3.49118750571466</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12411,7 +12598,7 @@
   <dimension ref="A1:AJ97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="AM69:AM96 A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
- Updated milestone tracking files
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="172">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -64,229 +64,241 @@
     <t xml:space="preserve">GIO</t>
   </si>
   <si>
+    <t xml:space="preserve">JSON-GLib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSSDP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUPnP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pango</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GtkPlus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GtkBuilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SourceViewGTK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebkitGTK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMTK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEPL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GooCanvas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WNCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COGL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GtkClutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Champlain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GStreamer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSVG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CardDecks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICal-GLib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VisualGrammar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoreTemps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BABL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebService-EveOnline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be9afbd88567debe355828f21b40d87c52bfce22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(since May 2018)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parser-SQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0df477626c94dba789710095dbbc53dfc6e0a312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon-AWS-EC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As of June 3, 2019</t>
+  </si>
+  <si>
     <t xml:space="preserve">ICal:</t>
   </si>
   <si>
-    <t xml:space="preserve">JSON-GLib</t>
-  </si>
-  <si>
     <t xml:space="preserve">GLib:</t>
   </si>
   <si>
-    <t xml:space="preserve">SOUP</t>
-  </si>
-  <si>
     <t xml:space="preserve">GIR:</t>
   </si>
   <si>
-    <t xml:space="preserve">GSSDP</t>
-  </si>
-  <si>
     <t xml:space="preserve">ATK:</t>
   </si>
   <si>
-    <t xml:space="preserve">GUPnP</t>
-  </si>
-  <si>
     <t xml:space="preserve">GIO:</t>
   </si>
   <si>
-    <t xml:space="preserve">Pango</t>
+    <t xml:space="preserve">As of June 9, 2019 – LOL!</t>
   </si>
   <si>
     <t xml:space="preserve">JSON-GLib:</t>
   </si>
   <si>
-    <t xml:space="preserve">GDK</t>
-  </si>
-  <si>
     <t xml:space="preserve">SOUP:</t>
   </si>
   <si>
-    <t xml:space="preserve">GtkPlus</t>
-  </si>
-  <si>
     <t xml:space="preserve">GSSDP:</t>
   </si>
   <si>
-    <t xml:space="preserve">GtkBuilder</t>
-  </si>
-  <si>
     <t xml:space="preserve">GUPnP:</t>
   </si>
   <si>
-    <t xml:space="preserve">SourceViewGTK</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pango:</t>
   </si>
   <si>
-    <t xml:space="preserve">WebkitGTK</t>
-  </si>
-  <si>
     <t xml:space="preserve">GDK:</t>
   </si>
   <si>
-    <t xml:space="preserve">AMTK</t>
-  </si>
-  <si>
     <t xml:space="preserve">GtkPlus:</t>
   </si>
   <si>
-    <t xml:space="preserve">TEPL</t>
-  </si>
-  <si>
     <t xml:space="preserve">GtkBuilder:</t>
   </si>
   <si>
-    <t xml:space="preserve">GooCanvas</t>
-  </si>
-  <si>
     <t xml:space="preserve">SourceViewGTK:</t>
   </si>
   <si>
-    <t xml:space="preserve">Slope</t>
-  </si>
-  <si>
     <t xml:space="preserve">WebkitGTK:</t>
   </si>
   <si>
-    <t xml:space="preserve">WNCK</t>
-  </si>
-  <si>
     <t xml:space="preserve">AMTK:</t>
   </si>
   <si>
-    <t xml:space="preserve">COGL</t>
-  </si>
-  <si>
     <t xml:space="preserve">TEPL:</t>
   </si>
   <si>
-    <t xml:space="preserve">Clutter</t>
-  </si>
-  <si>
     <t xml:space="preserve">GooCanvas:</t>
   </si>
   <si>
-    <t xml:space="preserve">GtkClutter</t>
+    <t xml:space="preserve">As of July 11, 2019!</t>
   </si>
   <si>
     <t xml:space="preserve">Slope:</t>
   </si>
   <si>
-    <t xml:space="preserve">Champlain</t>
-  </si>
-  <si>
     <t xml:space="preserve">WNCK:</t>
   </si>
   <si>
-    <t xml:space="preserve">GStreamer</t>
-  </si>
-  <si>
     <t xml:space="preserve">COGL:</t>
   </si>
   <si>
-    <t xml:space="preserve">RSVG</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clutter:</t>
   </si>
   <si>
-    <t xml:space="preserve">CardDecks</t>
-  </si>
-  <si>
     <t xml:space="preserve">GtkClutter:</t>
   </si>
   <si>
-    <t xml:space="preserve">VTE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Champlain:</t>
   </si>
   <si>
-    <t xml:space="preserve">ICal-GLib</t>
-  </si>
-  <si>
     <t xml:space="preserve">GStreamer:</t>
   </si>
   <si>
-    <t xml:space="preserve">EDS</t>
-  </si>
-  <si>
     <t xml:space="preserve">RSVG:</t>
   </si>
   <si>
-    <t xml:space="preserve">X11</t>
-  </si>
-  <si>
     <t xml:space="preserve">CardDeck:</t>
   </si>
   <si>
-    <t xml:space="preserve">Sheet</t>
-  </si>
-  <si>
     <t xml:space="preserve">VTE:</t>
   </si>
   <si>
-    <t xml:space="preserve">VisualGrammar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CoreTemps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BABL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WebService-EveOnline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">be9afbd88567debe355828f21b40d87c52bfce22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(since May 2018)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parser-SQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0df477626c94dba789710095dbbc53dfc6e0a312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon-AWS-EC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenVR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Totals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Projects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parallel x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Properly</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As of June 3, 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As of June 9, 2019 – LOL!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As of July 11, 2019!</t>
+    <t xml:space="preserve">GOA:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secret:</t>
   </si>
   <si>
     <t xml:space="preserve">As of August 10, 2019!</t>
@@ -1048,15 +1060,15 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right/>
-      <top style="hair"/>
+      <right style="hair"/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="hair"/>
-      <top/>
+      <right/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1137,7 +1149,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1166,10 +1178,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1178,11 +1186,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1190,11 +1198,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1211,6 +1215,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1286,15 +1294,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1334,7 +1350,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1352,6 +1368,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1449,13 +1469,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>738360</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>32760</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>186480</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1469,7 +1489,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="738360" y="9559440"/>
+          <a:off x="738360" y="10476000"/>
           <a:ext cx="9703800" cy="2053800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1485,15 +1505,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23400</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:colOff>24120</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>64440</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>43200</xdr:rowOff>
+      <xdr:colOff>65160</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1506,7 +1526,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2234160" y="12009600"/>
+          <a:off x="2234880" y="12926520"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1522,14 +1542,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23400</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:colOff>24120</xdr:colOff>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>15480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>29880</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:colOff>30600</xdr:colOff>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1543,7 +1563,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2234160" y="14624640"/>
+          <a:off x="2234880" y="15541200"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1559,15 +1579,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23400</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>32760</xdr:rowOff>
+      <xdr:colOff>24120</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>634320</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:colOff>635040</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1580,7 +1600,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2234160" y="16920360"/>
+          <a:off x="2234880" y="17836920"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1596,15 +1616,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23040</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>32760</xdr:rowOff>
+      <xdr:colOff>23760</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>587520</xdr:colOff>
-      <xdr:row>128</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:colOff>588240</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1617,7 +1637,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2233800" y="20075040"/>
+          <a:off x="2234520" y="20991600"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1633,15 +1653,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>52560</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:colOff>53280</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>612360</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:colOff>613080</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1654,7 +1674,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2263320" y="22854600"/>
+          <a:off x="2264040" y="23771520"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1670,15 +1690,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>20520</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>32760</xdr:rowOff>
+      <xdr:colOff>21240</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>257760</xdr:colOff>
-      <xdr:row>157</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:colOff>258480</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1691,7 +1711,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2231280" y="25332840"/>
+          <a:off x="2232000" y="26249400"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1708,14 +1728,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
-      <xdr:row>175</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>309600</xdr:colOff>
-      <xdr:row>187</xdr:row>
-      <xdr:rowOff>74160</xdr:rowOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1728,7 +1748,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3115080" y="30596760"/>
+          <a:off x="3115080" y="31513320"/>
           <a:ext cx="9708120" cy="2138400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1745,14 +1765,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>360360</xdr:colOff>
-      <xdr:row>160</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>271800</xdr:colOff>
-      <xdr:row>171</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1765,7 +1785,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3210120" y="27941760"/>
+          <a:off x="3210120" y="28858320"/>
           <a:ext cx="8718120" cy="1964880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1782,14 +1802,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>209880</xdr:colOff>
-      <xdr:row>189</xdr:row>
-      <xdr:rowOff>168840</xdr:rowOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>169560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>333720</xdr:colOff>
-      <xdr:row>202</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1802,7 +1822,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3059640" y="33180480"/>
+          <a:off x="3059640" y="34097400"/>
           <a:ext cx="9787680" cy="2191320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1819,14 +1839,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>306720</xdr:colOff>
-      <xdr:row>203</xdr:row>
-      <xdr:rowOff>115560</xdr:rowOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>123840</xdr:colOff>
-      <xdr:row>215</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1839,7 +1859,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3156480" y="35580600"/>
+          <a:off x="3156480" y="36497520"/>
           <a:ext cx="9480960" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1856,13 +1876,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>275040</xdr:colOff>
-      <xdr:row>216</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>38880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>629640</xdr:colOff>
-      <xdr:row>227</xdr:row>
+      <xdr:row>232</xdr:row>
       <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1876,7 +1896,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3124800" y="37782360"/>
+          <a:off x="3124800" y="38698920"/>
           <a:ext cx="9161280" cy="2044800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1893,14 +1913,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>382680</xdr:colOff>
-      <xdr:row>229</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:row>228</xdr:row>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>579960</xdr:colOff>
       <xdr:row>241</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1930,14 +1950,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>400680</xdr:colOff>
-      <xdr:row>243</xdr:row>
-      <xdr:rowOff>2520</xdr:rowOff>
+      <xdr:row>242</xdr:row>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>573840</xdr:colOff>
       <xdr:row>254</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1967,14 +1987,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>373320</xdr:colOff>
-      <xdr:row>256</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:row>255</xdr:row>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>533160</xdr:colOff>
-      <xdr:row>268</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2004,14 +2024,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>346320</xdr:colOff>
-      <xdr:row>269</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>563040</xdr:colOff>
-      <xdr:row>281</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:row>280</xdr:row>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2041,14 +2061,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>602280</xdr:colOff>
-      <xdr:row>283</xdr:row>
-      <xdr:rowOff>4680</xdr:rowOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>552600</xdr:colOff>
       <xdr:row>294</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2078,14 +2098,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>553680</xdr:colOff>
-      <xdr:row>296</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:row>295</xdr:row>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>541800</xdr:colOff>
       <xdr:row>306</xdr:row>
-      <xdr:rowOff>148320</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2116,13 +2136,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>428400</xdr:colOff>
       <xdr:row>307</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>548280</xdr:colOff>
       <xdr:row>319</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>116280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2152,14 +2172,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>550440</xdr:colOff>
-      <xdr:row>320</xdr:row>
-      <xdr:rowOff>13680</xdr:rowOff>
+      <xdr:row>319</xdr:row>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>567360</xdr:colOff>
-      <xdr:row>332</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:row>331</xdr:row>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2190,13 +2210,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>495000</xdr:colOff>
       <xdr:row>332</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>134640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>540360</xdr:colOff>
       <xdr:row>344</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2226,14 +2246,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>471960</xdr:colOff>
-      <xdr:row>346</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:row>345</xdr:row>
+      <xdr:rowOff>140760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>555480</xdr:colOff>
       <xdr:row>358</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2264,13 +2284,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>480240</xdr:colOff>
       <xdr:row>360</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>563760</xdr:colOff>
       <xdr:row>373</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2300,14 +2320,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>311040</xdr:colOff>
-      <xdr:row>375</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:row>374</xdr:row>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>537480</xdr:colOff>
       <xdr:row>386</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2337,14 +2357,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>465840</xdr:colOff>
-      <xdr:row>389</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:row>388</xdr:row>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>549360</xdr:colOff>
-      <xdr:row>401</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:row>400</xdr:row>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2374,14 +2394,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>509040</xdr:colOff>
-      <xdr:row>402</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:row>401</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>551520</xdr:colOff>
       <xdr:row>413</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2412,13 +2432,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>495000</xdr:colOff>
       <xdr:row>415</xdr:row>
-      <xdr:rowOff>172800</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>569160</xdr:colOff>
       <xdr:row>427</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>57240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2449,13 +2469,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>517680</xdr:colOff>
       <xdr:row>428</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>568080</xdr:colOff>
       <xdr:row>440</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2485,14 +2505,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>368640</xdr:colOff>
-      <xdr:row>441</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:row>440</xdr:row>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>556920</xdr:colOff>
       <xdr:row>452</xdr:row>
-      <xdr:rowOff>125280</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2522,14 +2542,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>362880</xdr:colOff>
-      <xdr:row>456</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:row>455</xdr:row>
+      <xdr:rowOff>166320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>553320</xdr:colOff>
       <xdr:row>467</xdr:row>
-      <xdr:rowOff>127800</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2559,14 +2579,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>313200</xdr:colOff>
-      <xdr:row>468</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:row>467</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>582840</xdr:colOff>
       <xdr:row>479</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2596,14 +2616,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>178920</xdr:colOff>
-      <xdr:row>481</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:row>480</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>555120</xdr:colOff>
       <xdr:row>493</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2634,13 +2654,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>123840</xdr:colOff>
       <xdr:row>494</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>536400</xdr:colOff>
-      <xdr:row>507</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:row>506</xdr:row>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2670,14 +2690,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>143640</xdr:colOff>
-      <xdr:row>508</xdr:row>
-      <xdr:rowOff>26280</xdr:rowOff>
+      <xdr:row>507</xdr:row>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>550800</xdr:colOff>
       <xdr:row>520</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2708,13 +2728,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>55080</xdr:colOff>
       <xdr:row>523</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>541800</xdr:colOff>
       <xdr:row>537</xdr:row>
-      <xdr:rowOff>126000</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2744,14 +2764,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>5760</xdr:colOff>
-      <xdr:row>538</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:row>537</xdr:row>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>532440</xdr:colOff>
       <xdr:row>551</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>68040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2782,13 +2802,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>552</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>533160</xdr:colOff>
       <xdr:row>566</xdr:row>
-      <xdr:rowOff>54360</xdr:rowOff>
+      <xdr:rowOff>14400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2819,13 +2839,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1308600</xdr:colOff>
       <xdr:row>566</xdr:row>
-      <xdr:rowOff>163800</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>516960</xdr:colOff>
-      <xdr:row>581</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:row>580</xdr:row>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2855,14 +2875,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>8280</xdr:colOff>
-      <xdr:row>585</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:row>584</xdr:row>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>551520</xdr:colOff>
       <xdr:row>598</xdr:row>
-      <xdr:rowOff>161640</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2892,14 +2912,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>601</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:row>600</xdr:row>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>612720</xdr:colOff>
-      <xdr:row>616</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:row>615</xdr:row>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2930,13 +2950,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1337040</xdr:colOff>
       <xdr:row>617</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>545400</xdr:colOff>
       <xdr:row>631</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2970,10 +2990,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X621"/>
+  <dimension ref="A1:X626"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E48" activeCellId="1" sqref="AM69:AM96 E48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3037,7 +3057,7 @@
       <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="0" t="n">
         <v>21021</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -3049,8 +3069,8 @@
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7" t="n">
-        <v>35374</v>
+      <c r="C6" s="0" t="n">
+        <v>35637</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>151</v>
@@ -3068,7 +3088,7 @@
       <c r="B7" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="0" t="n">
         <v>4649</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -3087,7 +3107,7 @@
       <c r="B8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="0" t="n">
         <v>6344</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -3107,8 +3127,8 @@
       <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5" t="n">
-        <v>56809</v>
+      <c r="C9" s="0" t="n">
+        <v>56910</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>285</v>
@@ -3117,9 +3137,6 @@
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!AB:AB)), Miletone_Tracking!AB:AB)</f>
         <v>Crossed 50,000 lines on 10/04/2020</v>
       </c>
-      <c r="K9" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
         <v>1608.31</v>
@@ -3131,16 +3148,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <v>5602</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>19</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>15</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="0" t="n">
@@ -3154,16 +3168,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <v>13418</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>65</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="0" t="n">
@@ -3177,16 +3188,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="n">
         <v>1821</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>11</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="0" t="n">
@@ -3200,16 +3208,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="7" t="n">
+        <v>16</v>
+      </c>
+      <c r="C13" s="0" t="n">
         <v>12474</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>80</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>21</v>
       </c>
       <c r="O13" s="4"/>
       <c r="P13" s="0" t="n">
@@ -3224,9 +3229,9 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="C14" s="0" t="n">
         <v>8998</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -3236,9 +3241,6 @@
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!M:M)), Miletone_Tracking!M:M)</f>
         <v>Crossed 10,000 on 12/02/2019</v>
       </c>
-      <c r="K14" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
         <v>347.14</v>
@@ -3251,16 +3253,13 @@
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
       <c r="B15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="C15" s="0" t="n">
         <v>15698</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>63</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
@@ -3273,10 +3272,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="7" t="n">
-        <v>89388</v>
+        <v>19</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>89658</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>395</v>
@@ -3285,9 +3284,6 @@
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!E:E)), Miletone_Tracking!E:E)</f>
         <v>Split to 85,550 on 01/04/20</v>
       </c>
-      <c r="K16" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
         <v>2779.73</v>
@@ -3299,16 +3295,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="C17" s="0" t="n">
         <v>2490</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>35</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
@@ -3321,16 +3314,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="C18" s="0" t="n">
         <v>11666</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>82</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
@@ -3343,9 +3333,9 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="C19" s="0" t="n">
         <v>15279</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -3355,9 +3345,6 @@
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!Q:Q)), Miletone_Tracking!Q:Q)</f>
         <v>Crossed 15,000 on 01/24/20</v>
       </c>
-      <c r="K19" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
         <v>847.06</v>
@@ -3369,16 +3356,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="5" t="n">
-        <v>2242</v>
+        <v>23</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2244</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>7</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
@@ -3391,16 +3375,13 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="5" t="n">
-        <v>4002</v>
+        <v>24</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4004</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>39</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>37</v>
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
@@ -3413,16 +3394,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="C22" s="0" t="n">
         <v>11420</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>53</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
@@ -3435,16 +3413,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="C23" s="0" t="n">
         <v>2936</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>27</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
@@ -3457,16 +3432,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>4261</v>
+        <v>27</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>4357</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>24</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
@@ -3479,16 +3451,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="C25" s="0" t="n">
         <v>11312</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>61</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="0" t="n">
@@ -3501,17 +3470,14 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="5" t="n">
+      <c r="B26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="0" t="n">
         <v>28579</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>126</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>47</v>
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
@@ -3524,16 +3490,13 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C27" s="0" t="n">
         <v>1404</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>10</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
@@ -3545,17 +3508,14 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="5" t="n">
+      <c r="B28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="0" t="n">
         <v>9645</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>52</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
@@ -3568,9 +3528,9 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="C29" s="0" t="n">
         <v>66230</v>
       </c>
       <c r="D29" s="0" t="n">
@@ -3580,9 +3540,6 @@
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!T:T)), Miletone_Tracking!T:T)</f>
         <v>Crossed 50,000 lines on 05/08/20</v>
       </c>
-      <c r="K29" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
         <v>1780.01</v>
@@ -3594,16 +3551,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="C30" s="0" t="n">
         <v>1044</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>3</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
@@ -3616,16 +3570,13 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="C31" s="0" t="n">
         <v>207</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>5</v>
-      </c>
-      <c r="K31" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="P31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
@@ -3636,46 +3587,40 @@
         <v>25.2621</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="5" t="n">
+    <row r="32" s="9" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="9" t="n">
         <v>3625</v>
       </c>
-      <c r="D32" s="10" t="n">
+      <c r="D32" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="K32" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="P32" s="11" t="n">
+      <c r="P32" s="10" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
         <v>170.28</v>
       </c>
-      <c r="Q32" s="11" t="n">
+      <c r="Q32" s="10" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
         <v>61.16896</v>
       </c>
-      <c r="R32" s="11"/>
+      <c r="R32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C33" s="5" t="n">
         <v>18796</v>
       </c>
-      <c r="K33" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="12"/>
-      <c r="R33" s="12"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
     </row>
     <row r="34" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5" t="n">
         <v>39684</v>
@@ -3684,14 +3629,11 @@
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!AF:AF)), Miletone_Tracking!AF:AF)</f>
         <v>Crossed 20,000 lines on 04/21/21</v>
       </c>
-      <c r="K34" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="O34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C35" s="5" t="n">
         <v>19623</v>
@@ -3700,23 +3642,17 @@
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!AJ:AJ)), Miletone_Tracking!AJ:AJ )</f>
         <v>Crossed 10,000 lines on 07/12/21</v>
       </c>
-      <c r="K35" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="O35" s="4"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-    </row>
-    <row r="36" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="14" t="n">
-        <v>5260</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>67</v>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+    </row>
+    <row r="36" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>5582</v>
       </c>
       <c r="L36" s="0"/>
       <c r="P36" s="0"/>
@@ -3727,371 +3663,541 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="12" t="n">
+        <v>5260</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="5" t="n">
         <v>878</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="5" t="n">
-        <v>190</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C40" s="5" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="5" t="n">
         <v>22184</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" s="5" t="n">
+    <row r="43" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="5" t="n">
         <v>825</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="0" t="n">
+    <row r="44" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="14.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="0" t="n">
         <f aca="false">4650-865</f>
         <v>3785</v>
       </c>
-      <c r="J44" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="0" t="n">
+      <c r="J49" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="0" t="n">
         <f aca="false">10319-580</f>
         <v>9739</v>
       </c>
-      <c r="J45" s="17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="0" t="n">
+      <c r="J50" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="0" t="n">
         <v>23768</v>
       </c>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" s="0" t="n">
+      <c r="F51" s="16"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="0" t="n">
         <v>3357</v>
       </c>
-      <c r="F47" s="18"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C49" s="5" t="n">
-        <f aca="false">SUM(C4:C47)</f>
-        <v>603392</v>
-      </c>
-      <c r="D49" s="0" t="n">
+      <c r="F52" s="16"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="5" t="n">
+        <f aca="false">SUM(C4:C52)</f>
+        <v>611312</v>
+      </c>
+      <c r="D54" s="0" t="n">
         <f aca="false">SUM(D5:D32)</f>
         <v>2410</v>
       </c>
-      <c r="F49" s="0" t="str">
+      <c r="F54" s="0" t="str">
         <f aca="false">LOOKUP(2, 1/(1-ISBLANK(Miletone_Tracking!A:A)), Miletone_Tracking!A:A)</f>
         <v>Crossed 600,000 on 7/19/21</v>
       </c>
-      <c r="O49" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="P49" s="0" t="n">
+      <c r="O54" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="P54" s="0" t="n">
         <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
         <v>16169.85</v>
       </c>
-      <c r="Q49" s="11" t="n">
+      <c r="Q54" s="17" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D35:ND35&lt;&gt;""),Parallel_Timings!D35:ND35)</f>
         <v>4631.61889</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="5" t="s">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="O55" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q55" s="18" t="n">
+        <f aca="false">P54/Q54</f>
+        <v>3.49118750571466</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q58" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S62" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R65" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R66" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R67" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R68" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R69" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="R70" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R71" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R72" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R73" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R74" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R75" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R76" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R77" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R78" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R79" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R80" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R81" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R82" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C83" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="R83" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R84" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="5" t="n">
-        <v>32</v>
-      </c>
-      <c r="O50" s="0" t="s">
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R85" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="Q50" s="19" t="n">
-        <f aca="false">P49/Q49</f>
-        <v>3.49118750571466</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R86" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="Q53" s="0" t="s">
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R87" s="0" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S57" s="0" t="s">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R88" s="0" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="0" t="s">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R89" s="0" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="0" t="s">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R90" s="0" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="0" t="s">
+      <c r="R91" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="0" t="s">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R92" s="0" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="0" t="s">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R93" s="0" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T147" s="20" t="n">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R94" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C96" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C112" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C127" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T152" s="19" t="n">
         <v>43729</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C159" s="0" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T163" s="20" t="n">
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C164" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T168" s="19" t="n">
         <v>43780</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C174" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T176" s="20" t="n">
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C179" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T181" s="19" t="n">
         <v>43765</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T191" s="20" t="n">
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T196" s="19" t="n">
         <v>43799</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T205" s="20" t="n">
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T210" s="19" t="n">
         <v>43814</v>
       </c>
     </row>
-    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T217" s="20" t="n">
+    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T222" s="19" t="n">
         <v>43827</v>
       </c>
     </row>
-    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T232" s="20" t="n">
+    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T237" s="19" t="n">
         <v>43930</v>
       </c>
     </row>
-    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T246" s="20" t="n">
+    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T251" s="19" t="n">
         <v>43939</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T259" s="20" t="n">
+    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T264" s="19" t="n">
         <v>43955</v>
       </c>
     </row>
-    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T267" s="20"/>
-    </row>
-    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T268" s="20"/>
-    </row>
-    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T269" s="20"/>
-    </row>
-    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T270" s="20"/>
-    </row>
-    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T271" s="20"/>
-    </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T272" s="20" t="n">
+      <c r="T272" s="19"/>
+    </row>
+    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T273" s="19"/>
+    </row>
+    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T274" s="19"/>
+    </row>
+    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T275" s="19"/>
+    </row>
+    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T276" s="19"/>
+    </row>
+    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T277" s="19" t="n">
         <v>43968</v>
       </c>
     </row>
-    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T286" s="20" t="n">
+    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T291" s="19" t="n">
         <v>44025</v>
       </c>
     </row>
-    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T299" s="20" t="n">
+    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T304" s="19" t="n">
         <v>44031</v>
       </c>
     </row>
-    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T311" s="20" t="n">
+    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T316" s="19" t="n">
         <v>44050</v>
       </c>
     </row>
-    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T325" s="20" t="n">
+    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T330" s="19" t="n">
         <v>44053</v>
       </c>
     </row>
-    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T338" s="20" t="n">
+    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T343" s="19" t="n">
         <v>44072</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T351" s="20" t="n">
+    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T356" s="19" t="n">
         <v>44094</v>
       </c>
     </row>
-    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T366" s="20" t="n">
+    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T371" s="19" t="n">
         <v>44101</v>
       </c>
     </row>
-    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T380" s="20" t="n">
+    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T385" s="19" t="n">
         <v>44125</v>
       </c>
     </row>
-    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T394" s="20" t="n">
+    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T399" s="19" t="n">
         <v>44130</v>
       </c>
     </row>
-    <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T407" s="20" t="n">
+    <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T412" s="19" t="n">
         <v>44136</v>
       </c>
     </row>
-    <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T421" s="20" t="n">
+    <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T426" s="19" t="n">
         <v>44157</v>
       </c>
     </row>
-    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T434" s="20" t="n">
+    <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T439" s="19" t="n">
         <v>44164</v>
       </c>
     </row>
-    <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T446" s="20" t="n">
+    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T451" s="19" t="n">
         <v>44171</v>
       </c>
     </row>
-    <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T461" s="20" t="n">
+    <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T466" s="19" t="n">
         <v>44199</v>
       </c>
     </row>
-    <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T473" s="20" t="n">
+    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T478" s="19" t="n">
         <v>44218</v>
       </c>
     </row>
-    <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T486" s="20" t="n">
+    <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T491" s="19" t="n">
         <v>44220</v>
       </c>
     </row>
-    <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T500" s="20" t="n">
+    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T505" s="19" t="n">
         <v>44241</v>
       </c>
     </row>
-    <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T513" s="20" t="n">
+    <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T518" s="19" t="n">
         <v>44241</v>
       </c>
     </row>
-    <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T529" s="20" t="n">
+    <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T534" s="19" t="n">
         <v>44284</v>
       </c>
     </row>
-    <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K542" s="0" t="n">
+    <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K547" s="0" t="n">
         <v>44</v>
       </c>
     </row>
-    <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T543" s="20" t="n">
+    <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T548" s="19" t="n">
         <v>44290</v>
       </c>
     </row>
-    <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T558" s="20" t="n">
+    <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T563" s="19" t="n">
         <v>44318</v>
       </c>
     </row>
-    <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T572" s="20" t="n">
+    <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T577" s="19" t="n">
         <v>44325</v>
       </c>
     </row>
-    <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T589" s="20" t="n">
+    <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T594" s="19" t="n">
         <v>44367</v>
       </c>
     </row>
-    <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T605" s="20" t="n">
+    <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T610" s="19" t="n">
         <v>44370</v>
       </c>
     </row>
-    <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T621" s="20" t="n">
+    <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T626" s="19" t="n">
         <v>44395</v>
       </c>
     </row>
@@ -4114,12 +4220,12 @@
   </sheetPr>
   <dimension ref="A2:BK109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="AI17" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AI1" activeCellId="0" sqref="AI1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="AM96" activeCellId="0" sqref="AM69:AM96"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AM96" activeCellId="0" sqref="AM96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4141,173 +4247,173 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" s="21" customFormat="true" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="22" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" s="20" customFormat="true" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C4" s="21" t="n">
         <v>44136</v>
       </c>
-      <c r="D4" s="22" t="n">
+      <c r="D4" s="21" t="n">
         <v>44143</v>
       </c>
-      <c r="E4" s="23" t="n">
+      <c r="E4" s="22" t="n">
         <v>44151</v>
       </c>
-      <c r="F4" s="23" t="n">
+      <c r="F4" s="22" t="n">
         <v>44157</v>
       </c>
-      <c r="G4" s="22" t="n">
+      <c r="G4" s="21" t="n">
         <v>44164</v>
       </c>
-      <c r="H4" s="23" t="n">
+      <c r="H4" s="22" t="n">
         <v>44171</v>
       </c>
-      <c r="I4" s="23" t="n">
+      <c r="I4" s="22" t="n">
         <v>44178</v>
       </c>
-      <c r="J4" s="23" t="n">
+      <c r="J4" s="22" t="n">
         <v>44185</v>
       </c>
-      <c r="K4" s="23" t="n">
+      <c r="K4" s="22" t="n">
         <v>44192</v>
       </c>
-      <c r="L4" s="23" t="n">
+      <c r="L4" s="22" t="n">
         <v>43833</v>
       </c>
-      <c r="M4" s="23" t="n">
+      <c r="M4" s="22" t="n">
         <v>44206</v>
       </c>
-      <c r="N4" s="23" t="n">
+      <c r="N4" s="22" t="n">
         <v>44213</v>
       </c>
-      <c r="O4" s="23" t="n">
+      <c r="O4" s="22" t="n">
         <v>44220</v>
       </c>
-      <c r="P4" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q4" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="R4" s="23" t="n">
+      <c r="P4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="R4" s="22" t="n">
         <v>44241</v>
       </c>
-      <c r="S4" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="T4" s="23" t="n">
+      <c r="S4" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="T4" s="22" t="n">
         <v>44255</v>
       </c>
-      <c r="U4" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="W4" s="25" t="n">
+      <c r="U4" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="V4" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="W4" s="24" t="n">
         <v>44276</v>
       </c>
-      <c r="X4" s="25" t="n">
+      <c r="X4" s="24" t="n">
         <v>44283</v>
       </c>
-      <c r="Y4" s="25" t="n">
+      <c r="Y4" s="24" t="n">
         <v>44290</v>
       </c>
-      <c r="Z4" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA4" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB4" s="23" t="n">
+      <c r="Z4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA4" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB4" s="22" t="n">
         <v>44311</v>
       </c>
-      <c r="AC4" s="23" t="n">
+      <c r="AC4" s="22" t="n">
         <v>44318</v>
       </c>
-      <c r="AD4" s="23" t="n">
+      <c r="AD4" s="22" t="n">
         <v>44325</v>
       </c>
-      <c r="AE4" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="AF4" s="23" t="n">
+      <c r="AE4" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF4" s="22" t="n">
         <v>44339</v>
       </c>
-      <c r="AG4" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH4" s="23" t="n">
+      <c r="AG4" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH4" s="22" t="n">
         <v>44353</v>
       </c>
-      <c r="AI4" s="23" t="n">
+      <c r="AI4" s="22" t="n">
         <v>44360</v>
       </c>
-      <c r="AJ4" s="23" t="n">
+      <c r="AJ4" s="22" t="n">
         <v>44367</v>
       </c>
-      <c r="AK4" s="23" t="n">
+      <c r="AK4" s="22" t="n">
         <v>44374</v>
       </c>
-      <c r="AL4" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="AM4" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="AN4" s="23" t="n">
+      <c r="AL4" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM4" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN4" s="22" t="n">
         <v>44395</v>
       </c>
-      <c r="AO4" s="27" t="n">
+      <c r="AO4" s="26" t="n">
         <v>44402</v>
       </c>
-      <c r="AP4" s="27" t="n">
+      <c r="AP4" s="26" t="n">
         <v>44409</v>
       </c>
-      <c r="AQ4" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="AR4" s="27" t="n">
+      <c r="AQ4" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="AR4" s="26" t="n">
         <v>44423</v>
       </c>
-      <c r="AS4" s="27" t="n">
+      <c r="AS4" s="26" t="n">
         <v>44430</v>
       </c>
-      <c r="AT4" s="27" t="n">
+      <c r="AT4" s="26" t="n">
         <v>44437</v>
       </c>
     </row>
-    <row r="5" s="30" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29" t="s">
+    <row r="5" s="29" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="33"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="32"/>
       <c r="AC5" s="0" t="n">
         <v>636.13</v>
       </c>
@@ -4363,15 +4469,15 @@
         <v>1160.42</v>
       </c>
     </row>
-    <row r="6" s="12" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
+    <row r="6" s="11" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="35" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="0" t="n">
         <v>509.17</v>
       </c>
-      <c r="D6" s="12" t="n">
+      <c r="D6" s="11" t="n">
         <v>561.22</v>
       </c>
       <c r="E6" s="0"/>
@@ -4423,7 +4529,7 @@
       <c r="U6" s="0" t="n">
         <v>682.7</v>
       </c>
-      <c r="V6" s="7" t="n">
+      <c r="V6" s="36" t="n">
         <v>730.42</v>
       </c>
       <c r="W6" s="0" t="n">
@@ -4900,7 +5006,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>109.49</v>
@@ -5037,7 +5143,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>329.82</v>
@@ -5174,7 +5280,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>87.98</v>
@@ -5284,7 +5390,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="37" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>511.4</v>
@@ -5382,7 +5488,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>248.23</v>
@@ -5519,7 +5625,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>309.51</v>
@@ -5656,7 +5762,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2194.98</v>
@@ -5793,7 +5899,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="AD17" s="0" t="n">
         <v>218.85</v>
@@ -5849,7 +5955,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>508.87</v>
@@ -5986,7 +6092,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>621.42</v>
@@ -6123,7 +6229,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>96.76</v>
@@ -6260,7 +6366,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>369.58</v>
@@ -6397,7 +6503,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>301.53</v>
@@ -6474,7 +6580,7 @@
       <c r="AA22" s="0" t="n">
         <v>407.53</v>
       </c>
-      <c r="AB22" s="10" t="n">
+      <c r="AB22" s="39" t="n">
         <v>375.94</v>
       </c>
       <c r="AC22" s="0" t="n">
@@ -6534,7 +6640,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>190.42</v>
@@ -6671,7 +6777,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>209.15</v>
@@ -6808,7 +6914,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>242.4</v>
@@ -6944,8 +7050,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="39" t="s">
-        <v>46</v>
+      <c r="A26" s="40" t="s">
+        <v>29</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>597.06</v>
@@ -7082,7 +7188,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="38" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>124.46</v>
@@ -7168,7 +7274,7 @@
       <c r="AD27" s="0" t="n">
         <v>167.39</v>
       </c>
-      <c r="AE27" s="7" t="n">
+      <c r="AE27" s="36" t="n">
         <v>168.41</v>
       </c>
       <c r="AF27" s="0" t="n">
@@ -7219,7 +7325,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="U28" s="0" t="n">
         <v>430.65</v>
@@ -7302,7 +7408,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="38" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>1348.93</v>
@@ -7439,7 +7545,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>30.85</v>
@@ -7576,7 +7682,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="37" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>22.21</v>
@@ -7713,7 +7819,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="37" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>117.34</v>
@@ -7850,12 +7956,12 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="37" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -8034,217 +8140,217 @@
         <v>16169.85</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40" t="n">
+    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41" t="n">
         <f aca="false">D35/C35</f>
         <v>1.0558825271854</v>
       </c>
-      <c r="E36" s="40" t="n">
+      <c r="E36" s="41" t="n">
         <f aca="false">E35/D35</f>
         <v>0.916849500061912</v>
       </c>
-      <c r="F36" s="40" t="n">
+      <c r="F36" s="41" t="n">
         <f aca="false">F35/E35</f>
         <v>1.10350896258914</v>
       </c>
-      <c r="G36" s="40" t="n">
+      <c r="G36" s="41" t="n">
         <f aca="false">G35/F35</f>
         <v>1.03987375176407</v>
       </c>
-      <c r="H36" s="40" t="n">
+      <c r="H36" s="41" t="n">
         <f aca="false">H35/G35</f>
         <v>1.06665722673939</v>
       </c>
-      <c r="I36" s="40" t="n">
+      <c r="I36" s="41" t="n">
         <f aca="false">I35/H35</f>
         <v>1.02227013104336</v>
       </c>
-      <c r="J36" s="40" t="n">
+      <c r="J36" s="41" t="n">
         <f aca="false">J35/I35</f>
         <v>0.968844995695285</v>
       </c>
-      <c r="K36" s="40" t="n">
+      <c r="K36" s="41" t="n">
         <f aca="false">K35/J35</f>
         <v>1.00756682988645</v>
       </c>
-      <c r="L36" s="40" t="n">
+      <c r="L36" s="41" t="n">
         <f aca="false">L35/K35</f>
         <v>1.03365334779935</v>
       </c>
-      <c r="M36" s="40" t="n">
+      <c r="M36" s="41" t="n">
         <f aca="false">M35/L35</f>
         <v>0.972899387020888</v>
       </c>
-      <c r="N36" s="40" t="n">
+      <c r="N36" s="41" t="n">
         <f aca="false">N35/M35</f>
         <v>1.06944594764067</v>
       </c>
-      <c r="O36" s="40" t="n">
+      <c r="O36" s="41" t="n">
         <f aca="false">O35/N35</f>
         <v>1.03914029657021</v>
       </c>
-      <c r="P36" s="40" t="n">
+      <c r="P36" s="41" t="n">
         <f aca="false">P35/O35</f>
         <v>1.0268997847368</v>
       </c>
-      <c r="Q36" s="40" t="n">
+      <c r="Q36" s="41" t="n">
         <f aca="false">Q35/P35</f>
         <v>1.00478259658715</v>
       </c>
-      <c r="R36" s="40" t="n">
+      <c r="R36" s="41" t="n">
         <f aca="false">R35/Q35</f>
         <v>1.02439095646859</v>
       </c>
-      <c r="S36" s="40" t="n">
+      <c r="S36" s="41" t="n">
         <f aca="false">S35/R35</f>
         <v>0.994786033590229</v>
       </c>
-      <c r="T36" s="40" t="n">
+      <c r="T36" s="41" t="n">
         <f aca="false">T35/S35</f>
         <v>0.995561439657853</v>
       </c>
-      <c r="U36" s="40" t="n">
+      <c r="U36" s="41" t="n">
         <f aca="false">U35/T35</f>
         <v>1.10342734655874</v>
       </c>
-      <c r="V36" s="40" t="n">
+      <c r="V36" s="41" t="n">
         <f aca="false">V35/U35</f>
         <v>0.949124255714387</v>
       </c>
-      <c r="W36" s="40" t="n">
+      <c r="W36" s="41" t="n">
         <f aca="false">W35/V35</f>
         <v>0.990510153289931</v>
       </c>
-      <c r="X36" s="40" t="n">
+      <c r="X36" s="41" t="n">
         <f aca="false">X35/W35</f>
         <v>0.963401613497919</v>
       </c>
-      <c r="Y36" s="40" t="n">
+      <c r="Y36" s="41" t="n">
         <f aca="false">Y35/X35</f>
         <v>1.04446534528375</v>
       </c>
-      <c r="Z36" s="40" t="n">
+      <c r="Z36" s="41" t="n">
         <f aca="false">Z35/Y35</f>
         <v>0.902660745410508</v>
       </c>
-      <c r="AA36" s="40" t="n">
+      <c r="AA36" s="41" t="n">
         <f aca="false">AA35/Z35</f>
         <v>1.14252240687931</v>
       </c>
-      <c r="AB36" s="40" t="n">
+      <c r="AB36" s="41" t="n">
         <f aca="false">AB35/AA35</f>
         <v>0.936850704356737</v>
       </c>
-      <c r="AC36" s="40" t="n">
+      <c r="AC36" s="41" t="n">
         <f aca="false">AC35/AB35</f>
         <v>1.03187444677672</v>
       </c>
-      <c r="AD36" s="40" t="n">
+      <c r="AD36" s="41" t="n">
         <f aca="false">AD35/AC35</f>
         <v>1.11331883538682</v>
       </c>
-      <c r="AE36" s="40" t="n">
+      <c r="AE36" s="41" t="n">
         <f aca="false">AE35/AD35</f>
         <v>1.00181950741378</v>
       </c>
-      <c r="AF36" s="40" t="n">
+      <c r="AF36" s="41" t="n">
         <f aca="false">AF35/AE35</f>
         <v>1.03424321595765</v>
       </c>
-      <c r="AG36" s="40" t="n">
+      <c r="AG36" s="41" t="n">
         <f aca="false">AG35/AF35</f>
         <v>1.00792537781632</v>
       </c>
-      <c r="AH36" s="40" t="n">
+      <c r="AH36" s="41" t="n">
         <f aca="false">AH35/AG35</f>
         <v>0.970324194852549</v>
       </c>
-      <c r="AI36" s="40" t="n">
+      <c r="AI36" s="41" t="n">
         <f aca="false">AI35/AH35</f>
         <v>1.04927844854803</v>
       </c>
-      <c r="AJ36" s="40" t="n">
+      <c r="AJ36" s="41" t="n">
         <f aca="false">AJ35/AI35</f>
         <v>0.940307515998851</v>
       </c>
-      <c r="AK36" s="40" t="n">
+      <c r="AK36" s="41" t="n">
         <f aca="false">AK35/AJ35</f>
         <v>0.954601895704387</v>
       </c>
-      <c r="AL36" s="40" t="n">
+      <c r="AL36" s="41" t="n">
         <f aca="false">AL35/AK35</f>
         <v>1.03769659098725</v>
       </c>
-      <c r="AM36" s="40" t="n">
+      <c r="AM36" s="41" t="n">
         <f aca="false">AM35/AL35</f>
         <v>1.0523801464953</v>
       </c>
-      <c r="AN36" s="40" t="n">
+      <c r="AN36" s="41" t="n">
         <f aca="false">AN35/AM35</f>
         <v>0.956782989818056</v>
       </c>
-      <c r="AO36" s="40" t="n">
+      <c r="AO36" s="41" t="n">
         <f aca="false">AO35/AN35</f>
         <v>1.00844663575681</v>
       </c>
-      <c r="AP36" s="40" t="n">
+      <c r="AP36" s="41" t="n">
         <f aca="false">AP35/AO35</f>
         <v>1.0133417237966</v>
       </c>
-      <c r="AQ36" s="40" t="n">
+      <c r="AQ36" s="41" t="n">
         <f aca="false">AQ35/AP35</f>
         <v>0.979393821898833</v>
       </c>
-      <c r="AR36" s="40" t="n">
+      <c r="AR36" s="41" t="n">
         <f aca="false">AR35/AQ35</f>
         <v>1.04525807986157</v>
       </c>
-      <c r="AS36" s="40" t="n">
+      <c r="AS36" s="41" t="n">
         <f aca="false">AS35/AR35</f>
         <v>0.988925223111335</v>
       </c>
-      <c r="AT36" s="40" t="n">
+      <c r="AT36" s="41" t="n">
         <f aca="false">AT35/AS35</f>
         <v>0.998857819887648</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="L38" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="O38" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="P38" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="U38" s="42" t="s">
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="AC38" s="42" t="s">
+      <c r="L38" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="AD38" s="42" t="s">
+      <c r="O38" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="AL38" s="44"/>
+      <c r="P38" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="U38" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC38" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD38" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL38" s="45"/>
       <c r="AR38" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8301,7 +8407,7 @@
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI87" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="BJ87" s="0" t="n">
         <v>141.39</v>
@@ -8312,7 +8418,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI88" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="BJ88" s="0" t="n">
         <v>420.46</v>
@@ -8323,7 +8429,7 @@
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI89" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BJ89" s="0" t="n">
         <v>96.99</v>
@@ -8334,7 +8440,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI90" s="0" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="BJ90" s="0" t="n">
         <v>547.6</v>
@@ -8345,7 +8451,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI91" s="0" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="BJ91" s="0" t="n">
         <v>314.62</v>
@@ -8356,7 +8462,7 @@
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI92" s="0" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="BJ92" s="0" t="n">
         <v>400.01</v>
@@ -8367,7 +8473,7 @@
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI93" s="0" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="BJ93" s="0" t="n">
         <v>2630.57</v>
@@ -8378,12 +8484,12 @@
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI94" s="0" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI95" s="0" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="BJ95" s="0" t="n">
         <v>627.3</v>
@@ -8394,7 +8500,7 @@
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI96" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="BJ96" s="0" t="n">
         <v>793.5</v>
@@ -8405,7 +8511,7 @@
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI97" s="0" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="BJ97" s="0" t="n">
         <v>128.01</v>
@@ -8416,7 +8522,7 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI98" s="0" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="BJ98" s="0" t="n">
         <v>433.45</v>
@@ -8427,7 +8533,7 @@
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI99" s="0" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="BJ99" s="0" t="n">
         <v>384.37</v>
@@ -8438,7 +8544,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI100" s="0" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="BJ100" s="0" t="n">
         <v>241.07</v>
@@ -8449,7 +8555,7 @@
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI101" s="0" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="BJ101" s="0" t="n">
         <v>261.63</v>
@@ -8460,7 +8566,7 @@
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI102" s="0" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="BJ102" s="0" t="n">
         <v>309.31</v>
@@ -8471,7 +8577,7 @@
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI103" s="0" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="BJ103" s="0" t="n">
         <v>777.04</v>
@@ -8482,7 +8588,7 @@
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI104" s="0" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="BJ104" s="0" t="n">
         <v>159.26</v>
@@ -8493,7 +8599,7 @@
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI105" s="0" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="BJ105" s="0" t="n">
         <v>385.36</v>
@@ -8504,7 +8610,7 @@
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI106" s="0" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="BJ106" s="0" t="n">
         <v>1620.35</v>
@@ -8515,7 +8621,7 @@
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI107" s="0" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="BJ107" s="0" t="n">
         <v>38.92</v>
@@ -8526,7 +8632,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI108" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="BJ108" s="0" t="n">
         <v>27.54</v>
@@ -8537,7 +8643,7 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI109" s="0" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="BJ109" s="0" t="n">
         <v>148.48</v>
@@ -8569,7 +8675,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
-      <selection pane="bottomRight" activeCell="AT4" activeCellId="1" sqref="AM69:AM96 AT4"/>
+      <selection pane="bottomRight" activeCell="AT4" activeCellId="0" sqref="AT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8588,174 +8694,174 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" s="46" customFormat="true" ht="42.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="45" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" s="47" customFormat="true" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="46" t="n">
         <v>44136</v>
       </c>
-      <c r="D4" s="45" t="n">
+      <c r="D4" s="46" t="n">
         <v>44144</v>
       </c>
-      <c r="E4" s="45" t="n">
+      <c r="E4" s="46" t="n">
         <v>44151</v>
       </c>
-      <c r="F4" s="45" t="n">
+      <c r="F4" s="46" t="n">
         <v>44157</v>
       </c>
-      <c r="G4" s="45" t="n">
+      <c r="G4" s="46" t="n">
         <v>44164</v>
       </c>
-      <c r="H4" s="45" t="n">
+      <c r="H4" s="46" t="n">
         <v>44171</v>
       </c>
-      <c r="I4" s="45" t="n">
+      <c r="I4" s="46" t="n">
         <v>44178</v>
       </c>
-      <c r="J4" s="45" t="n">
+      <c r="J4" s="46" t="n">
         <v>44185</v>
       </c>
-      <c r="K4" s="45" t="n">
+      <c r="K4" s="46" t="n">
         <v>44192</v>
       </c>
-      <c r="L4" s="45" t="n">
+      <c r="L4" s="46" t="n">
         <v>43833</v>
       </c>
-      <c r="M4" s="45" t="n">
+      <c r="M4" s="46" t="n">
         <v>44206</v>
       </c>
-      <c r="N4" s="45" t="n">
+      <c r="N4" s="46" t="n">
         <v>44213</v>
       </c>
-      <c r="O4" s="45" t="n">
+      <c r="O4" s="46" t="n">
         <v>44220</v>
       </c>
-      <c r="P4" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q4" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="R4" s="25" t="n">
+      <c r="P4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="R4" s="24" t="n">
         <v>44241</v>
       </c>
-      <c r="S4" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="T4" s="25" t="n">
+      <c r="S4" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="T4" s="24" t="n">
         <v>44255</v>
       </c>
-      <c r="U4" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="V4" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="W4" s="25" t="n">
+      <c r="U4" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="V4" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="W4" s="24" t="n">
         <v>44276</v>
       </c>
-      <c r="X4" s="25" t="n">
+      <c r="X4" s="24" t="n">
         <v>44276</v>
       </c>
-      <c r="Y4" s="25" t="n">
+      <c r="Y4" s="24" t="n">
         <v>44290</v>
       </c>
-      <c r="Z4" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA4" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="AB4" s="23" t="n">
+      <c r="Z4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA4" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB4" s="22" t="n">
         <v>44311</v>
       </c>
-      <c r="AC4" s="23" t="n">
+      <c r="AC4" s="22" t="n">
         <v>44318</v>
       </c>
-      <c r="AD4" s="45" t="n">
+      <c r="AD4" s="46" t="n">
         <v>44325</v>
       </c>
-      <c r="AE4" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="AG4" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH4" s="23" t="n">
+      <c r="AE4" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG4" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH4" s="22" t="n">
         <v>44353</v>
       </c>
-      <c r="AI4" s="23" t="n">
+      <c r="AI4" s="22" t="n">
         <v>44360</v>
       </c>
-      <c r="AJ4" s="23" t="n">
+      <c r="AJ4" s="22" t="n">
         <v>44367</v>
       </c>
-      <c r="AK4" s="23" t="n">
+      <c r="AK4" s="22" t="n">
         <v>44374</v>
       </c>
-      <c r="AL4" s="23" t="n">
+      <c r="AL4" s="22" t="n">
         <v>44383</v>
       </c>
-      <c r="AM4" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="AN4" s="23" t="n">
+      <c r="AM4" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN4" s="22" t="n">
         <v>44395</v>
       </c>
-      <c r="AO4" s="23" t="n">
+      <c r="AO4" s="22" t="n">
         <v>44402</v>
       </c>
-      <c r="AP4" s="23" t="n">
+      <c r="AP4" s="22" t="n">
         <v>44409</v>
       </c>
-      <c r="AQ4" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="AR4" s="23" t="n">
+      <c r="AQ4" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="AR4" s="22" t="n">
         <v>44423</v>
       </c>
-      <c r="AS4" s="47" t="n">
+      <c r="AS4" s="48" t="n">
         <v>44430</v>
       </c>
-      <c r="AT4" s="47" t="n">
+      <c r="AT4" s="48" t="n">
         <v>44437</v>
       </c>
     </row>
-    <row r="5" s="50" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="51" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="33"/>
-      <c r="AB5" s="33"/>
-      <c r="AC5" s="7" t="n">
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="32"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="32"/>
+      <c r="AC5" s="36" t="n">
         <v>272.20742</v>
       </c>
       <c r="AD5" s="0" t="n">
@@ -8807,15 +8913,15 @@
         <v>252.89731</v>
       </c>
     </row>
-    <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>125.35355</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="17" t="n">
         <v>144.04571</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -9334,7 +9440,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>33.85712</v>
@@ -9468,7 +9574,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>90.30445</v>
@@ -9602,7 +9708,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="37" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>33.5291</v>
@@ -9709,7 +9815,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>134.91832</v>
@@ -9804,7 +9910,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="38" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>74.7034</v>
@@ -9938,7 +10044,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="38" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>101.31368</v>
@@ -9964,7 +10070,7 @@
       <c r="J15" s="0" t="n">
         <v>106.81782</v>
       </c>
-      <c r="K15" s="10" t="n">
+      <c r="K15" s="39" t="n">
         <v>111.0613</v>
       </c>
       <c r="L15" s="0" t="n">
@@ -10072,7 +10178,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="38" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>523.34115</v>
@@ -10206,7 +10312,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="38" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="AD17" s="0" t="n">
         <v>53.44944</v>
@@ -10256,7 +10362,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="38" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>136.269</v>
@@ -10390,7 +10496,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="38" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>165.00564</v>
@@ -10524,7 +10630,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="38" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>43.42474</v>
@@ -10658,7 +10764,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="38" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>109.78636</v>
@@ -10792,7 +10898,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="38" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>93.06885</v>
@@ -10869,7 +10975,7 @@
       <c r="AA22" s="0" t="n">
         <v>113.63319</v>
       </c>
-      <c r="AB22" s="10" t="n">
+      <c r="AB22" s="39" t="n">
         <v>114.35779</v>
       </c>
       <c r="AC22" s="0" t="n">
@@ -10926,7 +11032,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="38" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>66.16259</v>
@@ -11060,7 +11166,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="38" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>66.85539</v>
@@ -11194,7 +11300,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="38" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>64.77227</v>
@@ -11327,8 +11433,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="39" t="s">
-        <v>46</v>
+      <c r="B26" s="40" t="s">
+        <v>29</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>170.8217</v>
@@ -11462,7 +11568,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="38" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>34.37503</v>
@@ -11596,7 +11702,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="38" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="U28" s="0" t="n">
         <v>70.84659</v>
@@ -11676,7 +11782,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="38" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>338.33972</v>
@@ -11810,7 +11916,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="38" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>14.4627</v>
@@ -11944,7 +12050,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="37" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>6.41945</v>
@@ -12078,7 +12184,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>45.24003</v>
@@ -12212,12 +12318,12 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="37" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -12394,177 +12500,177 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="C36" s="51" t="n">
+        <v>123</v>
+      </c>
+      <c r="C36" s="52" t="n">
         <f aca="false">1/(C35/Regular_Timings!C35)</f>
         <v>3.74749121272531</v>
       </c>
-      <c r="D36" s="51" t="n">
+      <c r="D36" s="52" t="n">
         <f aca="false">1/(D35/Regular_Timings!D35)</f>
         <v>3.41302620041922</v>
       </c>
-      <c r="E36" s="51" t="n">
+      <c r="E36" s="52" t="n">
         <f aca="false">1/(E35/Regular_Timings!E35)</f>
         <v>3.58035321194409</v>
       </c>
-      <c r="F36" s="51" t="n">
+      <c r="F36" s="52" t="n">
         <f aca="false">1/(F35/Regular_Timings!F35)</f>
         <v>3.77604759094586</v>
       </c>
-      <c r="G36" s="51" t="n">
+      <c r="G36" s="52" t="n">
         <f aca="false">1/(G35/Regular_Timings!G35)</f>
         <v>3.60534646208669</v>
       </c>
-      <c r="H36" s="51" t="n">
+      <c r="H36" s="52" t="n">
         <f aca="false">1/(H35/Regular_Timings!H35)</f>
         <v>3.71338155532446</v>
       </c>
-      <c r="I36" s="51" t="n">
+      <c r="I36" s="52" t="n">
         <f aca="false">1/(I35/Regular_Timings!I35)</f>
         <v>3.87995098100785</v>
       </c>
-      <c r="J36" s="51" t="n">
+      <c r="J36" s="52" t="n">
         <f aca="false">1/(J35/Regular_Timings!J35)</f>
         <v>3.77692817787917</v>
       </c>
-      <c r="K36" s="51" t="n">
+      <c r="K36" s="52" t="n">
         <f aca="false">1/(K35/Regular_Timings!K35)</f>
         <v>3.64724155744514</v>
       </c>
-      <c r="L36" s="51" t="n">
+      <c r="L36" s="52" t="n">
         <f aca="false">1/(L35/Regular_Timings!L35)</f>
         <v>3.74020943453721</v>
       </c>
-      <c r="M36" s="51" t="n">
+      <c r="M36" s="52" t="n">
         <f aca="false">1/(M35/Regular_Timings!M35)</f>
         <v>3.50672105722098</v>
       </c>
-      <c r="N36" s="51" t="n">
+      <c r="N36" s="52" t="n">
         <f aca="false">1/(N35/Regular_Timings!N35)</f>
         <v>3.73405080495359</v>
       </c>
-      <c r="O36" s="51" t="n">
+      <c r="O36" s="52" t="n">
         <f aca="false">1/(O35/Regular_Timings!O35)</f>
         <v>3.48066002524706</v>
       </c>
-      <c r="P36" s="51" t="n">
+      <c r="P36" s="52" t="n">
         <f aca="false">1/(P35/Regular_Timings!P35)</f>
         <v>3.64532320360124</v>
       </c>
-      <c r="Q36" s="51" t="n">
+      <c r="Q36" s="52" t="n">
         <f aca="false">1/(Q35/Regular_Timings!Q35)</f>
         <v>3.69283488712217</v>
       </c>
-      <c r="R36" s="51" t="n">
+      <c r="R36" s="52" t="n">
         <f aca="false">1/(R35/Regular_Timings!R35)</f>
         <v>3.91914079157363</v>
       </c>
-      <c r="S36" s="51" t="n">
+      <c r="S36" s="52" t="n">
         <f aca="false">1/(S35/Regular_Timings!S35)</f>
         <v>3.70850736443567</v>
       </c>
-      <c r="T36" s="51" t="n">
+      <c r="T36" s="52" t="n">
         <f aca="false">1/(T35/Regular_Timings!T35)</f>
         <v>3.75420891553771</v>
       </c>
-      <c r="U36" s="51" t="n">
+      <c r="U36" s="52" t="n">
         <f aca="false">1/(U35/Regular_Timings!U35)</f>
         <v>3.84853896938329</v>
       </c>
-      <c r="V36" s="51" t="n">
+      <c r="V36" s="52" t="n">
         <f aca="false">Regular_Timings!V35/V35</f>
         <v>3.72104488019434</v>
       </c>
-      <c r="W36" s="51" t="n">
+      <c r="W36" s="52" t="n">
         <f aca="false">Regular_Timings!W35/W35</f>
         <v>3.67572728059469</v>
       </c>
-      <c r="X36" s="51" t="n">
+      <c r="X36" s="52" t="n">
         <f aca="false">Regular_Timings!X35/X35</f>
         <v>4.19080065811635</v>
       </c>
-      <c r="Y36" s="51" t="n">
+      <c r="Y36" s="52" t="n">
         <f aca="false">Regular_Timings!Y35/Y35</f>
         <v>3.89406092958739</v>
       </c>
-      <c r="Z36" s="51" t="n">
+      <c r="Z36" s="52" t="n">
         <f aca="false">Regular_Timings!Z35/Z35</f>
         <v>3.55407794695691</v>
       </c>
-      <c r="AA36" s="51" t="n">
+      <c r="AA36" s="52" t="n">
         <f aca="false">Regular_Timings!AA35/AA35</f>
         <v>4.00488485600993</v>
       </c>
-      <c r="AB36" s="51" t="n">
+      <c r="AB36" s="52" t="n">
         <f aca="false">Regular_Timings!AB35/AB35</f>
         <v>3.66631773819967</v>
       </c>
-      <c r="AC36" s="51" t="n">
+      <c r="AC36" s="52" t="n">
         <f aca="false">Regular_Timings!AC35/AC35</f>
         <v>3.56831780200242</v>
       </c>
-      <c r="AD36" s="51" t="n">
+      <c r="AD36" s="52" t="n">
         <f aca="false">Regular_Timings!AD35/AD35</f>
         <v>3.7717099313906</v>
       </c>
-      <c r="AE36" s="51" t="n">
+      <c r="AE36" s="52" t="n">
         <f aca="false">Regular_Timings!AE35/AE35</f>
         <v>3.65797605865082</v>
       </c>
-      <c r="AG36" s="51" t="n">
+      <c r="AG36" s="52" t="n">
         <f aca="false">Regular_Timings!AG35/AG35</f>
         <v>3.6639766566581</v>
       </c>
-      <c r="AH36" s="51" t="n">
+      <c r="AH36" s="52" t="n">
         <f aca="false">Regular_Timings!AH35/AH35</f>
         <v>3.88981824858324</v>
       </c>
-      <c r="AI36" s="51" t="n">
+      <c r="AI36" s="52" t="n">
         <f aca="false">Regular_Timings!AI35/AI35</f>
         <v>3.95034639182564</v>
       </c>
-      <c r="AJ36" s="51" t="n">
+      <c r="AJ36" s="52" t="n">
         <f aca="false">Regular_Timings!AJ35/AJ35</f>
         <v>3.61276930976272</v>
       </c>
-      <c r="AK36" s="51" t="n">
+      <c r="AK36" s="52" t="n">
         <f aca="false">Regular_Timings!AK35/AK35</f>
         <v>3.47176276903545</v>
       </c>
-      <c r="AL36" s="51" t="n">
+      <c r="AL36" s="52" t="n">
         <f aca="false">Regular_Timings!AL35/AL35</f>
         <v>3.42704556536553</v>
       </c>
-      <c r="AM36" s="51" t="n">
+      <c r="AM36" s="52" t="n">
         <f aca="false">Regular_Timings!AM35/AM35</f>
         <v>3.62119345537265</v>
       </c>
-      <c r="AN36" s="51" t="n">
+      <c r="AN36" s="52" t="n">
         <f aca="false">Regular_Timings!AN35/AN35</f>
         <v>3.45756053775267</v>
       </c>
-      <c r="AO36" s="51" t="n">
+      <c r="AO36" s="52" t="n">
         <f aca="false">Regular_Timings!AO35/AO35</f>
         <v>3.39502062222087</v>
       </c>
-      <c r="AP36" s="51" t="n">
+      <c r="AP36" s="52" t="n">
         <f aca="false">Regular_Timings!AP35/AP35</f>
         <v>3.44119135284858</v>
       </c>
-      <c r="AQ36" s="51" t="n">
+      <c r="AQ36" s="52" t="n">
         <f aca="false">Regular_Timings!AQ35/AQ35</f>
         <v>3.37549763471932</v>
       </c>
-      <c r="AR36" s="51" t="n">
+      <c r="AR36" s="52" t="n">
         <f aca="false">Regular_Timings!AR35/AR35</f>
         <v>3.49581063859572</v>
       </c>
-      <c r="AS36" s="51" t="n">
+      <c r="AS36" s="52" t="n">
         <f aca="false">Regular_Timings!AS35/AS35</f>
         <v>3.56861246229986</v>
       </c>
-      <c r="AT36" s="51" t="n">
+      <c r="AT36" s="52" t="n">
         <f aca="false">Regular_Timings!AT35/AT35</f>
         <v>3.49118750571466</v>
       </c>
@@ -12572,11 +12678,11 @@
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="AC37" s="42"/>
+      <c r="AC37" s="43"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AC38" s="52" t="s">
-        <v>120</v>
+      <c r="AC38" s="53" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -12598,7 +12704,7 @@
   <dimension ref="A1:AJ97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="1" sqref="AM69:AM96 A33"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12612,232 +12718,232 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="X1" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AB1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q3" s="53" t="s">
-        <v>126</v>
+        <v>129</v>
+      </c>
+      <c r="Q3" s="54" t="s">
+        <v>130</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AJ3" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>143</v>
+        <v>146</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12847,7 +12953,7 @@
       <c r="J86" s="5"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J87" s="14"/>
+      <c r="J87" s="55"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J88" s="5"/>

</xml_diff>

<commit_message>
- Updated milestone, timeing and linecount tracking
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="142">
   <si>
     <t xml:space="preserve">Projects Since June 15, 2018</t>
   </si>
@@ -205,100 +205,10 @@
     <t xml:space="preserve">As of June 3, 2019</t>
   </si>
   <si>
-    <t xml:space="preserve">ICal:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLib:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIR:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATK:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIO:</t>
-  </si>
-  <si>
     <t xml:space="preserve">As of June 9, 2019 – LOL!</t>
   </si>
   <si>
-    <t xml:space="preserve">JSON-GLib:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOUP:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSSDP:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GUPnP:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pango:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDK:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GtkPlus:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GtkBuilder:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SourceViewGTK:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WebkitGTK:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMTK:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEPL:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GooCanvas:</t>
-  </si>
-  <si>
     <t xml:space="preserve">As of July 11, 2019!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slope:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WNCK:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COGL:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clutter:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GtkClutter:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Champlain:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GStreamer:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RSVG:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CardDeck:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTE:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOA:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secret:</t>
   </si>
   <si>
     <t xml:space="preserve">As of August 10, 2019!</t>
@@ -1470,13 +1380,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>738360</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>186480</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1489,7 +1399,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="738360" y="10476000"/>
+          <a:off x="738360" y="10476360"/>
           <a:ext cx="9703800" cy="2053800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1505,15 +1415,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>24120</xdr:colOff>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>65160</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>43920</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1526,7 +1436,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2234880" y="12926520"/>
+          <a:off x="2235240" y="12926880"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1542,13 +1452,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>24120</xdr:colOff>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>89</xdr:row>
       <xdr:rowOff>15480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>30600</xdr:colOff>
+      <xdr:colOff>30960</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
@@ -1563,7 +1473,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2234880" y="15541200"/>
+          <a:off x="2235240" y="15541200"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1579,15 +1489,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>24120</xdr:colOff>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>102</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
+      <xdr:colOff>635400</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1600,7 +1510,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2234880" y="17836920"/>
+          <a:off x="2235240" y="17837280"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1616,15 +1526,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>23760</xdr:colOff>
+      <xdr:colOff>24120</xdr:colOff>
       <xdr:row>120</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>588240</xdr:colOff>
+      <xdr:colOff>588600</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>84600</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1637,7 +1547,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2234520" y="20991600"/>
+          <a:off x="2234880" y="20991960"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1653,13 +1563,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>53280</xdr:colOff>
+      <xdr:colOff>53640</xdr:colOff>
       <xdr:row>136</xdr:row>
       <xdr:rowOff>8640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>613080</xdr:colOff>
+      <xdr:colOff>613440</xdr:colOff>
       <xdr:row>148</xdr:row>
       <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
@@ -1674,7 +1584,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2264040" y="23771520"/>
+          <a:off x="2264400" y="23771520"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1690,15 +1600,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>21240</xdr:colOff>
+      <xdr:colOff>21600</xdr:colOff>
       <xdr:row>150</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
+      <xdr:colOff>258840</xdr:colOff>
       <xdr:row>162</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1711,7 +1621,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2232000" y="26249400"/>
+          <a:off x="2232360" y="26249760"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1729,13 +1639,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
       <xdr:row>180</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>309600</xdr:colOff>
       <xdr:row>192</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1748,7 +1658,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3115080" y="31513320"/>
+          <a:off x="3115080" y="31513680"/>
           <a:ext cx="9708120" cy="2138400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1803,13 +1713,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>209880</xdr:colOff>
       <xdr:row>194</xdr:row>
-      <xdr:rowOff>169560</xdr:rowOff>
+      <xdr:rowOff>169920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>333720</xdr:colOff>
       <xdr:row>207</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1822,7 +1732,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3059640" y="34097400"/>
+          <a:off x="3059640" y="34097760"/>
           <a:ext cx="9787680" cy="2191320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2992,8 +2902,8 @@
   </sheetPr>
   <dimension ref="A1:X626"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S62" activeCellId="0" sqref="S62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3077,11 +2987,11 @@
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>748.28</v>
+        <v>754.52</v>
       </c>
       <c r="Q6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>210.2638</v>
+        <v>205.40968</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3096,11 +3006,11 @@
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>214.7</v>
+        <v>214.99</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>89.32501</v>
+        <v>87.29099</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3115,11 +3025,11 @@
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>295.13</v>
+        <v>294.56</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>89.27404</v>
+        <v>88.54707</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,11 +3049,11 @@
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1608.31</v>
+        <v>1641.63</v>
       </c>
       <c r="Q9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>402.9341</v>
+        <v>398.5639</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3159,11 +3069,11 @@
       <c r="O10" s="4"/>
       <c r="P10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>160.19</v>
+        <v>159.17</v>
       </c>
       <c r="Q10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>51.34159</v>
+        <v>50.66426</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3179,11 +3089,11 @@
       <c r="O11" s="4"/>
       <c r="P11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>141.63361</v>
+        <v>141.3976</v>
       </c>
       <c r="Q11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>141.63361</v>
+        <v>141.3976</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3199,11 +3109,11 @@
       <c r="O12" s="4"/>
       <c r="P12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>113.14</v>
+        <v>112.9</v>
       </c>
       <c r="Q12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>45.53721</v>
+        <v>44.7714</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3219,11 +3129,11 @@
       <c r="O13" s="4"/>
       <c r="P13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>610.03</v>
+        <v>606.02</v>
       </c>
       <c r="Q13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>164.25094</v>
+        <v>157.88911</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,11 +3153,11 @@
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>347.14</v>
+        <v>344.28</v>
       </c>
       <c r="Q14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>122.76784</v>
+        <v>119.24336</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,11 +3173,11 @@
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>426.34</v>
+        <v>425.22</v>
       </c>
       <c r="Q15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>142.33849</v>
+        <v>138.78989</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3286,11 +3196,11 @@
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>2779.73</v>
+        <v>2770.42</v>
       </c>
       <c r="Q16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>706.54516</v>
+        <v>702.72608</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3305,11 +3215,11 @@
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>252.51</v>
+        <v>250.75</v>
       </c>
       <c r="Q17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
-        <v>57.20562</v>
+        <v>56.91452</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3324,11 +3234,11 @@
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>694.36</v>
+        <v>691.04</v>
       </c>
       <c r="Q18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>197.45861</v>
+        <v>200.34936</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,11 +3257,11 @@
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>847.06</v>
+        <v>843.51</v>
       </c>
       <c r="Q19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>248.03044</v>
+        <v>234.65922</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,11 +3276,11 @@
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>138.82</v>
+        <v>138.07</v>
       </c>
       <c r="Q20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>57.76155</v>
+        <v>57.39666</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3385,11 +3295,11 @@
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>473.33</v>
+        <v>471.94</v>
       </c>
       <c r="Q21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>161.27427</v>
+        <v>155.16865</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3404,11 +3314,11 @@
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>428.78</v>
+        <v>426.63</v>
       </c>
       <c r="Q22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>137.73073</v>
+        <v>134.23404</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3423,11 +3333,11 @@
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>267.23</v>
+        <v>264.97</v>
       </c>
       <c r="Q23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>103.11229</v>
+        <v>98.32562</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,11 +3352,11 @@
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>289.86</v>
+        <v>288.62</v>
       </c>
       <c r="Q24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>92.93745</v>
+        <v>90.04957</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3462,11 +3372,11 @@
       <c r="O25" s="1"/>
       <c r="P25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>342.92</v>
+        <v>341.36</v>
       </c>
       <c r="Q25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>102.59401</v>
+        <v>99.55833</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3481,11 +3391,11 @@
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>839.5</v>
+        <v>831.34</v>
       </c>
       <c r="Q26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>255.02598</v>
+        <v>253.4455</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3500,11 +3410,11 @@
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>186.46</v>
+        <v>184.31</v>
       </c>
       <c r="Q27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>58.78364</v>
+        <v>53.8565</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,11 +3429,11 @@
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>438.13</v>
+        <v>433.6</v>
       </c>
       <c r="Q28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>144.56536</v>
+        <v>128.04166</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3542,11 +3452,11 @@
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1780.01</v>
+        <v>1767.51</v>
       </c>
       <c r="Q29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>487.48703</v>
+        <v>474.37795</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3561,11 +3471,11 @@
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>46.13</v>
+        <v>45.15</v>
       </c>
       <c r="Q30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>22.11175</v>
+        <v>21.95764</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,11 +3490,11 @@
       </c>
       <c r="P31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>33.2</v>
+        <v>32.52</v>
       </c>
       <c r="Q31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>25.2621</v>
+        <v>24.4971</v>
       </c>
     </row>
     <row r="32" s="9" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3599,11 +3509,11 @@
       </c>
       <c r="P32" s="10" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>170.28</v>
+        <v>167.71</v>
       </c>
       <c r="Q32" s="10" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>61.16896</v>
+        <v>59.25021</v>
       </c>
       <c r="R32" s="10"/>
     </row>
@@ -3790,11 +3700,11 @@
       </c>
       <c r="P54" s="0" t="n">
         <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
-        <v>16169.85</v>
+        <v>16123.04</v>
       </c>
       <c r="Q54" s="17" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D35:ND35&lt;&gt;""),Parallel_Timings!D35:ND35)</f>
-        <v>4631.61889</v>
+        <v>4525.68907</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3809,7 +3719,7 @@
       </c>
       <c r="Q55" s="18" t="n">
         <f aca="false">P54/Q54</f>
-        <v>3.49118750571466</v>
+        <v>3.56256025339363</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3825,175 +3735,29 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R65" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R66" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R67" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R68" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R69" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="R70" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R71" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R72" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R73" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R74" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R75" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R76" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R77" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R78" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R79" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R80" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R81" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R82" s="0" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="R83" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R84" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R85" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R86" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R87" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R88" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R89" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R90" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R91" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R92" s="0" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R93" s="0" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R94" s="0" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C112" s="0" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="0" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +3767,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C164" s="0" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4013,7 +3777,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C179" s="0" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4221,11 +3985,11 @@
   <dimension ref="A2:BK109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="AR5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="AR1" activeCellId="0" sqref="AR1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AM96" activeCellId="0" sqref="AM96"/>
+      <selection pane="bottomRight" activeCell="AU4" activeCellId="0" sqref="AU4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4247,7 +4011,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" s="20" customFormat="true" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4291,25 +4055,25 @@
         <v>44220</v>
       </c>
       <c r="P4" s="23" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="R4" s="22" t="n">
         <v>44241</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="T4" s="22" t="n">
         <v>44255</v>
       </c>
       <c r="U4" s="23" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="V4" s="23" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="W4" s="24" t="n">
         <v>44276</v>
@@ -4321,10 +4085,10 @@
         <v>44290</v>
       </c>
       <c r="Z4" s="23" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="AA4" s="23" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="AB4" s="22" t="n">
         <v>44311</v>
@@ -4336,13 +4100,13 @@
         <v>44325</v>
       </c>
       <c r="AE4" s="25" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="AF4" s="22" t="n">
         <v>44339</v>
       </c>
       <c r="AG4" s="25" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="AH4" s="22" t="n">
         <v>44353</v>
@@ -4357,10 +4121,10 @@
         <v>44374</v>
       </c>
       <c r="AL4" s="25" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="AM4" s="25" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="AN4" s="22" t="n">
         <v>44395</v>
@@ -4372,7 +4136,7 @@
         <v>44409</v>
       </c>
       <c r="AQ4" s="27" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="AR4" s="26" t="n">
         <v>44423</v>
@@ -4382,6 +4146,12 @@
       </c>
       <c r="AT4" s="26" t="n">
         <v>44437</v>
+      </c>
+      <c r="AU4" s="26" t="n">
+        <v>44444</v>
+      </c>
+      <c r="AV4" s="26" t="n">
+        <v>44451</v>
       </c>
     </row>
     <row r="5" s="29" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4468,6 +4238,12 @@
       <c r="AT5" s="0" t="n">
         <v>1160.42</v>
       </c>
+      <c r="AU5" s="0" t="n">
+        <v>1187.38</v>
+      </c>
+      <c r="AV5" s="0" t="n">
+        <v>1144.68</v>
+      </c>
     </row>
     <row r="6" s="11" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="35" t="s">
@@ -4604,6 +4380,12 @@
       <c r="AT6" s="0" t="n">
         <v>748.28</v>
       </c>
+      <c r="AU6" s="0" t="n">
+        <v>767.07</v>
+      </c>
+      <c r="AV6" s="0" t="n">
+        <v>754.52</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
@@ -4741,6 +4523,12 @@
       <c r="AT7" s="0" t="n">
         <v>214.7</v>
       </c>
+      <c r="AU7" s="0" t="n">
+        <v>217.41</v>
+      </c>
+      <c r="AV7" s="0" t="n">
+        <v>214.99</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="37" t="s">
@@ -4866,6 +4654,12 @@
       <c r="AT8" s="0" t="n">
         <v>295.13</v>
       </c>
+      <c r="AU8" s="0" t="n">
+        <v>297.8</v>
+      </c>
+      <c r="AV8" s="0" t="n">
+        <v>294.56</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
@@ -5003,6 +4797,12 @@
       <c r="AT9" s="0" t="n">
         <v>1608.31</v>
       </c>
+      <c r="AU9" s="0" t="n">
+        <v>1616.35</v>
+      </c>
+      <c r="AV9" s="0" t="n">
+        <v>1641.63</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
@@ -5140,6 +4940,12 @@
       <c r="AT10" s="0" t="n">
         <v>160.19</v>
       </c>
+      <c r="AU10" s="0" t="n">
+        <v>160.61</v>
+      </c>
+      <c r="AV10" s="0" t="n">
+        <v>159.17</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
@@ -5277,6 +5083,12 @@
       <c r="AT11" s="0" t="n">
         <v>477.86</v>
       </c>
+      <c r="AU11" s="0" t="n">
+        <v>477.19</v>
+      </c>
+      <c r="AV11" s="0" t="n">
+        <v>475.62</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
@@ -5387,6 +5199,12 @@
       <c r="AT12" s="0" t="n">
         <v>113.14</v>
       </c>
+      <c r="AU12" s="0" t="n">
+        <v>113.37</v>
+      </c>
+      <c r="AV12" s="0" t="n">
+        <v>112.9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="37" t="s">
@@ -5485,6 +5303,12 @@
       <c r="AT13" s="0" t="n">
         <v>610.03</v>
       </c>
+      <c r="AU13" s="0" t="n">
+        <v>602.81</v>
+      </c>
+      <c r="AV13" s="0" t="n">
+        <v>606.02</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
@@ -5622,6 +5446,12 @@
       <c r="AT14" s="0" t="n">
         <v>347.14</v>
       </c>
+      <c r="AU14" s="0" t="n">
+        <v>343.85</v>
+      </c>
+      <c r="AV14" s="0" t="n">
+        <v>344.28</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38" t="s">
@@ -5759,6 +5589,12 @@
       <c r="AT15" s="0" t="n">
         <v>426.34</v>
       </c>
+      <c r="AU15" s="0" t="n">
+        <v>423.33</v>
+      </c>
+      <c r="AV15" s="0" t="n">
+        <v>425.22</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38" t="s">
@@ -5896,6 +5732,12 @@
       <c r="AT16" s="0" t="n">
         <v>2779.73</v>
       </c>
+      <c r="AU16" s="0" t="n">
+        <v>2751.68</v>
+      </c>
+      <c r="AV16" s="0" t="n">
+        <v>2770.42</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38" t="s">
@@ -5952,6 +5794,12 @@
       <c r="AT17" s="0" t="n">
         <v>252.51</v>
       </c>
+      <c r="AU17" s="0" t="n">
+        <v>248.12</v>
+      </c>
+      <c r="AV17" s="0" t="n">
+        <v>250.75</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38" t="s">
@@ -6089,6 +5937,12 @@
       <c r="AT18" s="0" t="n">
         <v>694.36</v>
       </c>
+      <c r="AU18" s="0" t="n">
+        <v>687.71</v>
+      </c>
+      <c r="AV18" s="0" t="n">
+        <v>691.04</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38" t="s">
@@ -6226,6 +6080,12 @@
       <c r="AT19" s="0" t="n">
         <v>847.06</v>
       </c>
+      <c r="AU19" s="0" t="n">
+        <v>838.59</v>
+      </c>
+      <c r="AV19" s="0" t="n">
+        <v>843.51</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38" t="s">
@@ -6363,6 +6223,12 @@
       <c r="AT20" s="0" t="n">
         <v>138.82</v>
       </c>
+      <c r="AU20" s="0" t="n">
+        <v>137.73</v>
+      </c>
+      <c r="AV20" s="0" t="n">
+        <v>138.07</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38" t="s">
@@ -6500,6 +6366,12 @@
       <c r="AT21" s="0" t="n">
         <v>473.33</v>
       </c>
+      <c r="AU21" s="0" t="n">
+        <v>467.57</v>
+      </c>
+      <c r="AV21" s="0" t="n">
+        <v>471.94</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38" t="s">
@@ -6637,6 +6509,12 @@
       <c r="AT22" s="0" t="n">
         <v>428.78</v>
       </c>
+      <c r="AU22" s="0" t="n">
+        <v>423.41</v>
+      </c>
+      <c r="AV22" s="0" t="n">
+        <v>426.63</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38" t="s">
@@ -6774,6 +6652,12 @@
       <c r="AT23" s="0" t="n">
         <v>267.23</v>
       </c>
+      <c r="AU23" s="0" t="n">
+        <v>264.23</v>
+      </c>
+      <c r="AV23" s="0" t="n">
+        <v>264.97</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38" t="s">
@@ -6911,6 +6795,12 @@
       <c r="AT24" s="0" t="n">
         <v>289.86</v>
       </c>
+      <c r="AU24" s="0" t="n">
+        <v>287.04</v>
+      </c>
+      <c r="AV24" s="0" t="n">
+        <v>288.62</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38" t="s">
@@ -7048,6 +6938,12 @@
       <c r="AT25" s="0" t="n">
         <v>342.92</v>
       </c>
+      <c r="AU25" s="0" t="n">
+        <v>338.69</v>
+      </c>
+      <c r="AV25" s="0" t="n">
+        <v>341.36</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
@@ -7185,6 +7081,12 @@
       <c r="AT26" s="0" t="n">
         <v>839.5</v>
       </c>
+      <c r="AU26" s="0" t="n">
+        <v>830.58</v>
+      </c>
+      <c r="AV26" s="0" t="n">
+        <v>831.34</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="38" t="s">
@@ -7322,6 +7224,12 @@
       <c r="AT27" s="0" t="n">
         <v>186.46</v>
       </c>
+      <c r="AU27" s="0" t="n">
+        <v>183.56</v>
+      </c>
+      <c r="AV27" s="0" t="n">
+        <v>184.31</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38" t="s">
@@ -7405,6 +7313,12 @@
       <c r="AT28" s="0" t="n">
         <v>438.13</v>
       </c>
+      <c r="AU28" s="0" t="n">
+        <v>432.28</v>
+      </c>
+      <c r="AV28" s="0" t="n">
+        <v>433.6</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="38" t="s">
@@ -7542,6 +7456,12 @@
       <c r="AT29" s="0" t="n">
         <v>1780.01</v>
       </c>
+      <c r="AU29" s="0" t="n">
+        <v>1761.27</v>
+      </c>
+      <c r="AV29" s="0" t="n">
+        <v>1767.51</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38" t="s">
@@ -7679,6 +7599,12 @@
       <c r="AT30" s="0" t="n">
         <v>46.13</v>
       </c>
+      <c r="AU30" s="0" t="n">
+        <v>45.32</v>
+      </c>
+      <c r="AV30" s="0" t="n">
+        <v>45.15</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="37" t="s">
@@ -7816,6 +7742,12 @@
       <c r="AT31" s="0" t="n">
         <v>33.2</v>
       </c>
+      <c r="AU31" s="0" t="n">
+        <v>32.69</v>
+      </c>
+      <c r="AV31" s="0" t="n">
+        <v>32.52</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="37" t="s">
@@ -7953,6 +7885,12 @@
       <c r="AT32" s="0" t="n">
         <v>170.28</v>
       </c>
+      <c r="AU32" s="0" t="n">
+        <v>168.01</v>
+      </c>
+      <c r="AV32" s="0" t="n">
+        <v>167.71</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="37" t="s">
@@ -7961,7 +7899,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -8139,10 +8077,18 @@
         <f aca="false">SUM(AT$5:AT$32)</f>
         <v>16169.85</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU35" s="0" t="n">
+        <f aca="false">SUM(AU$5:AU$32)</f>
+        <v>16105.65</v>
+      </c>
+      <c r="AV35" s="0" t="n">
+        <f aca="false">SUM(AV$5:AV$32)</f>
+        <v>16123.04</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="36" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C36" s="41"/>
       <c r="D36" s="41" t="n">
@@ -8317,10 +8263,18 @@
         <f aca="false">AT35/AS35</f>
         <v>0.998857819887648</v>
       </c>
+      <c r="AU36" s="41" t="n">
+        <f aca="false">AU35/AT35</f>
+        <v>0.996029647770387</v>
+      </c>
+      <c r="AV36" s="41" t="n">
+        <f aca="false">AV35/AU35</f>
+        <v>1.00107974530677</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
@@ -8328,29 +8282,29 @@
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
       <c r="H38" s="42" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="L38" s="43" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="O38" s="44" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="P38" s="43" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="U38" s="43" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="AC38" s="43" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="AD38" s="43" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="AL38" s="45"/>
       <c r="AR38" s="0" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8632,7 +8586,7 @@
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="BI108" s="0" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="BJ108" s="0" t="n">
         <v>27.54</v>
@@ -8668,14 +8622,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AT38"/>
+  <dimension ref="A2:AV38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="AM11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
-      <selection pane="bottomRight" activeCell="AT4" activeCellId="0" sqref="AT4"/>
+      <selection pane="topRight" activeCell="AM1" activeCellId="0" sqref="AM1"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="AU30" activeCellId="0" sqref="AU30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8694,10 +8648,10 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" s="47" customFormat="true" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" s="47" customFormat="true" ht="42.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="46" t="n">
@@ -8740,25 +8694,25 @@
         <v>44220</v>
       </c>
       <c r="P4" s="23" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="R4" s="24" t="n">
         <v>44241</v>
       </c>
       <c r="S4" s="23" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="T4" s="24" t="n">
         <v>44255</v>
       </c>
       <c r="U4" s="23" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="V4" s="23" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="W4" s="24" t="n">
         <v>44276</v>
@@ -8770,10 +8724,10 @@
         <v>44290</v>
       </c>
       <c r="Z4" s="23" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="AA4" s="23" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="AB4" s="22" t="n">
         <v>44311</v>
@@ -8785,10 +8739,10 @@
         <v>44325</v>
       </c>
       <c r="AE4" s="25" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="AG4" s="25" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="AH4" s="22" t="n">
         <v>44353</v>
@@ -8806,7 +8760,7 @@
         <v>44383</v>
       </c>
       <c r="AM4" s="25" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="AN4" s="22" t="n">
         <v>44395</v>
@@ -8818,7 +8772,7 @@
         <v>44409</v>
       </c>
       <c r="AQ4" s="23" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="AR4" s="22" t="n">
         <v>44423</v>
@@ -8828,6 +8782,12 @@
       </c>
       <c r="AT4" s="48" t="n">
         <v>44437</v>
+      </c>
+      <c r="AU4" s="26" t="n">
+        <v>44444</v>
+      </c>
+      <c r="AV4" s="26" t="n">
+        <v>44451</v>
       </c>
     </row>
     <row r="5" s="51" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8912,6 +8872,12 @@
       <c r="AT5" s="0" t="n">
         <v>252.89731</v>
       </c>
+      <c r="AU5" s="0" t="n">
+        <v>252.91979</v>
+      </c>
+      <c r="AV5" s="0" t="n">
+        <v>248.3132</v>
+      </c>
     </row>
     <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -9047,6 +9013,12 @@
       <c r="AT6" s="0" t="n">
         <v>210.2638</v>
       </c>
+      <c r="AU6" s="0" t="n">
+        <v>214.33064</v>
+      </c>
+      <c r="AV6" s="0" t="n">
+        <v>205.40968</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
@@ -9181,6 +9153,12 @@
       <c r="AT7" s="0" t="n">
         <v>89.32501</v>
       </c>
+      <c r="AU7" s="0" t="n">
+        <v>91.49466</v>
+      </c>
+      <c r="AV7" s="0" t="n">
+        <v>87.29099</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
@@ -9303,6 +9281,12 @@
       <c r="AT8" s="0" t="n">
         <v>89.27404</v>
       </c>
+      <c r="AU8" s="0" t="n">
+        <v>91.51357</v>
+      </c>
+      <c r="AV8" s="0" t="n">
+        <v>88.54707</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="38" t="s">
@@ -9437,6 +9421,12 @@
       <c r="AT9" s="0" t="n">
         <v>402.9341</v>
       </c>
+      <c r="AU9" s="0" t="n">
+        <v>414.24903</v>
+      </c>
+      <c r="AV9" s="0" t="n">
+        <v>398.5639</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="37" t="s">
@@ -9571,6 +9561,12 @@
       <c r="AT10" s="0" t="n">
         <v>51.34159</v>
       </c>
+      <c r="AU10" s="0" t="n">
+        <v>51.96557</v>
+      </c>
+      <c r="AV10" s="0" t="n">
+        <v>50.66426</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
@@ -9705,6 +9701,12 @@
       <c r="AT11" s="0" t="n">
         <v>141.63361</v>
       </c>
+      <c r="AU11" s="0" t="n">
+        <v>144.9393</v>
+      </c>
+      <c r="AV11" s="0" t="n">
+        <v>141.3976</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="37" t="s">
@@ -9812,6 +9814,12 @@
       <c r="AT12" s="0" t="n">
         <v>45.53721</v>
       </c>
+      <c r="AU12" s="0" t="n">
+        <v>46.37073</v>
+      </c>
+      <c r="AV12" s="0" t="n">
+        <v>44.7714</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
@@ -9907,6 +9915,12 @@
       <c r="AT13" s="0" t="n">
         <v>164.25094</v>
       </c>
+      <c r="AU13" s="0" t="n">
+        <v>164.63836</v>
+      </c>
+      <c r="AV13" s="0" t="n">
+        <v>157.88911</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="38" t="s">
@@ -10041,6 +10055,12 @@
       <c r="AT14" s="0" t="n">
         <v>122.76784</v>
       </c>
+      <c r="AU14" s="0" t="n">
+        <v>125.27021</v>
+      </c>
+      <c r="AV14" s="0" t="n">
+        <v>119.24336</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="38" t="s">
@@ -10175,6 +10195,12 @@
       <c r="AT15" s="0" t="n">
         <v>142.33849</v>
       </c>
+      <c r="AU15" s="0" t="n">
+        <v>145.43458</v>
+      </c>
+      <c r="AV15" s="0" t="n">
+        <v>138.78989</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="38" t="s">
@@ -10309,6 +10335,12 @@
       <c r="AT16" s="0" t="n">
         <v>706.54516</v>
       </c>
+      <c r="AU16" s="0" t="n">
+        <v>721.50994</v>
+      </c>
+      <c r="AV16" s="0" t="n">
+        <v>702.72608</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="38" t="s">
@@ -10359,6 +10391,12 @@
       <c r="AT17" s="0" t="n">
         <v>57.20562</v>
       </c>
+      <c r="AU17" s="0" t="n">
+        <v>59.10345</v>
+      </c>
+      <c r="AV17" s="0" t="n">
+        <v>56.91452</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="38" t="s">
@@ -10493,6 +10531,12 @@
       <c r="AT18" s="0" t="n">
         <v>197.45861</v>
       </c>
+      <c r="AU18" s="0" t="n">
+        <v>203.1654</v>
+      </c>
+      <c r="AV18" s="0" t="n">
+        <v>200.34936</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="38" t="s">
@@ -10627,6 +10671,12 @@
       <c r="AT19" s="0" t="n">
         <v>248.03044</v>
       </c>
+      <c r="AU19" s="0" t="n">
+        <v>239.94694</v>
+      </c>
+      <c r="AV19" s="0" t="n">
+        <v>234.65922</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="38" t="s">
@@ -10761,6 +10811,12 @@
       <c r="AT20" s="0" t="n">
         <v>57.76155</v>
       </c>
+      <c r="AU20" s="0" t="n">
+        <v>59.43</v>
+      </c>
+      <c r="AV20" s="0" t="n">
+        <v>57.39666</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="38" t="s">
@@ -10895,6 +10951,12 @@
       <c r="AT21" s="0" t="n">
         <v>161.27427</v>
       </c>
+      <c r="AU21" s="0" t="n">
+        <v>162.08396</v>
+      </c>
+      <c r="AV21" s="0" t="n">
+        <v>155.16865</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="38" t="s">
@@ -11029,6 +11091,12 @@
       <c r="AT22" s="0" t="n">
         <v>137.73073</v>
       </c>
+      <c r="AU22" s="0" t="n">
+        <v>140.10591</v>
+      </c>
+      <c r="AV22" s="0" t="n">
+        <v>134.23404</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="38" t="s">
@@ -11163,6 +11231,12 @@
       <c r="AT23" s="0" t="n">
         <v>103.11229</v>
       </c>
+      <c r="AU23" s="0" t="n">
+        <v>102.91722</v>
+      </c>
+      <c r="AV23" s="0" t="n">
+        <v>98.32562</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="38" t="s">
@@ -11297,6 +11371,12 @@
       <c r="AT24" s="0" t="n">
         <v>92.93745</v>
       </c>
+      <c r="AU24" s="0" t="n">
+        <v>93.44129</v>
+      </c>
+      <c r="AV24" s="0" t="n">
+        <v>90.04957</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="38" t="s">
@@ -11431,6 +11511,12 @@
       <c r="AT25" s="0" t="n">
         <v>102.59401</v>
       </c>
+      <c r="AU25" s="0" t="n">
+        <v>101.27234</v>
+      </c>
+      <c r="AV25" s="0" t="n">
+        <v>99.55833</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="40" t="s">
@@ -11565,6 +11651,12 @@
       <c r="AT26" s="0" t="n">
         <v>255.02598</v>
       </c>
+      <c r="AU26" s="0" t="n">
+        <v>258.89419</v>
+      </c>
+      <c r="AV26" s="0" t="n">
+        <v>253.4455</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="38" t="s">
@@ -11699,6 +11791,12 @@
       <c r="AT27" s="0" t="n">
         <v>58.78364</v>
       </c>
+      <c r="AU27" s="0" t="n">
+        <v>55.28499</v>
+      </c>
+      <c r="AV27" s="0" t="n">
+        <v>53.8565</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="38" t="s">
@@ -11779,6 +11877,12 @@
       <c r="AT28" s="0" t="n">
         <v>144.56536</v>
       </c>
+      <c r="AU28" s="0" t="n">
+        <v>132.90942</v>
+      </c>
+      <c r="AV28" s="0" t="n">
+        <v>128.04166</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="38" t="s">
@@ -11913,6 +12017,12 @@
       <c r="AT29" s="0" t="n">
         <v>487.48703</v>
       </c>
+      <c r="AU29" s="0" t="n">
+        <v>497.48826</v>
+      </c>
+      <c r="AV29" s="0" t="n">
+        <v>474.37795</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="38" t="s">
@@ -12047,6 +12157,12 @@
       <c r="AT30" s="0" t="n">
         <v>22.11175</v>
       </c>
+      <c r="AU30" s="0" t="n">
+        <v>22.78173</v>
+      </c>
+      <c r="AV30" s="0" t="n">
+        <v>21.95764</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="37" t="s">
@@ -12181,6 +12297,12 @@
       <c r="AT31" s="0" t="n">
         <v>25.2621</v>
       </c>
+      <c r="AU31" s="0" t="n">
+        <v>25.87995</v>
+      </c>
+      <c r="AV31" s="0" t="n">
+        <v>24.4971</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
@@ -12315,6 +12437,12 @@
       <c r="AT32" s="0" t="n">
         <v>61.16896</v>
       </c>
+      <c r="AU32" s="0" t="n">
+        <v>62.19667</v>
+      </c>
+      <c r="AV32" s="0" t="n">
+        <v>59.25021</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="37" t="s">
@@ -12323,7 +12451,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">SUM(C$6:C$32)</f>
@@ -12497,10 +12625,18 @@
         <f aca="false">SUM(AT$5:AT$32)</f>
         <v>4631.61889</v>
       </c>
+      <c r="AU35" s="0" t="n">
+        <f aca="false">SUM(AU$5:AU$32)</f>
+        <v>4681.5381</v>
+      </c>
+      <c r="AV35" s="0" t="n">
+        <f aca="false">SUM(AV$5:AV$32)</f>
+        <v>4525.68907</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="C36" s="52" t="n">
         <f aca="false">1/(C35/Regular_Timings!C35)</f>
@@ -12673,6 +12809,14 @@
       <c r="AT36" s="52" t="n">
         <f aca="false">Regular_Timings!AT35/AT35</f>
         <v>3.49118750571466</v>
+      </c>
+      <c r="AU36" s="52" t="n">
+        <f aca="false">Regular_Timings!AU35/AU35</f>
+        <v>3.44024755453769</v>
+      </c>
+      <c r="AV36" s="52" t="n">
+        <f aca="false">Regular_Timings!AV35/AV35</f>
+        <v>3.56256025339363</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12682,7 +12826,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AC38" s="53" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -12721,7 +12865,7 @@
         <v>54</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>44</v>
@@ -12750,200 +12894,200 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="Q3" s="54" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="AF3" s="0" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="AJ3" s="0" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
- Updated timings for 9/19/2021
</commit_message>
<xml_diff>
--- a/doc/Perl6 Projects Line Counts.xlsx
+++ b/doc/Perl6 Projects Line Counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -1380,13 +1380,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>738360</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>186480</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1399,7 +1399,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="738360" y="10476360"/>
+          <a:off x="738360" y="10476720"/>
           <a:ext cx="9703800" cy="2053800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1415,15 +1415,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>24480</xdr:colOff>
+      <xdr:colOff>24840</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>30240</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>65520</xdr:colOff>
+      <xdr:colOff>65880</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>44280</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1436,7 +1436,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2235240" y="12926880"/>
+          <a:off x="2235600" y="12927240"/>
           <a:ext cx="9486720" cy="2117160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1452,13 +1452,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>24480</xdr:colOff>
+      <xdr:colOff>24840</xdr:colOff>
       <xdr:row>89</xdr:row>
       <xdr:rowOff>15480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>30960</xdr:colOff>
+      <xdr:colOff>31320</xdr:colOff>
       <xdr:row>100</xdr:row>
       <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
@@ -1473,7 +1473,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2235240" y="15541200"/>
+          <a:off x="2235600" y="15541200"/>
           <a:ext cx="9452160" cy="1995840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1489,15 +1489,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>24480</xdr:colOff>
+      <xdr:colOff>24840</xdr:colOff>
       <xdr:row>102</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>635400</xdr:colOff>
+      <xdr:colOff>635760</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1510,7 +1510,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2235240" y="17837280"/>
+          <a:off x="2235600" y="17837640"/>
           <a:ext cx="9294840" cy="2612880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1526,15 +1526,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>24120</xdr:colOff>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>120</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>588600</xdr:colOff>
+      <xdr:colOff>588960</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1547,7 +1547,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2234880" y="20991960"/>
+          <a:off x="2235240" y="20992320"/>
           <a:ext cx="9248400" cy="2329920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1563,13 +1563,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>53640</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>136</xdr:row>
       <xdr:rowOff>8640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>613440</xdr:colOff>
+      <xdr:colOff>613800</xdr:colOff>
       <xdr:row>148</xdr:row>
       <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
@@ -1584,7 +1584,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2264400" y="23771520"/>
+          <a:off x="2264760" y="23771520"/>
           <a:ext cx="9243720" cy="2110320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1600,15 +1600,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>21600</xdr:colOff>
+      <xdr:colOff>21960</xdr:colOff>
       <xdr:row>150</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
+      <xdr:colOff>259200</xdr:colOff>
       <xdr:row>162</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1621,7 +1621,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2232360" y="26249760"/>
+          <a:off x="2232720" y="26250120"/>
           <a:ext cx="9682920" cy="2109240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1639,13 +1639,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
       <xdr:row>180</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>309600</xdr:colOff>
       <xdr:row>192</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1658,7 +1658,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3115080" y="31513680"/>
+          <a:off x="3115080" y="31514040"/>
           <a:ext cx="9708120" cy="2138400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1713,13 +1713,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>209880</xdr:colOff>
       <xdr:row>194</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>333720</xdr:colOff>
       <xdr:row>207</xdr:row>
-      <xdr:rowOff>82800</xdr:rowOff>
+      <xdr:rowOff>83160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1732,7 +1732,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3059640" y="34097760"/>
+          <a:off x="3059640" y="34098120"/>
           <a:ext cx="9787680" cy="2191320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2987,11 +2987,11 @@
       </c>
       <c r="P6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C6:NC6&lt;&gt;""),Regular_Timings!C6:NC6)</f>
-        <v>754.52</v>
+        <v>766.8</v>
       </c>
       <c r="Q6" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D6:ND6&lt;&gt;""),Parallel_Timings!D6:ND6)</f>
-        <v>205.40968</v>
+        <v>229.41247</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3006,11 +3006,11 @@
       </c>
       <c r="P7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C7:NC7&lt;&gt;""),Regular_Timings!C7:NC7)</f>
-        <v>214.99</v>
+        <v>223.46</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D7:ND7&lt;&gt;""),Parallel_Timings!D7:ND7)</f>
-        <v>87.29099</v>
+        <v>99.46526</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3025,11 +3025,11 @@
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C8:NC8&lt;&gt;""),Regular_Timings!C8:NC8)</f>
-        <v>294.56</v>
+        <v>309.07</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D8:ND8&lt;&gt;""),Parallel_Timings!D8:ND8)</f>
-        <v>88.54707</v>
+        <v>100.1719</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,11 +3049,11 @@
       </c>
       <c r="P9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C9:NC9&lt;&gt;""),Regular_Timings!C9:NC9)</f>
-        <v>1641.63</v>
+        <v>1673.78</v>
       </c>
       <c r="Q9" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D9:ND9&lt;&gt;""),Parallel_Timings!D9:ND9)</f>
-        <v>398.5639</v>
+        <v>438.20262</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3069,11 +3069,11 @@
       <c r="O10" s="4"/>
       <c r="P10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C10:NC10&lt;&gt;""),Regular_Timings!C10:NC10)</f>
-        <v>159.17</v>
+        <v>169.18</v>
       </c>
       <c r="Q10" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D10:ND10&lt;&gt;""),Parallel_Timings!D10:ND10)</f>
-        <v>50.66426</v>
+        <v>55.67297</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3089,11 +3089,11 @@
       <c r="O11" s="4"/>
       <c r="P11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!C11:NC11&lt;&gt;""),Parallel_Timings!C11:NC11)</f>
-        <v>141.3976</v>
+        <v>152.34697</v>
       </c>
       <c r="Q11" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D11:ND11&lt;&gt;""),Parallel_Timings!D11:ND11)</f>
-        <v>141.3976</v>
+        <v>152.34697</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3109,11 +3109,11 @@
       <c r="O12" s="4"/>
       <c r="P12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C12:NC12&lt;&gt;""),Regular_Timings!C12:NC12)</f>
-        <v>112.9</v>
+        <v>117.53</v>
       </c>
       <c r="Q12" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D12:ND12&lt;&gt;""),Parallel_Timings!D12:ND12)</f>
-        <v>44.7714</v>
+        <v>49.49824</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3129,11 +3129,11 @@
       <c r="O13" s="4"/>
       <c r="P13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C13:NC13&lt;&gt;""),Regular_Timings!C13:NC13)</f>
-        <v>606.02</v>
+        <v>630.2</v>
       </c>
       <c r="Q13" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D13:ND13&lt;&gt;""),Parallel_Timings!D13:ND13)</f>
-        <v>157.88911</v>
+        <v>174.40043</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,11 +3153,11 @@
       </c>
       <c r="P14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C14:NC14&lt;&gt;""),Regular_Timings!C14:NC14)</f>
-        <v>344.28</v>
+        <v>360.3</v>
       </c>
       <c r="Q14" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D14:ND14&lt;&gt;""),Parallel_Timings!D14:ND14)</f>
-        <v>119.24336</v>
+        <v>134.84069</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3173,11 +3173,11 @@
       </c>
       <c r="P15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C15:NC15&lt;&gt;""),Regular_Timings!C15:NC15)</f>
-        <v>425.22</v>
+        <v>447.45</v>
       </c>
       <c r="Q15" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D15:ND15&lt;&gt;""),Parallel_Timings!D15:ND15)</f>
-        <v>138.78989</v>
+        <v>156.21393</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,11 +3196,11 @@
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C16:NC16&lt;&gt;""),Regular_Timings!C16:NC16)</f>
-        <v>2770.42</v>
+        <v>2894.6</v>
       </c>
       <c r="Q16" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D16:ND16&lt;&gt;""),Parallel_Timings!D16:ND16)</f>
-        <v>702.72608</v>
+        <v>756.15061</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3215,11 +3215,11 @@
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C17:NC17&lt;&gt;""),Regular_Timings!C17:NC17)</f>
-        <v>250.75</v>
+        <v>260.14</v>
       </c>
       <c r="Q17" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D17:ND17&lt;&gt;""),Parallel_Timings!D17:ND17)</f>
-        <v>56.91452</v>
+        <v>62.61951</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3234,11 +3234,11 @@
       </c>
       <c r="P18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C18:NC18&lt;&gt;""),Regular_Timings!C18:NC18)</f>
-        <v>691.04</v>
+        <v>716.91</v>
       </c>
       <c r="Q18" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D18:ND18&lt;&gt;""),Parallel_Timings!D18:ND18)</f>
-        <v>200.34936</v>
+        <v>214.81789</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3257,11 +3257,11 @@
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C19:NC19&lt;&gt;""),Regular_Timings!C19:NC19)</f>
-        <v>843.51</v>
+        <v>879.33</v>
       </c>
       <c r="Q19" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D19:ND19&lt;&gt;""),Parallel_Timings!D19:ND19)</f>
-        <v>234.65922</v>
+        <v>253.92047</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,11 +3276,11 @@
       </c>
       <c r="P20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C20:NC20&lt;&gt;""),Regular_Timings!C20:NC20)</f>
-        <v>138.07</v>
+        <v>143.49</v>
       </c>
       <c r="Q20" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D20:ND20&lt;&gt;""),Parallel_Timings!D20:ND20)</f>
-        <v>57.39666</v>
+        <v>63.37292</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3295,11 +3295,11 @@
       </c>
       <c r="P21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C21:NC21&lt;&gt;""),Regular_Timings!C21:NC21)</f>
-        <v>471.94</v>
+        <v>494.31</v>
       </c>
       <c r="Q21" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D21:ND21&lt;&gt;""),Parallel_Timings!D21:ND21)</f>
-        <v>155.16865</v>
+        <v>173.97629</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3314,11 +3314,11 @@
       </c>
       <c r="P22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C22:NC22&lt;&gt;""),Regular_Timings!C22:NC22)</f>
-        <v>426.63</v>
+        <v>446.43</v>
       </c>
       <c r="Q22" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D22:ND22&lt;&gt;""),Parallel_Timings!D22:ND22)</f>
-        <v>134.23404</v>
+        <v>149.31761</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="P23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C23:NC23&lt;&gt;""),Regular_Timings!C23:NC23)</f>
-        <v>264.97</v>
+        <v>276.46</v>
       </c>
       <c r="Q23" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D23:ND23&lt;&gt;""),Parallel_Timings!D23:ND23)</f>
-        <v>98.32562</v>
+        <v>108.48016</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3352,11 +3352,11 @@
       </c>
       <c r="P24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C24:NC24&lt;&gt;""),Regular_Timings!C24:NC24)</f>
-        <v>288.62</v>
+        <v>303.18</v>
       </c>
       <c r="Q24" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D24:ND24&lt;&gt;""),Parallel_Timings!D24:ND24)</f>
-        <v>90.04957</v>
+        <v>98.59967</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3372,11 +3372,11 @@
       <c r="O25" s="1"/>
       <c r="P25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C25:NC25&lt;&gt;""),Regular_Timings!C25:NC25)</f>
-        <v>341.36</v>
+        <v>361.36</v>
       </c>
       <c r="Q25" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D25:ND25&lt;&gt;""),Parallel_Timings!D25:ND25)</f>
-        <v>99.55833</v>
+        <v>106.70906</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3391,11 +3391,11 @@
       </c>
       <c r="P26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C26:NC26&lt;&gt;""),Regular_Timings!C26:NC26)</f>
-        <v>831.34</v>
+        <v>870.57</v>
       </c>
       <c r="Q26" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D26:ND26&lt;&gt;""),Parallel_Timings!D26:ND26)</f>
-        <v>253.4455</v>
+        <v>275.35122</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,11 +3410,11 @@
       </c>
       <c r="P27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C27:NC27&lt;&gt;""),Regular_Timings!C27:NC27)</f>
-        <v>184.31</v>
+        <v>194.36</v>
       </c>
       <c r="Q27" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D27:ND27&lt;&gt;""),Parallel_Timings!D27:ND27)</f>
-        <v>53.8565</v>
+        <v>59.38946</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,11 +3429,11 @@
       </c>
       <c r="P28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C28:NC28&lt;&gt;""),Regular_Timings!C28:NC28)</f>
-        <v>433.6</v>
+        <v>461.55</v>
       </c>
       <c r="Q28" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D28:ND28&lt;&gt;""),Parallel_Timings!D28:ND28)</f>
-        <v>128.04166</v>
+        <v>142.65758</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3452,11 +3452,11 @@
       </c>
       <c r="P29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C29:NC29&lt;&gt;""),Regular_Timings!C29:NC29)</f>
-        <v>1767.51</v>
+        <v>1857.39</v>
       </c>
       <c r="Q29" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D29:ND29&lt;&gt;""),Parallel_Timings!D29:ND29)</f>
-        <v>474.37795</v>
+        <v>532.41282</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3471,11 +3471,11 @@
       </c>
       <c r="P30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C30:NC30&lt;&gt;""),Regular_Timings!C30:NC30)</f>
-        <v>45.15</v>
+        <v>48.14</v>
       </c>
       <c r="Q30" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D30:ND30&lt;&gt;""),Parallel_Timings!D30:ND30)</f>
-        <v>21.95764</v>
+        <v>24.95392</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3490,11 +3490,11 @@
       </c>
       <c r="P31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C31:NC31&lt;&gt;""),Regular_Timings!C31:NC31)</f>
-        <v>32.52</v>
+        <v>34.56</v>
       </c>
       <c r="Q31" s="0" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D31:ND31&lt;&gt;""),Parallel_Timings!D31:ND31)</f>
-        <v>24.4971</v>
+        <v>28.04647</v>
       </c>
     </row>
     <row r="32" s="9" customFormat="true" ht="12.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3509,11 +3509,11 @@
       </c>
       <c r="P32" s="10" t="n">
         <f aca="false">LOOKUP(2,1/(Regular_Timings!C32:NC32&lt;&gt;""),Regular_Timings!C32:NC32)</f>
-        <v>167.71</v>
+        <v>178.03</v>
       </c>
       <c r="Q32" s="10" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D32:ND32&lt;&gt;""),Parallel_Timings!D32:ND32)</f>
-        <v>59.25021</v>
+        <v>65.87584</v>
       </c>
       <c r="R32" s="10"/>
     </row>
@@ -3700,11 +3700,11 @@
       </c>
       <c r="P54" s="0" t="n">
         <f aca="false">INDEX(Regular_Timings!35:35,COUNT(Regular_Timings!35:35,1,1))</f>
-        <v>16123.04</v>
+        <v>16749.57</v>
       </c>
       <c r="Q54" s="17" t="n">
         <f aca="false">LOOKUP(2,1/(Parallel_Timings!D35:ND35&lt;&gt;""),Parallel_Timings!D35:ND35)</f>
-        <v>4525.68907</v>
+        <v>4981.28445</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3719,7 +3719,7 @@
       </c>
       <c r="Q55" s="18" t="n">
         <f aca="false">P54/Q54</f>
-        <v>3.56256025339363</v>
+        <v>3.36250020815414</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3984,12 +3984,12 @@
   </sheetPr>
   <dimension ref="A2:BK109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="AR5" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="AR17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="AR1" activeCellId="0" sqref="AR1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AU4" activeCellId="0" sqref="AU4"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="AY3" activeCellId="0" sqref="AY3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4152,6 +4152,9 @@
       </c>
       <c r="AV4" s="26" t="n">
         <v>44451</v>
+      </c>
+      <c r="AW4" s="26" t="n">
+        <v>44458</v>
       </c>
     </row>
     <row r="5" s="29" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4244,6 +4247,9 @@
       <c r="AV5" s="0" t="n">
         <v>1144.68</v>
       </c>
+      <c r="AW5" s="0" t="n">
+        <v>1131.51</v>
+      </c>
     </row>
     <row r="6" s="11" customFormat="true" ht="12.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="35" t="s">
@@ -4386,6 +4392,9 @@
       <c r="AV6" s="0" t="n">
         <v>754.52</v>
       </c>
+      <c r="AW6" s="0" t="n">
+        <v>766.8</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="37" t="s">
@@ -4529,6 +4538,9 @@
       <c r="AV7" s="0" t="n">
         <v>214.99</v>
       </c>
+      <c r="AW7" s="0" t="n">
+        <v>223.46</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="37" t="s">
@@ -4660,6 +4672,9 @@
       <c r="AV8" s="0" t="n">
         <v>294.56</v>
       </c>
+      <c r="AW8" s="0" t="n">
+        <v>309.07</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38" t="s">
@@ -4803,6 +4818,9 @@
       <c r="AV9" s="0" t="n">
         <v>1641.63</v>
       </c>
+      <c r="AW9" s="0" t="n">
+        <v>1673.78</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="37" t="s">
@@ -4946,6 +4964,9 @@
       <c r="AV10" s="0" t="n">
         <v>159.17</v>
       </c>
+      <c r="AW10" s="0" t="n">
+        <v>169.18</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="37" t="s">
@@ -5089,6 +5110,9 @@
       <c r="AV11" s="0" t="n">
         <v>475.62</v>
       </c>
+      <c r="AW11" s="0" t="n">
+        <v>499.48</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="37" t="s">
@@ -5205,6 +5229,9 @@
       <c r="AV12" s="0" t="n">
         <v>112.9</v>
       </c>
+      <c r="AW12" s="0" t="n">
+        <v>117.53</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="37" t="s">
@@ -5309,6 +5336,9 @@
       <c r="AV13" s="0" t="n">
         <v>606.02</v>
       </c>
+      <c r="AW13" s="0" t="n">
+        <v>630.2</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38" t="s">
@@ -5452,6 +5482,9 @@
       <c r="AV14" s="0" t="n">
         <v>344.28</v>
       </c>
+      <c r="AW14" s="0" t="n">
+        <v>360.3</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38" t="s">
@@ -5595,6 +5628,9 @@
       <c r="AV15" s="0" t="n">
         <v>425.22</v>
       </c>
+      <c r="AW15" s="0" t="n">
+        <v>447.45</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38" t="s">
@@ -5738,6 +5774,9 @@
       <c r="AV16" s="0" t="n">
         <v>2770.42</v>
       </c>
+      <c r="AW16" s="0" t="n">
+        <v>2894.6</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38" t="s">
@@ -5800,6 +5839,9 @@
       <c r="AV17" s="0" t="n">
         <v>250.75</v>
       </c>
+      <c r="AW17" s="0" t="n">
+        <v>260.14</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38" t="s">
@@ -5943,6 +5985,9 @@
       <c r="AV18" s="0" t="n">
         <v>691.04</v>
       </c>
+      <c r="AW18" s="0" t="n">
+        <v>716.91</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38" t="s">
@@ -6086,6 +6131,9 @@
       <c r="AV19" s="0" t="n">
         <v>843.51</v>
       </c>
+      <c r="AW19" s="0" t="n">
+        <v>879.33</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38" t="s">
@@ -6229,6 +6277,9 @@
       <c r="AV20" s="0" t="n">
         <v>138.07</v>
       </c>
+      <c r="AW20" s="0" t="n">
+        <v>143.49</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38" t="s">
@@ -6372,6 +6423,9 @@
       <c r="AV21" s="0" t="n">
         <v>471.94</v>
       </c>
+      <c r="AW21" s="0" t="n">
+        <v>494.31</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="38" t="s">
@@ -6515,6 +6569,9 @@
       <c r="AV22" s="0" t="n">
         <v>426.63</v>
       </c>
+      <c r="AW22" s="0" t="n">
+        <v>446.43</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="38" t="s">
@@ -6658,6 +6715,9 @@
       <c r="AV23" s="0" t="n">
         <v>264.97</v>
       </c>
+      <c r="AW23" s="0" t="n">
+        <v>276.46</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="38" t="s">
@@ -6801,6 +6861,9 @@
       <c r="AV24" s="0" t="n">
         <v>288.62</v>
       </c>
+      <c r="AW24" s="0" t="n">
+        <v>303.18</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="38" t="s">
@@ -6944,6 +7007,9 @@
       <c r="AV25" s="0" t="n">
         <v>341.36</v>
       </c>
+      <c r="AW25" s="0" t="n">
+        <v>361.36</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
@@ -7087,6 +7153,9 @@
       <c r="AV26" s="0" t="n">
         <v>831.34</v>
       </c>
+      <c r="AW26" s="0" t="n">
+        <v>870.57</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="38" t="s">
@@ -7230,6 +7299,9 @@
       <c r="AV27" s="0" t="n">
         <v>184.31</v>
       </c>
+      <c r="AW27" s="0" t="n">
+        <v>194.36</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="38" t="s">
@@ -7319,6 +7391,9 @@
       <c r="AV28" s="0" t="n">
         <v>433.6</v>
       </c>
+      <c r="AW28" s="0" t="n">
+        <v>461.55</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="38" t="s">
@@ -7462,6 +7537,9 @@
       <c r="AV29" s="0" t="n">
         <v>1767.51</v>
       </c>
+      <c r="AW29" s="0" t="n">
+        <v>1857.39</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="38" t="s">
@@ -7605,6 +7683,9 @@
       <c r="AV30" s="0" t="n">
         <v>45.15</v>
       </c>
+      <c r="AW30" s="0" t="n">
+        <v>48.14</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="37" t="s">
@@ -7748,6 +7829,9 @@
       <c r="AV31" s="0" t="n">
         <v>32.52</v>
       </c>
+      <c r="AW31" s="0" t="n">
+        <v>34.56</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="37" t="s">
@@ -7891,6 +7975,9 @@
       <c r="AV32" s="0" t="n">
         <v>167.71</v>
       </c>
+      <c r="AW32" s="0" t="n">
+        <v>178.03</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="37" t="s">
@@ -8084,6 +8171,10 @@
       <c r="AV35" s="0" t="n">
         <f aca="false">SUM(AV$5:AV$32)</f>
         <v>16123.04</v>
+      </c>
+      <c r="AW35" s="0" t="n">
+        <f aca="false">SUM(AW$5:AW$32)</f>
+        <v>16749.57</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8270,6 +8361,10 @@
       <c r="AV36" s="41" t="n">
         <f aca="false">AV35/AU35</f>
         <v>1.00107974530677</v>
+      </c>
+      <c r="AW36" s="41" t="n">
+        <f aca="false">AW35/AV35</f>
+        <v>1.03885929700602</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8622,14 +8717,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:AV38"/>
+  <dimension ref="A2:AW38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="AM11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="AM1" activeCellId="0" sqref="AM1"/>
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="AU30" activeCellId="0" sqref="AU30"/>
+      <selection pane="bottomRight" activeCell="AW39" activeCellId="0" sqref="AW39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8788,6 +8883,9 @@
       </c>
       <c r="AV4" s="26" t="n">
         <v>44451</v>
+      </c>
+      <c r="AW4" s="26" t="n">
+        <v>44458</v>
       </c>
     </row>
     <row r="5" s="51" customFormat="true" ht="14.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8878,6 +8976,9 @@
       <c r="AV5" s="0" t="n">
         <v>248.3132</v>
       </c>
+      <c r="AW5" s="0" t="n">
+        <v>274.40747</v>
+      </c>
     </row>
     <row r="6" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -9019,6 +9120,9 @@
       <c r="AV6" s="0" t="n">
         <v>205.40968</v>
       </c>
+      <c r="AW6" s="0" t="n">
+        <v>229.41247</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="37" t="s">
@@ -9159,6 +9263,9 @@
       <c r="AV7" s="0" t="n">
         <v>87.29099</v>
       </c>
+      <c r="AW7" s="0" t="n">
+        <v>99.46526</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="37" t="s">
@@ -9287,6 +9394,9 @@
       <c r="AV8" s="0" t="n">
         <v>88.54707</v>
       </c>
+      <c r="AW8" s="0" t="n">
+        <v>100.1719</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="38" t="s">
@@ -9427,6 +9537,9 @@
       <c r="AV9" s="0" t="n">
         <v>398.5639</v>
       </c>
+      <c r="AW9" s="0" t="n">
+        <v>438.20262</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="37" t="s">
@@ -9567,6 +9680,9 @@
       <c r="AV10" s="0" t="n">
         <v>50.66426</v>
       </c>
+      <c r="AW10" s="0" t="n">
+        <v>55.67297</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="37" t="s">
@@ -9707,6 +9823,9 @@
       <c r="AV11" s="0" t="n">
         <v>141.3976</v>
       </c>
+      <c r="AW11" s="0" t="n">
+        <v>152.34697</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="37" t="s">
@@ -9820,6 +9939,9 @@
       <c r="AV12" s="0" t="n">
         <v>44.7714</v>
       </c>
+      <c r="AW12" s="0" t="n">
+        <v>49.49824</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="37" t="s">
@@ -9921,6 +10043,9 @@
       <c r="AV13" s="0" t="n">
         <v>157.88911</v>
       </c>
+      <c r="AW13" s="0" t="n">
+        <v>174.40043</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="38" t="s">
@@ -10061,6 +10186,9 @@
       <c r="AV14" s="0" t="n">
         <v>119.24336</v>
       </c>
+      <c r="AW14" s="0" t="n">
+        <v>134.84069</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="38" t="s">
@@ -10201,6 +10329,9 @@
       <c r="AV15" s="0" t="n">
         <v>138.78989</v>
       </c>
+      <c r="AW15" s="0" t="n">
+        <v>156.21393</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="38" t="s">
@@ -10341,6 +10472,9 @@
       <c r="AV16" s="0" t="n">
         <v>702.72608</v>
       </c>
+      <c r="AW16" s="0" t="n">
+        <v>756.15061</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="38" t="s">
@@ -10397,6 +10531,9 @@
       <c r="AV17" s="0" t="n">
         <v>56.91452</v>
       </c>
+      <c r="AW17" s="0" t="n">
+        <v>62.61951</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="38" t="s">
@@ -10537,6 +10674,9 @@
       <c r="AV18" s="0" t="n">
         <v>200.34936</v>
       </c>
+      <c r="AW18" s="0" t="n">
+        <v>214.81789</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="38" t="s">
@@ -10677,6 +10817,9 @@
       <c r="AV19" s="0" t="n">
         <v>234.65922</v>
       </c>
+      <c r="AW19" s="0" t="n">
+        <v>253.92047</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="38" t="s">
@@ -10817,6 +10960,9 @@
       <c r="AV20" s="0" t="n">
         <v>57.39666</v>
       </c>
+      <c r="AW20" s="0" t="n">
+        <v>63.37292</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="38" t="s">
@@ -10957,6 +11103,9 @@
       <c r="AV21" s="0" t="n">
         <v>155.16865</v>
       </c>
+      <c r="AW21" s="0" t="n">
+        <v>173.97629</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="38" t="s">
@@ -11097,6 +11246,9 @@
       <c r="AV22" s="0" t="n">
         <v>134.23404</v>
       </c>
+      <c r="AW22" s="0" t="n">
+        <v>149.31761</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="38" t="s">
@@ -11237,6 +11389,9 @@
       <c r="AV23" s="0" t="n">
         <v>98.32562</v>
       </c>
+      <c r="AW23" s="0" t="n">
+        <v>108.48016</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="38" t="s">
@@ -11377,6 +11532,9 @@
       <c r="AV24" s="0" t="n">
         <v>90.04957</v>
       </c>
+      <c r="AW24" s="0" t="n">
+        <v>98.59967</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="38" t="s">
@@ -11517,6 +11675,9 @@
       <c r="AV25" s="0" t="n">
         <v>99.55833</v>
       </c>
+      <c r="AW25" s="0" t="n">
+        <v>106.70906</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="40" t="s">
@@ -11657,6 +11818,9 @@
       <c r="AV26" s="0" t="n">
         <v>253.4455</v>
       </c>
+      <c r="AW26" s="0" t="n">
+        <v>275.35122</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="38" t="s">
@@ -11797,6 +11961,9 @@
       <c r="AV27" s="0" t="n">
         <v>53.8565</v>
       </c>
+      <c r="AW27" s="0" t="n">
+        <v>59.38946</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="38" t="s">
@@ -11883,6 +12050,9 @@
       <c r="AV28" s="0" t="n">
         <v>128.04166</v>
       </c>
+      <c r="AW28" s="0" t="n">
+        <v>142.65758</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="38" t="s">
@@ -12023,6 +12193,9 @@
       <c r="AV29" s="0" t="n">
         <v>474.37795</v>
       </c>
+      <c r="AW29" s="0" t="n">
+        <v>532.41282</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="38" t="s">
@@ -12163,6 +12336,9 @@
       <c r="AV30" s="0" t="n">
         <v>21.95764</v>
       </c>
+      <c r="AW30" s="0" t="n">
+        <v>24.95392</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="37" t="s">
@@ -12303,6 +12479,9 @@
       <c r="AV31" s="0" t="n">
         <v>24.4971</v>
       </c>
+      <c r="AW31" s="0" t="n">
+        <v>28.04647</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="37" t="s">
@@ -12443,6 +12622,9 @@
       <c r="AV32" s="0" t="n">
         <v>59.25021</v>
       </c>
+      <c r="AW32" s="0" t="n">
+        <v>65.87584</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="37" t="s">
@@ -12633,6 +12815,10 @@
         <f aca="false">SUM(AV$5:AV$32)</f>
         <v>4525.68907</v>
       </c>
+      <c r="AW35" s="0" t="n">
+        <f aca="false">SUM(AW$5:AW$32)</f>
+        <v>4981.28445</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
@@ -12817,6 +13003,10 @@
       <c r="AV36" s="52" t="n">
         <f aca="false">Regular_Timings!AV35/AV35</f>
         <v>3.56256025339363</v>
+      </c>
+      <c r="AW36" s="52" t="n">
+        <f aca="false">Regular_Timings!AW35/AW35</f>
+        <v>3.36250020815414</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>